<commit_message>
Update automatico via Actualizar 06-07-2020 18-03-41
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23005"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1270" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E04AA15-DA51-43E8-8DBD-DC637BF26940}"/>
+  <xr:revisionPtr revIDLastSave="1287" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77CD62FD-F3CB-416D-B6D5-27AB2A4B6090}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -116,7 +116,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -137,11 +137,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -151,6 +162,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,8 +226,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C89" totalsRowShown="0">
-  <autoFilter ref="A1:C89" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C90" totalsRowShown="0">
+  <autoFilter ref="A1:C90" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -227,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M90" totalsRowShown="0">
-  <autoFilter ref="A1:M90" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M91" totalsRowShown="0">
+  <autoFilter ref="A1:M91" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -253,8 +266,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C89" totalsRowShown="0">
-  <autoFilter ref="A1:C89" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C90" totalsRowShown="0">
+  <autoFilter ref="A1:C90" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -563,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC93"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3189,7 +3202,16 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="1"/>
+      <c r="A90" s="4">
+        <v>43988</v>
+      </c>
+      <c r="B90">
+        <v>10118</v>
+      </c>
+      <c r="C90">
+        <f>B90-B89</f>
+        <v>399</v>
+      </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1"/>
@@ -3213,11 +3235,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B82" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B91" sqref="B91"/>
+      <pane xSplit="1" topLeftCell="B81" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6914,10 +6936,62 @@
         <f>IFERROR(B90-B89,"")</f>
         <v>419</v>
       </c>
+      <c r="D90">
+        <v>205</v>
+      </c>
       <c r="E90" s="8">
         <f>C90-D90</f>
-        <v>419</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="F90">
+        <v>31</v>
+      </c>
+      <c r="G90">
+        <v>24</v>
+      </c>
+      <c r="H90">
+        <v>98</v>
+      </c>
+      <c r="I90">
+        <v>86</v>
+      </c>
+      <c r="J90">
+        <v>75</v>
+      </c>
+      <c r="K90">
+        <v>54</v>
+      </c>
+      <c r="L90">
+        <v>46</v>
+      </c>
+      <c r="M90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
+      <c r="A91" s="9">
+        <v>43988</v>
+      </c>
+      <c r="B91" s="6">
+        <v>16004</v>
+      </c>
+      <c r="C91" s="10">
+        <f>IFERROR(B91-B90,"")</f>
+        <v>541</v>
+      </c>
+      <c r="D91" s="6"/>
+      <c r="E91" s="10">
+        <f>C91-D91</f>
+        <v>541</v>
+      </c>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6929,10 +7003,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -7983,6 +8057,18 @@
         <v>7</v>
       </c>
     </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="4">
+        <v>43988</v>
+      </c>
+      <c r="B90">
+        <v>386</v>
+      </c>
+      <c r="C90">
+        <f>B90-B89</f>
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-08-2020 21-17-31
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1381" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AB90758-251A-4C9E-AEAC-8A164D4C6F01}"/>
+  <xr:revisionPtr revIDLastSave="1399" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{376670FD-B4FE-4B0A-8134-D31404E5131D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -3425,8 +3425,8 @@
   <dimension ref="A1:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="B83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -7166,19 +7166,37 @@
         <f>IFERROR(B91-B90,"")</f>
         <v>541</v>
       </c>
-      <c r="D91" s="6"/>
+      <c r="D91" s="6">
+        <v>255</v>
+      </c>
       <c r="E91" s="10">
         <f>C91-D91</f>
-        <v>541</v>
-      </c>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
-      <c r="H91" s="6"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="6"/>
-      <c r="K91" s="6"/>
-      <c r="L91" s="6"/>
-      <c r="M91" s="6"/>
+        <v>286</v>
+      </c>
+      <c r="F91" s="6">
+        <v>54</v>
+      </c>
+      <c r="G91" s="6">
+        <v>37</v>
+      </c>
+      <c r="H91" s="6">
+        <v>149</v>
+      </c>
+      <c r="I91" s="6">
+        <v>111</v>
+      </c>
+      <c r="J91" s="6">
+        <v>73</v>
+      </c>
+      <c r="K91" s="6">
+        <v>63</v>
+      </c>
+      <c r="L91" s="6">
+        <v>43</v>
+      </c>
+      <c r="M91" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="9">
@@ -7191,19 +7209,37 @@
         <f>IFERROR(B92-B91,"")</f>
         <v>421</v>
       </c>
-      <c r="D92" s="6"/>
+      <c r="D92" s="6">
+        <v>192</v>
+      </c>
       <c r="E92" s="10">
         <f>C92-D92</f>
-        <v>421</v>
-      </c>
-      <c r="F92" s="6"/>
-      <c r="G92" s="6"/>
-      <c r="H92" s="6"/>
-      <c r="I92" s="6"/>
-      <c r="J92" s="6"/>
-      <c r="K92" s="6"/>
-      <c r="L92" s="6"/>
-      <c r="M92" s="6"/>
+        <v>229</v>
+      </c>
+      <c r="F92" s="6">
+        <v>23</v>
+      </c>
+      <c r="G92" s="6">
+        <v>33</v>
+      </c>
+      <c r="H92" s="6">
+        <v>118</v>
+      </c>
+      <c r="I92" s="6">
+        <v>68</v>
+      </c>
+      <c r="J92" s="6">
+        <v>75</v>
+      </c>
+      <c r="K92" s="6">
+        <v>44</v>
+      </c>
+      <c r="L92" s="6">
+        <v>48</v>
+      </c>
+      <c r="M92" s="6">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-09-2020 05-18-14
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1399" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{376670FD-B4FE-4B0A-8134-D31404E5131D}"/>
+  <xr:revisionPtr revIDLastSave="1415" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E6D1CD1-4DBB-4AC8-BBFA-7AA2B418A971}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C91" totalsRowShown="0">
-  <autoFilter ref="A1:C91" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C92" totalsRowShown="0">
+  <autoFilter ref="A1:C92" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M92" totalsRowShown="0">
-  <autoFilter ref="A1:M92" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M93" totalsRowShown="0">
+  <autoFilter ref="A1:M93" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -375,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C91" totalsRowShown="0">
-  <autoFilter ref="A1:C91" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C92" totalsRowShown="0">
+  <autoFilter ref="A1:C92" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC93"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3404,7 +3404,16 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="1"/>
+      <c r="A92" s="4">
+        <v>43990</v>
+      </c>
+      <c r="B92">
+        <v>10401</v>
+      </c>
+      <c r="C92">
+        <f>B92-B91</f>
+        <v>183</v>
+      </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1"/>
@@ -3422,11 +3431,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N93" sqref="N93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -7241,6 +7250,49 @@
         <v>12</v>
       </c>
     </row>
+    <row r="93" spans="1:13">
+      <c r="A93" s="9">
+        <v>43990</v>
+      </c>
+      <c r="B93" s="6">
+        <v>16854</v>
+      </c>
+      <c r="C93" s="10">
+        <f>IFERROR(B93-B92,"")</f>
+        <v>429</v>
+      </c>
+      <c r="D93" s="6">
+        <v>181</v>
+      </c>
+      <c r="E93" s="10">
+        <f>C93-D93</f>
+        <v>248</v>
+      </c>
+      <c r="F93" s="6">
+        <v>22</v>
+      </c>
+      <c r="G93" s="6">
+        <v>34</v>
+      </c>
+      <c r="H93" s="6">
+        <v>125</v>
+      </c>
+      <c r="I93" s="6">
+        <v>86</v>
+      </c>
+      <c r="J93" s="6">
+        <v>71</v>
+      </c>
+      <c r="K93" s="6">
+        <v>40</v>
+      </c>
+      <c r="L93" s="6">
+        <v>42</v>
+      </c>
+      <c r="M93" s="6">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7251,10 +7303,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+      <selection activeCell="C91" sqref="C91:C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8327,6 +8379,18 @@
       <c r="C91">
         <f>B91-B90</f>
         <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="4">
+        <v>43990</v>
+      </c>
+      <c r="B92">
+        <v>398</v>
+      </c>
+      <c r="C92">
+        <f>B92-B91</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -15878,85 +15942,85 @@
       </c>
     </row>
     <row r="93" spans="1:20">
-      <c r="A93" s="4" t="str">
+      <c r="A93" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B93" t="str">
+        <v>43990</v>
+      </c>
+      <c r="B93">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C93" t="str">
+        <v>16854</v>
+      </c>
+      <c r="C93">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>429</v>
       </c>
       <c r="D93">
         <f>+IFERROR('Fallecidos Diarios'!B92,"")</f>
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="E93">
         <f>+IFERROR('Fallecidos Diarios'!C92,"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F93">
         <f>+IFERROR('Recuperados Diarios'!B92,"")</f>
-        <v>0</v>
+        <v>10401</v>
       </c>
       <c r="G93">
         <f>+IFERROR('Recuperados Diarios'!C92,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H93" t="str">
+        <v>183</v>
+      </c>
+      <c r="H93">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I93" t="str">
+        <v>6055</v>
+      </c>
+      <c r="I93">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J93" t="str">
+        <v>241</v>
+      </c>
+      <c r="J93">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K93" t="str">
+        <v>2.3614572208377833E-2</v>
+      </c>
+      <c r="K93">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L93" t="str">
+        <v>0.61712353150587396</v>
+      </c>
+      <c r="L93">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M93" t="str">
+        <v>0.35926189628574817</v>
+      </c>
+      <c r="M93">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N93" t="str">
+        <v>1194.114946325351</v>
+      </c>
+      <c r="N93">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O93" t="str">
+        <v>1.2562814070351759E-2</v>
+      </c>
+      <c r="O93">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P93" t="str">
+        <v>1.7594462070954716E-2</v>
+      </c>
+      <c r="P93">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q93" t="str">
+        <v>3.9801816680429397E-2</v>
+      </c>
+      <c r="Q93">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4052.4164462611207</v>
       </c>
       <c r="R93">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>95.696080788651116</v>
       </c>
       <c r="S93">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T93" t="str">
+        <v>2500.8415484491466</v>
+      </c>
+      <c r="T93">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1455.8788170233229</v>
       </c>
     </row>
     <row r="94" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-10-2020 03-53-05
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1415" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1E6D1CD1-4DBB-4AC8-BBFA-7AA2B418A971}"/>
+  <xr:revisionPtr revIDLastSave="1424" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF8423E4-9052-44C2-88F5-E9D335161A2B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C92" totalsRowShown="0">
-  <autoFilter ref="A1:C92" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C93" totalsRowShown="0">
+  <autoFilter ref="A1:C93" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M93" totalsRowShown="0">
-  <autoFilter ref="A1:M93" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M94" totalsRowShown="0">
+  <autoFilter ref="A1:M94" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -375,8 +375,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C92" totalsRowShown="0">
-  <autoFilter ref="A1:C92" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C93" totalsRowShown="0">
+  <autoFilter ref="A1:C93" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3416,7 +3416,16 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="1"/>
+      <c r="A93" s="4">
+        <v>43991</v>
+      </c>
+      <c r="B93">
+        <v>10561</v>
+      </c>
+      <c r="C93">
+        <f>B93-B92</f>
+        <v>160</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
@@ -3431,11 +3440,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N93" sqref="N93"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -7293,6 +7302,31 @@
         <v>9</v>
       </c>
     </row>
+    <row r="94" spans="1:13">
+      <c r="A94" s="9">
+        <v>43991</v>
+      </c>
+      <c r="B94" s="6">
+        <v>17233</v>
+      </c>
+      <c r="C94" s="10">
+        <f>IFERROR(B94-B93,"")</f>
+        <v>379</v>
+      </c>
+      <c r="D94" s="6"/>
+      <c r="E94" s="10">
+        <f>C94-D94</f>
+        <v>379</v>
+      </c>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7303,10 +7337,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91:C92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88:C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8353,7 +8387,7 @@
         <v>370</v>
       </c>
       <c r="C89">
-        <f>B89-B88</f>
+        <f t="shared" ref="C89:C93" si="0">B89-B88</f>
         <v>7</v>
       </c>
     </row>
@@ -8365,7 +8399,7 @@
         <v>386</v>
       </c>
       <c r="C90">
-        <f>B90-B89</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
@@ -8377,7 +8411,7 @@
         <v>393</v>
       </c>
       <c r="C91">
-        <f>B91-B90</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -8389,7 +8423,19 @@
         <v>398</v>
       </c>
       <c r="C92">
-        <f>B92-B91</f>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="4">
+        <v>43991</v>
+      </c>
+      <c r="B93">
+        <v>403</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -16024,85 +16070,85 @@
       </c>
     </row>
     <row r="94" spans="1:20">
-      <c r="A94" s="4" t="str">
+      <c r="A94" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B94" t="str">
+        <v>43991</v>
+      </c>
+      <c r="B94">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C94" t="str">
+        <v>17233</v>
+      </c>
+      <c r="C94">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>379</v>
       </c>
       <c r="D94">
         <f>+IFERROR('Fallecidos Diarios'!B93,"")</f>
-        <v>0</v>
+        <v>403</v>
       </c>
       <c r="E94">
         <f>+IFERROR('Fallecidos Diarios'!C93,"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F94">
         <f>+IFERROR('Recuperados Diarios'!B93,"")</f>
-        <v>0</v>
+        <v>10561</v>
       </c>
       <c r="G94">
         <f>+IFERROR('Recuperados Diarios'!C93,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H94" t="str">
+        <v>160</v>
+      </c>
+      <c r="H94">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I94" t="str">
+        <v>6269</v>
+      </c>
+      <c r="I94">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J94" t="str">
+        <v>214</v>
+      </c>
+      <c r="J94">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K94" t="str">
+        <v>2.3385365287529738E-2</v>
+      </c>
+      <c r="K94">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L94" t="str">
+        <v>0.61283583821737364</v>
+      </c>
+      <c r="L94">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M94" t="str">
+        <v>0.36377879649509659</v>
+      </c>
+      <c r="M94">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N94" t="str">
+        <v>1041.8419205614932</v>
+      </c>
+      <c r="N94">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O94" t="str">
+        <v>1.2406947890818859E-2</v>
+      </c>
+      <c r="O94">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P94" t="str">
+        <v>1.5150080484802576E-2</v>
+      </c>
+      <c r="P94">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q94" t="str">
+        <v>3.4136225873345034E-2</v>
+      </c>
+      <c r="Q94">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4143.5441211829766</v>
       </c>
       <c r="R94">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>96.898292858860302</v>
       </c>
       <c r="S94">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T94" t="str">
+        <v>2539.3123346958405</v>
+      </c>
+      <c r="T94">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1507.3334936282761</v>
       </c>
     </row>
     <row r="95" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-10-2020 15-54-26
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1424" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF8423E4-9052-44C2-88F5-E9D335161A2B}"/>
+  <xr:revisionPtr revIDLastSave="1478" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06CD8E72-2815-4506-AB0D-7CC1418B754C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC93"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -831,6 +831,12 @@
       <c r="A2" s="4">
         <v>43900</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -887,6 +893,12 @@
       <c r="A3" s="4">
         <v>43901</v>
       </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -943,6 +955,12 @@
       <c r="A4" s="4">
         <v>43902</v>
       </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -999,6 +1017,12 @@
       <c r="A5" s="4">
         <v>43903</v>
       </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1055,6 +1079,12 @@
       <c r="A6" s="4">
         <v>43904</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1111,6 +1141,12 @@
       <c r="A7" s="4">
         <v>43905</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1167,6 +1203,12 @@
       <c r="A8" s="4">
         <v>43906</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1223,6 +1265,12 @@
       <c r="A9" s="4">
         <v>43907</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1279,6 +1327,12 @@
       <c r="A10" s="4">
         <v>43908</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1335,6 +1389,13 @@
       <c r="A11" s="4">
         <v>43909</v>
       </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>B11-B10</f>
+        <v>1</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1391,6 +1452,13 @@
       <c r="A12" s="4">
         <v>43910</v>
       </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C35" si="0">B12-B11</f>
+        <v>0</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1447,6 +1515,13 @@
       <c r="A13" s="4">
         <v>43911</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1503,6 +1578,13 @@
       <c r="A14" s="4">
         <v>43912</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1559,6 +1641,13 @@
       <c r="A15" s="4">
         <v>43913</v>
       </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1615,6 +1704,13 @@
       <c r="A16" s="4">
         <v>43914</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1671,6 +1767,13 @@
       <c r="A17" s="4">
         <v>43915</v>
       </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1727,6 +1830,13 @@
       <c r="A18" s="4">
         <v>43916</v>
       </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1783,6 +1893,13 @@
       <c r="A19" s="4">
         <v>43917</v>
       </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1839,6 +1956,13 @@
       <c r="A20" s="4">
         <v>43918</v>
       </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1895,6 +2019,13 @@
       <c r="A21" s="4">
         <v>43919</v>
       </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1951,6 +2082,13 @@
       <c r="A22" s="4">
         <v>43920</v>
       </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2007,6 +2145,13 @@
       <c r="A23" s="4">
         <v>43921</v>
       </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -2063,6 +2208,13 @@
       <c r="A24" s="4">
         <v>43922</v>
       </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -2119,6 +2271,13 @@
       <c r="A25" s="4">
         <v>43923</v>
       </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -2175,6 +2334,13 @@
       <c r="A26" s="4">
         <v>43924</v>
       </c>
+      <c r="B26">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -2231,6 +2397,13 @@
       <c r="A27" s="4">
         <v>43925</v>
       </c>
+      <c r="B27">
+        <v>13</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -2287,6 +2460,13 @@
       <c r="A28" s="4">
         <v>43926</v>
       </c>
+      <c r="B28">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -2343,6 +2523,13 @@
       <c r="A29" s="4">
         <v>43927</v>
       </c>
+      <c r="B29">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -2399,6 +2586,13 @@
       <c r="A30" s="4">
         <v>43928</v>
       </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2455,6 +2649,13 @@
       <c r="A31" s="4">
         <v>43929</v>
       </c>
+      <c r="B31">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -2511,6 +2712,13 @@
       <c r="A32" s="4">
         <v>43930</v>
       </c>
+      <c r="B32">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -2567,6 +2775,13 @@
       <c r="A33" s="4">
         <v>43931</v>
       </c>
+      <c r="B33">
+        <v>17</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2623,6 +2838,13 @@
       <c r="A34" s="4">
         <v>43932</v>
       </c>
+      <c r="B34">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -2679,6 +2901,13 @@
       <c r="A35" s="4">
         <v>43933</v>
       </c>
+      <c r="B35">
+        <v>29</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -2763,7 +2992,7 @@
         <v>1884</v>
       </c>
       <c r="C38">
-        <f t="shared" ref="C38:C69" si="0">B38-B37</f>
+        <f t="shared" ref="C38:C69" si="1">B38-B37</f>
         <v>3</v>
       </c>
     </row>
@@ -2775,7 +3004,7 @@
         <v>1907</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
     </row>
@@ -2787,7 +3016,7 @@
         <v>1931</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
@@ -2799,7 +3028,7 @@
         <v>1949</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
@@ -2811,7 +3040,7 @@
         <v>1974</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
@@ -2823,7 +3052,7 @@
         <v>2013</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
     </row>
@@ -2835,7 +3064,7 @@
         <v>2040</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -2847,7 +3076,7 @@
         <v>2482</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>442</v>
       </c>
     </row>
@@ -2859,7 +3088,7 @@
         <v>2531</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
     </row>
@@ -2871,7 +3100,7 @@
         <v>2546</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
@@ -2883,7 +3112,7 @@
         <v>2762</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>216</v>
       </c>
     </row>
@@ -2895,7 +3124,7 @@
         <v>2824</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
     </row>
@@ -2907,7 +3136,7 @@
         <v>2910</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
@@ -2919,7 +3148,7 @@
         <v>2939</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
     </row>
@@ -2931,7 +3160,7 @@
         <v>3011</v>
       </c>
       <c r="C52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
     </row>
@@ -2943,7 +3172,7 @@
         <v>3060</v>
       </c>
       <c r="C53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
     </row>
@@ -2955,7 +3184,7 @@
         <v>3106</v>
       </c>
       <c r="C54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
@@ -2967,7 +3196,7 @@
         <v>3144</v>
       </c>
       <c r="C55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
     </row>
@@ -2979,7 +3208,7 @@
         <v>3144</v>
       </c>
       <c r="C56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2991,7 +3220,7 @@
         <v>3229</v>
       </c>
       <c r="C57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
@@ -3003,7 +3232,7 @@
         <v>4441</v>
       </c>
       <c r="C58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1212</v>
       </c>
     </row>
@@ -3015,7 +3244,7 @@
         <v>4477</v>
       </c>
       <c r="C59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
     </row>
@@ -3027,7 +3256,7 @@
         <v>4504</v>
       </c>
       <c r="C60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
     </row>
@@ -3039,7 +3268,7 @@
         <v>4500</v>
       </c>
       <c r="C61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-4</v>
       </c>
     </row>
@@ -3051,7 +3280,7 @@
         <v>4501</v>
       </c>
       <c r="C62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3063,7 +3292,7 @@
         <v>4687</v>
       </c>
       <c r="C63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
     </row>
@@ -3075,7 +3304,7 @@
         <v>4687</v>
       </c>
       <c r="C64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3087,7 +3316,7 @@
         <v>6021</v>
       </c>
       <c r="C65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1334</v>
       </c>
     </row>
@@ -3099,7 +3328,7 @@
         <v>6067</v>
       </c>
       <c r="C66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
@@ -3111,7 +3340,7 @@
         <v>6080</v>
       </c>
       <c r="C67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
@@ -3123,7 +3352,7 @@
         <v>6080</v>
       </c>
       <c r="C68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3135,7 +3364,7 @@
         <v>6081</v>
       </c>
       <c r="C69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3147,7 +3376,7 @@
         <v>6081</v>
       </c>
       <c r="C70">
-        <f t="shared" ref="C70:C88" si="1">B70-B69</f>
+        <f t="shared" ref="C70:C88" si="2">B70-B69</f>
         <v>0</v>
       </c>
     </row>
@@ -3159,7 +3388,7 @@
         <v>6085</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3171,7 +3400,7 @@
         <v>6194</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
     </row>
@@ -3183,7 +3412,7 @@
         <v>6194</v>
       </c>
       <c r="C73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3195,7 +3424,7 @@
         <v>6245</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
     </row>
@@ -3207,7 +3436,7 @@
         <v>6275</v>
       </c>
       <c r="C75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
     </row>
@@ -3219,7 +3448,7 @@
         <v>6279</v>
       </c>
       <c r="C76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -3231,7 +3460,7 @@
         <v>6279</v>
       </c>
       <c r="C77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3243,7 +3472,7 @@
         <v>6279</v>
       </c>
       <c r="C78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3255,7 +3484,7 @@
         <v>6379</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -3267,7 +3496,7 @@
         <v>7379</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
     </row>
@@ -3279,7 +3508,7 @@
         <v>7379</v>
       </c>
       <c r="C81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3291,7 +3520,7 @@
         <v>7540</v>
       </c>
       <c r="C82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>161</v>
       </c>
     </row>
@@ -3303,7 +3532,7 @@
         <v>9414</v>
       </c>
       <c r="C83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1874</v>
       </c>
     </row>
@@ -3315,7 +3544,7 @@
         <v>9514</v>
       </c>
       <c r="C84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -3327,7 +3556,7 @@
         <v>9514</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3339,7 +3568,7 @@
         <v>9514</v>
       </c>
       <c r="C86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -3351,7 +3580,7 @@
         <v>9519</v>
       </c>
       <c r="C87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -3363,7 +3592,7 @@
         <v>9619</v>
       </c>
       <c r="C88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
     </row>
@@ -3442,9 +3671,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -7313,19 +7542,37 @@
         <f>IFERROR(B94-B93,"")</f>
         <v>379</v>
       </c>
-      <c r="D94" s="6"/>
+      <c r="D94" s="6">
+        <v>164</v>
+      </c>
       <c r="E94" s="10">
         <f>C94-D94</f>
-        <v>379</v>
-      </c>
-      <c r="F94" s="6"/>
-      <c r="G94" s="6"/>
-      <c r="H94" s="6"/>
-      <c r="I94" s="6"/>
-      <c r="J94" s="6"/>
-      <c r="K94" s="6"/>
-      <c r="L94" s="6"/>
-      <c r="M94" s="6"/>
+        <v>215</v>
+      </c>
+      <c r="F94" s="6">
+        <v>15</v>
+      </c>
+      <c r="G94" s="6">
+        <v>17</v>
+      </c>
+      <c r="H94" s="6">
+        <v>102</v>
+      </c>
+      <c r="I94" s="6">
+        <v>78</v>
+      </c>
+      <c r="J94" s="6">
+        <v>71</v>
+      </c>
+      <c r="K94" s="6">
+        <v>56</v>
+      </c>
+      <c r="L94" s="6">
+        <v>35</v>
+      </c>
+      <c r="M94" s="6">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7339,7 +7586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView topLeftCell="A83" workbookViewId="0">
       <selection activeCell="C88" sqref="C88:C93"/>
     </sheetView>
   </sheetViews>
@@ -9368,19 +9615,19 @@
       </c>
       <c r="F12">
         <f>+IFERROR('Recuperados Diarios'!B11,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <f>+IFERROR('Recuperados Diarios'!C11,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I12">
         <f t="shared" si="12"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
@@ -9388,27 +9635,27 @@
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.2992700729927005E-3</v>
       </c>
       <c r="L12">
         <f t="shared" si="3"/>
-        <v>0.99270072992700731</v>
+        <v>0.98540145985401462</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>28.205882352941178</v>
+        <v>28.414814814814815</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O12" t="str">
+      <c r="O12">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="P12">
         <f t="shared" si="7"/>
-        <v>0.20588235294117646</v>
+        <v>0.2</v>
       </c>
       <c r="Q12">
         <f t="shared" si="8"/>
@@ -9420,11 +9667,11 @@
       </c>
       <c r="S12">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T12">
         <f t="shared" si="11"/>
-        <v>32.700168309689829</v>
+        <v>32.459725895647992</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -9450,7 +9697,7 @@
       </c>
       <c r="F13">
         <f>+IFERROR('Recuperados Diarios'!B12,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>+IFERROR('Recuperados Diarios'!C12,"")</f>
@@ -9458,7 +9705,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I13">
         <f t="shared" si="12"/>
@@ -9470,27 +9717,27 @@
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L13">
         <f t="shared" si="3"/>
-        <v>0.995</v>
+        <v>0.99</v>
       </c>
       <c r="M13">
         <f t="shared" si="4"/>
-        <v>63.316582914572862</v>
+        <v>63.63636363636364</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O13" t="str">
+      <c r="O13">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P13">
         <f t="shared" si="7"/>
-        <v>0.3165829145728643</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="Q13">
         <f t="shared" si="8"/>
@@ -9502,11 +9749,11 @@
       </c>
       <c r="S13">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T13">
         <f t="shared" si="11"/>
-        <v>47.848040394325558</v>
+        <v>47.607597980283721</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -9532,7 +9779,7 @@
       </c>
       <c r="F14">
         <f>+IFERROR('Recuperados Diarios'!B13,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f>+IFERROR('Recuperados Diarios'!C13,"")</f>
@@ -9540,7 +9787,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I14">
         <f t="shared" si="12"/>
@@ -9552,27 +9799,27 @@
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.0816326530612249E-3</v>
       </c>
       <c r="L14">
         <f t="shared" si="3"/>
-        <v>0.99591836734693873</v>
+        <v>0.99183673469387756</v>
       </c>
       <c r="M14">
         <f t="shared" si="4"/>
-        <v>45.184426229508198</v>
+        <v>45.370370370370367</v>
       </c>
       <c r="N14">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O14" t="str">
+      <c r="O14">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P14">
         <f t="shared" si="7"/>
-        <v>0.18442622950819673</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="Q14">
         <f t="shared" si="8"/>
@@ -9584,11 +9831,11 @@
       </c>
       <c r="S14">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T14">
         <f t="shared" si="11"/>
-        <v>58.667949026208227</v>
+        <v>58.42750661216639</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -9614,7 +9861,7 @@
       </c>
       <c r="F15">
         <f>+IFERROR('Recuperados Diarios'!B14,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <f>+IFERROR('Recuperados Diarios'!C14,"")</f>
@@ -9622,7 +9869,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I15">
         <f t="shared" si="12"/>
@@ -9634,27 +9881,27 @@
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.1948881789137379E-3</v>
       </c>
       <c r="L15">
         <f t="shared" si="3"/>
-        <v>0.99041533546325877</v>
+        <v>0.98722044728434499</v>
       </c>
       <c r="M15">
         <f t="shared" si="4"/>
-        <v>68.658064516129031</v>
+        <v>68.880258899676377</v>
       </c>
       <c r="N15">
         <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O15" t="str">
+      <c r="O15">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P15">
         <f t="shared" si="7"/>
-        <v>0.2129032258064516</v>
+        <v>0.21359223300970873</v>
       </c>
       <c r="Q15">
         <f t="shared" si="8"/>
@@ -9666,11 +9913,11 @@
       </c>
       <c r="S15">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T15">
         <f t="shared" si="11"/>
-        <v>74.537148352969467</v>
+        <v>74.29670593892763</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -9696,7 +9943,7 @@
       </c>
       <c r="F16">
         <f>+IFERROR('Recuperados Diarios'!B15,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
         <f>+IFERROR('Recuperados Diarios'!C15,"")</f>
@@ -9704,7 +9951,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I16">
         <f t="shared" si="12"/>
@@ -9716,27 +9963,27 @@
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.8985507246376812E-3</v>
       </c>
       <c r="L16">
         <f t="shared" si="3"/>
-        <v>0.9826086956521739</v>
+        <v>0.97971014492753628</v>
       </c>
       <c r="M16">
         <f t="shared" si="4"/>
-        <v>32.56637168141593</v>
+        <v>32.662721893491124</v>
       </c>
       <c r="N16">
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
-      <c r="O16" t="str">
+      <c r="O16">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P16">
         <f t="shared" si="7"/>
-        <v>8.5545722713864306E-2</v>
+        <v>8.5798816568047331E-2</v>
       </c>
       <c r="Q16">
         <f t="shared" si="8"/>
@@ -9748,11 +9995,11 @@
       </c>
       <c r="S16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T16">
         <f t="shared" si="11"/>
-        <v>81.509978360182743</v>
+        <v>81.269535946140905</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -9778,7 +10025,7 @@
       </c>
       <c r="F17">
         <f>+IFERROR('Recuperados Diarios'!B16,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <f>+IFERROR('Recuperados Diarios'!C16,"")</f>
@@ -9786,7 +10033,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I17">
         <f t="shared" si="12"/>
@@ -9798,27 +10045,27 @@
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.257336343115124E-3</v>
       </c>
       <c r="L17">
         <f t="shared" si="3"/>
-        <v>0.98645598194130923</v>
+        <v>0.98419864559819414</v>
       </c>
       <c r="M17">
         <f t="shared" si="4"/>
-        <v>99.345537757437071</v>
+        <v>99.573394495412842</v>
       </c>
       <c r="N17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O17" t="str">
+      <c r="O17">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P17">
         <f t="shared" si="7"/>
-        <v>0.22425629290617849</v>
+        <v>0.22477064220183487</v>
       </c>
       <c r="Q17">
         <f t="shared" si="8"/>
@@ -9830,11 +10077,11 @@
       </c>
       <c r="S17">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.240442414041837</v>
       </c>
       <c r="T17">
         <f t="shared" si="11"/>
-        <v>105.07333493628276</v>
+        <v>104.83289252224093</v>
       </c>
     </row>
     <row r="18" spans="1:20">
@@ -9860,19 +10107,19 @@
       </c>
       <c r="F18">
         <f>+IFERROR('Recuperados Diarios'!B17,"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18">
         <f>+IFERROR('Recuperados Diarios'!C17,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I18">
         <f t="shared" si="12"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
@@ -9880,27 +10127,27 @@
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.5842293906810036E-3</v>
       </c>
       <c r="L18">
         <f t="shared" si="3"/>
-        <v>0.98566308243727596</v>
+        <v>0.98207885304659504</v>
       </c>
       <c r="M18">
         <f t="shared" si="4"/>
-        <v>116.67272727272727</v>
+        <v>117.0985401459854</v>
       </c>
       <c r="N18">
         <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
-      <c r="O18" t="str">
+      <c r="O18">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="P18">
         <f t="shared" si="7"/>
-        <v>0.20545454545454545</v>
+        <v>0.20437956204379562</v>
       </c>
       <c r="Q18">
         <f t="shared" si="8"/>
@@ -9912,11 +10159,11 @@
       </c>
       <c r="S18">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.480884828083674</v>
       </c>
       <c r="T18">
         <f t="shared" si="11"/>
-        <v>132.24332772301034</v>
+        <v>131.76244289492666</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -9942,7 +10189,7 @@
       </c>
       <c r="F19">
         <f>+IFERROR('Recuperados Diarios'!B18,"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <f>+IFERROR('Recuperados Diarios'!C18,"")</f>
@@ -9950,7 +10197,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I19">
         <f t="shared" si="12"/>
@@ -9962,27 +10209,27 @@
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.967359050445104E-3</v>
       </c>
       <c r="L19">
         <f t="shared" si="3"/>
-        <v>0.98813056379821962</v>
+        <v>0.98516320474777452</v>
       </c>
       <c r="M19">
         <f t="shared" si="4"/>
-        <v>117.3933933933934</v>
+        <v>117.74698795180723</v>
       </c>
       <c r="N19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O19" t="str">
+      <c r="O19">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P19">
         <f t="shared" si="7"/>
-        <v>0.17417417417417416</v>
+        <v>0.1746987951807229</v>
       </c>
       <c r="Q19">
         <f t="shared" si="8"/>
@@ -9994,11 +10241,11 @@
       </c>
       <c r="S19">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.480884828083674</v>
       </c>
       <c r="T19">
         <f t="shared" si="11"/>
-        <v>160.13464775186344</v>
+        <v>159.65376292377977</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -10024,19 +10271,19 @@
       </c>
       <c r="F20">
         <f>+IFERROR('Recuperados Diarios'!B19,"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <f>+IFERROR('Recuperados Diarios'!C19,"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="I20">
         <f t="shared" si="12"/>
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
@@ -10044,27 +10291,27 @@
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.0890585241730284E-3</v>
       </c>
       <c r="L20">
         <f t="shared" si="3"/>
-        <v>0.98854961832061072</v>
+        <v>0.98346055979643765</v>
       </c>
       <c r="M20">
         <f t="shared" si="4"/>
-        <v>113.29729729729729</v>
+        <v>113.88357050452781</v>
       </c>
       <c r="N20">
         <f t="shared" si="5"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="O20" t="str">
+      <c r="O20">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="P20">
         <f t="shared" si="7"/>
-        <v>0.14285714285714285</v>
+        <v>0.14100905562742561</v>
       </c>
       <c r="Q20">
         <f t="shared" si="8"/>
@@ -10076,11 +10323,11 @@
       </c>
       <c r="S20">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.961769656167348</v>
       </c>
       <c r="T20">
         <f t="shared" si="11"/>
-        <v>186.82375571050736</v>
+        <v>185.86198605434001</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -10106,7 +10353,7 @@
       </c>
       <c r="F21">
         <f>+IFERROR('Recuperados Diarios'!B20,"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21">
         <f>+IFERROR('Recuperados Diarios'!C20,"")</f>
@@ -10114,7 +10361,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="0"/>
-        <v>887</v>
+        <v>883</v>
       </c>
       <c r="I21">
         <f t="shared" si="12"/>
@@ -10126,27 +10373,27 @@
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.4395116537180911E-3</v>
       </c>
       <c r="L21">
         <f t="shared" si="3"/>
-        <v>0.98446170921198672</v>
+        <v>0.98002219755826858</v>
       </c>
       <c r="M21">
         <f t="shared" si="4"/>
-        <v>116.815107102593</v>
+        <v>117.34428086070216</v>
       </c>
       <c r="N21">
         <f t="shared" si="5"/>
         <v>0.35714285714285715</v>
       </c>
-      <c r="O21" t="str">
+      <c r="O21">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P21">
         <f t="shared" si="7"/>
-        <v>0.12401352874859076</v>
+        <v>0.1245753114382786</v>
       </c>
       <c r="Q21">
         <f t="shared" si="8"/>
@@ -10158,11 +10405,11 @@
       </c>
       <c r="S21">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.961769656167348</v>
       </c>
       <c r="T21">
         <f t="shared" si="11"/>
-        <v>213.27242125510941</v>
+        <v>212.31065159894206</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -10188,7 +10435,7 @@
       </c>
       <c r="F22">
         <f>+IFERROR('Recuperados Diarios'!B21,"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <f>+IFERROR('Recuperados Diarios'!C21,"")</f>
@@ -10196,7 +10443,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="0"/>
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="I22">
         <f t="shared" si="12"/>
@@ -10208,27 +10455,27 @@
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.0444893832153692E-3</v>
       </c>
       <c r="L22">
         <f t="shared" si="3"/>
-        <v>0.98281092012133464</v>
+        <v>0.97876643073811931</v>
       </c>
       <c r="M22">
         <f t="shared" si="4"/>
-        <v>89.539094650205769</v>
+        <v>89.909090909090907</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="O22" t="str">
+      <c r="O22">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P22">
         <f t="shared" si="7"/>
-        <v>8.7448559670781897E-2</v>
+        <v>8.78099173553719E-2</v>
       </c>
       <c r="Q22">
         <f t="shared" si="8"/>
@@ -10240,11 +10487,11 @@
       </c>
       <c r="S22">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.961769656167348</v>
       </c>
       <c r="T22">
         <f t="shared" si="11"/>
-        <v>233.71002644866556</v>
+        <v>232.74825679249821</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -10270,7 +10517,7 @@
       </c>
       <c r="F23">
         <f>+IFERROR('Recuperados Diarios'!B22,"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G23">
         <f>+IFERROR('Recuperados Diarios'!C22,"")</f>
@@ -10278,7 +10525,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="0"/>
-        <v>1051</v>
+        <v>1047</v>
       </c>
       <c r="I23">
         <f t="shared" si="12"/>
@@ -10290,27 +10537,27 @@
       </c>
       <c r="K23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.7209302325581397E-3</v>
       </c>
       <c r="L23">
         <f t="shared" si="3"/>
-        <v>0.97767441860465121</v>
+        <v>0.97395348837209306</v>
       </c>
       <c r="M23">
         <f t="shared" si="4"/>
-        <v>87.963843958135101</v>
+        <v>88.299904489016228</v>
       </c>
       <c r="N23">
         <f t="shared" si="5"/>
         <v>0.29166666666666669</v>
       </c>
-      <c r="O23" t="str">
+      <c r="O23">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P23">
         <f t="shared" si="7"/>
-        <v>7.516650808753568E-2</v>
+        <v>7.5453677172874878E-2</v>
       </c>
       <c r="Q23">
         <f t="shared" si="8"/>
@@ -10322,11 +10569,11 @@
       </c>
       <c r="S23">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.961769656167348</v>
       </c>
       <c r="T23">
         <f t="shared" si="11"/>
-        <v>252.70497715797069</v>
+        <v>251.74320750180334</v>
       </c>
     </row>
     <row r="24" spans="1:20">
@@ -10352,19 +10599,19 @@
       </c>
       <c r="F24">
         <f>+IFERROR('Recuperados Diarios'!B23,"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G24">
         <f>+IFERROR('Recuperados Diarios'!C23,"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <f t="shared" si="0"/>
-        <v>1151</v>
+        <v>1142</v>
       </c>
       <c r="I24">
         <f t="shared" si="12"/>
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J24">
         <f t="shared" si="1"/>
@@ -10372,27 +10619,27 @@
       </c>
       <c r="K24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.6206604572396277E-3</v>
       </c>
       <c r="L24">
         <f t="shared" si="3"/>
-        <v>0.97459779847586792</v>
+        <v>0.96697713801862828</v>
       </c>
       <c r="M24">
         <f t="shared" si="4"/>
-        <v>108.76281494352736</v>
+        <v>109.6199649737303</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
-      <c r="O24" t="str">
+      <c r="O24">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.55555555555555558</v>
       </c>
       <c r="P24">
         <f t="shared" si="7"/>
-        <v>8.6880973066898348E-2</v>
+        <v>8.3187390542907177E-2</v>
       </c>
       <c r="Q24">
         <f t="shared" si="8"/>
@@ -10404,11 +10651,11 @@
       </c>
       <c r="S24">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.1639817263765329</v>
       </c>
       <c r="T24">
         <f t="shared" si="11"/>
-        <v>276.7492185621544</v>
+        <v>274.58523683577783</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -10434,7 +10681,7 @@
       </c>
       <c r="F25">
         <f>+IFERROR('Recuperados Diarios'!B24,"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G25">
         <f>+IFERROR('Recuperados Diarios'!C24,"")</f>
@@ -10442,7 +10689,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="0"/>
-        <v>1287</v>
+        <v>1278</v>
       </c>
       <c r="I25">
         <f t="shared" si="12"/>
@@ -10454,27 +10701,27 @@
       </c>
       <c r="K25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.8337129840546698E-3</v>
       </c>
       <c r="L25">
         <f t="shared" si="3"/>
-        <v>0.97722095671981779</v>
+        <v>0.97038724373576313</v>
       </c>
       <c r="M25">
         <f t="shared" si="4"/>
-        <v>139.17016317016316</v>
+        <v>140.15023474178403</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O25" t="str">
+      <c r="O25">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P25">
         <f t="shared" si="7"/>
-        <v>0.10567210567210568</v>
+        <v>0.10641627543035993</v>
       </c>
       <c r="Q25">
         <f t="shared" si="8"/>
@@ -10486,11 +10733,11 @@
       </c>
       <c r="S25">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.1639817263765329</v>
       </c>
       <c r="T25">
         <f t="shared" si="11"/>
-        <v>309.44938687184418</v>
+        <v>307.28540514546768</v>
       </c>
     </row>
     <row r="26" spans="1:20">
@@ -10516,19 +10763,19 @@
       </c>
       <c r="F26">
         <f>+IFERROR('Recuperados Diarios'!B25,"")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G26">
         <f>+IFERROR('Recuperados Diarios'!C25,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f t="shared" si="0"/>
-        <v>1443</v>
+        <v>1433</v>
       </c>
       <c r="I26">
         <f t="shared" si="12"/>
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J26">
         <f t="shared" si="1"/>
@@ -10536,27 +10783,27 @@
       </c>
       <c r="K26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.7796610169491523E-3</v>
       </c>
       <c r="L26">
         <f t="shared" si="3"/>
-        <v>0.97830508474576272</v>
+        <v>0.97152542372881356</v>
       </c>
       <c r="M26">
         <f t="shared" si="4"/>
-        <v>161.50381150381151</v>
+        <v>162.63084438241452</v>
       </c>
       <c r="N26">
         <f t="shared" si="5"/>
         <v>6.25E-2</v>
       </c>
-      <c r="O26" t="str">
+      <c r="O26">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.1</v>
       </c>
       <c r="P26">
         <f t="shared" si="7"/>
-        <v>0.10810810810810811</v>
+        <v>0.10816468946266573</v>
       </c>
       <c r="Q26">
         <f t="shared" si="8"/>
@@ -10568,11 +10815,11 @@
       </c>
       <c r="S26">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>2.4044241404183699</v>
       </c>
       <c r="T26">
         <f t="shared" si="11"/>
-        <v>346.95840346237077</v>
+        <v>344.5539793219524</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -10598,19 +10845,19 @@
       </c>
       <c r="F27">
         <f>+IFERROR('Recuperados Diarios'!B26,"")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G27">
         <f>+IFERROR('Recuperados Diarios'!C26,"")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H27">
         <f t="shared" si="0"/>
-        <v>1636</v>
+        <v>1623</v>
       </c>
       <c r="I27">
         <f t="shared" si="12"/>
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J27">
         <f t="shared" si="1"/>
@@ -10618,27 +10865,27 @@
       </c>
       <c r="K27">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.7704722056186493E-3</v>
       </c>
       <c r="L27">
         <f t="shared" si="3"/>
-        <v>0.9778840406455469</v>
+        <v>0.97011356843992824</v>
       </c>
       <c r="M27">
         <f t="shared" si="4"/>
-        <v>202.47799511002447</v>
+        <v>204.09981515711647</v>
       </c>
       <c r="N27">
         <f t="shared" si="5"/>
         <v>0.13513513513513514</v>
       </c>
-      <c r="O27" t="str">
+      <c r="O27">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.23076923076923078</v>
       </c>
       <c r="P27">
         <f t="shared" si="7"/>
-        <v>0.11797066014669927</v>
+        <v>0.1170671595810228</v>
       </c>
       <c r="Q27">
         <f t="shared" si="8"/>
@@ -10650,11 +10897,11 @@
       </c>
       <c r="S27">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.1257513825438807</v>
       </c>
       <c r="T27">
         <f t="shared" si="11"/>
-        <v>393.3637893724453</v>
+        <v>390.23803798990144</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -10680,7 +10927,7 @@
       </c>
       <c r="F28">
         <f>+IFERROR('Recuperados Diarios'!B27,"")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G28">
         <f>+IFERROR('Recuperados Diarios'!C27,"")</f>
@@ -10688,7 +10935,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="0"/>
-        <v>1760</v>
+        <v>1747</v>
       </c>
       <c r="I28">
         <f t="shared" si="12"/>
@@ -10700,27 +10947,27 @@
       </c>
       <c r="K28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.2182121043864516E-3</v>
       </c>
       <c r="L28">
         <f t="shared" si="3"/>
-        <v>0.97723486951693506</v>
+        <v>0.97001665741254861</v>
       </c>
       <c r="M28">
         <f t="shared" si="4"/>
-        <v>130.98181818181817</v>
+        <v>131.95649685174584</v>
       </c>
       <c r="N28">
         <f t="shared" si="5"/>
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="O28" t="str">
+      <c r="O28">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P28">
         <f t="shared" si="7"/>
-        <v>7.045454545454545E-2</v>
+        <v>7.0978820835718368E-2</v>
       </c>
       <c r="Q28">
         <f t="shared" si="8"/>
@@ -10732,11 +10979,11 @@
       </c>
       <c r="S28">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.1257513825438807</v>
       </c>
       <c r="T28">
         <f t="shared" si="11"/>
-        <v>423.17864871363309</v>
+        <v>420.05289733108924</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -10762,7 +11009,7 @@
       </c>
       <c r="F29">
         <f>+IFERROR('Recuperados Diarios'!B28,"")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G29">
         <f>+IFERROR('Recuperados Diarios'!C28,"")</f>
@@ -10770,7 +11017,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="0"/>
-        <v>1942</v>
+        <v>1929</v>
       </c>
       <c r="I29">
         <f t="shared" si="12"/>
@@ -10782,27 +11029,27 @@
       </c>
       <c r="K29">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5392354124748494E-3</v>
       </c>
       <c r="L29">
         <f t="shared" si="3"/>
-        <v>0.97686116700201209</v>
+        <v>0.97032193158953728</v>
       </c>
       <c r="M29">
         <f t="shared" si="4"/>
-        <v>191.42945417095777</v>
+        <v>192.71954380508035</v>
       </c>
       <c r="N29">
         <f t="shared" si="5"/>
         <v>0.10869565217391304</v>
       </c>
-      <c r="O29" t="str">
+      <c r="O29">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P29">
         <f t="shared" si="7"/>
-        <v>9.3717816683831098E-2</v>
+        <v>9.4349403836184551E-2</v>
       </c>
       <c r="Q29">
         <f t="shared" si="8"/>
@@ -10814,11 +11061,11 @@
       </c>
       <c r="S29">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.1257513825438807</v>
       </c>
       <c r="T29">
         <f t="shared" si="11"/>
-        <v>466.93916806924744</v>
+        <v>463.81341668670353</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -10844,19 +11091,19 @@
       </c>
       <c r="F30">
         <f>+IFERROR('Recuperados Diarios'!B29,"")</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <f>+IFERROR('Recuperados Diarios'!C29,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>2046</v>
+        <v>2032</v>
       </c>
       <c r="I30">
         <f t="shared" si="12"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J30">
         <f t="shared" si="1"/>
@@ -10864,27 +11111,27 @@
       </c>
       <c r="K30">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.6666666666666671E-3</v>
       </c>
       <c r="L30">
         <f t="shared" si="3"/>
-        <v>0.97428571428571431</v>
+        <v>0.9676190476190476</v>
       </c>
       <c r="M30">
         <f t="shared" si="4"/>
-        <v>114.95601173020528</v>
+        <v>115.74803149606299</v>
       </c>
       <c r="N30">
         <f t="shared" si="5"/>
         <v>0.14814814814814814</v>
       </c>
-      <c r="O30" t="str">
+      <c r="O30">
         <f t="shared" si="6"/>
-        <v/>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="P30">
         <f t="shared" si="7"/>
-        <v>5.0830889540566963E-2</v>
+        <v>5.0688976377952756E-2</v>
       </c>
       <c r="Q30">
         <f t="shared" si="8"/>
@@ -10896,11 +11143,11 @@
       </c>
       <c r="S30">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.3661937965857178</v>
       </c>
       <c r="T30">
         <f t="shared" si="11"/>
-        <v>491.9451791295985</v>
+        <v>488.57898533301278</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -10926,19 +11173,19 @@
       </c>
       <c r="F31">
         <f>+IFERROR('Recuperados Diarios'!B30,"")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G31">
         <f>+IFERROR('Recuperados Diarios'!C30,"")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H31">
         <f t="shared" si="0"/>
-        <v>2194</v>
+        <v>2178</v>
       </c>
       <c r="I31">
         <f t="shared" si="12"/>
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J31">
         <f t="shared" si="1"/>
@@ -10946,27 +11193,27 @@
       </c>
       <c r="K31">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.1142730102267673E-3</v>
       </c>
       <c r="L31">
         <f t="shared" si="3"/>
-        <v>0.97554468652734549</v>
+        <v>0.96843041351711867</v>
       </c>
       <c r="M31">
         <f t="shared" si="4"/>
-        <v>152.73518687329079</v>
+        <v>153.85720844811755</v>
       </c>
       <c r="N31">
         <f t="shared" si="5"/>
         <v>1.8181818181818181E-2</v>
       </c>
-      <c r="O31" t="str">
+      <c r="O31">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.125</v>
       </c>
       <c r="P31">
         <f t="shared" si="7"/>
-        <v>6.7456700091157701E-2</v>
+        <v>6.7033976124885222E-2</v>
       </c>
       <c r="Q31">
         <f t="shared" si="8"/>
@@ -10978,11 +11225,11 @@
       </c>
       <c r="S31">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.847078624669392</v>
       </c>
       <c r="T31">
         <f t="shared" si="11"/>
-        <v>527.53065640779039</v>
+        <v>523.683577783121</v>
       </c>
     </row>
     <row r="32" spans="1:20">
@@ -11008,7 +11255,7 @@
       </c>
       <c r="F32">
         <f>+IFERROR('Recuperados Diarios'!B31,"")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G32">
         <f>+IFERROR('Recuperados Diarios'!C31,"")</f>
@@ -11016,7 +11263,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="0"/>
-        <v>2469</v>
+        <v>2453</v>
       </c>
       <c r="I32">
         <f t="shared" si="12"/>
@@ -11028,27 +11275,27 @@
       </c>
       <c r="K32">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.3291139240506328E-3</v>
       </c>
       <c r="L32">
         <f t="shared" si="3"/>
-        <v>0.97666139240506333</v>
+        <v>0.97033227848101267</v>
       </c>
       <c r="M32">
         <f t="shared" si="4"/>
-        <v>285.66707168894288</v>
+        <v>287.53037097431718</v>
       </c>
       <c r="N32">
         <f t="shared" si="5"/>
         <v>6.7796610169491525E-2</v>
       </c>
-      <c r="O32" t="str">
+      <c r="O32">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P32">
         <f t="shared" si="7"/>
-        <v>0.11138112596192791</v>
+        <v>0.11210762331838565</v>
       </c>
       <c r="Q32">
         <f t="shared" si="8"/>
@@ -11060,11 +11307,11 @@
       </c>
       <c r="S32">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.847078624669392</v>
       </c>
       <c r="T32">
         <f t="shared" si="11"/>
-        <v>593.6523202692955</v>
+        <v>589.80524164462611</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -11090,7 +11337,7 @@
       </c>
       <c r="F33">
         <f>+IFERROR('Recuperados Diarios'!B32,"")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G33">
         <f>+IFERROR('Recuperados Diarios'!C32,"")</f>
@@ -11098,7 +11345,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="0"/>
-        <v>2689</v>
+        <v>2673</v>
       </c>
       <c r="I33">
         <f t="shared" si="12"/>
@@ -11110,27 +11357,27 @@
       </c>
       <c r="K33">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.8139534883720929E-3</v>
       </c>
       <c r="L33">
         <f t="shared" si="3"/>
-        <v>0.97710755813953487</v>
+        <v>0.97129360465116277</v>
       </c>
       <c r="M33">
         <f t="shared" si="4"/>
-        <v>229.24804760133878</v>
+        <v>230.62027684249907</v>
       </c>
       <c r="N33">
         <f t="shared" si="5"/>
         <v>6.3492063492063489E-2</v>
       </c>
-      <c r="O33" t="str">
+      <c r="O33">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="P33">
         <f t="shared" si="7"/>
-        <v>8.1814801041279292E-2</v>
+        <v>8.2304526748971193E-2</v>
       </c>
       <c r="Q33">
         <f t="shared" si="8"/>
@@ -11142,11 +11389,11 @@
       </c>
       <c r="S33">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3.847078624669392</v>
       </c>
       <c r="T33">
         <f t="shared" si="11"/>
-        <v>646.54965135849966</v>
+        <v>642.70257273383027</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -11172,19 +11419,19 @@
       </c>
       <c r="F34">
         <f>+IFERROR('Recuperados Diarios'!B33,"")</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G34">
         <f>+IFERROR('Recuperados Diarios'!C33,"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <f t="shared" si="0"/>
-        <v>2908</v>
+        <v>2891</v>
       </c>
       <c r="I34">
         <f t="shared" si="12"/>
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J34">
         <f t="shared" si="1"/>
@@ -11192,27 +11439,27 @@
       </c>
       <c r="K34">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.7162071284465365E-3</v>
       </c>
       <c r="L34">
         <f t="shared" si="3"/>
-        <v>0.97780766644250172</v>
+        <v>0.97209145931405516</v>
       </c>
       <c r="M34">
         <f t="shared" si="4"/>
-        <v>227.0385144429161</v>
+        <v>228.37357315807679</v>
       </c>
       <c r="N34">
         <f t="shared" si="5"/>
         <v>4.5454545454545456E-2</v>
       </c>
-      <c r="O34" t="str">
+      <c r="O34">
         <f t="shared" si="6"/>
-        <v/>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="P34">
         <f t="shared" si="7"/>
-        <v>7.5309491059147179E-2</v>
+        <v>7.5406433759944658E-2</v>
       </c>
       <c r="Q34">
         <f t="shared" si="8"/>
@@ -11224,11 +11471,11 @@
       </c>
       <c r="S34">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4.0875210387112286</v>
       </c>
       <c r="T34">
         <f t="shared" si="11"/>
-        <v>699.20654003366201</v>
+        <v>695.11901899495069</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -11254,19 +11501,19 @@
       </c>
       <c r="F35">
         <f>+IFERROR('Recuperados Diarios'!B34,"")</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G35">
         <f>+IFERROR('Recuperados Diarios'!C34,"")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H35">
         <f t="shared" si="0"/>
-        <v>3160</v>
+        <v>3137</v>
       </c>
       <c r="I35">
         <f t="shared" si="12"/>
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J35">
         <f t="shared" si="1"/>
@@ -11274,27 +11521,27 @@
       </c>
       <c r="K35">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.1119356833642547E-3</v>
       </c>
       <c r="L35">
         <f t="shared" si="3"/>
-        <v>0.97711811997526288</v>
+        <v>0.97000618429189855</v>
       </c>
       <c r="M35">
         <f t="shared" si="4"/>
-        <v>266.08860759493672</v>
+        <v>268.03952821166723</v>
       </c>
       <c r="N35">
         <f t="shared" si="5"/>
         <v>0.10810810810810811</v>
       </c>
-      <c r="O35" t="str">
+      <c r="O35">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.2608695652173913</v>
       </c>
       <c r="P35">
         <f t="shared" si="7"/>
-        <v>7.9746835443037969E-2</v>
+        <v>7.8418871533312076E-2</v>
       </c>
       <c r="Q35">
         <f t="shared" si="8"/>
@@ -11306,11 +11553,11 @@
       </c>
       <c r="S35">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5.5301755229622511</v>
       </c>
       <c r="T35">
         <f t="shared" si="11"/>
-        <v>759.79802837220484</v>
+        <v>754.26785284924267</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -11336,19 +11583,19 @@
       </c>
       <c r="F36">
         <f>+IFERROR('Recuperados Diarios'!B35,"")</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G36">
         <f>+IFERROR('Recuperados Diarios'!C35,"")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H36">
         <f t="shared" si="0"/>
-        <v>3321</v>
+        <v>3292</v>
       </c>
       <c r="I36">
         <f t="shared" si="12"/>
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J36">
         <f t="shared" si="1"/>
@@ -11356,27 +11603,27 @@
       </c>
       <c r="K36">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8.5294117647058826E-3</v>
       </c>
       <c r="L36">
         <f t="shared" si="3"/>
-        <v>0.97676470588235298</v>
+        <v>0.96823529411764708</v>
       </c>
       <c r="M36">
         <f t="shared" si="4"/>
-        <v>169.9488105992171</v>
+        <v>171.44592952612393</v>
       </c>
       <c r="N36">
         <f t="shared" si="5"/>
         <v>6.3291139240506333E-2</v>
       </c>
-      <c r="O36" t="str">
+      <c r="O36">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0.20689655172413793</v>
       </c>
       <c r="P36">
         <f t="shared" si="7"/>
-        <v>4.8479373682625712E-2</v>
+        <v>4.7083839611178617E-2</v>
       </c>
       <c r="Q36">
         <f t="shared" si="8"/>
@@ -11388,11 +11635,11 @@
       </c>
       <c r="S36">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>6.9728300072132727</v>
       </c>
       <c r="T36">
         <f t="shared" si="11"/>
-        <v>798.5092570329407</v>
+        <v>791.53642702572733</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -11430,7 +11677,7 @@
       </c>
       <c r="I37">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="J37">
         <f t="shared" si="1"/>
@@ -11458,7 +11705,7 @@
       </c>
       <c r="P37">
         <f t="shared" si="7"/>
-        <v>9.025270758122744E-4</v>
+        <v>9.6269554753309269E-3</v>
       </c>
       <c r="Q37">
         <f t="shared" si="8"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-11-2020 00-39-56
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1478" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{06CD8E72-2815-4506-AB0D-7CC1418B754C}"/>
+  <xr:revisionPtr revIDLastSave="1479" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B63A2F0-0385-47FA-8557-4BE9E929A4E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
-    <sheet name="Confirmados Diarios" sheetId="4" r:id="rId2"/>
-    <sheet name="Fallecidos Diarios" sheetId="5" r:id="rId3"/>
+    <sheet name="Fallecidos Diarios" sheetId="5" r:id="rId2"/>
+    <sheet name="Confirmados Diarios" sheetId="4" r:id="rId3"/>
     <sheet name="Resumen" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$93</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Nuevos Recuperados</t>
+  </si>
+  <si>
+    <t>Fallecidos Acumulados</t>
+  </si>
+  <si>
+    <t>Nuevos Fallecidos</t>
   </si>
   <si>
     <t>Confirmados Acumulados</t>
@@ -82,12 +88,6 @@
   </si>
   <si>
     <t>81-100 años</t>
-  </si>
-  <si>
-    <t>Fallecidos Acumulados</t>
-  </si>
-  <si>
-    <t>Nuevos Fallecidos</t>
   </si>
   <si>
     <t>Activos</t>
@@ -279,9 +279,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -321,6 +318,9 @@
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -349,16 +349,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C93" totalsRowShown="0">
+  <autoFilter ref="A1:C93" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
+    <tableColumn id="3" xr3:uid="{953C86B5-D930-4CD8-BDD6-7B2F6016F7B8}" name="Nuevos Fallecidos"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M94" totalsRowShown="0">
   <autoFilter ref="A1:M94" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
-    <tableColumn id="3" xr3:uid="{9702B7CB-3CBF-4BD3-A6FB-6E7476D20E04}" name="Nuevos Confirmados" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{9702B7CB-3CBF-4BD3-A6FB-6E7476D20E04}" name="Nuevos Confirmados" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(B2-B1,"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{4D67C206-6947-4A9D-A86B-9696EC92AE7B}" name="Femenino"/>
-    <tableColumn id="5" xr3:uid="{2C5FE086-42D4-4CE1-8D75-61AEC82F25CC}" name="Masculino" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{2C5FE086-42D4-4CE1-8D75-61AEC82F25CC}" name="Masculino" dataDxfId="2">
       <calculatedColumnFormula>C2-D2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{ECA607ED-046A-4D30-8CB5-AF268A116D81}" name="0-10 años"/>
@@ -369,18 +381,6 @@
     <tableColumn id="11" xr3:uid="{868DED38-8C57-4C53-8CB8-6344AF644B0D}" name="51-60 años"/>
     <tableColumn id="12" xr3:uid="{9CE13132-B6F5-4B6E-8F32-9E05767252DE}" name="61-80 años"/>
     <tableColumn id="13" xr3:uid="{D4A45927-765E-4403-980D-0EED5C0A5994}" name="81-100 años"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C93" totalsRowShown="0">
-  <autoFilter ref="A1:C93" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
-    <tableColumn id="3" xr3:uid="{953C86B5-D930-4CD8-BDD6-7B2F6016F7B8}" name="Nuevos Fallecidos"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3668,11 +3668,1123 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
+  <dimension ref="A1:E93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88:C93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4">
+        <v>43900</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4">
+        <v>43901</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4">
+        <v>43902</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4">
+        <v>43903</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4">
+        <v>43904</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4">
+        <v>43905</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4">
+        <v>43906</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4">
+        <v>43907</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4">
+        <v>43908</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4">
+        <v>43909</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4">
+        <v>43910</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4">
+        <v>43911</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4">
+        <v>43912</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4">
+        <v>43913</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4">
+        <v>43914</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4">
+        <v>43915</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4">
+        <v>43916</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4">
+        <v>43917</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4">
+        <v>43918</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4">
+        <v>43919</v>
+      </c>
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4">
+        <v>43920</v>
+      </c>
+      <c r="B22">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4">
+        <v>43921</v>
+      </c>
+      <c r="B23">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4">
+        <v>43922</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4">
+        <v>43923</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4">
+        <v>43924</v>
+      </c>
+      <c r="B26">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4">
+        <v>43925</v>
+      </c>
+      <c r="B27">
+        <v>41</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4">
+        <v>43926</v>
+      </c>
+      <c r="B28">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4">
+        <v>43927</v>
+      </c>
+      <c r="B29">
+        <v>54</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4">
+        <v>43928</v>
+      </c>
+      <c r="B30">
+        <v>55</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4">
+        <v>43929</v>
+      </c>
+      <c r="B31">
+        <v>59</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4">
+        <v>43930</v>
+      </c>
+      <c r="B32">
+        <v>63</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>43931</v>
+      </c>
+      <c r="B33">
+        <v>66</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4">
+        <v>43932</v>
+      </c>
+      <c r="B34">
+        <v>74</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4">
+        <v>43933</v>
+      </c>
+      <c r="B35">
+        <v>79</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4">
+        <v>43934</v>
+      </c>
+      <c r="B36">
+        <v>87</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>43935</v>
+      </c>
+      <c r="B37">
+        <v>94</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4">
+        <v>43936</v>
+      </c>
+      <c r="B38">
+        <v>95</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4">
+        <v>43937</v>
+      </c>
+      <c r="B39">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
+        <v>43938</v>
+      </c>
+      <c r="B40">
+        <v>109</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4">
+        <v>43939</v>
+      </c>
+      <c r="B41">
+        <v>116</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4">
+        <v>43940</v>
+      </c>
+      <c r="B42">
+        <v>120</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4">
+        <v>43941</v>
+      </c>
+      <c r="B43">
+        <v>126</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4">
+        <v>43942</v>
+      </c>
+      <c r="B44">
+        <v>136</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="E44" s="5"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4">
+        <v>43943</v>
+      </c>
+      <c r="B45">
+        <v>141</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4">
+        <v>43944</v>
+      </c>
+      <c r="B46">
+        <v>146</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4">
+        <v>43945</v>
+      </c>
+      <c r="B47">
+        <v>154</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4">
+        <v>43946</v>
+      </c>
+      <c r="B48">
+        <v>159</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4">
+        <v>43947</v>
+      </c>
+      <c r="B49">
+        <v>165</v>
+      </c>
+      <c r="C49">
+        <v>6</v>
+      </c>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4">
+        <v>43948</v>
+      </c>
+      <c r="B50">
+        <v>167</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4">
+        <v>43949</v>
+      </c>
+      <c r="B51">
+        <v>167</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4">
+        <v>43950</v>
+      </c>
+      <c r="B52">
+        <v>178</v>
+      </c>
+      <c r="C52">
+        <v>11</v>
+      </c>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4">
+        <v>43951</v>
+      </c>
+      <c r="B53">
+        <v>188</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="E53" s="5"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4">
+        <v>43952</v>
+      </c>
+      <c r="B54">
+        <v>192</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4">
+        <v>43953</v>
+      </c>
+      <c r="B55">
+        <v>197</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4">
+        <v>43954</v>
+      </c>
+      <c r="B56">
+        <v>197</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4">
+        <v>43955</v>
+      </c>
+      <c r="B57">
+        <v>200</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4">
+        <v>43956</v>
+      </c>
+      <c r="B58">
+        <v>210</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4">
+        <v>43957</v>
+      </c>
+      <c r="B59">
+        <v>218</v>
+      </c>
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4">
+        <v>43958</v>
+      </c>
+      <c r="B60">
+        <v>225</v>
+      </c>
+      <c r="C60">
+        <v>7</v>
+      </c>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4">
+        <v>43959</v>
+      </c>
+      <c r="B61">
+        <v>231</v>
+      </c>
+      <c r="C61">
+        <v>6</v>
+      </c>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="4">
+        <v>43960</v>
+      </c>
+      <c r="B62">
+        <v>237</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4">
+        <v>43961</v>
+      </c>
+      <c r="B63">
+        <v>244</v>
+      </c>
+      <c r="C63">
+        <v>7</v>
+      </c>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4">
+        <v>43962</v>
+      </c>
+      <c r="B64">
+        <v>249</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4">
+        <v>43963</v>
+      </c>
+      <c r="B65">
+        <v>252</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
+      </c>
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4">
+        <v>43964</v>
+      </c>
+      <c r="B66">
+        <v>256</v>
+      </c>
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4">
+        <v>43965</v>
+      </c>
+      <c r="B67">
+        <v>260</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4">
+        <v>43966</v>
+      </c>
+      <c r="B68">
+        <v>266</v>
+      </c>
+      <c r="C68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4">
+        <v>43967</v>
+      </c>
+      <c r="B69">
+        <v>269</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4">
+        <v>43968</v>
+      </c>
+      <c r="B70">
+        <v>275</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4">
+        <v>43969</v>
+      </c>
+      <c r="B71">
+        <v>279</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4">
+        <v>43970</v>
+      </c>
+      <c r="B72">
+        <v>281</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4">
+        <v>43971</v>
+      </c>
+      <c r="B73">
+        <v>287</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4">
+        <v>43972</v>
+      </c>
+      <c r="B74">
+        <v>291</v>
+      </c>
+      <c r="C74">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="4">
+        <v>43973</v>
+      </c>
+      <c r="B75">
+        <v>295</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4">
+        <v>43974</v>
+      </c>
+      <c r="B76">
+        <v>299</v>
+      </c>
+      <c r="C76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4">
+        <v>43975</v>
+      </c>
+      <c r="B77">
+        <v>306</v>
+      </c>
+      <c r="C77">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4">
+        <v>43976</v>
+      </c>
+      <c r="B78">
+        <v>310</v>
+      </c>
+      <c r="C78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4">
+        <v>43977</v>
+      </c>
+      <c r="B79">
+        <v>313</v>
+      </c>
+      <c r="C79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4">
+        <v>43978</v>
+      </c>
+      <c r="B80">
+        <v>315</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="4">
+        <v>43979</v>
+      </c>
+      <c r="B81">
+        <v>320</v>
+      </c>
+      <c r="C81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="4">
+        <v>43980</v>
+      </c>
+      <c r="B82">
+        <v>326</v>
+      </c>
+      <c r="C82">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="4">
+        <v>43981</v>
+      </c>
+      <c r="B83">
+        <v>330</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="4">
+        <v>43982</v>
+      </c>
+      <c r="B84">
+        <v>336</v>
+      </c>
+      <c r="C84">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="4">
+        <v>43983</v>
+      </c>
+      <c r="B85">
+        <v>344</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="4">
+        <v>43984</v>
+      </c>
+      <c r="B86">
+        <v>352</v>
+      </c>
+      <c r="C86">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="4">
+        <v>43985</v>
+      </c>
+      <c r="B87">
+        <v>357</v>
+      </c>
+      <c r="C87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="4">
+        <v>43986</v>
+      </c>
+      <c r="B88">
+        <v>363</v>
+      </c>
+      <c r="C88">
+        <f>B88-B87</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="4">
+        <v>43987</v>
+      </c>
+      <c r="B89">
+        <v>370</v>
+      </c>
+      <c r="C89">
+        <f t="shared" ref="C89:C93" si="0">B89-B88</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="4">
+        <v>43988</v>
+      </c>
+      <c r="B90">
+        <v>386</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="4">
+        <v>43989</v>
+      </c>
+      <c r="B91">
+        <v>393</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="4">
+        <v>43990</v>
+      </c>
+      <c r="B92">
+        <v>398</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="4">
+        <v>43991</v>
+      </c>
+      <c r="B93">
+        <v>403</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B89" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
@@ -3693,40 +4805,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -7571,1118 +8683,6 @@
         <v>35</v>
       </c>
       <c r="M94" s="6">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E93"/>
-  <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88:C93"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4">
-        <v>43900</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4">
-        <v>43901</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4">
-        <v>43902</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4">
-        <v>43903</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4">
-        <v>43904</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4">
-        <v>43905</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4">
-        <v>43906</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4">
-        <v>43907</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="4">
-        <v>43908</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4">
-        <v>43909</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4">
-        <v>43910</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4">
-        <v>43911</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="4">
-        <v>43912</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4">
-        <v>43913</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="4">
-        <v>43914</v>
-      </c>
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="4">
-        <v>43915</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4">
-        <v>43916</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4">
-        <v>43917</v>
-      </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="4">
-        <v>43918</v>
-      </c>
-      <c r="B20">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4">
-        <v>43919</v>
-      </c>
-      <c r="B21">
-        <v>17</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="4">
-        <v>43920</v>
-      </c>
-      <c r="B22">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>7</v>
-      </c>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="4">
-        <v>43921</v>
-      </c>
-      <c r="B23">
-        <v>30</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="4">
-        <v>43922</v>
-      </c>
-      <c r="B24">
-        <v>30</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="4">
-        <v>43923</v>
-      </c>
-      <c r="B25">
-        <v>32</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="4">
-        <v>43924</v>
-      </c>
-      <c r="B26">
-        <v>37</v>
-      </c>
-      <c r="C26">
-        <v>5</v>
-      </c>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="4">
-        <v>43925</v>
-      </c>
-      <c r="B27">
-        <v>41</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="4">
-        <v>43926</v>
-      </c>
-      <c r="B28">
-        <v>46</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="4">
-        <v>43927</v>
-      </c>
-      <c r="B29">
-        <v>54</v>
-      </c>
-      <c r="C29">
-        <v>8</v>
-      </c>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="4">
-        <v>43928</v>
-      </c>
-      <c r="B30">
-        <v>55</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="4">
-        <v>43929</v>
-      </c>
-      <c r="B31">
-        <v>59</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="4">
-        <v>43930</v>
-      </c>
-      <c r="B32">
-        <v>63</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="4">
-        <v>43931</v>
-      </c>
-      <c r="B33">
-        <v>66</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="4">
-        <v>43932</v>
-      </c>
-      <c r="B34">
-        <v>74</v>
-      </c>
-      <c r="C34">
-        <v>8</v>
-      </c>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="4">
-        <v>43933</v>
-      </c>
-      <c r="B35">
-        <v>79</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="4">
-        <v>43934</v>
-      </c>
-      <c r="B36">
-        <v>87</v>
-      </c>
-      <c r="C36">
-        <v>8</v>
-      </c>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4">
-        <v>43935</v>
-      </c>
-      <c r="B37">
-        <v>94</v>
-      </c>
-      <c r="C37">
-        <v>7</v>
-      </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="4">
-        <v>43936</v>
-      </c>
-      <c r="B38">
-        <v>95</v>
-      </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="4">
-        <v>43937</v>
-      </c>
-      <c r="B39">
-        <v>103</v>
-      </c>
-      <c r="C39">
-        <v>8</v>
-      </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4">
-        <v>43938</v>
-      </c>
-      <c r="B40">
-        <v>109</v>
-      </c>
-      <c r="C40">
-        <v>6</v>
-      </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="4">
-        <v>43939</v>
-      </c>
-      <c r="B41">
-        <v>116</v>
-      </c>
-      <c r="C41">
-        <v>7</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="4">
-        <v>43940</v>
-      </c>
-      <c r="B42">
-        <v>120</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="4">
-        <v>43941</v>
-      </c>
-      <c r="B43">
-        <v>126</v>
-      </c>
-      <c r="C43">
-        <v>6</v>
-      </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="4">
-        <v>43942</v>
-      </c>
-      <c r="B44">
-        <v>136</v>
-      </c>
-      <c r="C44">
-        <v>10</v>
-      </c>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="4">
-        <v>43943</v>
-      </c>
-      <c r="B45">
-        <v>141</v>
-      </c>
-      <c r="C45">
-        <v>5</v>
-      </c>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="4">
-        <v>43944</v>
-      </c>
-      <c r="B46">
-        <v>146</v>
-      </c>
-      <c r="C46">
-        <v>5</v>
-      </c>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="4">
-        <v>43945</v>
-      </c>
-      <c r="B47">
-        <v>154</v>
-      </c>
-      <c r="C47">
-        <v>8</v>
-      </c>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="4">
-        <v>43946</v>
-      </c>
-      <c r="B48">
-        <v>159</v>
-      </c>
-      <c r="C48">
-        <v>5</v>
-      </c>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="4">
-        <v>43947</v>
-      </c>
-      <c r="B49">
-        <v>165</v>
-      </c>
-      <c r="C49">
-        <v>6</v>
-      </c>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="4">
-        <v>43948</v>
-      </c>
-      <c r="B50">
-        <v>167</v>
-      </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="4">
-        <v>43949</v>
-      </c>
-      <c r="B51">
-        <v>167</v>
-      </c>
-      <c r="C51">
-        <v>0</v>
-      </c>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4">
-        <v>43950</v>
-      </c>
-      <c r="B52">
-        <v>178</v>
-      </c>
-      <c r="C52">
-        <v>11</v>
-      </c>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="4">
-        <v>43951</v>
-      </c>
-      <c r="B53">
-        <v>188</v>
-      </c>
-      <c r="C53">
-        <v>10</v>
-      </c>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="4">
-        <v>43952</v>
-      </c>
-      <c r="B54">
-        <v>192</v>
-      </c>
-      <c r="C54">
-        <v>4</v>
-      </c>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="4">
-        <v>43953</v>
-      </c>
-      <c r="B55">
-        <v>197</v>
-      </c>
-      <c r="C55">
-        <v>5</v>
-      </c>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="4">
-        <v>43954</v>
-      </c>
-      <c r="B56">
-        <v>197</v>
-      </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="E56" s="5"/>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="4">
-        <v>43955</v>
-      </c>
-      <c r="B57">
-        <v>200</v>
-      </c>
-      <c r="C57">
-        <v>3</v>
-      </c>
-      <c r="E57" s="5"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="4">
-        <v>43956</v>
-      </c>
-      <c r="B58">
-        <v>210</v>
-      </c>
-      <c r="C58">
-        <v>10</v>
-      </c>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="4">
-        <v>43957</v>
-      </c>
-      <c r="B59">
-        <v>218</v>
-      </c>
-      <c r="C59">
-        <v>8</v>
-      </c>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="4">
-        <v>43958</v>
-      </c>
-      <c r="B60">
-        <v>225</v>
-      </c>
-      <c r="C60">
-        <v>7</v>
-      </c>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="4">
-        <v>43959</v>
-      </c>
-      <c r="B61">
-        <v>231</v>
-      </c>
-      <c r="C61">
-        <v>6</v>
-      </c>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="4">
-        <v>43960</v>
-      </c>
-      <c r="B62">
-        <v>237</v>
-      </c>
-      <c r="C62">
-        <v>6</v>
-      </c>
-      <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="4">
-        <v>43961</v>
-      </c>
-      <c r="B63">
-        <v>244</v>
-      </c>
-      <c r="C63">
-        <v>7</v>
-      </c>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="4">
-        <v>43962</v>
-      </c>
-      <c r="B64">
-        <v>249</v>
-      </c>
-      <c r="C64">
-        <v>5</v>
-      </c>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="4">
-        <v>43963</v>
-      </c>
-      <c r="B65">
-        <v>252</v>
-      </c>
-      <c r="C65">
-        <v>3</v>
-      </c>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="4">
-        <v>43964</v>
-      </c>
-      <c r="B66">
-        <v>256</v>
-      </c>
-      <c r="C66">
-        <v>4</v>
-      </c>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="4">
-        <v>43965</v>
-      </c>
-      <c r="B67">
-        <v>260</v>
-      </c>
-      <c r="C67">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="4">
-        <v>43966</v>
-      </c>
-      <c r="B68">
-        <v>266</v>
-      </c>
-      <c r="C68">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="4">
-        <v>43967</v>
-      </c>
-      <c r="B69">
-        <v>269</v>
-      </c>
-      <c r="C69">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="4">
-        <v>43968</v>
-      </c>
-      <c r="B70">
-        <v>275</v>
-      </c>
-      <c r="C70">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="4">
-        <v>43969</v>
-      </c>
-      <c r="B71">
-        <v>279</v>
-      </c>
-      <c r="C71">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" s="4">
-        <v>43970</v>
-      </c>
-      <c r="B72">
-        <v>281</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="4">
-        <v>43971</v>
-      </c>
-      <c r="B73">
-        <v>287</v>
-      </c>
-      <c r="C73">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" s="4">
-        <v>43972</v>
-      </c>
-      <c r="B74">
-        <v>291</v>
-      </c>
-      <c r="C74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="4">
-        <v>43973</v>
-      </c>
-      <c r="B75">
-        <v>295</v>
-      </c>
-      <c r="C75">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="4">
-        <v>43974</v>
-      </c>
-      <c r="B76">
-        <v>299</v>
-      </c>
-      <c r="C76">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="4">
-        <v>43975</v>
-      </c>
-      <c r="B77">
-        <v>306</v>
-      </c>
-      <c r="C77">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="4">
-        <v>43976</v>
-      </c>
-      <c r="B78">
-        <v>310</v>
-      </c>
-      <c r="C78">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="4">
-        <v>43977</v>
-      </c>
-      <c r="B79">
-        <v>313</v>
-      </c>
-      <c r="C79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" s="4">
-        <v>43978</v>
-      </c>
-      <c r="B80">
-        <v>315</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="4">
-        <v>43979</v>
-      </c>
-      <c r="B81">
-        <v>320</v>
-      </c>
-      <c r="C81">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="4">
-        <v>43980</v>
-      </c>
-      <c r="B82">
-        <v>326</v>
-      </c>
-      <c r="C82">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="4">
-        <v>43981</v>
-      </c>
-      <c r="B83">
-        <v>330</v>
-      </c>
-      <c r="C83">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="4">
-        <v>43982</v>
-      </c>
-      <c r="B84">
-        <v>336</v>
-      </c>
-      <c r="C84">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="4">
-        <v>43983</v>
-      </c>
-      <c r="B85">
-        <v>344</v>
-      </c>
-      <c r="C85">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="4">
-        <v>43984</v>
-      </c>
-      <c r="B86">
-        <v>352</v>
-      </c>
-      <c r="C86">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="4">
-        <v>43985</v>
-      </c>
-      <c r="B87">
-        <v>357</v>
-      </c>
-      <c r="C87">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="4">
-        <v>43986</v>
-      </c>
-      <c r="B88">
-        <v>363</v>
-      </c>
-      <c r="C88">
-        <f>B88-B87</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="4">
-        <v>43987</v>
-      </c>
-      <c r="B89">
-        <v>370</v>
-      </c>
-      <c r="C89">
-        <f t="shared" ref="C89:C93" si="0">B89-B88</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="4">
-        <v>43988</v>
-      </c>
-      <c r="B90">
-        <v>386</v>
-      </c>
-      <c r="C90">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="4">
-        <v>43989</v>
-      </c>
-      <c r="B91">
-        <v>393</v>
-      </c>
-      <c r="C91">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="4">
-        <v>43990</v>
-      </c>
-      <c r="B92">
-        <v>398</v>
-      </c>
-      <c r="C92">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="4">
-        <v>43991</v>
-      </c>
-      <c r="B93">
-        <v>403</v>
-      </c>
-      <c r="C93">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -8732,16 +8732,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>16</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-11-2020 22-33-15
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1479" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B63A2F0-0385-47FA-8557-4BE9E929A4E2}"/>
+  <xr:revisionPtr revIDLastSave="1486" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA4D1DC-D0CA-4781-B956-E32E70DBFF11}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$94</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C93" totalsRowShown="0">
-  <autoFilter ref="A1:C93" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C94" totalsRowShown="0">
+  <autoFilter ref="A1:C94" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C93" totalsRowShown="0">
-  <autoFilter ref="A1:C93" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C94" totalsRowShown="0">
+  <autoFilter ref="A1:C94" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M94" totalsRowShown="0">
-  <autoFilter ref="A1:M94" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M95" totalsRowShown="0">
+  <autoFilter ref="A1:M95" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC93"/>
+  <dimension ref="A1:BC94"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3656,6 +3656,18 @@
         <v>160</v>
       </c>
     </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="4">
+        <v>43992</v>
+      </c>
+      <c r="B94">
+        <v>10977</v>
+      </c>
+      <c r="C94">
+        <f>B94-B93</f>
+        <v>416</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3669,10 +3681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88:C93"/>
+      <selection activeCell="C93" sqref="C93:C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4719,7 +4731,7 @@
         <v>370</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89:C93" si="0">B89-B88</f>
+        <f t="shared" ref="C89:C94" si="0">B89-B88</f>
         <v>7</v>
       </c>
     </row>
@@ -4769,6 +4781,18 @@
       <c r="C93">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="4">
+        <v>43992</v>
+      </c>
+      <c r="B94">
+        <v>413</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4781,11 +4805,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N94" sqref="N94"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8685,6 +8709,31 @@
       <c r="M94" s="6">
         <v>5</v>
       </c>
+    </row>
+    <row r="95" spans="1:13">
+      <c r="A95" s="9">
+        <v>43992</v>
+      </c>
+      <c r="B95" s="6">
+        <v>17889</v>
+      </c>
+      <c r="C95" s="10">
+        <f>IFERROR(B95-B94,"")</f>
+        <v>656</v>
+      </c>
+      <c r="D95" s="6"/>
+      <c r="E95" s="10">
+        <f>C95-D95</f>
+        <v>656</v>
+      </c>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16399,85 +16448,85 @@
       </c>
     </row>
     <row r="95" spans="1:20">
-      <c r="A95" s="4" t="str">
+      <c r="A95" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B95" t="str">
+        <v>43992</v>
+      </c>
+      <c r="B95">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C95" t="str">
+        <v>17889</v>
+      </c>
+      <c r="C95">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>656</v>
       </c>
       <c r="D95">
         <f>+IFERROR('Fallecidos Diarios'!B94,"")</f>
-        <v>0</v>
+        <v>413</v>
       </c>
       <c r="E95">
         <f>+IFERROR('Fallecidos Diarios'!C94,"")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F95">
         <f>+IFERROR('Recuperados Diarios'!B94,"")</f>
-        <v>0</v>
+        <v>10977</v>
       </c>
       <c r="G95">
         <f>+IFERROR('Recuperados Diarios'!C94,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H95" t="str">
+        <v>416</v>
+      </c>
+      <c r="H95">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I95" t="str">
+        <v>6499</v>
+      </c>
+      <c r="I95">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J95" t="str">
+        <v>230</v>
+      </c>
+      <c r="J95">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K95" t="str">
+        <v>2.3086813125384315E-2</v>
+      </c>
+      <c r="K95">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L95" t="str">
+        <v>0.61361730672480297</v>
+      </c>
+      <c r="L95">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M95" t="str">
+        <v>0.36329588014981273</v>
+      </c>
+      <c r="M95">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N95" t="str">
+        <v>1805.6907216494844</v>
+      </c>
+      <c r="N95">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O95" t="str">
+        <v>2.4213075060532687E-2</v>
+      </c>
+      <c r="O95">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P95" t="str">
+        <v>3.7897421882117151E-2</v>
+      </c>
+      <c r="P95">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q95" t="str">
+        <v>3.5390060009232192E-2</v>
+      </c>
+      <c r="Q95">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4301.2743447944222</v>
       </c>
       <c r="R95">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>99.302716999278672</v>
       </c>
       <c r="S95">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T95" t="str">
+        <v>2639.3363789372447</v>
+      </c>
+      <c r="T95">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1562.6352488578987</v>
       </c>
     </row>
     <row r="96" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-12-2020 02-33-38
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1486" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FA4D1DC-D0CA-4781-B956-E32E70DBFF11}"/>
+  <xr:revisionPtr revIDLastSave="1493" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49965F50-B8D0-44D7-8994-204E019A71C4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$94</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$95</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C94" totalsRowShown="0">
-  <autoFilter ref="A1:C94" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C95" totalsRowShown="0">
+  <autoFilter ref="A1:C95" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C94" totalsRowShown="0">
-  <autoFilter ref="A1:C94" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C95" totalsRowShown="0">
+  <autoFilter ref="A1:C95" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M95" totalsRowShown="0">
-  <autoFilter ref="A1:M95" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M96" totalsRowShown="0">
+  <autoFilter ref="A1:M96" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC94"/>
+  <dimension ref="A1:BC95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3668,6 +3668,18 @@
         <v>416</v>
       </c>
     </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B95">
+        <v>11077</v>
+      </c>
+      <c r="C95">
+        <f>B95-B94</f>
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3681,10 +3693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93:C94"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94:C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4731,7 +4743,7 @@
         <v>370</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89:C94" si="0">B89-B88</f>
+        <f t="shared" ref="C89:C95" si="0">B89-B88</f>
         <v>7</v>
       </c>
     </row>
@@ -4793,6 +4805,18 @@
       <c r="C94">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="4">
+        <v>43993</v>
+      </c>
+      <c r="B95">
+        <v>418</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4805,11 +4829,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M95"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
+      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8734,6 +8758,31 @@
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
       <c r="M95" s="6"/>
+    </row>
+    <row r="96" spans="1:13">
+      <c r="A96" s="9">
+        <v>43993</v>
+      </c>
+      <c r="B96" s="6">
+        <v>18586</v>
+      </c>
+      <c r="C96" s="10">
+        <f>IFERROR(B96-B95,"")</f>
+        <v>697</v>
+      </c>
+      <c r="D96" s="6"/>
+      <c r="E96" s="10">
+        <f>C96-D96</f>
+        <v>697</v>
+      </c>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16530,85 +16579,85 @@
       </c>
     </row>
     <row r="96" spans="1:20">
-      <c r="A96" s="4" t="str">
+      <c r="A96" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B96" t="str">
+        <v>43993</v>
+      </c>
+      <c r="B96">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C96" t="str">
+        <v>18586</v>
+      </c>
+      <c r="C96">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>697</v>
       </c>
       <c r="D96">
         <f>+IFERROR('Fallecidos Diarios'!B95,"")</f>
-        <v>0</v>
+        <v>418</v>
       </c>
       <c r="E96">
         <f>+IFERROR('Fallecidos Diarios'!C95,"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F96">
         <f>+IFERROR('Recuperados Diarios'!B95,"")</f>
-        <v>0</v>
+        <v>11077</v>
       </c>
       <c r="G96">
         <f>+IFERROR('Recuperados Diarios'!C95,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H96" t="str">
+        <v>100</v>
+      </c>
+      <c r="H96">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I96" t="str">
+        <v>7091</v>
+      </c>
+      <c r="I96">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J96" t="str">
+        <v>592</v>
+      </c>
+      <c r="J96">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K96" t="str">
+        <v>2.2490046271387065E-2</v>
+      </c>
+      <c r="K96">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L96" t="str">
+        <v>0.59598622619175723</v>
+      </c>
+      <c r="L96">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M96" t="str">
+        <v>0.38152372753685571</v>
+      </c>
+      <c r="M96">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N96" t="str">
+        <v>1826.8850655760823</v>
+      </c>
+      <c r="N96">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O96" t="str">
+        <v>1.1961722488038277E-2</v>
+      </c>
+      <c r="O96">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P96" t="str">
+        <v>9.0277150853119072E-3</v>
+      </c>
+      <c r="P96">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q96" t="str">
+        <v>8.3486109152446766E-2</v>
+      </c>
+      <c r="Q96">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4468.8627073815824</v>
       </c>
       <c r="R96">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>100.50492906948786</v>
       </c>
       <c r="S96">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T96" t="str">
+        <v>2663.3806203414283</v>
+      </c>
+      <c r="T96">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1704.9771579706662</v>
       </c>
     </row>
     <row r="97" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-12-2020 18-35-10
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1493" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49965F50-B8D0-44D7-8994-204E019A71C4}"/>
+  <xr:revisionPtr revIDLastSave="1511" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF6AA370-539A-49B2-8704-C123409C03E2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -754,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+    <sheetView topLeftCell="A84" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -4831,9 +4831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M97" sqref="M97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8745,19 +8745,37 @@
         <f>IFERROR(B95-B94,"")</f>
         <v>656</v>
       </c>
-      <c r="D95" s="6"/>
+      <c r="D95" s="6">
+        <v>316</v>
+      </c>
       <c r="E95" s="10">
         <f>C95-D95</f>
-        <v>656</v>
-      </c>
-      <c r="F95" s="6"/>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
-      <c r="I95" s="6"/>
-      <c r="J95" s="6"/>
-      <c r="K95" s="6"/>
-      <c r="L95" s="6"/>
-      <c r="M95" s="6"/>
+        <v>340</v>
+      </c>
+      <c r="F95" s="6">
+        <v>39</v>
+      </c>
+      <c r="G95" s="6">
+        <v>35</v>
+      </c>
+      <c r="H95" s="6">
+        <v>191</v>
+      </c>
+      <c r="I95" s="6">
+        <v>155</v>
+      </c>
+      <c r="J95" s="6">
+        <v>117</v>
+      </c>
+      <c r="K95" s="6">
+        <v>79</v>
+      </c>
+      <c r="L95" s="6">
+        <v>45</v>
+      </c>
+      <c r="M95" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="9">
@@ -8770,19 +8788,37 @@
         <f>IFERROR(B96-B95,"")</f>
         <v>697</v>
       </c>
-      <c r="D96" s="6"/>
+      <c r="D96" s="6">
+        <v>297</v>
+      </c>
       <c r="E96" s="10">
         <f>C96-D96</f>
-        <v>697</v>
-      </c>
-      <c r="F96" s="6"/>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
-      <c r="I96" s="6"/>
-      <c r="J96" s="6"/>
-      <c r="K96" s="6"/>
-      <c r="L96" s="6"/>
-      <c r="M96" s="6"/>
+        <v>400</v>
+      </c>
+      <c r="F96" s="6">
+        <v>50</v>
+      </c>
+      <c r="G96" s="6">
+        <v>42</v>
+      </c>
+      <c r="H96" s="6">
+        <v>189</v>
+      </c>
+      <c r="I96" s="6">
+        <v>143</v>
+      </c>
+      <c r="J96" s="6">
+        <v>116</v>
+      </c>
+      <c r="K96" s="6">
+        <v>77</v>
+      </c>
+      <c r="L96" s="6">
+        <v>65</v>
+      </c>
+      <c r="M96" s="6">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-13-2020 14-51-10
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1511" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF6AA370-539A-49B2-8704-C123409C03E2}"/>
+  <xr:revisionPtr revIDLastSave="1518" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{093F0A47-9784-4C2B-AA21-E75383D5D8D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$96</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C95" totalsRowShown="0">
-  <autoFilter ref="A1:C95" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C96" totalsRowShown="0">
+  <autoFilter ref="A1:C96" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C95" totalsRowShown="0">
-  <autoFilter ref="A1:C95" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C96" totalsRowShown="0">
+  <autoFilter ref="A1:C96" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M96" totalsRowShown="0">
-  <autoFilter ref="A1:M96" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M97" totalsRowShown="0">
+  <autoFilter ref="A1:M97" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC95"/>
+  <dimension ref="A1:BC96"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3680,6 +3680,18 @@
         <v>100</v>
       </c>
     </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B96">
+        <v>13759</v>
+      </c>
+      <c r="C96">
+        <f>B96-B95</f>
+        <v>2682</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3693,10 +3705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94:C95"/>
+      <selection activeCell="C95" sqref="C95:C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4743,7 +4755,7 @@
         <v>370</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89:C95" si="0">B89-B88</f>
+        <f t="shared" ref="C89:C96" si="0">B89-B88</f>
         <v>7</v>
       </c>
     </row>
@@ -4817,6 +4829,18 @@
       <c r="C95">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="4">
+        <v>43994</v>
+      </c>
+      <c r="B96">
+        <v>421</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4829,11 +4853,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M97" sqref="M97"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8819,6 +8843,31 @@
       <c r="M96" s="6">
         <v>6</v>
       </c>
+    </row>
+    <row r="97" spans="1:13">
+      <c r="A97" s="9">
+        <v>43994</v>
+      </c>
+      <c r="B97" s="6">
+        <v>19211</v>
+      </c>
+      <c r="C97" s="10">
+        <f>IFERROR(B97-B96,"")</f>
+        <v>625</v>
+      </c>
+      <c r="D97" s="6"/>
+      <c r="E97" s="10">
+        <f>C97-D97</f>
+        <v>625</v>
+      </c>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16697,85 +16746,85 @@
       </c>
     </row>
     <row r="97" spans="1:20">
-      <c r="A97" s="4" t="str">
+      <c r="A97" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B97" t="str">
+        <v>43994</v>
+      </c>
+      <c r="B97">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C97" t="str">
+        <v>19211</v>
+      </c>
+      <c r="C97">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>625</v>
       </c>
       <c r="D97">
         <f>+IFERROR('Fallecidos Diarios'!B96,"")</f>
-        <v>0</v>
+        <v>421</v>
       </c>
       <c r="E97">
         <f>+IFERROR('Fallecidos Diarios'!C96,"")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F97">
         <f>+IFERROR('Recuperados Diarios'!B96,"")</f>
-        <v>0</v>
+        <v>13759</v>
       </c>
       <c r="G97">
         <f>+IFERROR('Recuperados Diarios'!C96,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H97" t="str">
+        <v>2682</v>
+      </c>
+      <c r="H97">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I97" t="str">
+        <v>5031</v>
+      </c>
+      <c r="I97">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J97" t="str">
+        <v>-2060</v>
+      </c>
+      <c r="J97">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K97" t="str">
+        <v>2.1914528134922701E-2</v>
+      </c>
+      <c r="K97">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L97" t="str">
+        <v>0.71620425797720055</v>
+      </c>
+      <c r="L97">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M97" t="str">
+        <v>0.26188121388787672</v>
+      </c>
+      <c r="M97">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N97" t="str">
+        <v>2386.5782150665873</v>
+      </c>
+      <c r="N97">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O97" t="str">
+        <v>7.1258907363420431E-3</v>
+      </c>
+      <c r="O97">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P97" t="str">
+        <v>0.19492695690093756</v>
+      </c>
+      <c r="P97">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q97" t="str">
+        <v>-0.40946133969389781</v>
+      </c>
+      <c r="Q97">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4619.1392161577305</v>
       </c>
       <c r="R97">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>101.22625631161337</v>
       </c>
       <c r="S97">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T97" t="str">
+        <v>3308.2471748016351</v>
+      </c>
+      <c r="T97">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1209.6657850444819</v>
       </c>
     </row>
     <row r="98" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-14-2020 02-20-04
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1518" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{093F0A47-9784-4C2B-AA21-E75383D5D8D1}"/>
+  <xr:revisionPtr revIDLastSave="1526" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CA48D36-B818-4F9C-BD74-132996F918E8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$97</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C96" totalsRowShown="0">
-  <autoFilter ref="A1:C96" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C97" totalsRowShown="0">
+  <autoFilter ref="A1:C97" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C96" totalsRowShown="0">
-  <autoFilter ref="A1:C96" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C97" totalsRowShown="0">
+  <autoFilter ref="A1:C97" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M97" totalsRowShown="0">
-  <autoFilter ref="A1:M97" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M98" totalsRowShown="0">
+  <autoFilter ref="A1:M98" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC96"/>
+  <dimension ref="A1:BC97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3692,6 +3692,18 @@
         <v>2682</v>
       </c>
     </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="4">
+        <v>43995</v>
+      </c>
+      <c r="B97">
+        <v>13759</v>
+      </c>
+      <c r="C97">
+        <f>B97-B96</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3705,10 +3717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95:C96"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4839,8 +4851,20 @@
         <v>421</v>
       </c>
       <c r="C96">
-        <f t="shared" si="0"/>
+        <f>B96-B95</f>
         <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="4">
+        <v>43995</v>
+      </c>
+      <c r="B97">
+        <v>429</v>
+      </c>
+      <c r="C97">
+        <f>B97-B96</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -4853,11 +4877,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
+      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8868,6 +8892,31 @@
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
       <c r="M97" s="6"/>
+    </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="9">
+        <v>43995</v>
+      </c>
+      <c r="B98" s="6">
+        <v>20059</v>
+      </c>
+      <c r="C98" s="10">
+        <f>IFERROR(B98-B97,"")</f>
+        <v>848</v>
+      </c>
+      <c r="D98" s="6"/>
+      <c r="E98" s="10">
+        <f>C98-D98</f>
+        <v>848</v>
+      </c>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16828,85 +16877,85 @@
       </c>
     </row>
     <row r="98" spans="1:20">
-      <c r="A98" s="4" t="str">
+      <c r="A98" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B98" t="str">
+        <v>43995</v>
+      </c>
+      <c r="B98">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C98" t="str">
+        <v>20059</v>
+      </c>
+      <c r="C98">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>848</v>
       </c>
       <c r="D98">
         <f>+IFERROR('Fallecidos Diarios'!B97,"")</f>
-        <v>0</v>
+        <v>429</v>
       </c>
       <c r="E98">
         <f>+IFERROR('Fallecidos Diarios'!C97,"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F98">
         <f>+IFERROR('Recuperados Diarios'!B97,"")</f>
-        <v>0</v>
+        <v>13759</v>
       </c>
       <c r="G98">
         <f>+IFERROR('Recuperados Diarios'!C97,"")</f>
         <v>0</v>
       </c>
-      <c r="H98" t="str">
+      <c r="H98">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I98" t="str">
+        <v>5871</v>
+      </c>
+      <c r="I98">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J98" t="str">
+        <v>840</v>
+      </c>
+      <c r="J98">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K98" t="str">
+        <v>2.1386908619572261E-2</v>
+      </c>
+      <c r="K98">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L98" t="str">
+        <v>0.6859265167755122</v>
+      </c>
+      <c r="L98">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M98" t="str">
+        <v>0.29268657460491548</v>
+      </c>
+      <c r="M98">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N98" t="str">
+        <v>2897.2972236416285</v>
+      </c>
+      <c r="N98">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O98" t="str">
+        <v>1.8648018648018648E-2</v>
+      </c>
+      <c r="O98">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P98" t="str">
+        <v>0</v>
+      </c>
+      <c r="P98">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q98" t="str">
+        <v>0.14307613694430249</v>
+      </c>
+      <c r="Q98">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4823.0343832652079</v>
       </c>
       <c r="R98">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>103.14979562394807</v>
       </c>
       <c r="S98">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T98" t="str">
+        <v>3308.2471748016351</v>
+      </c>
+      <c r="T98">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1411.6374128396251</v>
       </c>
     </row>
     <row r="99" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-16-2020 00-26-02
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23007"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1526" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CA48D36-B818-4F9C-BD74-132996F918E8}"/>
+  <xr:revisionPtr revIDLastSave="1567" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB4AE087-6111-4FF7-8E4D-A410D0432145}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$99</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C97" totalsRowShown="0">
-  <autoFilter ref="A1:C97" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C99" totalsRowShown="0">
+  <autoFilter ref="A1:C99" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C97" totalsRowShown="0">
-  <autoFilter ref="A1:C97" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C99" totalsRowShown="0">
+  <autoFilter ref="A1:C99" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M98" totalsRowShown="0">
-  <autoFilter ref="A1:M98" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M100" totalsRowShown="0">
+  <autoFilter ref="A1:M100" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC97"/>
+  <dimension ref="A1:BC99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3704,6 +3704,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="4">
+        <v>43996</v>
+      </c>
+      <c r="B98">
+        <v>13766</v>
+      </c>
+      <c r="C98">
+        <f>B98-B97</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="4">
+        <v>43997</v>
+      </c>
+      <c r="B99">
+        <v>13766</v>
+      </c>
+      <c r="C99">
+        <f>B99-B98</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3717,10 +3741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4867,6 +4891,30 @@
         <v>8</v>
       </c>
     </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="4">
+        <v>43996</v>
+      </c>
+      <c r="B98">
+        <v>437</v>
+      </c>
+      <c r="C98">
+        <f>B98-B97</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="4">
+        <v>43997</v>
+      </c>
+      <c r="B99">
+        <v>448</v>
+      </c>
+      <c r="C99">
+        <f>B99-B98</f>
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4877,11 +4925,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8884,14 +8932,18 @@
         <f>C97-D97</f>
         <v>625</v>
       </c>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-      <c r="I97" s="6"/>
-      <c r="J97" s="6"/>
-      <c r="K97" s="6"/>
-      <c r="L97" s="6"/>
-      <c r="M97" s="6"/>
+      <c r="F97">
+        <v>43</v>
+      </c>
+      <c r="G97">
+        <v>38</v>
+      </c>
+      <c r="H97">
+        <v>204</v>
+      </c>
+      <c r="I97">
+        <v>117</v>
+      </c>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="9">
@@ -8909,14 +8961,96 @@
         <f>C98-D98</f>
         <v>848</v>
       </c>
-      <c r="F98" s="6"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="6"/>
-      <c r="I98" s="6"/>
-      <c r="J98" s="6"/>
-      <c r="K98" s="6"/>
-      <c r="L98" s="6"/>
-      <c r="M98" s="6"/>
+      <c r="F98" s="6">
+        <v>55</v>
+      </c>
+      <c r="G98" s="6">
+        <v>49</v>
+      </c>
+      <c r="H98" s="6">
+        <v>243</v>
+      </c>
+      <c r="I98" s="6">
+        <v>168</v>
+      </c>
+      <c r="J98" s="6">
+        <v>155</v>
+      </c>
+      <c r="K98" s="6">
+        <v>87</v>
+      </c>
+      <c r="L98" s="6">
+        <v>82</v>
+      </c>
+      <c r="M98" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
+      <c r="A99" s="9">
+        <v>43996</v>
+      </c>
+      <c r="B99">
+        <v>20686</v>
+      </c>
+      <c r="C99" s="10">
+        <f t="shared" ref="C99:C100" si="6">IFERROR(B99-B98,"")</f>
+        <v>627</v>
+      </c>
+      <c r="D99" s="6"/>
+      <c r="E99" s="10">
+        <f>C99-D99</f>
+        <v>627</v>
+      </c>
+      <c r="F99" s="6">
+        <v>28</v>
+      </c>
+      <c r="G99" s="6">
+        <v>45</v>
+      </c>
+      <c r="H99" s="6">
+        <v>187</v>
+      </c>
+      <c r="I99" s="6">
+        <v>119</v>
+      </c>
+      <c r="J99" s="6">
+        <v>105</v>
+      </c>
+      <c r="K99" s="6">
+        <v>82</v>
+      </c>
+      <c r="L99" s="6">
+        <v>47</v>
+      </c>
+      <c r="M99" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
+      <c r="A100" s="9">
+        <v>43997</v>
+      </c>
+      <c r="B100" s="6">
+        <v>21422</v>
+      </c>
+      <c r="C100" s="10">
+        <f t="shared" si="6"/>
+        <v>736</v>
+      </c>
+      <c r="D100" s="6"/>
+      <c r="E100" s="10">
+        <f>C100-D100</f>
+        <v>736</v>
+      </c>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16959,167 +17093,167 @@
       </c>
     </row>
     <row r="99" spans="1:20">
-      <c r="A99" s="4" t="str">
+      <c r="A99" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B99" t="str">
+        <v>43996</v>
+      </c>
+      <c r="B99">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C99" t="str">
+        <v>20686</v>
+      </c>
+      <c r="C99">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>627</v>
       </c>
       <c r="D99">
         <f>+IFERROR('Fallecidos Diarios'!B98,"")</f>
-        <v>0</v>
+        <v>437</v>
       </c>
       <c r="E99">
         <f>+IFERROR('Fallecidos Diarios'!C98,"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F99">
         <f>+IFERROR('Recuperados Diarios'!B98,"")</f>
-        <v>0</v>
+        <v>13766</v>
       </c>
       <c r="G99">
         <f>+IFERROR('Recuperados Diarios'!C98,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H99" t="str">
+        <v>7</v>
+      </c>
+      <c r="H99">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I99" t="str">
+        <v>6483</v>
+      </c>
+      <c r="I99">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J99" t="str">
+        <v>612</v>
+      </c>
+      <c r="J99">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K99" t="str">
+        <v>2.1125398820458281E-2</v>
+      </c>
+      <c r="K99">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L99" t="str">
+        <v>0.66547423378130133</v>
+      </c>
+      <c r="L99">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M99" t="str">
+        <v>0.31340036739824034</v>
+      </c>
+      <c r="M99">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N99" t="str">
+        <v>2000.6358167515041</v>
+      </c>
+      <c r="N99">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O99" t="str">
+        <v>1.8306636155606407E-2</v>
+      </c>
+      <c r="O99">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P99" t="str">
+        <v>5.0849920092982707E-4</v>
+      </c>
+      <c r="P99">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q99" t="str">
+        <v>9.4400740397963909E-2</v>
+      </c>
+      <c r="Q99">
         <f t="shared" si="21"/>
-        <v/>
+        <v>4973.7917768694397</v>
       </c>
       <c r="R99">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>105.07333493628276</v>
       </c>
       <c r="S99">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T99" t="str">
+        <v>3309.9302716999282</v>
+      </c>
+      <c r="T99">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1558.7881702332293</v>
       </c>
     </row>
     <row r="100" spans="1:20">
-      <c r="A100" s="4" t="str">
+      <c r="A100" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B100" t="str">
+        <v>43997</v>
+      </c>
+      <c r="B100">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C100" t="str">
+        <v>21422</v>
+      </c>
+      <c r="C100">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>736</v>
       </c>
       <c r="D100">
         <f>+IFERROR('Fallecidos Diarios'!B99,"")</f>
-        <v>0</v>
+        <v>448</v>
       </c>
       <c r="E100">
         <f>+IFERROR('Fallecidos Diarios'!C99,"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F100">
         <f>+IFERROR('Recuperados Diarios'!B99,"")</f>
-        <v>0</v>
+        <v>13766</v>
       </c>
       <c r="G100">
         <f>+IFERROR('Recuperados Diarios'!C99,"")</f>
         <v>0</v>
       </c>
-      <c r="H100" t="str">
+      <c r="H100">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I100" t="str">
+        <v>7208</v>
+      </c>
+      <c r="I100">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J100" t="str">
+        <v>725</v>
+      </c>
+      <c r="J100">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K100" t="str">
+        <v>2.0913080011203435E-2</v>
+      </c>
+      <c r="K100">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L100" t="str">
+        <v>0.64261040052282703</v>
+      </c>
+      <c r="L100">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M100" t="str">
+        <v>0.33647651946596957</v>
+      </c>
+      <c r="M100">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N100" t="str">
+        <v>2187.3740288568256</v>
+      </c>
+      <c r="N100">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O100" t="str">
+        <v>2.4553571428571428E-2</v>
+      </c>
+      <c r="O100">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P100" t="str">
+        <v>0</v>
+      </c>
+      <c r="P100">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q100" t="str">
+        <v>0.1005826859045505</v>
+      </c>
+      <c r="Q100">
         <f t="shared" si="21"/>
-        <v/>
+        <v>5150.7573936042318</v>
       </c>
       <c r="R100">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>107.71820149074297</v>
       </c>
       <c r="S100">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T100" t="str">
+        <v>3309.9302716999282</v>
+      </c>
+      <c r="T100">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1733.108920413561</v>
       </c>
     </row>
     <row r="101" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-16-2020 04-26-44
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1567" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB4AE087-6111-4FF7-8E4D-A410D0432145}"/>
+  <xr:revisionPtr revIDLastSave="1571" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{91DEA401-A687-4135-9977-23CFD52B5857}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4928,8 +4928,8 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J97" sqref="J97"/>
+      <pane ySplit="1" topLeftCell="B92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -8943,6 +8943,18 @@
       </c>
       <c r="I97">
         <v>117</v>
+      </c>
+      <c r="J97">
+        <v>103</v>
+      </c>
+      <c r="K97">
+        <v>56</v>
+      </c>
+      <c r="L97">
+        <v>56</v>
+      </c>
+      <c r="M97">
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:13">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-18-2020 16-35-50
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1583" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A917CE58-ACE1-4022-9A0D-98E34CBB5597}"/>
+  <xr:revisionPtr revIDLastSave="1598" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9EF00F3B-B9E9-4682-B563-CFFDDA4481CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$101</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C99" totalsRowShown="0">
-  <autoFilter ref="A1:C99" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C99" totalsRowShown="0">
-  <autoFilter ref="A1:C99" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C101" totalsRowShown="0">
+  <autoFilter ref="A1:C101" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M100" totalsRowShown="0">
-  <autoFilter ref="A1:M100" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M102" totalsRowShown="0">
+  <autoFilter ref="A1:M102" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC99"/>
+  <dimension ref="A1:BC101"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3728,6 +3728,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="4">
+        <v>43998</v>
+      </c>
+      <c r="B100">
+        <v>13774</v>
+      </c>
+      <c r="C100">
+        <f>B100-B99</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="4">
+        <v>43999</v>
+      </c>
+      <c r="B101">
+        <v>13774</v>
+      </c>
+      <c r="C101">
+        <f>B101-B100</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3741,10 +3765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4915,6 +4939,30 @@
         <v>11</v>
       </c>
     </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="4">
+        <v>43998</v>
+      </c>
+      <c r="B100">
+        <v>457</v>
+      </c>
+      <c r="C100">
+        <f t="shared" ref="C100:C101" si="1">B100-B99</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="4">
+        <v>43999</v>
+      </c>
+      <c r="B101">
+        <v>470</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4925,11 +4973,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M100"/>
+  <dimension ref="A1:M102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N100" sqref="N100"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9087,6 +9135,58 @@
       <c r="M100" s="6">
         <v>17</v>
       </c>
+    </row>
+    <row r="101" spans="1:13">
+      <c r="A101" s="9">
+        <v>43998</v>
+      </c>
+      <c r="B101" s="6">
+        <v>21962</v>
+      </c>
+      <c r="C101" s="10">
+        <f>IFERROR(B101-B100,"")</f>
+        <v>540</v>
+      </c>
+      <c r="D101" s="6">
+        <v>254</v>
+      </c>
+      <c r="E101" s="10">
+        <f>C101-D101</f>
+        <v>286</v>
+      </c>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+    </row>
+    <row r="102" spans="1:13">
+      <c r="A102" s="9">
+        <v>43999</v>
+      </c>
+      <c r="B102" s="6">
+        <v>22597</v>
+      </c>
+      <c r="C102" s="10">
+        <f>IFERROR(B102-B101,"")</f>
+        <v>635</v>
+      </c>
+      <c r="D102" s="6"/>
+      <c r="E102" s="10">
+        <f>C102-D102</f>
+        <v>635</v>
+      </c>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17293,167 +17393,167 @@
       </c>
     </row>
     <row r="101" spans="1:20">
-      <c r="A101" s="4" t="str">
+      <c r="A101" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B101" t="str">
+        <v>43998</v>
+      </c>
+      <c r="B101">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C101" t="str">
+        <v>21962</v>
+      </c>
+      <c r="C101">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>540</v>
       </c>
       <c r="D101">
         <f>+IFERROR('Fallecidos Diarios'!B100,"")</f>
-        <v>0</v>
+        <v>457</v>
       </c>
       <c r="E101">
         <f>+IFERROR('Fallecidos Diarios'!C100,"")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F101">
         <f>+IFERROR('Recuperados Diarios'!B100,"")</f>
-        <v>0</v>
+        <v>13774</v>
       </c>
       <c r="G101">
         <f>+IFERROR('Recuperados Diarios'!C100,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H101" t="str">
+        <v>8</v>
+      </c>
+      <c r="H101">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I101" t="str">
+        <v>7731</v>
+      </c>
+      <c r="I101">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J101" t="str">
+        <v>523</v>
+      </c>
+      <c r="J101">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K101" t="str">
+        <v>2.0808669520080137E-2</v>
+      </c>
+      <c r="K101">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L101" t="str">
+        <v>0.62717420999908935</v>
+      </c>
+      <c r="L101">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M101" t="str">
+        <v>0.3520171204808305</v>
+      </c>
+      <c r="M101">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N101" t="str">
+        <v>1534.0162980209548</v>
+      </c>
+      <c r="N101">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O101" t="str">
+        <v>1.9693654266958426E-2</v>
+      </c>
+      <c r="O101">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P101" t="str">
+        <v>5.8080441411354725E-4</v>
+      </c>
+      <c r="P101">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q101" t="str">
+        <v>6.7649721898848797E-2</v>
+      </c>
+      <c r="Q101">
         <f t="shared" si="21"/>
-        <v/>
+        <v>5280.5962971868239</v>
       </c>
       <c r="R101">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>109.8821832171195</v>
       </c>
       <c r="S101">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T101" t="str">
+        <v>3311.8538110122627</v>
+      </c>
+      <c r="T101">
         <f t="shared" si="24"/>
-        <v/>
+        <v>1858.8603029574417</v>
       </c>
     </row>
     <row r="102" spans="1:20">
-      <c r="A102" s="4" t="str">
+      <c r="A102" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B102" t="str">
+        <v>43999</v>
+      </c>
+      <c r="B102">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C102" t="str">
+        <v>22597</v>
+      </c>
+      <c r="C102">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>635</v>
       </c>
       <c r="D102">
         <f>+IFERROR('Fallecidos Diarios'!B101,"")</f>
-        <v>0</v>
+        <v>470</v>
       </c>
       <c r="E102">
         <f>+IFERROR('Fallecidos Diarios'!C101,"")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F102">
         <f>+IFERROR('Recuperados Diarios'!B101,"")</f>
-        <v>0</v>
+        <v>13774</v>
       </c>
       <c r="G102">
         <f>+IFERROR('Recuperados Diarios'!C101,"")</f>
         <v>0</v>
       </c>
-      <c r="H102" t="str">
+      <c r="H102">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I102" t="str">
+        <v>8353</v>
+      </c>
+      <c r="I102">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J102" t="str">
+        <v>622</v>
+      </c>
+      <c r="J102">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K102" t="str">
+        <v>2.0799221135548968E-2</v>
+      </c>
+      <c r="K102">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L102" t="str">
+        <v>0.60954994025755627</v>
+      </c>
+      <c r="L102">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M102" t="str">
+        <v>0.36965083860689474</v>
+      </c>
+      <c r="M102">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N102" t="str">
+        <v>1717.8373039626481</v>
+      </c>
+      <c r="N102">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O102" t="str">
+        <v>2.7659574468085105E-2</v>
+      </c>
+      <c r="O102">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P102" t="str">
+        <v>0</v>
+      </c>
+      <c r="P102">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q102" t="str">
+        <v>7.4464264336166652E-2</v>
+      </c>
+      <c r="Q102">
         <f t="shared" si="21"/>
-        <v/>
+        <v>5433.2772301033901</v>
       </c>
       <c r="R102">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>113.00793459966339</v>
       </c>
       <c r="S102">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T102" t="str">
+        <v>3311.8538110122627</v>
+      </c>
+      <c r="T102">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2008.4154844914644</v>
       </c>
     </row>
     <row r="103" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-19-2020 16-38-53
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1598" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9EF00F3B-B9E9-4682-B563-CFFDDA4481CF}"/>
+  <xr:revisionPtr revIDLastSave="1631" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{44FEB833-C0A0-4127-9379-B5E42B1344DE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$102</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C102" totalsRowShown="0">
+  <autoFilter ref="A1:C102" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C101" totalsRowShown="0">
-  <autoFilter ref="A1:C101" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C102" totalsRowShown="0">
+  <autoFilter ref="A1:C102" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M102" totalsRowShown="0">
-  <autoFilter ref="A1:M102" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M103" totalsRowShown="0">
+  <autoFilter ref="A1:M103" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC101"/>
+  <dimension ref="A1:BC102"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3752,6 +3752,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="4">
+        <v>44000</v>
+      </c>
+      <c r="B102">
+        <v>13782</v>
+      </c>
+      <c r="C102">
+        <f>B102-B101</f>
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3765,10 +3777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="C101" sqref="C101:C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4947,7 +4959,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C101" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C102" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -4961,6 +4973,18 @@
       <c r="C101">
         <f t="shared" si="1"/>
         <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="4">
+        <v>44000</v>
+      </c>
+      <c r="B102">
+        <v>475</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4973,11 +4997,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M102"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O103" sqref="O103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9154,14 +9178,30 @@
         <f>C101-D101</f>
         <v>286</v>
       </c>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="6"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
+      <c r="F101" s="6">
+        <v>39</v>
+      </c>
+      <c r="G101" s="6">
+        <v>37</v>
+      </c>
+      <c r="H101" s="6">
+        <v>141</v>
+      </c>
+      <c r="I101" s="6">
+        <v>113</v>
+      </c>
+      <c r="J101" s="6">
+        <v>87</v>
+      </c>
+      <c r="K101" s="6">
+        <v>58</v>
+      </c>
+      <c r="L101" s="6">
+        <v>55</v>
+      </c>
+      <c r="M101" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="9">
@@ -9174,19 +9214,80 @@
         <f>IFERROR(B102-B101,"")</f>
         <v>635</v>
       </c>
-      <c r="D102" s="6"/>
+      <c r="D102" s="6">
+        <v>317</v>
+      </c>
       <c r="E102" s="10">
         <f>C102-D102</f>
-        <v>635</v>
-      </c>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
+        <v>318</v>
+      </c>
+      <c r="F102" s="6">
+        <v>44</v>
+      </c>
+      <c r="G102" s="6">
+        <v>49</v>
+      </c>
+      <c r="H102" s="6">
+        <v>162</v>
+      </c>
+      <c r="I102" s="6">
+        <v>131</v>
+      </c>
+      <c r="J102" s="6">
+        <v>114</v>
+      </c>
+      <c r="K102" s="6">
+        <v>69</v>
+      </c>
+      <c r="L102" s="6">
+        <v>57</v>
+      </c>
+      <c r="M102" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13">
+      <c r="A103" s="9">
+        <v>44000</v>
+      </c>
+      <c r="B103" s="6">
+        <v>23351</v>
+      </c>
+      <c r="C103" s="10">
+        <f>IFERROR(B103-B102,"")</f>
+        <v>754</v>
+      </c>
+      <c r="D103" s="6">
+        <v>328</v>
+      </c>
+      <c r="E103" s="10">
+        <f>C103-D103</f>
+        <v>426</v>
+      </c>
+      <c r="F103" s="6">
+        <v>32</v>
+      </c>
+      <c r="G103" s="6">
+        <v>49</v>
+      </c>
+      <c r="H103" s="6">
+        <v>201</v>
+      </c>
+      <c r="I103" s="6">
+        <v>166</v>
+      </c>
+      <c r="J103" s="6">
+        <v>141</v>
+      </c>
+      <c r="K103" s="6">
+        <v>89</v>
+      </c>
+      <c r="L103" s="6">
+        <v>67</v>
+      </c>
+      <c r="M103" s="6">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17557,85 +17658,85 @@
       </c>
     </row>
     <row r="103" spans="1:20">
-      <c r="A103" s="4" t="str">
+      <c r="A103" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B103" t="str">
+        <v>44000</v>
+      </c>
+      <c r="B103">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C103" t="str">
+        <v>23351</v>
+      </c>
+      <c r="C103">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>754</v>
       </c>
       <c r="D103">
         <f>+IFERROR('Fallecidos Diarios'!B102,"")</f>
-        <v>0</v>
+        <v>475</v>
       </c>
       <c r="E103">
         <f>+IFERROR('Fallecidos Diarios'!C102,"")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F103">
         <f>+IFERROR('Recuperados Diarios'!B102,"")</f>
-        <v>0</v>
+        <v>13782</v>
       </c>
       <c r="G103">
         <f>+IFERROR('Recuperados Diarios'!C102,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H103" t="str">
+        <v>8</v>
+      </c>
+      <c r="H103">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I103" t="str">
+        <v>9094</v>
+      </c>
+      <c r="I103">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J103" t="str">
+        <v>741</v>
+      </c>
+      <c r="J103">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K103" t="str">
+        <v>2.034174125305126E-2</v>
+      </c>
+      <c r="K103">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L103" t="str">
+        <v>0.59021026936747889</v>
+      </c>
+      <c r="L103">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M103" t="str">
+        <v>0.38944798937946984</v>
+      </c>
+      <c r="M103">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N103" t="str">
+        <v>1936.0736749505168</v>
+      </c>
+      <c r="N103">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O103" t="str">
+        <v>1.0526315789473684E-2</v>
+      </c>
+      <c r="O103">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P103" t="str">
+        <v>5.8046727615730664E-4</v>
+      </c>
+      <c r="P103">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q103" t="str">
+        <v>8.1482296019353417E-2</v>
+      </c>
+      <c r="Q103">
         <f t="shared" si="21"/>
-        <v/>
+        <v>5614.5708102909357</v>
       </c>
       <c r="R103">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>114.21014666987257</v>
       </c>
       <c r="S103">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T103" t="str">
+        <v>3313.7773503245976</v>
+      </c>
+      <c r="T103">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2186.5833132964658</v>
       </c>
     </row>
     <row r="104" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-20-2020 18-08-09
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1631" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{44FEB833-C0A0-4127-9379-B5E42B1344DE}"/>
+  <xr:revisionPtr revIDLastSave="1647" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E46CFCE-5F06-485A-A720-612ED6D2D3A7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$103</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C102" totalsRowShown="0">
-  <autoFilter ref="A1:C102" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C103" totalsRowShown="0">
+  <autoFilter ref="A1:C103" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C102" totalsRowShown="0">
-  <autoFilter ref="A1:C102" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C103" totalsRowShown="0">
+  <autoFilter ref="A1:C103" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M103" totalsRowShown="0">
-  <autoFilter ref="A1:M103" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M104" totalsRowShown="0">
+  <autoFilter ref="A1:M104" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC102"/>
+  <dimension ref="A1:BC103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3764,6 +3764,18 @@
         <v>8</v>
       </c>
     </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="4">
+        <v>44001</v>
+      </c>
+      <c r="B103">
+        <v>14359</v>
+      </c>
+      <c r="C103">
+        <f>B103-B102</f>
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3777,10 +3789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101:C102"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4959,7 +4971,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C102" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C103" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -4985,6 +4997,18 @@
       <c r="C102">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="4">
+        <v>44001</v>
+      </c>
+      <c r="B103">
+        <v>485</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4997,11 +5021,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O103" sqref="O103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9287,6 +9311,49 @@
       </c>
       <c r="M103" s="6">
         <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13">
+      <c r="A104" s="9">
+        <v>44001</v>
+      </c>
+      <c r="B104" s="6">
+        <v>24274</v>
+      </c>
+      <c r="C104" s="10">
+        <f>IFERROR(B104-B103,"")</f>
+        <v>923</v>
+      </c>
+      <c r="D104" s="6">
+        <v>437</v>
+      </c>
+      <c r="E104" s="10">
+        <f>C104-D104</f>
+        <v>486</v>
+      </c>
+      <c r="F104" s="6">
+        <v>61</v>
+      </c>
+      <c r="G104" s="6">
+        <v>45</v>
+      </c>
+      <c r="H104" s="6">
+        <v>248</v>
+      </c>
+      <c r="I104" s="6">
+        <v>185</v>
+      </c>
+      <c r="J104" s="6">
+        <v>161</v>
+      </c>
+      <c r="K104" s="6">
+        <v>120</v>
+      </c>
+      <c r="L104" s="6">
+        <v>91</v>
+      </c>
+      <c r="M104" s="6">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -17740,85 +17807,85 @@
       </c>
     </row>
     <row r="104" spans="1:20">
-      <c r="A104" s="4" t="str">
+      <c r="A104" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B104" t="str">
+        <v>44001</v>
+      </c>
+      <c r="B104">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C104" t="str">
+        <v>24274</v>
+      </c>
+      <c r="C104">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>923</v>
       </c>
       <c r="D104">
         <f>+IFERROR('Fallecidos Diarios'!B103,"")</f>
-        <v>0</v>
+        <v>485</v>
       </c>
       <c r="E104">
         <f>+IFERROR('Fallecidos Diarios'!C103,"")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F104">
         <f>+IFERROR('Recuperados Diarios'!B103,"")</f>
-        <v>0</v>
+        <v>14359</v>
       </c>
       <c r="G104">
         <f>+IFERROR('Recuperados Diarios'!C103,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H104" t="str">
+        <v>577</v>
+      </c>
+      <c r="H104">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I104" t="str">
+        <v>9430</v>
+      </c>
+      <c r="I104">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J104" t="str">
+        <v>336</v>
+      </c>
+      <c r="J104">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K104" t="str">
+        <v>1.9980225755952871E-2</v>
+      </c>
+      <c r="K104">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L104" t="str">
+        <v>0.5915382714014995</v>
+      </c>
+      <c r="L104">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M104" t="str">
+        <v>0.38848150284254757</v>
+      </c>
+      <c r="M104">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N104" t="str">
+        <v>2375.9174973488866</v>
+      </c>
+      <c r="N104">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O104" t="str">
+        <v>2.0618556701030927E-2</v>
+      </c>
+      <c r="O104">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P104" t="str">
+        <v>4.0183856814541404E-2</v>
+      </c>
+      <c r="P104">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q104" t="str">
+        <v>3.5630965005302224E-2</v>
+      </c>
+      <c r="Q104">
         <f t="shared" si="21"/>
-        <v/>
+        <v>5836.499158451551</v>
       </c>
       <c r="R104">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>116.61457081029094</v>
       </c>
       <c r="S104">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T104" t="str">
+        <v>3452.5126232267376</v>
+      </c>
+      <c r="T104">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2267.3719644145226</v>
       </c>
     </row>
     <row r="105" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-21-2020 04-14-18
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1647" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0E46CFCE-5F06-485A-A720-612ED6D2D3A7}"/>
+  <xr:revisionPtr revIDLastSave="1654" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E1A6647-8D10-4D0A-8E0B-2454AD01BB1D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C103" totalsRowShown="0">
-  <autoFilter ref="A1:C103" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C104" totalsRowShown="0">
+  <autoFilter ref="A1:C104" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C103" totalsRowShown="0">
-  <autoFilter ref="A1:C103" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C104" totalsRowShown="0">
+  <autoFilter ref="A1:C104" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M104" totalsRowShown="0">
-  <autoFilter ref="A1:M104" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M105" totalsRowShown="0">
+  <autoFilter ref="A1:M105" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,7 +752,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC103"/>
+  <dimension ref="A1:BC104"/>
   <sheetViews>
     <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="C105" sqref="C105"/>
@@ -3776,6 +3776,18 @@
         <v>577</v>
       </c>
     </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="4">
+        <v>44002</v>
+      </c>
+      <c r="B104">
+        <v>14359</v>
+      </c>
+      <c r="C104">
+        <f>B104-B103</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3789,10 +3801,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4971,7 +4983,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C103" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C104" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5009,6 +5021,18 @@
       <c r="C103">
         <f t="shared" si="1"/>
         <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="4">
+        <v>44002</v>
+      </c>
+      <c r="B104">
+        <v>493</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5021,11 +5045,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9355,6 +9379,31 @@
       <c r="M104" s="6">
         <v>12</v>
       </c>
+    </row>
+    <row r="105" spans="1:13">
+      <c r="A105" s="9">
+        <v>44002</v>
+      </c>
+      <c r="B105" s="6">
+        <v>25222</v>
+      </c>
+      <c r="C105" s="10">
+        <f>IFERROR(B105-B104,"")</f>
+        <v>948</v>
+      </c>
+      <c r="D105" s="6"/>
+      <c r="E105" s="10">
+        <f>C105-D105</f>
+        <v>948</v>
+      </c>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17889,85 +17938,85 @@
       </c>
     </row>
     <row r="105" spans="1:20">
-      <c r="A105" s="4" t="str">
+      <c r="A105" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B105" t="str">
+        <v>44002</v>
+      </c>
+      <c r="B105">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C105" t="str">
+        <v>25222</v>
+      </c>
+      <c r="C105">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>948</v>
       </c>
       <c r="D105">
         <f>+IFERROR('Fallecidos Diarios'!B104,"")</f>
-        <v>0</v>
+        <v>493</v>
       </c>
       <c r="E105">
         <f>+IFERROR('Fallecidos Diarios'!C104,"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F105">
         <f>+IFERROR('Recuperados Diarios'!B104,"")</f>
-        <v>0</v>
+        <v>14359</v>
       </c>
       <c r="G105">
         <f>+IFERROR('Recuperados Diarios'!C104,"")</f>
         <v>0</v>
       </c>
-      <c r="H105" t="str">
+      <c r="H105">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I105" t="str">
+        <v>10370</v>
+      </c>
+      <c r="I105">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J105" t="str">
+        <v>940</v>
+      </c>
+      <c r="J105">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K105" t="str">
+        <v>1.9546427721830149E-2</v>
+      </c>
+      <c r="K105">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L105" t="str">
+        <v>0.56930457537070811</v>
+      </c>
+      <c r="L105">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M105" t="str">
+        <v>0.41114899690746176</v>
+      </c>
+      <c r="M105">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N105" t="str">
+        <v>2305.733461909354</v>
+      </c>
+      <c r="N105">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O105" t="str">
+        <v>1.6227180527383367E-2</v>
+      </c>
+      <c r="O105">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P105" t="str">
+        <v>0</v>
+      </c>
+      <c r="P105">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q105" t="str">
+        <v>9.0646094503375116E-2</v>
+      </c>
+      <c r="Q105">
         <f t="shared" si="21"/>
-        <v/>
+        <v>6064.4385669632129</v>
       </c>
       <c r="R105">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>118.53811012262564</v>
       </c>
       <c r="S105">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T105" t="str">
+        <v>3452.5126232267376</v>
+      </c>
+      <c r="T105">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2493.3878336138496</v>
       </c>
     </row>
     <row r="106" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-21-2020 20-15-59
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23017"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1654" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E1A6647-8D10-4D0A-8E0B-2454AD01BB1D}"/>
+  <xr:revisionPtr revIDLastSave="1663" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF3EC13A-B089-457A-ADF5-D498B38D96EF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -3803,7 +3803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
@@ -5047,9 +5047,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
   <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L111" sqref="L111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9391,19 +9391,37 @@
         <f>IFERROR(B105-B104,"")</f>
         <v>948</v>
       </c>
-      <c r="D105" s="6"/>
+      <c r="D105" s="6">
+        <v>426</v>
+      </c>
       <c r="E105" s="10">
         <f>C105-D105</f>
-        <v>948</v>
-      </c>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
-      <c r="J105" s="6"/>
-      <c r="K105" s="6"/>
-      <c r="L105" s="6"/>
-      <c r="M105" s="6"/>
+        <v>522</v>
+      </c>
+      <c r="F105" s="6">
+        <v>82</v>
+      </c>
+      <c r="G105" s="6">
+        <v>64</v>
+      </c>
+      <c r="H105" s="6">
+        <v>257</v>
+      </c>
+      <c r="I105" s="6">
+        <v>164</v>
+      </c>
+      <c r="J105" s="6">
+        <v>159</v>
+      </c>
+      <c r="K105" s="6">
+        <v>125</v>
+      </c>
+      <c r="L105" s="6">
+        <v>80</v>
+      </c>
+      <c r="M105" s="6">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-22-2020 16-05-07
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1663" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF3EC13A-B089-457A-ADF5-D498B38D96EF}"/>
+  <xr:revisionPtr revIDLastSave="1679" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED08100C-79D7-4C9F-9AC6-E405A622B116}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$105</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C104" totalsRowShown="0">
-  <autoFilter ref="A1:C104" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C105" totalsRowShown="0">
+  <autoFilter ref="A1:C105" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C104" totalsRowShown="0">
-  <autoFilter ref="A1:C104" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C105" totalsRowShown="0">
+  <autoFilter ref="A1:C105" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M105" totalsRowShown="0">
-  <autoFilter ref="A1:M105" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M106" totalsRowShown="0">
+  <autoFilter ref="A1:M106" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC104"/>
+  <dimension ref="A1:BC105"/>
   <sheetViews>
     <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3788,6 +3788,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="4">
+        <v>44003</v>
+      </c>
+      <c r="B105">
+        <v>14359</v>
+      </c>
+      <c r="C105">
+        <f>B105-B104</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3801,10 +3813,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4983,7 +4995,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C104" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C105" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5031,6 +5043,18 @@
         <v>493</v>
       </c>
       <c r="C104">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="4">
+        <v>44003</v>
+      </c>
+      <c r="B105">
+        <v>501</v>
+      </c>
+      <c r="C105">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -5045,11 +5069,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L111" sqref="L111"/>
+      <pane ySplit="1" topLeftCell="B96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9421,6 +9445,49 @@
       </c>
       <c r="M105" s="6">
         <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13">
+      <c r="A106" s="9">
+        <v>44003</v>
+      </c>
+      <c r="B106" s="6">
+        <v>26030</v>
+      </c>
+      <c r="C106" s="10">
+        <f>IFERROR(B106-B105,"")</f>
+        <v>808</v>
+      </c>
+      <c r="D106" s="6">
+        <v>366</v>
+      </c>
+      <c r="E106" s="10">
+        <f>C106-D106</f>
+        <v>442</v>
+      </c>
+      <c r="F106" s="6">
+        <v>39</v>
+      </c>
+      <c r="G106" s="6">
+        <v>48</v>
+      </c>
+      <c r="H106" s="6">
+        <v>209</v>
+      </c>
+      <c r="I106" s="6">
+        <v>160</v>
+      </c>
+      <c r="J106" s="6">
+        <v>137</v>
+      </c>
+      <c r="K106" s="6">
+        <v>101</v>
+      </c>
+      <c r="L106" s="6">
+        <v>90</v>
+      </c>
+      <c r="M106" s="6">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -18038,85 +18105,85 @@
       </c>
     </row>
     <row r="106" spans="1:20">
-      <c r="A106" s="4" t="str">
+      <c r="A106" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B106" t="str">
+        <v>44003</v>
+      </c>
+      <c r="B106">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C106" t="str">
+        <v>26030</v>
+      </c>
+      <c r="C106">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>808</v>
       </c>
       <c r="D106">
         <f>+IFERROR('Fallecidos Diarios'!B105,"")</f>
-        <v>0</v>
+        <v>501</v>
       </c>
       <c r="E106">
         <f>+IFERROR('Fallecidos Diarios'!C105,"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F106">
         <f>+IFERROR('Recuperados Diarios'!B105,"")</f>
-        <v>0</v>
+        <v>14359</v>
       </c>
       <c r="G106">
         <f>+IFERROR('Recuperados Diarios'!C105,"")</f>
         <v>0</v>
       </c>
-      <c r="H106" t="str">
+      <c r="H106">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I106" t="str">
+        <v>11170</v>
+      </c>
+      <c r="I106">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J106" t="str">
+        <v>800</v>
+      </c>
+      <c r="J106">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K106" t="str">
+        <v>1.9247022666154436E-2</v>
+      </c>
+      <c r="K106">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L106" t="str">
+        <v>0.55163273146369574</v>
+      </c>
+      <c r="L106">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M106" t="str">
+        <v>0.42912024587014985</v>
+      </c>
+      <c r="M106">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N106" t="str">
+        <v>1882.9221128021486</v>
+      </c>
+      <c r="N106">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O106" t="str">
+        <v>1.5968063872255488E-2</v>
+      </c>
+      <c r="O106">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P106" t="str">
+        <v>0</v>
+      </c>
+      <c r="P106">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q106" t="str">
+        <v>7.1620411817367946E-2</v>
+      </c>
+      <c r="Q106">
         <f t="shared" si="21"/>
-        <v/>
+        <v>6258.716037509017</v>
       </c>
       <c r="R106">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>120.46164943496034</v>
       </c>
       <c r="S106">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T106" t="str">
+        <v>3452.5126232267376</v>
+      </c>
+      <c r="T106">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2685.7417648473192</v>
       </c>
     </row>
     <row r="107" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-23-2020 19-02-35
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23017"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23022"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1679" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ED08100C-79D7-4C9F-9AC6-E405A622B116}"/>
+  <xr:revisionPtr revIDLastSave="1695" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3790F157-92BB-4B28-A240-C27E4CA614D9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$106</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C105" totalsRowShown="0">
-  <autoFilter ref="A1:C105" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C106" totalsRowShown="0">
+  <autoFilter ref="A1:C106" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C105" totalsRowShown="0">
-  <autoFilter ref="A1:C105" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C106" totalsRowShown="0">
+  <autoFilter ref="A1:C106" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M106" totalsRowShown="0">
-  <autoFilter ref="A1:M106" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M107" totalsRowShown="0">
+  <autoFilter ref="A1:M107" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC105"/>
+  <dimension ref="A1:BC106"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3800,6 +3800,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B106">
+        <v>14664</v>
+      </c>
+      <c r="C106">
+        <f>B106-B105</f>
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3813,10 +3825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4995,7 +5007,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C105" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C106" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5057,6 +5069,18 @@
       <c r="C105">
         <f t="shared" si="1"/>
         <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="4">
+        <v>44004</v>
+      </c>
+      <c r="B106">
+        <v>521</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5069,11 +5093,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+      <pane ySplit="1" topLeftCell="B103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M108" sqref="M108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9488,6 +9512,49 @@
       </c>
       <c r="M106" s="6">
         <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13">
+      <c r="A107" s="9">
+        <v>44004</v>
+      </c>
+      <c r="B107" s="6">
+        <v>26752</v>
+      </c>
+      <c r="C107" s="10">
+        <f>IFERROR(B107-B106,"")</f>
+        <v>722</v>
+      </c>
+      <c r="D107" s="6">
+        <v>337</v>
+      </c>
+      <c r="E107" s="10">
+        <f>C107-D107</f>
+        <v>385</v>
+      </c>
+      <c r="F107" s="6">
+        <v>40</v>
+      </c>
+      <c r="G107" s="6">
+        <v>54</v>
+      </c>
+      <c r="H107" s="6">
+        <v>164</v>
+      </c>
+      <c r="I107" s="6">
+        <v>140</v>
+      </c>
+      <c r="J107" s="6">
+        <v>135</v>
+      </c>
+      <c r="K107" s="6">
+        <v>94</v>
+      </c>
+      <c r="L107" s="6">
+        <v>77</v>
+      </c>
+      <c r="M107" s="6">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -18187,85 +18254,85 @@
       </c>
     </row>
     <row r="107" spans="1:20">
-      <c r="A107" s="4" t="str">
+      <c r="A107" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B107" t="str">
+        <v>44004</v>
+      </c>
+      <c r="B107">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C107" t="str">
+        <v>26752</v>
+      </c>
+      <c r="C107">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>722</v>
       </c>
       <c r="D107">
         <f>+IFERROR('Fallecidos Diarios'!B106,"")</f>
-        <v>0</v>
+        <v>521</v>
       </c>
       <c r="E107">
         <f>+IFERROR('Fallecidos Diarios'!C106,"")</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F107">
         <f>+IFERROR('Recuperados Diarios'!B106,"")</f>
-        <v>0</v>
+        <v>14664</v>
       </c>
       <c r="G107">
         <f>+IFERROR('Recuperados Diarios'!C106,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H107" t="str">
+        <v>305</v>
+      </c>
+      <c r="H107">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I107" t="str">
+        <v>11567</v>
+      </c>
+      <c r="I107">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J107" t="str">
+        <v>397</v>
+      </c>
+      <c r="J107">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K107" t="str">
+        <v>1.9475179425837319E-2</v>
+      </c>
+      <c r="K107">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L107" t="str">
+        <v>0.5481459330143541</v>
+      </c>
+      <c r="L107">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M107" t="str">
+        <v>0.43237888755980863</v>
+      </c>
+      <c r="M107">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N107" t="str">
+        <v>1669.831762773407</v>
+      </c>
+      <c r="N107">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O107" t="str">
+        <v>3.8387715930902108E-2</v>
+      </c>
+      <c r="O107">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P107" t="str">
+        <v>2.079923622476814E-2</v>
+      </c>
+      <c r="P107">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q107" t="str">
+        <v>3.4321777470389905E-2</v>
+      </c>
+      <c r="Q107">
         <f t="shared" si="21"/>
-        <v/>
+        <v>6432.3154604472229</v>
       </c>
       <c r="R107">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>125.27049771579708</v>
       </c>
       <c r="S107">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T107" t="str">
+        <v>3525.8475595094978</v>
+      </c>
+      <c r="T107">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2781.1974032219287</v>
       </c>
     </row>
     <row r="108" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-25-2020 03-07-13
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23023"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1695" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3790F157-92BB-4B28-A240-C27E4CA614D9}"/>
+  <xr:revisionPtr revIDLastSave="1702" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B4E585C-BBB7-4A62-8B67-2ACDB4EA482C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$107</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C106" totalsRowShown="0">
-  <autoFilter ref="A1:C106" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C107" totalsRowShown="0">
+  <autoFilter ref="A1:C107" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C106" totalsRowShown="0">
-  <autoFilter ref="A1:C106" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C107" totalsRowShown="0">
+  <autoFilter ref="A1:C107" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M107" totalsRowShown="0">
-  <autoFilter ref="A1:M107" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M108" totalsRowShown="0">
+  <autoFilter ref="A1:M108" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC106"/>
+  <dimension ref="A1:BC107"/>
   <sheetViews>
-    <sheetView topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3812,6 +3812,18 @@
         <v>305</v>
       </c>
     </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="4">
+        <v>44005</v>
+      </c>
+      <c r="B107">
+        <v>14694</v>
+      </c>
+      <c r="C107">
+        <f>B107-B106</f>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3825,10 +3837,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E106"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5007,7 +5019,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C106" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C107" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5081,6 +5093,18 @@
       <c r="C106">
         <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="4">
+        <v>44005</v>
+      </c>
+      <c r="B107">
+        <v>536</v>
+      </c>
+      <c r="C107">
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -5093,11 +5117,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M107"/>
+  <dimension ref="A1:M108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M108" sqref="M108"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9556,6 +9580,31 @@
       <c r="M107" s="6">
         <v>18</v>
       </c>
+    </row>
+    <row r="108" spans="1:13">
+      <c r="A108" s="9">
+        <v>44005</v>
+      </c>
+      <c r="B108" s="6">
+        <v>27314</v>
+      </c>
+      <c r="C108" s="10">
+        <f>IFERROR(B108-B107,"")</f>
+        <v>562</v>
+      </c>
+      <c r="D108" s="6"/>
+      <c r="E108" s="10">
+        <f>C108-D108</f>
+        <v>562</v>
+      </c>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18336,85 +18385,85 @@
       </c>
     </row>
     <row r="108" spans="1:20">
-      <c r="A108" s="4" t="str">
+      <c r="A108" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B108" t="str">
+        <v>44005</v>
+      </c>
+      <c r="B108">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C108" t="str">
+        <v>27314</v>
+      </c>
+      <c r="C108">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>562</v>
       </c>
       <c r="D108">
         <f>+IFERROR('Fallecidos Diarios'!B107,"")</f>
-        <v>0</v>
+        <v>536</v>
       </c>
       <c r="E108">
         <f>+IFERROR('Fallecidos Diarios'!C107,"")</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F108">
         <f>+IFERROR('Recuperados Diarios'!B107,"")</f>
-        <v>0</v>
+        <v>14694</v>
       </c>
       <c r="G108">
         <f>+IFERROR('Recuperados Diarios'!C107,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H108" t="str">
+        <v>30</v>
+      </c>
+      <c r="H108">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I108" t="str">
+        <v>12084</v>
+      </c>
+      <c r="I108">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J108" t="str">
+        <v>517</v>
+      </c>
+      <c r="J108">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K108" t="str">
+        <v>1.9623636230504504E-2</v>
+      </c>
+      <c r="K108">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L108" t="str">
+        <v>0.53796587830416631</v>
+      </c>
+      <c r="L108">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M108" t="str">
+        <v>0.44241048546532913</v>
+      </c>
+      <c r="M108">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N108" t="str">
+        <v>1270.3134723601456</v>
+      </c>
+      <c r="N108">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O108" t="str">
+        <v>2.7985074626865673E-2</v>
+      </c>
+      <c r="O108">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P108" t="str">
+        <v>2.0416496529195591E-3</v>
+      </c>
+      <c r="P108">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q108" t="str">
+        <v>4.2783846408474012E-2</v>
+      </c>
+      <c r="Q108">
         <f t="shared" si="21"/>
-        <v/>
+        <v>6567.4440971387357</v>
       </c>
       <c r="R108">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>128.87713392642462</v>
       </c>
       <c r="S108">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T108" t="str">
+        <v>3533.0608319307526</v>
+      </c>
+      <c r="T108">
         <f t="shared" si="24"/>
-        <v/>
+        <v>2905.5061312815583</v>
       </c>
     </row>
     <row r="109" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-26-2020 03-11-26
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1702" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B4E585C-BBB7-4A62-8B67-2ACDB4EA482C}"/>
+  <xr:revisionPtr revIDLastSave="1730" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{608F0A08-2338-48CC-9402-05BFF48451E0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,9 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$109</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C107" totalsRowShown="0">
-  <autoFilter ref="A1:C107" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C109" totalsRowShown="0">
+  <autoFilter ref="A1:C109" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C107" totalsRowShown="0">
-  <autoFilter ref="A1:C107" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C109" totalsRowShown="0">
+  <autoFilter ref="A1:C109" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M108" totalsRowShown="0">
-  <autoFilter ref="A1:M108" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M110" totalsRowShown="0">
+  <autoFilter ref="A1:M110" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC107"/>
+  <dimension ref="A1:BC109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3824,6 +3824,27 @@
         <v>30</v>
       </c>
     </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="4">
+        <v>44006</v>
+      </c>
+      <c r="B108">
+        <v>14794</v>
+      </c>
+      <c r="C108">
+        <f>B108-B107</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="4">
+        <v>44007</v>
+      </c>
+      <c r="C109">
+        <f>B109-B108</f>
+        <v>-14794</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3837,10 +3858,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5019,7 +5040,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C107" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C109" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5105,6 +5126,27 @@
       <c r="C107">
         <f t="shared" si="1"/>
         <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="4">
+        <v>44006</v>
+      </c>
+      <c r="B108">
+        <v>547</v>
+      </c>
+      <c r="C108">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="4">
+        <v>44007</v>
+      </c>
+      <c r="C109">
+        <f t="shared" si="1"/>
+        <v>-547</v>
       </c>
     </row>
   </sheetData>
@@ -5117,11 +5159,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M108"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9592,19 +9634,103 @@
         <f>IFERROR(B108-B107,"")</f>
         <v>562</v>
       </c>
-      <c r="D108" s="6"/>
+      <c r="D108" s="6">
+        <v>280</v>
+      </c>
       <c r="E108" s="10">
         <f>C108-D108</f>
-        <v>562</v>
-      </c>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
-      <c r="I108" s="6"/>
-      <c r="J108" s="6"/>
-      <c r="K108" s="6"/>
-      <c r="L108" s="6"/>
-      <c r="M108" s="6"/>
+        <v>282</v>
+      </c>
+      <c r="F108" s="6">
+        <v>37</v>
+      </c>
+      <c r="G108" s="6">
+        <v>29</v>
+      </c>
+      <c r="H108" s="6">
+        <v>132</v>
+      </c>
+      <c r="I108" s="6">
+        <v>102</v>
+      </c>
+      <c r="J108" s="6">
+        <v>113</v>
+      </c>
+      <c r="K108" s="6">
+        <v>81</v>
+      </c>
+      <c r="L108" s="6">
+        <v>51</v>
+      </c>
+      <c r="M108" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13">
+      <c r="A109" s="9">
+        <v>44006</v>
+      </c>
+      <c r="B109" s="6">
+        <v>28030</v>
+      </c>
+      <c r="C109" s="10">
+        <f>IFERROR(B109-B108,"")</f>
+        <v>716</v>
+      </c>
+      <c r="D109" s="6">
+        <v>343</v>
+      </c>
+      <c r="E109" s="10">
+        <f>C109-D109</f>
+        <v>373</v>
+      </c>
+      <c r="F109" s="6">
+        <v>35</v>
+      </c>
+      <c r="G109" s="6">
+        <v>32</v>
+      </c>
+      <c r="H109" s="6">
+        <v>167</v>
+      </c>
+      <c r="I109" s="6">
+        <v>146</v>
+      </c>
+      <c r="J109" s="6">
+        <v>149</v>
+      </c>
+      <c r="K109" s="6">
+        <v>104</v>
+      </c>
+      <c r="L109" s="6">
+        <v>65</v>
+      </c>
+      <c r="M109" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13">
+      <c r="A110" s="9">
+        <v>44007</v>
+      </c>
+      <c r="B110" s="6"/>
+      <c r="C110" s="10">
+        <f>IFERROR(B110-B109,"")</f>
+        <v>-28030</v>
+      </c>
+      <c r="D110" s="6"/>
+      <c r="E110" s="10">
+        <f>C110-D110</f>
+        <v>-28030</v>
+      </c>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18467,99 +18593,99 @@
       </c>
     </row>
     <row r="109" spans="1:20">
-      <c r="A109" s="4" t="str">
+      <c r="A109" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B109" t="str">
+        <v>44006</v>
+      </c>
+      <c r="B109">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C109" t="str">
+        <v>28030</v>
+      </c>
+      <c r="C109">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>716</v>
       </c>
       <c r="D109">
         <f>+IFERROR('Fallecidos Diarios'!B108,"")</f>
-        <v>0</v>
+        <v>547</v>
       </c>
       <c r="E109">
         <f>+IFERROR('Fallecidos Diarios'!C108,"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F109">
         <f>+IFERROR('Recuperados Diarios'!B108,"")</f>
-        <v>0</v>
+        <v>14794</v>
       </c>
       <c r="G109">
         <f>+IFERROR('Recuperados Diarios'!C108,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H109" t="str">
+        <v>100</v>
+      </c>
+      <c r="H109">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I109" t="str">
+        <v>12689</v>
+      </c>
+      <c r="I109">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J109" t="str">
+        <v>605</v>
+      </c>
+      <c r="J109">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K109" t="str">
+        <v>1.9514805565465573E-2</v>
+      </c>
+      <c r="K109">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L109" t="str">
+        <v>0.52779165180164112</v>
+      </c>
+      <c r="L109">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M109" t="str">
+        <v>0.45269354263289335</v>
+      </c>
+      <c r="M109">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N109" t="str">
+        <v>1581.6439435731736</v>
+      </c>
+      <c r="N109">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O109" t="str">
+        <v>2.0109689213893969E-2</v>
+      </c>
+      <c r="O109">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P109" t="str">
+        <v>6.7594970934162502E-3</v>
+      </c>
+      <c r="P109">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q109" t="str">
+        <v>4.767909212703917E-2</v>
+      </c>
+      <c r="Q109">
         <f t="shared" si="21"/>
-        <v/>
+        <v>6739.6008655926908</v>
       </c>
       <c r="R109">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>131.52200048088483</v>
       </c>
       <c r="S109">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T109" t="str">
+        <v>3557.1050733349366</v>
+      </c>
+      <c r="T109">
         <f t="shared" si="24"/>
-        <v/>
+        <v>3050.9737917768698</v>
       </c>
     </row>
     <row r="110" spans="1:20">
-      <c r="A110" s="4" t="str">
+      <c r="A110" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B110" t="str">
+        <v>44007</v>
+      </c>
+      <c r="B110">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C110" t="str">
+        <v>0</v>
+      </c>
+      <c r="C110">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>-28030</v>
       </c>
       <c r="D110">
         <f>+IFERROR('Fallecidos Diarios'!B109,"")</f>
@@ -18567,7 +18693,7 @@
       </c>
       <c r="E110">
         <f>+IFERROR('Fallecidos Diarios'!C109,"")</f>
-        <v>0</v>
+        <v>-547</v>
       </c>
       <c r="F110">
         <f>+IFERROR('Recuperados Diarios'!B109,"")</f>
@@ -18575,15 +18701,15 @@
       </c>
       <c r="G110">
         <f>+IFERROR('Recuperados Diarios'!C109,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H110" t="str">
+        <v>-14794</v>
+      </c>
+      <c r="H110">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I110" t="str">
+        <v>0</v>
+      </c>
+      <c r="I110">
         <f t="shared" si="25"/>
-        <v/>
+        <v>-12689</v>
       </c>
       <c r="J110" t="str">
         <f t="shared" si="14"/>
@@ -18613,9 +18739,9 @@
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="Q110" t="str">
+      <c r="Q110">
         <f t="shared" si="21"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R110">
         <f t="shared" si="22"/>
@@ -18625,9 +18751,9 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="T110" t="str">
+      <c r="T110">
         <f t="shared" si="24"/>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-27-2020 19-16-23
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1730" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{608F0A08-2338-48CC-9402-05BFF48451E0}"/>
+  <xr:revisionPtr revIDLastSave="1749" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B69692EA-AD74-482A-8340-45469726F465}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$110</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C109" totalsRowShown="0">
-  <autoFilter ref="A1:C109" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C110" totalsRowShown="0">
+  <autoFilter ref="A1:C110" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C109" totalsRowShown="0">
-  <autoFilter ref="A1:C109" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C110" totalsRowShown="0">
+  <autoFilter ref="A1:C110" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M110" totalsRowShown="0">
-  <autoFilter ref="A1:M110" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M111" totalsRowShown="0">
+  <autoFilter ref="A1:M111" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC109"/>
+  <dimension ref="A1:BC110"/>
   <sheetViews>
-    <sheetView topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3840,9 +3840,24 @@
       <c r="A109" s="4">
         <v>44007</v>
       </c>
+      <c r="B109">
+        <v>14800</v>
+      </c>
       <c r="C109">
         <f>B109-B108</f>
-        <v>-14794</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="4">
+        <v>44008</v>
+      </c>
+      <c r="B110">
+        <v>15270</v>
+      </c>
+      <c r="C110">
+        <f>B110-B109</f>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -3858,10 +3873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5040,7 +5055,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C109" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C110" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5144,9 +5159,24 @@
       <c r="A109" s="4">
         <v>44007</v>
       </c>
+      <c r="B109">
+        <v>564</v>
+      </c>
       <c r="C109">
         <f t="shared" si="1"/>
-        <v>-547</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="4">
+        <v>44008</v>
+      </c>
+      <c r="B110">
+        <v>575</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -5159,11 +5189,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M110"/>
+  <dimension ref="A1:M111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="B103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M110" sqref="M110"/>
+      <selection pane="bottomLeft" activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9713,24 +9743,69 @@
       <c r="A110" s="9">
         <v>44007</v>
       </c>
-      <c r="B110" s="6"/>
+      <c r="B110" s="6">
+        <v>29037</v>
+      </c>
       <c r="C110" s="10">
         <f>IFERROR(B110-B109,"")</f>
-        <v>-28030</v>
-      </c>
-      <c r="D110" s="6"/>
+        <v>1007</v>
+      </c>
+      <c r="D110" s="6">
+        <v>469</v>
+      </c>
       <c r="E110" s="10">
         <f>C110-D110</f>
-        <v>-28030</v>
-      </c>
-      <c r="F110" s="6"/>
-      <c r="G110" s="6"/>
-      <c r="H110" s="6"/>
-      <c r="I110" s="6"/>
-      <c r="J110" s="6"/>
-      <c r="K110" s="6"/>
-      <c r="L110" s="6"/>
-      <c r="M110" s="6"/>
+        <v>538</v>
+      </c>
+      <c r="F110" s="6">
+        <v>45</v>
+      </c>
+      <c r="G110" s="6">
+        <v>55</v>
+      </c>
+      <c r="H110" s="6">
+        <v>278</v>
+      </c>
+      <c r="I110" s="6">
+        <v>252</v>
+      </c>
+      <c r="J110" s="6">
+        <v>144</v>
+      </c>
+      <c r="K110" s="6">
+        <v>135</v>
+      </c>
+      <c r="L110" s="6">
+        <v>85</v>
+      </c>
+      <c r="M110" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
+      <c r="A111" s="9">
+        <v>44008</v>
+      </c>
+      <c r="B111" s="6">
+        <v>29905</v>
+      </c>
+      <c r="C111" s="10">
+        <f>IFERROR(B111-B110,"")</f>
+        <v>868</v>
+      </c>
+      <c r="D111" s="6"/>
+      <c r="E111" s="10">
+        <f>C111-D111</f>
+        <v>868</v>
+      </c>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18681,161 +18756,161 @@
       </c>
       <c r="B110">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v>0</v>
+        <v>29037</v>
       </c>
       <c r="C110">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v>-28030</v>
+        <v>1007</v>
       </c>
       <c r="D110">
         <f>+IFERROR('Fallecidos Diarios'!B109,"")</f>
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="E110">
         <f>+IFERROR('Fallecidos Diarios'!C109,"")</f>
-        <v>-547</v>
+        <v>17</v>
       </c>
       <c r="F110">
         <f>+IFERROR('Recuperados Diarios'!B109,"")</f>
-        <v>0</v>
+        <v>14800</v>
       </c>
       <c r="G110">
         <f>+IFERROR('Recuperados Diarios'!C109,"")</f>
-        <v>-14794</v>
+        <v>6</v>
       </c>
       <c r="H110">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>13673</v>
       </c>
       <c r="I110">
         <f t="shared" si="25"/>
-        <v>-12689</v>
-      </c>
-      <c r="J110" t="str">
+        <v>984</v>
+      </c>
+      <c r="J110">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K110" t="str">
+        <v>1.9423494162620104E-2</v>
+      </c>
+      <c r="K110">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L110" t="str">
+        <v>0.5096945276715914</v>
+      </c>
+      <c r="L110">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M110" t="str">
+        <v>0.47088197816578847</v>
+      </c>
+      <c r="M110">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N110" t="str">
+        <v>2138.5401155562058</v>
+      </c>
+      <c r="N110">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O110" t="str">
+        <v>3.0141843971631204E-2</v>
+      </c>
+      <c r="O110">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P110" t="str">
+        <v>4.0540540540540538E-4</v>
+      </c>
+      <c r="P110">
         <f t="shared" si="20"/>
-        <v/>
+        <v>7.1966649601404226E-2</v>
       </c>
       <c r="Q110">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>6981.7263765328207</v>
       </c>
       <c r="R110">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>135.60952151959606</v>
       </c>
       <c r="S110">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3558.5477278191875</v>
       </c>
       <c r="T110">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>3287.5691271940373</v>
       </c>
     </row>
     <row r="111" spans="1:20">
-      <c r="A111" s="4" t="str">
+      <c r="A111" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B111" t="str">
+        <v>44008</v>
+      </c>
+      <c r="B111">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C111" t="str">
+        <v>29905</v>
+      </c>
+      <c r="C111">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>868</v>
       </c>
       <c r="D111">
         <f>+IFERROR('Fallecidos Diarios'!B110,"")</f>
-        <v>0</v>
+        <v>575</v>
       </c>
       <c r="E111">
         <f>+IFERROR('Fallecidos Diarios'!C110,"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F111">
         <f>+IFERROR('Recuperados Diarios'!B110,"")</f>
-        <v>0</v>
+        <v>15270</v>
       </c>
       <c r="G111">
         <f>+IFERROR('Recuperados Diarios'!C110,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H111" t="str">
+        <v>470</v>
+      </c>
+      <c r="H111">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I111" t="str">
+        <v>14060</v>
+      </c>
+      <c r="I111">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J111" t="str">
+        <v>387</v>
+      </c>
+      <c r="J111">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K111" t="str">
+        <v>1.9227553920749037E-2</v>
+      </c>
+      <c r="K111">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L111" t="str">
+        <v>0.51061695368667448</v>
+      </c>
+      <c r="L111">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M111" t="str">
+        <v>0.47015549239257648</v>
+      </c>
+      <c r="M111">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N111" t="str">
+        <v>1846.1977240398294</v>
+      </c>
+      <c r="N111">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O111" t="str">
+        <v>1.9130434782608695E-2</v>
+      </c>
+      <c r="O111">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P111" t="str">
+        <v>3.0779305828421741E-2</v>
+      </c>
+      <c r="P111">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q111" t="str">
+        <v>2.7524893314366999E-2</v>
+      </c>
+      <c r="Q111">
         <f t="shared" si="21"/>
-        <v/>
+        <v>7190.4303919211352</v>
       </c>
       <c r="R111">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>138.25438807405627</v>
       </c>
       <c r="S111">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T111" t="str">
+        <v>3671.5556624188507</v>
+      </c>
+      <c r="T111">
         <f t="shared" si="24"/>
-        <v/>
+        <v>3380.6203414282281</v>
       </c>
     </row>
     <row r="112" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-29-2020 19-22-02
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23023"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1749" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B69692EA-AD74-482A-8340-45469726F465}"/>
+  <xr:revisionPtr revIDLastSave="1780" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{125D7CD1-5980-4F7A-B326-6E6435B34142}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$112</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C110" totalsRowShown="0">
-  <autoFilter ref="A1:C110" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C112" totalsRowShown="0">
+  <autoFilter ref="A1:C112" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C110" totalsRowShown="0">
-  <autoFilter ref="A1:C110" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C112" totalsRowShown="0">
+  <autoFilter ref="A1:C112" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M111" totalsRowShown="0">
-  <autoFilter ref="A1:M111" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M113" totalsRowShown="0">
+  <autoFilter ref="A1:M113" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC110"/>
+  <dimension ref="A1:BC112"/>
   <sheetViews>
     <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3860,6 +3860,30 @@
         <v>470</v>
       </c>
     </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="4">
+        <v>44009</v>
+      </c>
+      <c r="B111">
+        <v>15370</v>
+      </c>
+      <c r="C111">
+        <f>B111-B110</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="4">
+        <v>44010</v>
+      </c>
+      <c r="B112">
+        <v>15470</v>
+      </c>
+      <c r="C112">
+        <f>B112-B111</f>
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3873,10 +3897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="B111" sqref="B111"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5055,7 +5079,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C110" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C112" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5177,6 +5201,30 @@
       <c r="C110">
         <f t="shared" si="1"/>
         <v>11</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="4">
+        <v>44009</v>
+      </c>
+      <c r="B111">
+        <v>592</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="4">
+        <v>44010</v>
+      </c>
+      <c r="B112">
+        <v>604</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5189,11 +5237,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M111"/>
+  <dimension ref="A1:M113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K112" sqref="K112"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9793,19 +9841,105 @@
         <f>IFERROR(B111-B110,"")</f>
         <v>868</v>
       </c>
-      <c r="D111" s="6"/>
+      <c r="D111" s="6">
+        <v>416</v>
+      </c>
       <c r="E111" s="10">
         <f>C111-D111</f>
-        <v>868</v>
-      </c>
-      <c r="F111" s="6"/>
-      <c r="G111" s="6"/>
-      <c r="H111" s="6"/>
-      <c r="I111" s="6"/>
-      <c r="J111" s="6"/>
-      <c r="K111" s="6"/>
-      <c r="L111" s="6"/>
-      <c r="M111" s="6"/>
+        <v>452</v>
+      </c>
+      <c r="F111" s="6">
+        <v>51</v>
+      </c>
+      <c r="G111" s="6">
+        <v>41</v>
+      </c>
+      <c r="H111" s="6">
+        <v>218</v>
+      </c>
+      <c r="I111" s="6">
+        <v>197</v>
+      </c>
+      <c r="J111" s="6">
+        <v>158</v>
+      </c>
+      <c r="K111" s="6">
+        <v>119</v>
+      </c>
+      <c r="L111" s="6">
+        <v>74</v>
+      </c>
+      <c r="M111" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13">
+      <c r="A112" s="9">
+        <v>44009</v>
+      </c>
+      <c r="B112" s="6">
+        <v>30658</v>
+      </c>
+      <c r="C112" s="10">
+        <f>IFERROR(B112-B111,"")</f>
+        <v>753</v>
+      </c>
+      <c r="D112" s="6">
+        <v>318</v>
+      </c>
+      <c r="E112" s="10">
+        <f>C112-D112</f>
+        <v>435</v>
+      </c>
+      <c r="F112" s="6">
+        <v>33</v>
+      </c>
+      <c r="G112" s="6">
+        <v>50</v>
+      </c>
+      <c r="H112" s="6">
+        <v>186</v>
+      </c>
+      <c r="I112" s="6">
+        <v>165</v>
+      </c>
+      <c r="J112" s="6">
+        <v>129</v>
+      </c>
+      <c r="K112" s="6">
+        <v>111</v>
+      </c>
+      <c r="L112" s="6">
+        <v>64</v>
+      </c>
+      <c r="M112" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13">
+      <c r="A113" s="9">
+        <v>44010</v>
+      </c>
+      <c r="B113" s="6">
+        <v>31686</v>
+      </c>
+      <c r="C113" s="10">
+        <f>IFERROR(B113-B112,"")</f>
+        <v>1028</v>
+      </c>
+      <c r="D113" s="6"/>
+      <c r="E113" s="10">
+        <f>C113-D113</f>
+        <v>1028</v>
+      </c>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18914,167 +19048,167 @@
       </c>
     </row>
     <row r="112" spans="1:20">
-      <c r="A112" s="4" t="str">
+      <c r="A112" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B112" t="str">
+        <v>44009</v>
+      </c>
+      <c r="B112">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C112" t="str">
+        <v>30658</v>
+      </c>
+      <c r="C112">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>753</v>
       </c>
       <c r="D112">
         <f>+IFERROR('Fallecidos Diarios'!B111,"")</f>
-        <v>0</v>
+        <v>592</v>
       </c>
       <c r="E112">
         <f>+IFERROR('Fallecidos Diarios'!C111,"")</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F112">
         <f>+IFERROR('Recuperados Diarios'!B111,"")</f>
-        <v>0</v>
+        <v>15370</v>
       </c>
       <c r="G112">
         <f>+IFERROR('Recuperados Diarios'!C111,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H112" t="str">
+        <v>100</v>
+      </c>
+      <c r="H112">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I112" t="str">
+        <v>14696</v>
+      </c>
+      <c r="I112">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J112" t="str">
+        <v>636</v>
+      </c>
+      <c r="J112">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K112" t="str">
+        <v>1.9309804944875726E-2</v>
+      </c>
+      <c r="K112">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L112" t="str">
+        <v>0.50133733446408768</v>
+      </c>
+      <c r="L112">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M112" t="str">
+        <v>0.4793528605910366</v>
+      </c>
+      <c r="M112">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N112" t="str">
+        <v>1570.8678551986934</v>
+      </c>
+      <c r="N112">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O112" t="str">
+        <v>2.8716216216216218E-2</v>
+      </c>
+      <c r="O112">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P112" t="str">
+        <v>6.5061808718282366E-3</v>
+      </c>
+      <c r="P112">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q112" t="str">
+        <v>4.3277082199237885E-2</v>
+      </c>
+      <c r="Q112">
         <f t="shared" si="21"/>
-        <v/>
+        <v>7371.4835296946385</v>
       </c>
       <c r="R112">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>142.3419091127675</v>
       </c>
       <c r="S112">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T112" t="str">
+        <v>3695.5999038230348</v>
+      </c>
+      <c r="T112">
         <f t="shared" si="24"/>
-        <v/>
+        <v>3533.5417167588366</v>
       </c>
     </row>
     <row r="113" spans="1:20">
-      <c r="A113" s="4" t="str">
+      <c r="A113" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B113" t="str">
+        <v>44010</v>
+      </c>
+      <c r="B113">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C113" t="str">
+        <v>31686</v>
+      </c>
+      <c r="C113">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1028</v>
       </c>
       <c r="D113">
         <f>+IFERROR('Fallecidos Diarios'!B112,"")</f>
-        <v>0</v>
+        <v>604</v>
       </c>
       <c r="E113">
         <f>+IFERROR('Fallecidos Diarios'!C112,"")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F113">
         <f>+IFERROR('Recuperados Diarios'!B112,"")</f>
-        <v>0</v>
+        <v>15470</v>
       </c>
       <c r="G113">
         <f>+IFERROR('Recuperados Diarios'!C112,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H113" t="str">
+        <v>100</v>
+      </c>
+      <c r="H113">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I113" t="str">
+        <v>15612</v>
+      </c>
+      <c r="I113">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J113" t="str">
+        <v>916</v>
+      </c>
+      <c r="J113">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K113" t="str">
+        <v>1.906204632960929E-2</v>
+      </c>
+      <c r="K113">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L113" t="str">
+        <v>0.48822823960108563</v>
+      </c>
+      <c r="L113">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M113" t="str">
+        <v>0.49270971406930508</v>
+      </c>
+      <c r="M113">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N113" t="str">
+        <v>2086.4212144504227</v>
+      </c>
+      <c r="N113">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O113" t="str">
+        <v>1.9867549668874173E-2</v>
+      </c>
+      <c r="O113">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P113" t="str">
+        <v>6.4641241111829343E-3</v>
+      </c>
+      <c r="P113">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q113" t="str">
+        <v>5.867281578273123E-2</v>
+      </c>
+      <c r="Q113">
         <f t="shared" si="21"/>
-        <v/>
+        <v>7618.6583313296469</v>
       </c>
       <c r="R113">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>145.22721808126954</v>
       </c>
       <c r="S113">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T113" t="str">
+        <v>3719.6441452272184</v>
+      </c>
+      <c r="T113">
         <f t="shared" si="24"/>
-        <v/>
+        <v>3753.7869680211593</v>
       </c>
     </row>
     <row r="114" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-30-2020 23-25-33
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1780" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{125D7CD1-5980-4F7A-B326-6E6435B34142}"/>
+  <xr:revisionPtr revIDLastSave="1787" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F762E6F-FA0A-4F33-8830-6C892680E865}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$113</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C112" totalsRowShown="0">
-  <autoFilter ref="A1:C112" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C113" totalsRowShown="0">
+  <autoFilter ref="A1:C113" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C112" totalsRowShown="0">
-  <autoFilter ref="A1:C112" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C113" totalsRowShown="0">
+  <autoFilter ref="A1:C113" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M113" totalsRowShown="0">
-  <autoFilter ref="A1:M113" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M114" totalsRowShown="0">
+  <autoFilter ref="A1:M114" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC112"/>
+  <dimension ref="A1:BC113"/>
   <sheetViews>
-    <sheetView topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3884,6 +3884,18 @@
         <v>100</v>
       </c>
     </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="4">
+        <v>44011</v>
+      </c>
+      <c r="B113">
+        <v>15595</v>
+      </c>
+      <c r="C113">
+        <f>B113-B112</f>
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3897,10 +3909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E112"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+      <selection activeCell="C112" sqref="C112:C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5079,7 +5091,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C112" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C113" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5225,6 +5237,18 @@
       <c r="C112">
         <f t="shared" si="1"/>
         <v>12</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="4">
+        <v>44011</v>
+      </c>
+      <c r="B113">
+        <v>620</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -5237,11 +5261,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M113"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
+      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9940,6 +9964,31 @@
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
       <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="1:13">
+      <c r="A114" s="9">
+        <v>44011</v>
+      </c>
+      <c r="B114" s="6">
+        <v>32785</v>
+      </c>
+      <c r="C114" s="10">
+        <f>IFERROR(B114-B113,"")</f>
+        <v>1099</v>
+      </c>
+      <c r="D114" s="6"/>
+      <c r="E114" s="10">
+        <f>C114-D114</f>
+        <v>1099</v>
+      </c>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19212,85 +19261,85 @@
       </c>
     </row>
     <row r="114" spans="1:20">
-      <c r="A114" s="4" t="str">
+      <c r="A114" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B114" t="str">
+        <v>44011</v>
+      </c>
+      <c r="B114">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C114" t="str">
+        <v>32785</v>
+      </c>
+      <c r="C114">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1099</v>
       </c>
       <c r="D114">
         <f>+IFERROR('Fallecidos Diarios'!B113,"")</f>
-        <v>0</v>
+        <v>620</v>
       </c>
       <c r="E114">
         <f>+IFERROR('Fallecidos Diarios'!C113,"")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F114">
         <f>+IFERROR('Recuperados Diarios'!B113,"")</f>
-        <v>0</v>
+        <v>15595</v>
       </c>
       <c r="G114">
         <f>+IFERROR('Recuperados Diarios'!C113,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H114" t="str">
+        <v>125</v>
+      </c>
+      <c r="H114">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I114" t="str">
+        <v>16570</v>
+      </c>
+      <c r="I114">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J114" t="str">
+        <v>958</v>
+      </c>
+      <c r="J114">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K114" t="str">
+        <v>1.8911087387524783E-2</v>
+      </c>
+      <c r="K114">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L114" t="str">
+        <v>0.47567485130394999</v>
+      </c>
+      <c r="L114">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M114" t="str">
+        <v>0.50541406130852529</v>
+      </c>
+      <c r="M114">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N114" t="str">
+        <v>2174.4547374773683</v>
+      </c>
+      <c r="N114">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O114" t="str">
+        <v>2.5806451612903226E-2</v>
+      </c>
+      <c r="O114">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P114" t="str">
+        <v>8.0153895479320291E-3</v>
+      </c>
+      <c r="P114">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q114" t="str">
+        <v>5.7815328907664457E-2</v>
+      </c>
+      <c r="Q114">
         <f t="shared" si="21"/>
-        <v/>
+        <v>7882.904544361626</v>
       </c>
       <c r="R114">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>149.07429670593893</v>
       </c>
       <c r="S114">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T114" t="str">
+        <v>3749.6994469824481</v>
+      </c>
+      <c r="T114">
         <f t="shared" si="24"/>
-        <v/>
+        <v>3984.1308006732388</v>
       </c>
     </row>
     <row r="115" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-02-2020 19-30-19
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1787" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F762E6F-FA0A-4F33-8830-6C892680E865}"/>
+  <xr:revisionPtr revIDLastSave="1800" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AB6A6F2-D7B8-4C37-B898-A733DD7FCF9A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$115</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C113" totalsRowShown="0">
-  <autoFilter ref="A1:C113" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C115" totalsRowShown="0">
+  <autoFilter ref="A1:C115" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C113" totalsRowShown="0">
-  <autoFilter ref="A1:C113" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C115" totalsRowShown="0">
+  <autoFilter ref="A1:C115" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M114" totalsRowShown="0">
-  <autoFilter ref="A1:M114" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M116" totalsRowShown="0">
+  <autoFilter ref="A1:M116" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC113"/>
+  <dimension ref="A1:BC115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3896,6 +3896,30 @@
         <v>125</v>
       </c>
     </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="4">
+        <v>44012</v>
+      </c>
+      <c r="B114">
+        <v>15745</v>
+      </c>
+      <c r="C114">
+        <f>B114-B113</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="4">
+        <v>44013</v>
+      </c>
+      <c r="B115">
+        <v>15945</v>
+      </c>
+      <c r="C115">
+        <f>B115-B114</f>
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3909,10 +3933,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112:C113"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5091,7 +5115,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C113" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C115" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5249,6 +5273,30 @@
       <c r="C113">
         <f t="shared" si="1"/>
         <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="4">
+        <v>44012</v>
+      </c>
+      <c r="B114">
+        <v>631</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="4">
+        <v>44013</v>
+      </c>
+      <c r="B115">
+        <v>645</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -5261,11 +5309,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -9989,6 +10037,56 @@
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
       <c r="M114" s="6"/>
+    </row>
+    <row r="115" spans="1:13">
+      <c r="A115" s="9">
+        <v>44012</v>
+      </c>
+      <c r="B115" s="6">
+        <v>33550</v>
+      </c>
+      <c r="C115" s="10">
+        <f>IFERROR(B115-B114,"")</f>
+        <v>765</v>
+      </c>
+      <c r="D115" s="6"/>
+      <c r="E115" s="10">
+        <f>C115-D115</f>
+        <v>765</v>
+      </c>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+    </row>
+    <row r="116" spans="1:13">
+      <c r="A116" s="9">
+        <v>44013</v>
+      </c>
+      <c r="B116" s="6">
+        <v>34463</v>
+      </c>
+      <c r="C116" s="10">
+        <f>IFERROR(B116-B115,"")</f>
+        <v>913</v>
+      </c>
+      <c r="D116" s="6"/>
+      <c r="E116" s="10">
+        <f>C116-D116</f>
+        <v>913</v>
+      </c>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19343,167 +19441,167 @@
       </c>
     </row>
     <row r="115" spans="1:20">
-      <c r="A115" s="4" t="str">
+      <c r="A115" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B115" t="str">
+        <v>44012</v>
+      </c>
+      <c r="B115">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C115" t="str">
+        <v>33550</v>
+      </c>
+      <c r="C115">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>765</v>
       </c>
       <c r="D115">
         <f>+IFERROR('Fallecidos Diarios'!B114,"")</f>
-        <v>0</v>
+        <v>631</v>
       </c>
       <c r="E115">
         <f>+IFERROR('Fallecidos Diarios'!C114,"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F115">
         <f>+IFERROR('Recuperados Diarios'!B114,"")</f>
-        <v>0</v>
+        <v>15745</v>
       </c>
       <c r="G115">
         <f>+IFERROR('Recuperados Diarios'!C114,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H115" t="str">
+        <v>150</v>
+      </c>
+      <c r="H115">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I115" t="str">
+        <v>17174</v>
+      </c>
+      <c r="I115">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J115" t="str">
+        <v>604</v>
+      </c>
+      <c r="J115">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K115" t="str">
+        <v>1.8807749627421759E-2</v>
+      </c>
+      <c r="K115">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L115" t="str">
+        <v>0.46929955290611031</v>
+      </c>
+      <c r="L115">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M115" t="str">
+        <v>0.51189269746646793</v>
+      </c>
+      <c r="M115">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N115" t="str">
+        <v>1494.4538255502505</v>
+      </c>
+      <c r="N115">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O115" t="str">
+        <v>1.7432646592709985E-2</v>
+      </c>
+      <c r="O115">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P115" t="str">
+        <v>9.5268339155287398E-3</v>
+      </c>
+      <c r="P115">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q115" t="str">
+        <v>3.5169442180039596E-2</v>
+      </c>
+      <c r="Q115">
         <f t="shared" si="21"/>
-        <v/>
+        <v>8066.842991103631</v>
       </c>
       <c r="R115">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>151.71916326039914</v>
       </c>
       <c r="S115">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T115" t="str">
+        <v>3785.7658090887235</v>
+      </c>
+      <c r="T115">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4129.3580187545085</v>
       </c>
     </row>
     <row r="116" spans="1:20">
-      <c r="A116" s="4" t="str">
+      <c r="A116" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B116" t="str">
+        <v>44013</v>
+      </c>
+      <c r="B116">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C116" t="str">
+        <v>34463</v>
+      </c>
+      <c r="C116">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>913</v>
       </c>
       <c r="D116">
         <f>+IFERROR('Fallecidos Diarios'!B115,"")</f>
-        <v>0</v>
+        <v>645</v>
       </c>
       <c r="E116">
         <f>+IFERROR('Fallecidos Diarios'!C115,"")</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F116">
         <f>+IFERROR('Recuperados Diarios'!B115,"")</f>
-        <v>0</v>
+        <v>15945</v>
       </c>
       <c r="G116">
         <f>+IFERROR('Recuperados Diarios'!C115,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H116" t="str">
+        <v>200</v>
+      </c>
+      <c r="H116">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I116" t="str">
+        <v>17873</v>
+      </c>
+      <c r="I116">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J116" t="str">
+        <v>699</v>
+      </c>
+      <c r="J116">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K116" t="str">
+        <v>1.8715724109914983E-2</v>
+      </c>
+      <c r="K116">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L116" t="str">
+        <v>0.46267010997301455</v>
+      </c>
+      <c r="L116">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M116" t="str">
+        <v>0.51861416591707044</v>
+      </c>
+      <c r="M116">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N116" t="str">
+        <v>1760.460974654507</v>
+      </c>
+      <c r="N116">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O116" t="str">
+        <v>2.1705426356589147E-2</v>
+      </c>
+      <c r="O116">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P116" t="str">
+        <v>1.2543116964565695E-2</v>
+      </c>
+      <c r="P116">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q116" t="str">
+        <v>3.9109270967380969E-2</v>
+      </c>
+      <c r="Q116">
         <f t="shared" si="21"/>
-        <v/>
+        <v>8286.3669151238282</v>
       </c>
       <c r="R116">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>155.08535705698486</v>
       </c>
       <c r="S116">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T116" t="str">
+        <v>3833.8542918970907</v>
+      </c>
+      <c r="T116">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4297.4272661697523</v>
       </c>
     </row>
     <row r="117" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-03-2020 17-31-52
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1800" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AB6A6F2-D7B8-4C37-B898-A733DD7FCF9A}"/>
+  <xr:revisionPtr revIDLastSave="1807" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC89084A-872E-4576-918A-09BB7EB64338}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$116</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C115" totalsRowShown="0">
-  <autoFilter ref="A1:C115" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C116" totalsRowShown="0">
+  <autoFilter ref="A1:C116" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C115" totalsRowShown="0">
-  <autoFilter ref="A1:C115" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C116" totalsRowShown="0">
+  <autoFilter ref="A1:C116" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M116" totalsRowShown="0">
-  <autoFilter ref="A1:M116" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M117" totalsRowShown="0">
+  <autoFilter ref="A1:M117" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC115"/>
+  <dimension ref="A1:BC116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3920,6 +3920,18 @@
         <v>200</v>
       </c>
     </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B116">
+        <v>16445</v>
+      </c>
+      <c r="C116">
+        <f>B116-B115</f>
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3933,10 +3945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E115"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5115,7 +5127,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C115" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C116" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5297,6 +5309,18 @@
       <c r="C115">
         <f t="shared" si="1"/>
         <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="4">
+        <v>44014</v>
+      </c>
+      <c r="B116">
+        <v>667</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5309,11 +5333,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:M117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10087,6 +10111,31 @@
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
       <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="1:13">
+      <c r="A117" s="9">
+        <v>44014</v>
+      </c>
+      <c r="B117" s="6">
+        <v>35237</v>
+      </c>
+      <c r="C117" s="10">
+        <f>IFERROR(B117-B116,"")</f>
+        <v>774</v>
+      </c>
+      <c r="D117" s="6"/>
+      <c r="E117" s="10">
+        <f>C117-D117</f>
+        <v>774</v>
+      </c>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19605,85 +19654,85 @@
       </c>
     </row>
     <row r="117" spans="1:20">
-      <c r="A117" s="4" t="str">
+      <c r="A117" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B117" t="str">
+        <v>44014</v>
+      </c>
+      <c r="B117">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C117" t="str">
+        <v>35237</v>
+      </c>
+      <c r="C117">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>774</v>
       </c>
       <c r="D117">
         <f>+IFERROR('Fallecidos Diarios'!B116,"")</f>
-        <v>0</v>
+        <v>667</v>
       </c>
       <c r="E117">
         <f>+IFERROR('Fallecidos Diarios'!C116,"")</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F117">
         <f>+IFERROR('Recuperados Diarios'!B116,"")</f>
-        <v>0</v>
+        <v>16445</v>
       </c>
       <c r="G117">
         <f>+IFERROR('Recuperados Diarios'!C116,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H117" t="str">
+        <v>500</v>
+      </c>
+      <c r="H117">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I117" t="str">
+        <v>18125</v>
+      </c>
+      <c r="I117">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J117" t="str">
+        <v>252</v>
+      </c>
+      <c r="J117">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K117" t="str">
+        <v>1.892896671112751E-2</v>
+      </c>
+      <c r="K117">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L117" t="str">
+        <v>0.46669693787779892</v>
+      </c>
+      <c r="L117">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M117" t="str">
+        <v>0.5143740954110736</v>
+      </c>
+      <c r="M117">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N117" t="str">
+        <v>1504.7414068965518</v>
+      </c>
+      <c r="N117">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O117" t="str">
+        <v>3.2983508245877063E-2</v>
+      </c>
+      <c r="O117">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P117" t="str">
+        <v>3.0404378230465188E-2</v>
+      </c>
+      <c r="P117">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q117" t="str">
+        <v>1.3903448275862068E-2</v>
+      </c>
+      <c r="Q117">
         <f t="shared" si="21"/>
-        <v/>
+        <v>8472.4693435922109</v>
       </c>
       <c r="R117">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>160.37509016590528</v>
       </c>
       <c r="S117">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T117" t="str">
+        <v>3954.0754989180095</v>
+      </c>
+      <c r="T117">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4358.0187545082954</v>
       </c>
     </row>
     <row r="118" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-03-2020 21-37-20
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1807" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AC89084A-872E-4576-918A-09BB7EB64338}"/>
+  <xr:revisionPtr revIDLastSave="1854" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67AB31EF-0659-4556-AFD1-031B39C9A9CA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -5336,8 +5336,8 @@
   <dimension ref="A1:M117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10023,19 +10023,37 @@
         <f>IFERROR(B113-B112,"")</f>
         <v>1028</v>
       </c>
-      <c r="D113" s="6"/>
+      <c r="D113">
+        <v>449</v>
+      </c>
       <c r="E113" s="10">
-        <f>C113-D113</f>
-        <v>1028</v>
-      </c>
-      <c r="F113" s="6"/>
-      <c r="G113" s="6"/>
-      <c r="H113" s="6"/>
-      <c r="I113" s="6"/>
-      <c r="J113" s="6"/>
-      <c r="K113" s="6"/>
-      <c r="L113" s="6"/>
-      <c r="M113" s="6"/>
+        <f>C113-F113</f>
+        <v>964</v>
+      </c>
+      <c r="F113" s="6">
+        <v>64</v>
+      </c>
+      <c r="G113" s="6">
+        <v>67</v>
+      </c>
+      <c r="H113" s="6">
+        <v>250</v>
+      </c>
+      <c r="I113" s="6">
+        <v>236</v>
+      </c>
+      <c r="J113" s="6">
+        <v>163</v>
+      </c>
+      <c r="K113" s="6">
+        <v>130</v>
+      </c>
+      <c r="L113" s="6">
+        <v>98</v>
+      </c>
+      <c r="M113" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="114" spans="1:13">
       <c r="A114" s="9">
@@ -10048,19 +10066,37 @@
         <f>IFERROR(B114-B113,"")</f>
         <v>1099</v>
       </c>
-      <c r="D114" s="6"/>
+      <c r="D114">
+        <v>497</v>
+      </c>
       <c r="E114" s="10">
-        <f>C114-D114</f>
-        <v>1099</v>
-      </c>
-      <c r="F114" s="6"/>
-      <c r="G114" s="6"/>
-      <c r="H114" s="6"/>
-      <c r="I114" s="6"/>
-      <c r="J114" s="6"/>
-      <c r="K114" s="6"/>
-      <c r="L114" s="6"/>
-      <c r="M114" s="6"/>
+        <f>C114-F114</f>
+        <v>1031</v>
+      </c>
+      <c r="F114" s="6">
+        <v>68</v>
+      </c>
+      <c r="G114" s="6">
+        <v>65</v>
+      </c>
+      <c r="H114" s="6">
+        <v>310</v>
+      </c>
+      <c r="I114" s="6">
+        <v>238</v>
+      </c>
+      <c r="J114" s="6">
+        <v>165</v>
+      </c>
+      <c r="K114" s="6">
+        <v>123</v>
+      </c>
+      <c r="L114" s="6">
+        <v>115</v>
+      </c>
+      <c r="M114" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="115" spans="1:13">
       <c r="A115" s="9">
@@ -10073,19 +10109,37 @@
         <f>IFERROR(B115-B114,"")</f>
         <v>765</v>
       </c>
-      <c r="D115" s="6"/>
+      <c r="D115" s="6">
+        <v>346</v>
+      </c>
       <c r="E115" s="10">
         <f>C115-D115</f>
-        <v>765</v>
-      </c>
-      <c r="F115" s="6"/>
-      <c r="G115" s="6"/>
-      <c r="H115" s="6"/>
-      <c r="I115" s="6"/>
-      <c r="J115" s="6"/>
-      <c r="K115" s="6"/>
-      <c r="L115" s="6"/>
-      <c r="M115" s="6"/>
+        <v>419</v>
+      </c>
+      <c r="F115" s="6">
+        <v>27</v>
+      </c>
+      <c r="G115" s="6">
+        <v>41</v>
+      </c>
+      <c r="H115" s="6">
+        <v>210</v>
+      </c>
+      <c r="I115" s="6">
+        <v>143</v>
+      </c>
+      <c r="J115" s="6">
+        <v>134</v>
+      </c>
+      <c r="K115" s="6">
+        <v>100</v>
+      </c>
+      <c r="L115" s="6">
+        <v>94</v>
+      </c>
+      <c r="M115" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="116" spans="1:13">
       <c r="A116" s="9">
@@ -10098,19 +10152,37 @@
         <f>IFERROR(B116-B115,"")</f>
         <v>913</v>
       </c>
-      <c r="D116" s="6"/>
+      <c r="D116" s="6">
+        <v>426</v>
+      </c>
       <c r="E116" s="10">
         <f>C116-D116</f>
-        <v>913</v>
-      </c>
-      <c r="F116" s="6"/>
-      <c r="G116" s="6"/>
-      <c r="H116" s="6"/>
-      <c r="I116" s="6"/>
-      <c r="J116" s="6"/>
-      <c r="K116" s="6"/>
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
+        <v>487</v>
+      </c>
+      <c r="F116" s="6">
+        <v>53</v>
+      </c>
+      <c r="G116" s="6">
+        <v>45</v>
+      </c>
+      <c r="H116" s="6">
+        <v>234</v>
+      </c>
+      <c r="I116" s="6">
+        <v>181</v>
+      </c>
+      <c r="J116" s="6">
+        <v>162</v>
+      </c>
+      <c r="K116" s="6">
+        <v>122</v>
+      </c>
+      <c r="L116" s="6">
+        <v>95</v>
+      </c>
+      <c r="M116" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="9">
@@ -10123,19 +10195,37 @@
         <f>IFERROR(B117-B116,"")</f>
         <v>774</v>
       </c>
-      <c r="D117" s="6"/>
+      <c r="D117" s="6">
+        <v>369</v>
+      </c>
       <c r="E117" s="10">
         <f>C117-D117</f>
-        <v>774</v>
-      </c>
-      <c r="F117" s="6"/>
-      <c r="G117" s="6"/>
-      <c r="H117" s="6"/>
-      <c r="I117" s="6"/>
-      <c r="J117" s="6"/>
-      <c r="K117" s="6"/>
-      <c r="L117" s="6"/>
-      <c r="M117" s="6"/>
+        <v>405</v>
+      </c>
+      <c r="F117" s="6">
+        <v>39</v>
+      </c>
+      <c r="G117" s="6">
+        <v>45</v>
+      </c>
+      <c r="H117" s="6">
+        <v>188</v>
+      </c>
+      <c r="I117" s="6">
+        <v>178</v>
+      </c>
+      <c r="J117" s="6">
+        <v>141</v>
+      </c>
+      <c r="K117" s="6">
+        <v>96</v>
+      </c>
+      <c r="L117" s="6">
+        <v>71</v>
+      </c>
+      <c r="M117" s="6">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-04-2020 21-40-30
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1854" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{67AB31EF-0659-4556-AFD1-031B39C9A9CA}"/>
+  <xr:revisionPtr revIDLastSave="1869" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9BA6153-9B2A-420A-BE72-73DC34479C56}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$117</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C116" totalsRowShown="0">
-  <autoFilter ref="A1:C116" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C117" totalsRowShown="0">
+  <autoFilter ref="A1:C117" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C116" totalsRowShown="0">
-  <autoFilter ref="A1:C116" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C117" totalsRowShown="0">
+  <autoFilter ref="A1:C117" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M117" totalsRowShown="0">
-  <autoFilter ref="A1:M117" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M118" totalsRowShown="0">
+  <autoFilter ref="A1:M118" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC116"/>
+  <dimension ref="A1:BC117"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3932,6 +3932,18 @@
         <v>500</v>
       </c>
     </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="4">
+        <v>44015</v>
+      </c>
+      <c r="B117">
+        <v>16945</v>
+      </c>
+      <c r="C117">
+        <f>B117-B116</f>
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3945,10 +3957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116:C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5127,7 +5139,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C116" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C117" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5321,6 +5333,18 @@
       <c r="C116">
         <f t="shared" si="1"/>
         <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="4">
+        <v>44015</v>
+      </c>
+      <c r="B117">
+        <v>698</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5333,11 +5357,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M117"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
+      <pane ySplit="1" topLeftCell="B113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10225,6 +10249,47 @@
       </c>
       <c r="M117" s="6">
         <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13">
+      <c r="A118" s="9">
+        <v>44015</v>
+      </c>
+      <c r="B118" s="6">
+        <v>35995</v>
+      </c>
+      <c r="C118" s="10">
+        <f>IFERROR(B118-B117,"")</f>
+        <v>758</v>
+      </c>
+      <c r="D118" s="6"/>
+      <c r="E118" s="10">
+        <f>C118-D118</f>
+        <v>758</v>
+      </c>
+      <c r="F118" s="6">
+        <v>36</v>
+      </c>
+      <c r="G118" s="6">
+        <v>37</v>
+      </c>
+      <c r="H118" s="6">
+        <v>202</v>
+      </c>
+      <c r="I118" s="6">
+        <v>158</v>
+      </c>
+      <c r="J118" s="6">
+        <v>136</v>
+      </c>
+      <c r="K118" s="6">
+        <v>86</v>
+      </c>
+      <c r="L118" s="6">
+        <v>84</v>
+      </c>
+      <c r="M118" s="6">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -19826,85 +19891,85 @@
       </c>
     </row>
     <row r="118" spans="1:20">
-      <c r="A118" s="4" t="str">
+      <c r="A118" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B118" t="str">
+        <v>44015</v>
+      </c>
+      <c r="B118">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C118" t="str">
+        <v>35995</v>
+      </c>
+      <c r="C118">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>758</v>
       </c>
       <c r="D118">
         <f>+IFERROR('Fallecidos Diarios'!B117,"")</f>
-        <v>0</v>
+        <v>698</v>
       </c>
       <c r="E118">
         <f>+IFERROR('Fallecidos Diarios'!C117,"")</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F118">
         <f>+IFERROR('Recuperados Diarios'!B117,"")</f>
-        <v>0</v>
+        <v>16945</v>
       </c>
       <c r="G118">
         <f>+IFERROR('Recuperados Diarios'!C117,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H118" t="str">
+        <v>500</v>
+      </c>
+      <c r="H118">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I118" t="str">
+        <v>18352</v>
+      </c>
+      <c r="I118">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J118" t="str">
+        <v>227</v>
+      </c>
+      <c r="J118">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K118" t="str">
+        <v>1.9391582164189472E-2</v>
+      </c>
+      <c r="K118">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L118" t="str">
+        <v>0.47075982775385472</v>
+      </c>
+      <c r="L118">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M118" t="str">
+        <v>0.50984859008195582</v>
+      </c>
+      <c r="M118">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N118" t="str">
+        <v>1486.7158892763732</v>
+      </c>
+      <c r="N118">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O118" t="str">
+        <v>4.4412607449856735E-2</v>
+      </c>
+      <c r="O118">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P118" t="str">
+        <v>2.9507229271171435E-2</v>
+      </c>
+      <c r="P118">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q118" t="str">
+        <v>1.236922406277245E-2</v>
+      </c>
+      <c r="Q118">
         <f t="shared" si="21"/>
-        <v/>
+        <v>8654.7246934359227</v>
       </c>
       <c r="R118">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>167.82880500120223</v>
       </c>
       <c r="S118">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T118" t="str">
+        <v>4074.296705938928</v>
+      </c>
+      <c r="T118">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4412.5991824957928</v>
       </c>
     </row>
     <row r="119" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-05-2020 17-43-44
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1869" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E9BA6153-9B2A-420A-BE72-73DC34479C56}"/>
+  <xr:revisionPtr revIDLastSave="1877" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B7AA127-09C1-4942-9664-C42188128A63}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$118</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C117" totalsRowShown="0">
-  <autoFilter ref="A1:C117" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C118" totalsRowShown="0">
+  <autoFilter ref="A1:C118" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C117" totalsRowShown="0">
-  <autoFilter ref="A1:C117" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C118" totalsRowShown="0">
+  <autoFilter ref="A1:C118" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M118" totalsRowShown="0">
-  <autoFilter ref="A1:M118" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M119" totalsRowShown="0">
+  <autoFilter ref="A1:M119" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC117"/>
+  <dimension ref="A1:BC118"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3944,6 +3944,18 @@
         <v>500</v>
       </c>
     </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="4">
+        <v>44016</v>
+      </c>
+      <c r="B118">
+        <v>17761</v>
+      </c>
+      <c r="C118">
+        <f>B118-B117</f>
+        <v>816</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3957,10 +3969,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116:C117"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117:C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5139,7 +5151,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C117" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C118" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5345,6 +5357,18 @@
       <c r="C117">
         <f t="shared" si="1"/>
         <v>31</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="4">
+        <v>44016</v>
+      </c>
+      <c r="B118">
+        <v>720</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5357,11 +5381,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M118"/>
+  <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M119" sqref="M119"/>
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10262,10 +10286,12 @@
         <f>IFERROR(B118-B117,"")</f>
         <v>758</v>
       </c>
-      <c r="D118" s="6"/>
+      <c r="D118" s="6">
+        <v>324</v>
+      </c>
       <c r="E118" s="10">
         <f>C118-D118</f>
-        <v>758</v>
+        <v>434</v>
       </c>
       <c r="F118" s="6">
         <v>36</v>
@@ -10291,6 +10317,31 @@
       <c r="M118" s="6">
         <v>19</v>
       </c>
+    </row>
+    <row r="119" spans="1:13">
+      <c r="A119" s="9">
+        <v>44016</v>
+      </c>
+      <c r="B119" s="6">
+        <v>36983</v>
+      </c>
+      <c r="C119" s="10">
+        <f>IFERROR(B119-B118,"")</f>
+        <v>988</v>
+      </c>
+      <c r="D119" s="6"/>
+      <c r="E119" s="10">
+        <f>C119-D119</f>
+        <v>988</v>
+      </c>
+      <c r="F119" s="6"/>
+      <c r="G119" s="6"/>
+      <c r="H119" s="6"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19973,85 +20024,85 @@
       </c>
     </row>
     <row r="119" spans="1:20">
-      <c r="A119" s="4" t="str">
+      <c r="A119" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B119" t="str">
+        <v>44016</v>
+      </c>
+      <c r="B119">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C119" t="str">
+        <v>36983</v>
+      </c>
+      <c r="C119">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>988</v>
       </c>
       <c r="D119">
         <f>+IFERROR('Fallecidos Diarios'!B118,"")</f>
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E119">
         <f>+IFERROR('Fallecidos Diarios'!C118,"")</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F119">
         <f>+IFERROR('Recuperados Diarios'!B118,"")</f>
-        <v>0</v>
+        <v>17761</v>
       </c>
       <c r="G119">
         <f>+IFERROR('Recuperados Diarios'!C118,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H119" t="str">
+        <v>816</v>
+      </c>
+      <c r="H119">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I119" t="str">
+        <v>18502</v>
+      </c>
+      <c r="I119">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J119" t="str">
+        <v>150</v>
+      </c>
+      <c r="J119">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K119" t="str">
+        <v>1.9468404402022552E-2</v>
+      </c>
+      <c r="K119">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L119" t="str">
+        <v>0.4802476813671146</v>
+      </c>
+      <c r="L119">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M119" t="str">
+        <v>0.50028391423086283</v>
+      </c>
+      <c r="M119">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N119" t="str">
+        <v>1974.8786077180846</v>
+      </c>
+      <c r="N119">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O119" t="str">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="O119">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P119" t="str">
+        <v>4.594335904509881E-2</v>
+      </c>
+      <c r="P119">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q119" t="str">
+        <v>8.1072316506323634E-3</v>
+      </c>
+      <c r="Q119">
         <f t="shared" si="21"/>
-        <v/>
+        <v>8892.281798509257</v>
       </c>
       <c r="R119">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>173.11853811012264</v>
       </c>
       <c r="S119">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T119" t="str">
+        <v>4270.497715797067</v>
+      </c>
+      <c r="T119">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4448.6655446020677</v>
       </c>
     </row>
     <row r="120" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-06-2020 17-47-18
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23101"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1877" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B7AA127-09C1-4942-9664-C42188128A63}"/>
+  <xr:revisionPtr revIDLastSave="1902" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32E7DB36-D90A-4C78-AA5F-067095AD1EEA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$119</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C118" totalsRowShown="0">
-  <autoFilter ref="A1:C118" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C119" totalsRowShown="0">
+  <autoFilter ref="A1:C119" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C118" totalsRowShown="0">
-  <autoFilter ref="A1:C118" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C119" totalsRowShown="0">
+  <autoFilter ref="A1:C119" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M119" totalsRowShown="0">
-  <autoFilter ref="A1:M119" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M120" totalsRowShown="0">
+  <autoFilter ref="A1:M120" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC118"/>
+  <dimension ref="A1:BC119"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3956,6 +3956,18 @@
         <v>816</v>
       </c>
     </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="4">
+        <v>44017</v>
+      </c>
+      <c r="B119">
+        <v>17986</v>
+      </c>
+      <c r="C119">
+        <f>B119-B118</f>
+        <v>225</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3969,10 +3981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117:C118"/>
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5151,7 +5163,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C118" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C119" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5369,6 +5381,18 @@
       <c r="C118">
         <f t="shared" si="1"/>
         <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="4">
+        <v>44017</v>
+      </c>
+      <c r="B119">
+        <v>747</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -5381,11 +5405,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M119"/>
+  <dimension ref="A1:M120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D120" sqref="D120"/>
+      <pane ySplit="1" topLeftCell="B115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10329,19 +10353,80 @@
         <f>IFERROR(B119-B118,"")</f>
         <v>988</v>
       </c>
-      <c r="D119" s="6"/>
+      <c r="D119" s="6">
+        <v>468</v>
+      </c>
       <c r="E119" s="10">
         <f>C119-D119</f>
-        <v>988</v>
-      </c>
-      <c r="F119" s="6"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="6"/>
-      <c r="I119" s="6"/>
-      <c r="J119" s="6"/>
-      <c r="K119" s="6"/>
-      <c r="L119" s="6"/>
-      <c r="M119" s="6"/>
+        <v>520</v>
+      </c>
+      <c r="F119" s="6">
+        <v>65</v>
+      </c>
+      <c r="G119" s="6">
+        <v>45</v>
+      </c>
+      <c r="H119" s="6">
+        <v>273</v>
+      </c>
+      <c r="I119" s="6">
+        <v>180</v>
+      </c>
+      <c r="J119" s="6">
+        <v>187</v>
+      </c>
+      <c r="K119" s="6">
+        <v>135</v>
+      </c>
+      <c r="L119" s="6">
+        <v>95</v>
+      </c>
+      <c r="M119" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
+      <c r="A120" s="9">
+        <v>44017</v>
+      </c>
+      <c r="B120" s="6">
+        <v>38149</v>
+      </c>
+      <c r="C120" s="10">
+        <f>IFERROR(B120-B119,"")</f>
+        <v>1166</v>
+      </c>
+      <c r="D120" s="6">
+        <v>549</v>
+      </c>
+      <c r="E120" s="10">
+        <f>C120-D120</f>
+        <v>617</v>
+      </c>
+      <c r="F120" s="6">
+        <v>73</v>
+      </c>
+      <c r="G120" s="6">
+        <v>62</v>
+      </c>
+      <c r="H120" s="6">
+        <v>268</v>
+      </c>
+      <c r="I120" s="6">
+        <v>252</v>
+      </c>
+      <c r="J120" s="6">
+        <v>216</v>
+      </c>
+      <c r="K120" s="6">
+        <v>141</v>
+      </c>
+      <c r="L120" s="6">
+        <v>138</v>
+      </c>
+      <c r="M120" s="6">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20106,85 +20191,85 @@
       </c>
     </row>
     <row r="120" spans="1:20">
-      <c r="A120" s="4" t="str">
+      <c r="A120" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B120" t="str">
+        <v>44017</v>
+      </c>
+      <c r="B120">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C120" t="str">
+        <v>38149</v>
+      </c>
+      <c r="C120">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1166</v>
       </c>
       <c r="D120">
         <f>+IFERROR('Fallecidos Diarios'!B119,"")</f>
-        <v>0</v>
+        <v>747</v>
       </c>
       <c r="E120">
         <f>+IFERROR('Fallecidos Diarios'!C119,"")</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F120">
         <f>+IFERROR('Recuperados Diarios'!B119,"")</f>
-        <v>0</v>
+        <v>17986</v>
       </c>
       <c r="G120">
         <f>+IFERROR('Recuperados Diarios'!C119,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H120" t="str">
+        <v>225</v>
+      </c>
+      <c r="H120">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I120" t="str">
+        <v>19416</v>
+      </c>
+      <c r="I120">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J120" t="str">
+        <v>914</v>
+      </c>
+      <c r="J120">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K120" t="str">
+        <v>1.9581116149833547E-2</v>
+      </c>
+      <c r="K120">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L120" t="str">
+        <v>0.47146714199585832</v>
+      </c>
+      <c r="L120">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M120" t="str">
+        <v>0.50895174185430814</v>
+      </c>
+      <c r="M120">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N120" t="str">
+        <v>2290.9834157395962</v>
+      </c>
+      <c r="N120">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O120" t="str">
+        <v>3.614457831325301E-2</v>
+      </c>
+      <c r="O120">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P120" t="str">
+        <v>1.2509729789836539E-2</v>
+      </c>
+      <c r="P120">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q120" t="str">
+        <v>4.707457766790276E-2</v>
+      </c>
+      <c r="Q120">
         <f t="shared" si="21"/>
-        <v/>
+        <v>9172.6376532820395</v>
       </c>
       <c r="R120">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>179.61048328925224</v>
       </c>
       <c r="S120">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T120" t="str">
+        <v>4324.5972589564799</v>
+      </c>
+      <c r="T120">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4668.4299110363072</v>
       </c>
     </row>
     <row r="121" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-07-2020 21-51-41
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1902" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32E7DB36-D90A-4C78-AA5F-067095AD1EEA}"/>
+  <xr:revisionPtr revIDLastSave="1917" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC5B35E2-ADCD-438F-BDD4-502CE1EBD4FA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$120</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C119" totalsRowShown="0">
-  <autoFilter ref="A1:C119" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C120" totalsRowShown="0">
+  <autoFilter ref="A1:C120" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C119" totalsRowShown="0">
-  <autoFilter ref="A1:C119" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C120" totalsRowShown="0">
+  <autoFilter ref="A1:C120" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M120" totalsRowShown="0">
-  <autoFilter ref="A1:M120" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M121" totalsRowShown="0">
+  <autoFilter ref="A1:M121" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC119"/>
+  <dimension ref="A1:BC120"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3968,6 +3968,18 @@
         <v>225</v>
       </c>
     </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="4">
+        <v>44018</v>
+      </c>
+      <c r="B120">
+        <v>18036</v>
+      </c>
+      <c r="C120">
+        <f>B120-B119</f>
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3981,10 +3993,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5163,7 +5175,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C119" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C120" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5393,6 +5405,18 @@
       <c r="C119">
         <f t="shared" si="1"/>
         <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="4">
+        <v>44018</v>
+      </c>
+      <c r="B120">
+        <v>770</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5405,11 +5429,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:M121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M121" sqref="M121"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L123" sqref="L123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10426,6 +10450,47 @@
       </c>
       <c r="M120" s="6">
         <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13">
+      <c r="A121" s="9">
+        <v>44018</v>
+      </c>
+      <c r="B121" s="6">
+        <v>39334</v>
+      </c>
+      <c r="C121" s="10">
+        <f>IFERROR(B121-B120,"")</f>
+        <v>1185</v>
+      </c>
+      <c r="D121" s="6"/>
+      <c r="E121" s="10">
+        <f>C121-D121</f>
+        <v>1185</v>
+      </c>
+      <c r="F121" s="6">
+        <v>73</v>
+      </c>
+      <c r="G121" s="6">
+        <v>78</v>
+      </c>
+      <c r="H121" s="6">
+        <v>278</v>
+      </c>
+      <c r="I121" s="6">
+        <v>247</v>
+      </c>
+      <c r="J121" s="6">
+        <v>222</v>
+      </c>
+      <c r="K121" s="6">
+        <v>137</v>
+      </c>
+      <c r="L121" s="6">
+        <v>124</v>
+      </c>
+      <c r="M121" s="6">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -20273,85 +20338,85 @@
       </c>
     </row>
     <row r="121" spans="1:20">
-      <c r="A121" s="4" t="str">
+      <c r="A121" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B121" t="str">
+        <v>44018</v>
+      </c>
+      <c r="B121">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C121" t="str">
+        <v>39334</v>
+      </c>
+      <c r="C121">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1185</v>
       </c>
       <c r="D121">
         <f>+IFERROR('Fallecidos Diarios'!B120,"")</f>
-        <v>0</v>
+        <v>770</v>
       </c>
       <c r="E121">
         <f>+IFERROR('Fallecidos Diarios'!C120,"")</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F121">
         <f>+IFERROR('Recuperados Diarios'!B120,"")</f>
-        <v>0</v>
+        <v>18036</v>
       </c>
       <c r="G121">
         <f>+IFERROR('Recuperados Diarios'!C120,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H121" t="str">
+        <v>50</v>
+      </c>
+      <c r="H121">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I121" t="str">
+        <v>20528</v>
+      </c>
+      <c r="I121">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J121" t="str">
+        <v>1112</v>
+      </c>
+      <c r="J121">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K121" t="str">
+        <v>1.9575939390857781E-2</v>
+      </c>
+      <c r="K121">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L121" t="str">
+        <v>0.45853460110845579</v>
+      </c>
+      <c r="L121">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M121" t="str">
+        <v>0.52188945950068644</v>
+      </c>
+      <c r="M121">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N121" t="str">
+        <v>2270.5957716289945</v>
+      </c>
+      <c r="N121">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O121" t="str">
+        <v>2.987012987012987E-2</v>
+      </c>
+      <c r="O121">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P121" t="str">
+        <v>2.7722333111554667E-3</v>
+      </c>
+      <c r="P121">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q121" t="str">
+        <v>5.416991426344505E-2</v>
+      </c>
+      <c r="Q121">
         <f t="shared" si="21"/>
-        <v/>
+        <v>9457.561913921616</v>
       </c>
       <c r="R121">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>185.1406588122145</v>
       </c>
       <c r="S121">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T121" t="str">
+        <v>4336.6193796585721</v>
+      </c>
+      <c r="T121">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4935.8018754508294</v>
       </c>
     </row>
     <row r="122" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-09-2020 01-55-58
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1917" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BC5B35E2-ADCD-438F-BDD4-502CE1EBD4FA}"/>
+  <xr:revisionPtr revIDLastSave="1934" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB3A35C5-052C-4B32-A8EE-580B04CC0020}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$121</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C120" totalsRowShown="0">
-  <autoFilter ref="A1:C120" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C121" totalsRowShown="0">
+  <autoFilter ref="A1:C121" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C120" totalsRowShown="0">
-  <autoFilter ref="A1:C120" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C121" totalsRowShown="0">
+  <autoFilter ref="A1:C121" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M121" totalsRowShown="0">
-  <autoFilter ref="A1:M121" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M122" totalsRowShown="0">
+  <autoFilter ref="A1:M122" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC120"/>
+  <dimension ref="A1:BC121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3980,6 +3980,18 @@
         <v>50</v>
       </c>
     </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="4">
+        <v>44019</v>
+      </c>
+      <c r="B121">
+        <v>18726</v>
+      </c>
+      <c r="C121">
+        <f>B121-B120</f>
+        <v>690</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -3993,10 +4005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+      <selection activeCell="C120" sqref="C120:C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5175,7 +5187,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C120" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C121" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5417,6 +5429,18 @@
       <c r="C120">
         <f t="shared" si="1"/>
         <v>23</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="4">
+        <v>44019</v>
+      </c>
+      <c r="B121">
+        <v>799</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -5429,11 +5453,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M121"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L123" sqref="L123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="B118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M123" sqref="M123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10463,10 +10487,12 @@
         <f>IFERROR(B121-B120,"")</f>
         <v>1185</v>
       </c>
-      <c r="D121" s="6"/>
+      <c r="D121" s="6">
+        <v>553</v>
+      </c>
       <c r="E121" s="10">
         <f>C121-D121</f>
-        <v>1185</v>
+        <v>632</v>
       </c>
       <c r="F121" s="6">
         <v>73</v>
@@ -10491,6 +10517,49 @@
       </c>
       <c r="M121" s="6">
         <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13">
+      <c r="A122" s="9">
+        <v>44019</v>
+      </c>
+      <c r="B122" s="6">
+        <v>40291</v>
+      </c>
+      <c r="C122" s="10">
+        <f>IFERROR(B122-B121,"")</f>
+        <v>957</v>
+      </c>
+      <c r="D122" s="6">
+        <v>426</v>
+      </c>
+      <c r="E122" s="10">
+        <f>C122-D122</f>
+        <v>531</v>
+      </c>
+      <c r="F122" s="6">
+        <v>40</v>
+      </c>
+      <c r="G122" s="6">
+        <v>50</v>
+      </c>
+      <c r="H122" s="6">
+        <v>240</v>
+      </c>
+      <c r="I122" s="6">
+        <v>191</v>
+      </c>
+      <c r="J122" s="6">
+        <v>190</v>
+      </c>
+      <c r="K122" s="6">
+        <v>113</v>
+      </c>
+      <c r="L122" s="6">
+        <v>123</v>
+      </c>
+      <c r="M122" s="6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -20420,85 +20489,85 @@
       </c>
     </row>
     <row r="122" spans="1:20">
-      <c r="A122" s="4" t="str">
+      <c r="A122" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B122" t="str">
+        <v>44019</v>
+      </c>
+      <c r="B122">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C122" t="str">
+        <v>40291</v>
+      </c>
+      <c r="C122">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>957</v>
       </c>
       <c r="D122">
         <f>+IFERROR('Fallecidos Diarios'!B121,"")</f>
-        <v>0</v>
+        <v>799</v>
       </c>
       <c r="E122">
         <f>+IFERROR('Fallecidos Diarios'!C121,"")</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F122">
         <f>+IFERROR('Recuperados Diarios'!B121,"")</f>
-        <v>0</v>
+        <v>18726</v>
       </c>
       <c r="G122">
         <f>+IFERROR('Recuperados Diarios'!C121,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H122" t="str">
+        <v>690</v>
+      </c>
+      <c r="H122">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I122" t="str">
+        <v>20766</v>
+      </c>
+      <c r="I122">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J122" t="str">
+        <v>238</v>
+      </c>
+      <c r="J122">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K122" t="str">
+        <v>1.9830731428855081E-2</v>
+      </c>
+      <c r="K122">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L122" t="str">
+        <v>0.46476880692958727</v>
+      </c>
+      <c r="L122">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M122" t="str">
+        <v>0.51540046164155762</v>
+      </c>
+      <c r="M122">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N122" t="str">
+        <v>1856.8085813348746</v>
+      </c>
+      <c r="N122">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O122" t="str">
+        <v>3.629536921151439E-2</v>
+      </c>
+      <c r="O122">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P122" t="str">
+        <v>3.6847164370394106E-2</v>
+      </c>
+      <c r="P122">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q122" t="str">
+        <v>1.1461042088028508E-2</v>
+      </c>
+      <c r="Q122">
         <f t="shared" si="21"/>
-        <v/>
+        <v>9687.6653041596546</v>
       </c>
       <c r="R122">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>192.11348881942774</v>
       </c>
       <c r="S122">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T122" t="str">
+        <v>4502.5246453474392</v>
+      </c>
+      <c r="T122">
         <f t="shared" si="24"/>
-        <v/>
+        <v>4993.0271699927871</v>
       </c>
     </row>
     <row r="123" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-09-2020 21-58-29
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1934" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB3A35C5-052C-4B32-A8EE-580B04CC0020}"/>
+  <xr:revisionPtr revIDLastSave="1950" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36D9AC4F-39A6-4C70-97D8-F7932102C353}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$122</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C121" totalsRowShown="0">
-  <autoFilter ref="A1:C121" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C122" totalsRowShown="0">
+  <autoFilter ref="A1:C122" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C121" totalsRowShown="0">
-  <autoFilter ref="A1:C121" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C122" totalsRowShown="0">
+  <autoFilter ref="A1:C122" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M122" totalsRowShown="0">
-  <autoFilter ref="A1:M122" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M123" totalsRowShown="0">
+  <autoFilter ref="A1:M123" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC121"/>
+  <dimension ref="A1:BC122"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -3992,6 +3992,18 @@
         <v>690</v>
       </c>
     </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="4">
+        <v>44020</v>
+      </c>
+      <c r="B122">
+        <v>19469</v>
+      </c>
+      <c r="C122">
+        <f>B122-B121</f>
+        <v>743</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4005,10 +4017,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120:C121"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5187,7 +5199,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C121" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C122" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5441,6 +5453,18 @@
       <c r="C121">
         <f t="shared" si="1"/>
         <v>29</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="4">
+        <v>44020</v>
+      </c>
+      <c r="B122">
+        <v>819</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5453,11 +5477,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M123" sqref="M123"/>
+      <pane ySplit="1" topLeftCell="B116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M124" sqref="M124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10560,6 +10584,49 @@
       </c>
       <c r="M122" s="6">
         <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
+      <c r="A123" s="9">
+        <v>44020</v>
+      </c>
+      <c r="B123" s="6">
+        <v>41251</v>
+      </c>
+      <c r="C123" s="10">
+        <f>IFERROR(B123-B122,"")</f>
+        <v>960</v>
+      </c>
+      <c r="D123" s="6">
+        <v>419</v>
+      </c>
+      <c r="E123" s="10">
+        <f>C123-D123</f>
+        <v>541</v>
+      </c>
+      <c r="F123" s="6">
+        <v>46</v>
+      </c>
+      <c r="G123" s="6">
+        <v>31</v>
+      </c>
+      <c r="H123" s="6">
+        <v>255</v>
+      </c>
+      <c r="I123" s="6">
+        <v>201</v>
+      </c>
+      <c r="J123" s="6">
+        <v>188</v>
+      </c>
+      <c r="K123" s="6">
+        <v>125</v>
+      </c>
+      <c r="L123" s="6">
+        <v>95</v>
+      </c>
+      <c r="M123" s="6">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -20571,85 +20638,85 @@
       </c>
     </row>
     <row r="123" spans="1:20">
-      <c r="A123" s="4" t="str">
+      <c r="A123" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B123" t="str">
+        <v>44020</v>
+      </c>
+      <c r="B123">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C123" t="str">
+        <v>41251</v>
+      </c>
+      <c r="C123">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>960</v>
       </c>
       <c r="D123">
         <f>+IFERROR('Fallecidos Diarios'!B122,"")</f>
-        <v>0</v>
+        <v>819</v>
       </c>
       <c r="E123">
         <f>+IFERROR('Fallecidos Diarios'!C122,"")</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F123">
         <f>+IFERROR('Recuperados Diarios'!B122,"")</f>
-        <v>0</v>
+        <v>19469</v>
       </c>
       <c r="G123">
         <f>+IFERROR('Recuperados Diarios'!C122,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H123" t="str">
+        <v>743</v>
+      </c>
+      <c r="H123">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I123" t="str">
+        <v>20963</v>
+      </c>
+      <c r="I123">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J123" t="str">
+        <v>197</v>
+      </c>
+      <c r="J123">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K123" t="str">
+        <v>1.9854064143899543E-2</v>
+      </c>
+      <c r="K123">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L123" t="str">
+        <v>0.4719643160165814</v>
+      </c>
+      <c r="L123">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M123" t="str">
+        <v>0.50818161983951904</v>
+      </c>
+      <c r="M123">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N123" t="str">
+        <v>1889.0883938367599</v>
+      </c>
+      <c r="N123">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O123" t="str">
+        <v>2.442002442002442E-2</v>
+      </c>
+      <c r="O123">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P123" t="str">
+        <v>3.8163233858955259E-2</v>
+      </c>
+      <c r="P123">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q123" t="str">
+        <v>9.3975098983924057E-3</v>
+      </c>
+      <c r="Q123">
         <f t="shared" si="21"/>
-        <v/>
+        <v>9918.4900216398182</v>
       </c>
       <c r="R123">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>196.92233710026449</v>
       </c>
       <c r="S123">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T123" t="str">
+        <v>4681.1733589805244</v>
+      </c>
+      <c r="T123">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5040.3943255590284</v>
       </c>
     </row>
     <row r="124" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-11-2020 18-04-31
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1950" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{36D9AC4F-39A6-4C70-97D8-F7932102C353}"/>
+  <xr:revisionPtr revIDLastSave="1972" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0122BD23-A167-4AE8-ABA3-7C5F8C84622D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$124</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C122" totalsRowShown="0">
-  <autoFilter ref="A1:C122" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C124" totalsRowShown="0">
+  <autoFilter ref="A1:C124" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C122" totalsRowShown="0">
-  <autoFilter ref="A1:C122" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C124" totalsRowShown="0">
+  <autoFilter ref="A1:C124" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M123" totalsRowShown="0">
-  <autoFilter ref="A1:M123" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M125" totalsRowShown="0">
+  <autoFilter ref="A1:M125" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC122"/>
+  <dimension ref="A1:BC124"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4004,6 +4004,30 @@
         <v>743</v>
       </c>
     </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="4">
+        <v>44021</v>
+      </c>
+      <c r="B123">
+        <v>20437</v>
+      </c>
+      <c r="C123">
+        <f>B123-B122</f>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="4">
+        <v>44022</v>
+      </c>
+      <c r="B124">
+        <v>21426</v>
+      </c>
+      <c r="C124">
+        <f>B124-B123</f>
+        <v>989</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4017,10 +4041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E124"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121:C122"/>
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5199,7 +5223,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C122" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C124" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5465,6 +5489,30 @@
       <c r="C122">
         <f t="shared" si="1"/>
         <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="4">
+        <v>44021</v>
+      </c>
+      <c r="B123">
+        <v>839</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="4">
+        <v>44022</v>
+      </c>
+      <c r="B124">
+        <v>863</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5477,11 +5525,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M123"/>
+  <dimension ref="A1:M125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M124" sqref="M124"/>
+      <pane ySplit="1" topLeftCell="B118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N124" sqref="N124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10628,6 +10676,74 @@
       <c r="M123" s="6">
         <v>19</v>
       </c>
+    </row>
+    <row r="124" spans="1:13">
+      <c r="A124" s="9">
+        <v>44021</v>
+      </c>
+      <c r="B124" s="6">
+        <v>42216</v>
+      </c>
+      <c r="C124" s="10">
+        <f>IFERROR(B124-B123,"")</f>
+        <v>965</v>
+      </c>
+      <c r="D124" s="6">
+        <v>439</v>
+      </c>
+      <c r="E124" s="10">
+        <f>C124-D124</f>
+        <v>526</v>
+      </c>
+      <c r="F124" s="6">
+        <v>56</v>
+      </c>
+      <c r="G124" s="6">
+        <v>61</v>
+      </c>
+      <c r="H124" s="6">
+        <v>252</v>
+      </c>
+      <c r="I124" s="6">
+        <v>206</v>
+      </c>
+      <c r="J124" s="6">
+        <v>148</v>
+      </c>
+      <c r="K124" s="6">
+        <v>126</v>
+      </c>
+      <c r="L124" s="6">
+        <v>97</v>
+      </c>
+      <c r="M124" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
+      <c r="A125" s="9">
+        <v>44022</v>
+      </c>
+      <c r="B125" s="6">
+        <v>43257</v>
+      </c>
+      <c r="C125" s="10">
+        <f>IFERROR(B125-B124,"")</f>
+        <v>1041</v>
+      </c>
+      <c r="D125" s="6"/>
+      <c r="E125" s="10">
+        <f>C125-D125</f>
+        <v>1041</v>
+      </c>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="6"/>
+      <c r="I125" s="6"/>
+      <c r="J125" s="6"/>
+      <c r="K125" s="6"/>
+      <c r="L125" s="6"/>
+      <c r="M125" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20720,167 +20836,167 @@
       </c>
     </row>
     <row r="124" spans="1:20">
-      <c r="A124" s="4" t="str">
+      <c r="A124" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B124" t="str">
+        <v>44021</v>
+      </c>
+      <c r="B124">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C124" t="str">
+        <v>42216</v>
+      </c>
+      <c r="C124">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>965</v>
       </c>
       <c r="D124">
         <f>+IFERROR('Fallecidos Diarios'!B123,"")</f>
-        <v>0</v>
+        <v>839</v>
       </c>
       <c r="E124">
         <f>+IFERROR('Fallecidos Diarios'!C123,"")</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F124">
         <f>+IFERROR('Recuperados Diarios'!B123,"")</f>
-        <v>0</v>
+        <v>20437</v>
       </c>
       <c r="G124">
         <f>+IFERROR('Recuperados Diarios'!C123,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H124" t="str">
+        <v>968</v>
+      </c>
+      <c r="H124">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I124" t="str">
+        <v>20940</v>
+      </c>
+      <c r="I124">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J124" t="str">
+        <v>-23</v>
+      </c>
+      <c r="J124">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K124" t="str">
+        <v>1.9873981428842145E-2</v>
+      </c>
+      <c r="K124">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L124" t="str">
+        <v>0.48410555239719538</v>
+      </c>
+      <c r="L124">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M124" t="str">
+        <v>0.4960204661739625</v>
+      </c>
+      <c r="M124">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N124" t="str">
+        <v>1945.4842406876789</v>
+      </c>
+      <c r="N124">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O124" t="str">
+        <v>2.3837902264600714E-2</v>
+      </c>
+      <c r="O124">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P124" t="str">
+        <v>4.7365073151636738E-2</v>
+      </c>
+      <c r="P124">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q124" t="str">
+        <v>-1.0983763132760267E-3</v>
+      </c>
+      <c r="Q124">
         <f t="shared" si="21"/>
-        <v/>
+        <v>10150.516951190191</v>
       </c>
       <c r="R124">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>201.73118538110123</v>
       </c>
       <c r="S124">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T124" t="str">
+        <v>4913.9216157730225</v>
+      </c>
+      <c r="T124">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5034.8641500360663</v>
       </c>
     </row>
     <row r="125" spans="1:20">
-      <c r="A125" s="4" t="str">
+      <c r="A125" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B125" t="str">
+        <v>44022</v>
+      </c>
+      <c r="B125">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C125" t="str">
+        <v>43257</v>
+      </c>
+      <c r="C125">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1041</v>
       </c>
       <c r="D125">
         <f>+IFERROR('Fallecidos Diarios'!B124,"")</f>
-        <v>0</v>
+        <v>863</v>
       </c>
       <c r="E125">
         <f>+IFERROR('Fallecidos Diarios'!C124,"")</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F125">
         <f>+IFERROR('Recuperados Diarios'!B124,"")</f>
-        <v>0</v>
+        <v>21426</v>
       </c>
       <c r="G125">
         <f>+IFERROR('Recuperados Diarios'!C124,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H125" t="str">
+        <v>989</v>
+      </c>
+      <c r="H125">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I125" t="str">
+        <v>20968</v>
+      </c>
+      <c r="I125">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J125" t="str">
+        <v>28</v>
+      </c>
+      <c r="J125">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K125" t="str">
+        <v>1.9950528238204222E-2</v>
+      </c>
+      <c r="K125">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L125" t="str">
+        <v>0.4953186767459602</v>
+      </c>
+      <c r="L125">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M125" t="str">
+        <v>0.4847307950158356</v>
+      </c>
+      <c r="M125">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N125" t="str">
+        <v>2147.5837943533002</v>
+      </c>
+      <c r="N125">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O125" t="str">
+        <v>2.7809965237543453E-2</v>
+      </c>
+      <c r="O125">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P125" t="str">
+        <v>4.6158872398021099E-2</v>
+      </c>
+      <c r="P125">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q125" t="str">
+        <v>1.3353681800839375E-3</v>
+      </c>
+      <c r="Q125">
         <f t="shared" si="21"/>
-        <v/>
+        <v>10400.817504207742</v>
       </c>
       <c r="R125">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>207.50180331810532</v>
       </c>
       <c r="S125">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T125" t="str">
+        <v>5151.719163260399</v>
+      </c>
+      <c r="T125">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5041.5965376292379</v>
       </c>
     </row>
     <row r="126" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-12-2020 22-08-13
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1972" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0122BD23-A167-4AE8-ABA3-7C5F8C84622D}"/>
+  <xr:revisionPtr revIDLastSave="1988" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{987DBAA1-1D58-4C48-9BF5-D768188981BC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$125</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C124" totalsRowShown="0">
-  <autoFilter ref="A1:C124" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C125" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C124" totalsRowShown="0">
-  <autoFilter ref="A1:C124" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C125" totalsRowShown="0">
+  <autoFilter ref="A1:C125" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M125" totalsRowShown="0">
-  <autoFilter ref="A1:M125" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M126" totalsRowShown="0">
+  <autoFilter ref="A1:M126" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC124"/>
+  <dimension ref="A1:BC125"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4028,6 +4028,18 @@
         <v>989</v>
       </c>
     </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="4">
+        <v>44023</v>
+      </c>
+      <c r="B125">
+        <v>22170</v>
+      </c>
+      <c r="C125">
+        <f>B125-B124</f>
+        <v>744</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4041,10 +4053,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E124"/>
+  <dimension ref="A1:E125"/>
   <sheetViews>
     <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="C124" sqref="C124:C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5223,7 +5235,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C124" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C125" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5513,6 +5525,18 @@
       <c r="C124">
         <f t="shared" si="1"/>
         <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="4">
+        <v>44023</v>
+      </c>
+      <c r="B125">
+        <v>893</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5525,11 +5549,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M125"/>
+  <dimension ref="A1:M126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="B118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N124" sqref="N124"/>
+      <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10731,19 +10755,62 @@
         <f>IFERROR(B125-B124,"")</f>
         <v>1041</v>
       </c>
-      <c r="D125" s="6"/>
+      <c r="D125" s="6">
+        <v>487</v>
+      </c>
       <c r="E125" s="10">
         <f>C125-D125</f>
-        <v>1041</v>
-      </c>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
-      <c r="H125" s="6"/>
-      <c r="I125" s="6"/>
-      <c r="J125" s="6"/>
-      <c r="K125" s="6"/>
-      <c r="L125" s="6"/>
-      <c r="M125" s="6"/>
+        <v>554</v>
+      </c>
+      <c r="F125" s="6">
+        <v>63</v>
+      </c>
+      <c r="G125" s="6">
+        <v>43</v>
+      </c>
+      <c r="H125" s="6">
+        <v>277</v>
+      </c>
+      <c r="I125" s="6">
+        <v>210</v>
+      </c>
+      <c r="J125" s="6">
+        <v>172</v>
+      </c>
+      <c r="K125" s="6">
+        <v>135</v>
+      </c>
+      <c r="L125" s="6">
+        <v>117</v>
+      </c>
+      <c r="M125" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
+      <c r="A126" s="9">
+        <v>44023</v>
+      </c>
+      <c r="B126" s="6">
+        <v>44332</v>
+      </c>
+      <c r="C126" s="10">
+        <f>IFERROR(B126-B125,"")</f>
+        <v>1075</v>
+      </c>
+      <c r="D126" s="6"/>
+      <c r="E126" s="10">
+        <f>C126-D126</f>
+        <v>1075</v>
+      </c>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="6"/>
+      <c r="K126" s="6"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21000,85 +21067,85 @@
       </c>
     </row>
     <row r="126" spans="1:20">
-      <c r="A126" s="4" t="str">
+      <c r="A126" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B126" t="str">
+        <v>44023</v>
+      </c>
+      <c r="B126">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C126" t="str">
+        <v>44332</v>
+      </c>
+      <c r="C126">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1075</v>
       </c>
       <c r="D126">
         <f>+IFERROR('Fallecidos Diarios'!B125,"")</f>
-        <v>0</v>
+        <v>893</v>
       </c>
       <c r="E126">
         <f>+IFERROR('Fallecidos Diarios'!C125,"")</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F126">
         <f>+IFERROR('Recuperados Diarios'!B125,"")</f>
-        <v>0</v>
+        <v>22170</v>
       </c>
       <c r="G126">
         <f>+IFERROR('Recuperados Diarios'!C125,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H126" t="str">
+        <v>744</v>
+      </c>
+      <c r="H126">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I126" t="str">
+        <v>21269</v>
+      </c>
+      <c r="I126">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J126" t="str">
+        <v>301</v>
+      </c>
+      <c r="J126">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K126" t="str">
+        <v>2.0143462961292068E-2</v>
+      </c>
+      <c r="K126">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L126" t="str">
+        <v>0.50009022827754224</v>
+      </c>
+      <c r="L126">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M126" t="str">
+        <v>0.47976630876116577</v>
+      </c>
+      <c r="M126">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N126" t="str">
+        <v>2240.6742206967888</v>
+      </c>
+      <c r="N126">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O126" t="str">
+        <v>3.3594624860022397E-2</v>
+      </c>
+      <c r="O126">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P126" t="str">
+        <v>3.3558863328822734E-2</v>
+      </c>
+      <c r="P126">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q126" t="str">
+        <v>1.4152052282664911E-2</v>
+      </c>
+      <c r="Q126">
         <f t="shared" si="21"/>
-        <v/>
+        <v>10659.293099302717</v>
       </c>
       <c r="R126">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>214.71507573936043</v>
       </c>
       <c r="S126">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T126" t="str">
+        <v>5330.6083193075265</v>
+      </c>
+      <c r="T126">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5113.9697042558309</v>
       </c>
     </row>
     <row r="127" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-13-2020 18-10-37
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1988" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{987DBAA1-1D58-4C48-9BF5-D768188981BC}"/>
+  <xr:revisionPtr revIDLastSave="2013" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3995DB02-82B3-42AB-954F-256F4123F708}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$125</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$126</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C125" totalsRowShown="0">
-  <autoFilter ref="A1:C125" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C126" totalsRowShown="0">
+  <autoFilter ref="A1:C126" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C125" totalsRowShown="0">
-  <autoFilter ref="A1:C125" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C126" totalsRowShown="0">
+  <autoFilter ref="A1:C126" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M126" totalsRowShown="0">
-  <autoFilter ref="A1:M126" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M127" totalsRowShown="0">
+  <autoFilter ref="A1:M127" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC125"/>
+  <dimension ref="A1:BC126"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4040,6 +4040,18 @@
         <v>744</v>
       </c>
     </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="4">
+        <v>44024</v>
+      </c>
+      <c r="B126">
+        <v>23039</v>
+      </c>
+      <c r="C126">
+        <f>B126-B125</f>
+        <v>869</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4053,10 +4065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124:C125"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5235,7 +5247,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C125" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C126" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5537,6 +5549,18 @@
       <c r="C125">
         <f t="shared" si="1"/>
         <v>30</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="4">
+        <v>44024</v>
+      </c>
+      <c r="B126">
+        <v>909</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -5549,11 +5573,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
+      <pane ySplit="1" topLeftCell="B121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10756,35 +10780,35 @@
         <v>1041</v>
       </c>
       <c r="D125" s="6">
-        <v>487</v>
+        <v>967</v>
       </c>
       <c r="E125" s="10">
         <f>C125-D125</f>
-        <v>554</v>
+        <v>74</v>
       </c>
       <c r="F125" s="6">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="G125" s="6">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="H125" s="6">
-        <v>277</v>
+        <v>534</v>
       </c>
       <c r="I125" s="6">
+        <v>487</v>
+      </c>
+      <c r="J125" s="6">
+        <v>389</v>
+      </c>
+      <c r="K125" s="6">
+        <v>248</v>
+      </c>
+      <c r="L125" s="6">
         <v>210</v>
       </c>
-      <c r="J125" s="6">
-        <v>172</v>
-      </c>
-      <c r="K125" s="6">
-        <v>135</v>
-      </c>
-      <c r="L125" s="6">
-        <v>117</v>
-      </c>
       <c r="M125" s="6">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="126" spans="1:13">
@@ -10798,19 +10822,62 @@
         <f>IFERROR(B126-B125,"")</f>
         <v>1075</v>
       </c>
-      <c r="D126" s="6"/>
+      <c r="D126" s="6">
+        <v>572</v>
+      </c>
       <c r="E126" s="10">
         <f>C126-D126</f>
-        <v>1075</v>
-      </c>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
-      <c r="I126" s="6"/>
-      <c r="J126" s="6"/>
-      <c r="K126" s="6"/>
-      <c r="L126" s="6"/>
-      <c r="M126" s="6"/>
+        <v>503</v>
+      </c>
+      <c r="F126" s="6">
+        <v>72</v>
+      </c>
+      <c r="G126" s="6">
+        <v>75</v>
+      </c>
+      <c r="H126" s="6">
+        <v>351</v>
+      </c>
+      <c r="I126" s="6">
+        <v>257</v>
+      </c>
+      <c r="J126" s="6">
+        <v>214</v>
+      </c>
+      <c r="K126" s="6">
+        <v>171</v>
+      </c>
+      <c r="L126" s="6">
+        <v>123</v>
+      </c>
+      <c r="M126" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
+      <c r="A127" s="9">
+        <v>44024</v>
+      </c>
+      <c r="B127" s="6">
+        <v>45633</v>
+      </c>
+      <c r="C127" s="10">
+        <f>IFERROR(B127-B126,"")</f>
+        <v>1301</v>
+      </c>
+      <c r="D127" s="6"/>
+      <c r="E127" s="10">
+        <f>C127-D127</f>
+        <v>1301</v>
+      </c>
+      <c r="F127" s="6"/>
+      <c r="G127" s="6"/>
+      <c r="H127" s="6"/>
+      <c r="I127" s="6"/>
+      <c r="J127" s="6"/>
+      <c r="K127" s="6"/>
+      <c r="L127" s="6"/>
+      <c r="M127" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21149,85 +21216,85 @@
       </c>
     </row>
     <row r="127" spans="1:20">
-      <c r="A127" s="4" t="str">
+      <c r="A127" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B127" t="str">
+        <v>44024</v>
+      </c>
+      <c r="B127">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C127" t="str">
+        <v>45633</v>
+      </c>
+      <c r="C127">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1301</v>
       </c>
       <c r="D127">
         <f>+IFERROR('Fallecidos Diarios'!B126,"")</f>
-        <v>0</v>
+        <v>909</v>
       </c>
       <c r="E127">
         <f>+IFERROR('Fallecidos Diarios'!C126,"")</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F127">
         <f>+IFERROR('Recuperados Diarios'!B126,"")</f>
-        <v>0</v>
+        <v>23039</v>
       </c>
       <c r="G127">
         <f>+IFERROR('Recuperados Diarios'!C126,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H127" t="str">
+        <v>869</v>
+      </c>
+      <c r="H127">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I127" t="str">
+        <v>21685</v>
+      </c>
+      <c r="I127">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J127" t="str">
+        <v>416</v>
+      </c>
+      <c r="J127">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K127" t="str">
+        <v>1.9919794885280388E-2</v>
+      </c>
+      <c r="K127">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L127" t="str">
+        <v>0.50487585738391072</v>
+      </c>
+      <c r="L127">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M127" t="str">
+        <v>0.47520434773080883</v>
+      </c>
+      <c r="M127">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N127" t="str">
+        <v>2737.7695642148951</v>
+      </c>
+      <c r="N127">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O127" t="str">
+        <v>1.7601760176017601E-2</v>
+      </c>
+      <c r="O127">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P127" t="str">
+        <v>3.7718650983115588E-2</v>
+      </c>
+      <c r="P127">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q127" t="str">
+        <v>1.9183767581277381E-2</v>
+      </c>
+      <c r="Q127">
         <f t="shared" si="21"/>
-        <v/>
+        <v>10972.108679971147</v>
       </c>
       <c r="R127">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>218.56215436402982</v>
       </c>
       <c r="S127">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T127" t="str">
+        <v>5539.5527771098823</v>
+      </c>
+      <c r="T127">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5213.9937484972352</v>
       </c>
     </row>
     <row r="128" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-18-2020 02-28-28
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2013" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3995DB02-82B3-42AB-954F-256F4123F708}"/>
+  <xr:revisionPtr revIDLastSave="2076" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B75EFA39-0605-481C-A6D4-1A25F0A3CDA6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$130</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C126" totalsRowShown="0">
-  <autoFilter ref="A1:C126" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C130" totalsRowShown="0">
+  <autoFilter ref="A1:C130" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C126" totalsRowShown="0">
-  <autoFilter ref="A1:C126" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C130" totalsRowShown="0">
+  <autoFilter ref="A1:C130" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M127" totalsRowShown="0">
-  <autoFilter ref="A1:M127" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M131" totalsRowShown="0">
+  <autoFilter ref="A1:M131" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC126"/>
+  <dimension ref="A1:BC130"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4052,6 +4052,54 @@
         <v>869</v>
       </c>
     </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="4">
+        <v>44025</v>
+      </c>
+      <c r="B127">
+        <v>23919</v>
+      </c>
+      <c r="C127">
+        <f>B127-B126</f>
+        <v>880</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="4">
+        <v>44026</v>
+      </c>
+      <c r="B128">
+        <v>24667</v>
+      </c>
+      <c r="C128">
+        <f>B128-B127</f>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="4">
+        <v>44027</v>
+      </c>
+      <c r="B129">
+        <v>25417</v>
+      </c>
+      <c r="C129">
+        <f>B129-B128</f>
+        <v>750</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="4">
+        <v>44028</v>
+      </c>
+      <c r="B130">
+        <v>25842</v>
+      </c>
+      <c r="C130">
+        <f>B130-B129</f>
+        <v>425</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4065,10 +4113,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="D127" sqref="D127"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5247,7 +5295,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C126" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C130" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5561,6 +5609,54 @@
       <c r="C126">
         <f t="shared" si="1"/>
         <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="4">
+        <v>44025</v>
+      </c>
+      <c r="B127">
+        <v>932</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="4">
+        <v>44026</v>
+      </c>
+      <c r="B128">
+        <v>960</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="4">
+        <v>44027</v>
+      </c>
+      <c r="B129">
+        <v>982</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="4">
+        <v>44028</v>
+      </c>
+      <c r="B130">
+        <v>1000</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -5573,11 +5669,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D127" sqref="D127"/>
+      <pane ySplit="1" topLeftCell="B122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10865,19 +10961,191 @@
         <f>IFERROR(B127-B126,"")</f>
         <v>1301</v>
       </c>
-      <c r="D127" s="6"/>
+      <c r="D127" s="6">
+        <v>748</v>
+      </c>
       <c r="E127" s="10">
         <f>C127-D127</f>
-        <v>1301</v>
-      </c>
-      <c r="F127" s="6"/>
-      <c r="G127" s="6"/>
-      <c r="H127" s="6"/>
-      <c r="I127" s="6"/>
-      <c r="J127" s="6"/>
-      <c r="K127" s="6"/>
-      <c r="L127" s="6"/>
-      <c r="M127" s="6"/>
+        <v>553</v>
+      </c>
+      <c r="F127" s="6">
+        <v>114</v>
+      </c>
+      <c r="G127" s="6">
+        <v>97</v>
+      </c>
+      <c r="H127" s="6">
+        <v>372</v>
+      </c>
+      <c r="I127" s="6">
+        <v>279</v>
+      </c>
+      <c r="J127" s="6">
+        <v>274</v>
+      </c>
+      <c r="K127" s="6">
+        <v>214</v>
+      </c>
+      <c r="L127" s="6">
+        <v>168</v>
+      </c>
+      <c r="M127" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" s="9">
+        <v>44025</v>
+      </c>
+      <c r="B128" s="6">
+        <v>47173</v>
+      </c>
+      <c r="C128" s="10">
+        <f>IFERROR(B128-B127,"")</f>
+        <v>1540</v>
+      </c>
+      <c r="D128" s="6">
+        <v>413</v>
+      </c>
+      <c r="E128" s="10">
+        <f>C128-D128</f>
+        <v>1127</v>
+      </c>
+      <c r="F128" s="6">
+        <v>69</v>
+      </c>
+      <c r="G128" s="6">
+        <v>67</v>
+      </c>
+      <c r="H128" s="6">
+        <v>221</v>
+      </c>
+      <c r="I128" s="6">
+        <v>180</v>
+      </c>
+      <c r="J128" s="6">
+        <v>136</v>
+      </c>
+      <c r="K128" s="6">
+        <v>115</v>
+      </c>
+      <c r="L128" s="6">
+        <v>119</v>
+      </c>
+      <c r="M128" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13">
+      <c r="A129" s="9">
+        <v>44026</v>
+      </c>
+      <c r="B129" s="6">
+        <v>48096</v>
+      </c>
+      <c r="C129" s="10">
+        <f>IFERROR(B129-B128,"")</f>
+        <v>923</v>
+      </c>
+      <c r="D129" s="6">
+        <v>586</v>
+      </c>
+      <c r="E129" s="10">
+        <f>C129-D129</f>
+        <v>337</v>
+      </c>
+      <c r="F129" s="6">
+        <v>57</v>
+      </c>
+      <c r="G129" s="6">
+        <v>55</v>
+      </c>
+      <c r="H129" s="6">
+        <v>250</v>
+      </c>
+      <c r="I129" s="6">
+        <v>260</v>
+      </c>
+      <c r="J129" s="6">
+        <v>177</v>
+      </c>
+      <c r="K129" s="6">
+        <v>163</v>
+      </c>
+      <c r="L129" s="6">
+        <v>159</v>
+      </c>
+      <c r="M129" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13">
+      <c r="A130" s="9">
+        <v>44027</v>
+      </c>
+      <c r="B130" s="6">
+        <v>49243</v>
+      </c>
+      <c r="C130" s="10">
+        <f>IFERROR(B130-B129,"")</f>
+        <v>1147</v>
+      </c>
+      <c r="D130" s="6">
+        <v>346</v>
+      </c>
+      <c r="E130" s="10">
+        <f>C130-D130</f>
+        <v>801</v>
+      </c>
+      <c r="F130" s="6">
+        <v>60</v>
+      </c>
+      <c r="G130" s="6">
+        <v>33</v>
+      </c>
+      <c r="H130" s="6">
+        <v>185</v>
+      </c>
+      <c r="I130" s="6">
+        <v>158</v>
+      </c>
+      <c r="J130" s="6">
+        <v>117</v>
+      </c>
+      <c r="K130" s="6">
+        <v>99</v>
+      </c>
+      <c r="L130" s="6">
+        <v>81</v>
+      </c>
+      <c r="M130" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
+      <c r="A131" s="9">
+        <v>44028</v>
+      </c>
+      <c r="B131" s="6">
+        <v>50373</v>
+      </c>
+      <c r="C131" s="10">
+        <f>IFERROR(B131-B130,"")</f>
+        <v>1130</v>
+      </c>
+      <c r="D131" s="6"/>
+      <c r="E131" s="10">
+        <f>C131-D131</f>
+        <v>1130</v>
+      </c>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="6"/>
+      <c r="K131" s="6"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21298,331 +21566,331 @@
       </c>
     </row>
     <row r="128" spans="1:20">
-      <c r="A128" s="4" t="str">
+      <c r="A128" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B128" t="str">
+        <v>44025</v>
+      </c>
+      <c r="B128">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C128" t="str">
+        <v>47173</v>
+      </c>
+      <c r="C128">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1540</v>
       </c>
       <c r="D128">
         <f>+IFERROR('Fallecidos Diarios'!B127,"")</f>
-        <v>0</v>
+        <v>932</v>
       </c>
       <c r="E128">
         <f>+IFERROR('Fallecidos Diarios'!C127,"")</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F128">
         <f>+IFERROR('Recuperados Diarios'!B127,"")</f>
-        <v>0</v>
+        <v>23919</v>
       </c>
       <c r="G128">
         <f>+IFERROR('Recuperados Diarios'!C127,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H128" t="str">
+        <v>880</v>
+      </c>
+      <c r="H128">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I128" t="str">
+        <v>22322</v>
+      </c>
+      <c r="I128">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J128" t="str">
+        <v>637</v>
+      </c>
+      <c r="J128">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K128" t="str">
+        <v>1.9757064422445042E-2</v>
+      </c>
+      <c r="K128">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L128" t="str">
+        <v>0.50704852351981011</v>
+      </c>
+      <c r="L128">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M128" t="str">
+        <v>0.47319441205774487</v>
+      </c>
+      <c r="M128">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N128" t="str">
+        <v>3254.4763014066843</v>
+      </c>
+      <c r="N128">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O128" t="str">
+        <v>2.4678111587982832E-2</v>
+      </c>
+      <c r="O128">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P128" t="str">
+        <v>3.6790835737279988E-2</v>
+      </c>
+      <c r="P128">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q128" t="str">
+        <v>2.8536869456141922E-2</v>
+      </c>
+      <c r="Q128">
         <f t="shared" si="21"/>
-        <v/>
+        <v>11342.389997595576</v>
       </c>
       <c r="R128">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>224.09232988699208</v>
       </c>
       <c r="S128">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T128" t="str">
+        <v>5751.1421014666994</v>
+      </c>
+      <c r="T128">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5367.155566241885</v>
       </c>
     </row>
     <row r="129" spans="1:20">
-      <c r="A129" s="4" t="str">
+      <c r="A129" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B129" t="str">
+        <v>44026</v>
+      </c>
+      <c r="B129">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C129" t="str">
+        <v>48096</v>
+      </c>
+      <c r="C129">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>923</v>
       </c>
       <c r="D129">
         <f>+IFERROR('Fallecidos Diarios'!B128,"")</f>
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="E129">
         <f>+IFERROR('Fallecidos Diarios'!C128,"")</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F129">
         <f>+IFERROR('Recuperados Diarios'!B128,"")</f>
-        <v>0</v>
+        <v>24667</v>
       </c>
       <c r="G129">
         <f>+IFERROR('Recuperados Diarios'!C128,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H129" t="str">
+        <v>748</v>
+      </c>
+      <c r="H129">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I129" t="str">
+        <v>22469</v>
+      </c>
+      <c r="I129">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J129" t="str">
+        <v>147</v>
+      </c>
+      <c r="J129">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K129" t="str">
+        <v>1.9960079840319361E-2</v>
+      </c>
+      <c r="K129">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L129" t="str">
+        <v>0.51287009314703924</v>
+      </c>
+      <c r="L129">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M129" t="str">
+        <v>0.46716982701264137</v>
+      </c>
+      <c r="M129">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N129" t="str">
+        <v>1975.7269126351864</v>
+      </c>
+      <c r="N129">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O129" t="str">
+        <v>2.9166666666666667E-2</v>
+      </c>
+      <c r="O129">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P129" t="str">
+        <v>3.0323914541695383E-2</v>
+      </c>
+      <c r="P129">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q129" t="str">
+        <v>6.5423472339667986E-3</v>
+      </c>
+      <c r="Q129">
         <f t="shared" si="21"/>
-        <v/>
+        <v>11564.318345756192</v>
       </c>
       <c r="R129">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>230.82471748016351</v>
       </c>
       <c r="S129">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T129" t="str">
+        <v>5930.9930271699932</v>
+      </c>
+      <c r="T129">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5402.500601106035</v>
       </c>
     </row>
     <row r="130" spans="1:20">
-      <c r="A130" s="4" t="str">
+      <c r="A130" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B130" t="str">
+        <v>44027</v>
+      </c>
+      <c r="B130">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C130" t="str">
+        <v>49243</v>
+      </c>
+      <c r="C130">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1147</v>
       </c>
       <c r="D130">
         <f>+IFERROR('Fallecidos Diarios'!B129,"")</f>
-        <v>0</v>
+        <v>982</v>
       </c>
       <c r="E130">
         <f>+IFERROR('Fallecidos Diarios'!C129,"")</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F130">
         <f>+IFERROR('Recuperados Diarios'!B129,"")</f>
-        <v>0</v>
+        <v>25417</v>
       </c>
       <c r="G130">
         <f>+IFERROR('Recuperados Diarios'!C129,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H130" t="str">
+        <v>750</v>
+      </c>
+      <c r="H130">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I130" t="str">
+        <v>22844</v>
+      </c>
+      <c r="I130">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J130" t="str">
+        <v>375</v>
+      </c>
+      <c r="J130">
         <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="K130" t="str">
+        <v>1.994192067908129E-2</v>
+      </c>
+      <c r="K130">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="L130" t="str">
+        <v>0.51615458034644524</v>
+      </c>
+      <c r="L130">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="M130" t="str">
+        <v>0.46390349897447353</v>
+      </c>
+      <c r="M130">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="N130" t="str">
+        <v>2472.4969795132201</v>
+      </c>
+      <c r="N130">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="O130" t="str">
+        <v>2.2403258655804479E-2</v>
+      </c>
+      <c r="O130">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="P130" t="str">
+        <v>2.9507809733642837E-2</v>
+      </c>
+      <c r="P130">
         <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="Q130" t="str">
+        <v>1.6415689021187181E-2</v>
+      </c>
+      <c r="Q130">
         <f t="shared" si="21"/>
-        <v/>
+        <v>11840.105794662179</v>
       </c>
       <c r="R130">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>236.11445058908393</v>
       </c>
       <c r="S130">
         <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
-      <c r="T130" t="str">
+        <v>6111.3248377013706</v>
+      </c>
+      <c r="T130">
         <f t="shared" si="24"/>
-        <v/>
+        <v>5492.6665063717246</v>
       </c>
     </row>
     <row r="131" spans="1:20">
-      <c r="A131" s="4" t="str">
+      <c r="A131" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B131" t="str">
+        <v>44028</v>
+      </c>
+      <c r="B131">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C131" t="str">
+        <v>50373</v>
+      </c>
+      <c r="C131">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1130</v>
       </c>
       <c r="D131">
         <f>+IFERROR('Fallecidos Diarios'!B130,"")</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E131">
         <f>+IFERROR('Fallecidos Diarios'!C130,"")</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F131">
         <f>+IFERROR('Recuperados Diarios'!B130,"")</f>
-        <v>0</v>
+        <v>25842</v>
       </c>
       <c r="G131">
         <f>+IFERROR('Recuperados Diarios'!C130,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H131" t="str">
+        <v>425</v>
+      </c>
+      <c r="H131">
         <f t="shared" ref="H131:H194" si="26">+IFERROR(B131-D131-F131,"")</f>
-        <v/>
-      </c>
-      <c r="I131" t="str">
+        <v>23531</v>
+      </c>
+      <c r="I131">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="J131" t="str">
+        <v>687</v>
+      </c>
+      <c r="J131">
         <f t="shared" ref="J131:J194" si="27">+IFERROR(D131/B131,"")</f>
-        <v/>
-      </c>
-      <c r="K131" t="str">
+        <v>1.9851904790264625E-2</v>
+      </c>
+      <c r="K131">
         <f t="shared" ref="K131:K194" si="28">+IFERROR(F131/B131,"")</f>
-        <v/>
-      </c>
-      <c r="L131" t="str">
+        <v>0.51301292359001849</v>
+      </c>
+      <c r="L131">
         <f t="shared" ref="L131:L194" si="29">+IFERROR(H131/B131,"")</f>
-        <v/>
-      </c>
-      <c r="M131" t="str">
+        <v>0.4671351716197169</v>
+      </c>
+      <c r="M131">
         <f t="shared" ref="M131:M194" si="30">+IFERROR(C131/L131,"")</f>
-        <v/>
-      </c>
-      <c r="N131" t="str">
+        <v>2419.0000424971313</v>
+      </c>
+      <c r="N131">
         <f t="shared" ref="N131:N194" si="31">+IFERROR(E131/D131,"")</f>
-        <v/>
-      </c>
-      <c r="O131" t="str">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O131">
         <f t="shared" ref="O131:O194" si="32">+IFERROR(G131/F131,"")</f>
-        <v/>
-      </c>
-      <c r="P131" t="str">
+        <v>1.6446095503444006E-2</v>
+      </c>
+      <c r="P131">
         <f t="shared" ref="P131:P194" si="33">+IFERROR(I131/H131,"")</f>
-        <v/>
-      </c>
-      <c r="Q131" t="str">
+        <v>2.9195529301772129E-2</v>
+      </c>
+      <c r="Q131">
         <f t="shared" ref="Q131:Q194" si="34">+IFERROR(B131/4.159,"")</f>
-        <v/>
+        <v>12111.805722529454</v>
       </c>
       <c r="R131">
         <f t="shared" ref="R131:R194" si="35">+IFERROR(D131/4.159,"")</f>
-        <v>0</v>
+        <v>240.442414041837</v>
       </c>
       <c r="S131">
         <f t="shared" ref="S131:S194" si="36">+IFERROR(F131/4.159,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T131" t="str">
+        <v>6213.5128636691516</v>
+      </c>
+      <c r="T131">
         <f t="shared" ref="T131:T194" si="37">+IFERROR(H131/4.159,"")</f>
-        <v/>
+        <v>5657.8504448184658</v>
       </c>
     </row>
     <row r="132" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-19-2020 02-32-00
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2076" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B75EFA39-0605-481C-A6D4-1A25F0A3CDA6}"/>
+  <xr:revisionPtr revIDLastSave="2084" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6AFFF639-6158-4292-BE61-B3E3EEF7B94E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$131</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C130" totalsRowShown="0">
-  <autoFilter ref="A1:C130" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C131" totalsRowShown="0">
+  <autoFilter ref="A1:C131" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C130" totalsRowShown="0">
-  <autoFilter ref="A1:C130" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C131" totalsRowShown="0">
+  <autoFilter ref="A1:C131" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M131" totalsRowShown="0">
-  <autoFilter ref="A1:M131" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M132" totalsRowShown="0">
+  <autoFilter ref="A1:M132" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC130"/>
+  <dimension ref="A1:BC131"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4100,6 +4100,18 @@
         <v>425</v>
       </c>
     </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="4">
+        <v>44029</v>
+      </c>
+      <c r="B131">
+        <v>26520</v>
+      </c>
+      <c r="C131">
+        <f>B131-B130</f>
+        <v>678</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4113,10 +4125,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E131"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5295,7 +5307,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C130" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C131" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5657,6 +5669,18 @@
       <c r="C130">
         <f t="shared" si="1"/>
         <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="4">
+        <v>44029</v>
+      </c>
+      <c r="B131">
+        <v>1038</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -5669,11 +5693,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M131"/>
+  <dimension ref="A1:M132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="B122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M131" sqref="M131"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -11146,6 +11170,31 @@
       <c r="K131" s="6"/>
       <c r="L131" s="6"/>
       <c r="M131" s="6"/>
+    </row>
+    <row r="132" spans="1:13">
+      <c r="A132" s="9">
+        <v>44029</v>
+      </c>
+      <c r="B132" s="6">
+        <v>51408</v>
+      </c>
+      <c r="C132" s="10">
+        <f>IFERROR(B132-B131,"")</f>
+        <v>1035</v>
+      </c>
+      <c r="D132" s="6"/>
+      <c r="E132" s="10">
+        <f>C132-D132</f>
+        <v>1035</v>
+      </c>
+      <c r="F132" s="6"/>
+      <c r="G132" s="6"/>
+      <c r="H132" s="6"/>
+      <c r="I132" s="6"/>
+      <c r="J132" s="6"/>
+      <c r="K132" s="6"/>
+      <c r="L132" s="6"/>
+      <c r="M132" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21894,85 +21943,85 @@
       </c>
     </row>
     <row r="132" spans="1:20">
-      <c r="A132" s="4" t="str">
+      <c r="A132" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B132" t="str">
+        <v>44029</v>
+      </c>
+      <c r="B132">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C132" t="str">
+        <v>51408</v>
+      </c>
+      <c r="C132">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1035</v>
       </c>
       <c r="D132">
         <f>+IFERROR('Fallecidos Diarios'!B131,"")</f>
-        <v>0</v>
+        <v>1038</v>
       </c>
       <c r="E132">
         <f>+IFERROR('Fallecidos Diarios'!C131,"")</f>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F132">
         <f>+IFERROR('Recuperados Diarios'!B131,"")</f>
-        <v>0</v>
+        <v>26520</v>
       </c>
       <c r="G132">
         <f>+IFERROR('Recuperados Diarios'!C131,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H132" t="str">
+        <v>678</v>
+      </c>
+      <c r="H132">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I132" t="str">
+        <v>23850</v>
+      </c>
+      <c r="I132">
         <f t="shared" ref="I132:I195" si="38">+IFERROR(H132-H131,"")</f>
-        <v/>
-      </c>
-      <c r="J132" t="str">
+        <v>319</v>
+      </c>
+      <c r="J132">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K132" t="str">
+        <v>2.0191409897292251E-2</v>
+      </c>
+      <c r="K132">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L132" t="str">
+        <v>0.51587301587301593</v>
+      </c>
+      <c r="L132">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M132" t="str">
+        <v>0.46393557422969189</v>
+      </c>
+      <c r="M132">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N132" t="str">
+        <v>2230.9132075471698</v>
+      </c>
+      <c r="N132">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O132" t="str">
+        <v>3.6608863198458574E-2</v>
+      </c>
+      <c r="O132">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P132" t="str">
+        <v>2.5565610859728506E-2</v>
+      </c>
+      <c r="P132">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q132" t="str">
+        <v>1.3375262054507337E-2</v>
+      </c>
+      <c r="Q132">
         <f t="shared" si="34"/>
-        <v/>
+        <v>12360.663621062757</v>
       </c>
       <c r="R132">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>249.57922577542681</v>
       </c>
       <c r="S132">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T132" t="str">
+        <v>6376.5328203895169</v>
+      </c>
+      <c r="T132">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5734.5515748978123</v>
       </c>
     </row>
     <row r="133" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 07-22-2020 02-41-36
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2084" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6AFFF639-6158-4292-BE61-B3E3EEF7B94E}"/>
+  <xr:revisionPtr revIDLastSave="2103" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3D51BFC-738D-455A-AF68-FD5D76A36FD5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$131</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$134</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C131" totalsRowShown="0">
-  <autoFilter ref="A1:C131" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C134" totalsRowShown="0">
+  <autoFilter ref="A1:C134" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C131" totalsRowShown="0">
-  <autoFilter ref="A1:C131" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C134" totalsRowShown="0">
+  <autoFilter ref="A1:C134" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M132" totalsRowShown="0">
-  <autoFilter ref="A1:M132" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M135" totalsRowShown="0">
+  <autoFilter ref="A1:M135" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC131"/>
+  <dimension ref="A1:BC134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4112,6 +4112,42 @@
         <v>678</v>
       </c>
     </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="4">
+        <v>44030</v>
+      </c>
+      <c r="B132">
+        <v>27494</v>
+      </c>
+      <c r="C132">
+        <f>B132-B131</f>
+        <v>974</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="4">
+        <v>44031</v>
+      </c>
+      <c r="B133">
+        <v>28482</v>
+      </c>
+      <c r="C133">
+        <f>B133-B132</f>
+        <v>988</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="4">
+        <v>44032</v>
+      </c>
+      <c r="B134">
+        <v>29164</v>
+      </c>
+      <c r="C134">
+        <f>B134-B133</f>
+        <v>682</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
     <sortCondition descending="1" ref="A72:A1048573"/>
@@ -4125,10 +4161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5307,7 +5343,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C131" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C134" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5681,6 +5717,42 @@
       <c r="C131">
         <f t="shared" si="1"/>
         <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="4">
+        <v>44030</v>
+      </c>
+      <c r="B132">
+        <v>1071</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="4">
+        <v>44031</v>
+      </c>
+      <c r="B133">
+        <v>1096</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="4">
+        <v>44032</v>
+      </c>
+      <c r="B134">
+        <v>1127</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5693,11 +5765,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M132"/>
+  <dimension ref="A1:M135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C132" sqref="C132"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -11195,6 +11267,81 @@
       <c r="K132" s="6"/>
       <c r="L132" s="6"/>
       <c r="M132" s="6"/>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133" s="9">
+        <v>44030</v>
+      </c>
+      <c r="B133" s="6">
+        <v>52261</v>
+      </c>
+      <c r="C133" s="10">
+        <f>IFERROR(B133-B132,"")</f>
+        <v>853</v>
+      </c>
+      <c r="D133" s="6"/>
+      <c r="E133" s="10">
+        <f>C133-D133</f>
+        <v>853</v>
+      </c>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="6"/>
+      <c r="I133" s="6"/>
+      <c r="J133" s="6"/>
+      <c r="K133" s="6"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+    </row>
+    <row r="134" spans="1:13">
+      <c r="A134" s="9">
+        <v>44031</v>
+      </c>
+      <c r="B134" s="6">
+        <v>53468</v>
+      </c>
+      <c r="C134" s="10">
+        <f>IFERROR(B134-B133,"")</f>
+        <v>1207</v>
+      </c>
+      <c r="D134" s="6"/>
+      <c r="E134" s="10">
+        <f>C134-D134</f>
+        <v>1207</v>
+      </c>
+      <c r="F134" s="6"/>
+      <c r="G134" s="6"/>
+      <c r="H134" s="6"/>
+      <c r="I134" s="6"/>
+      <c r="J134" s="6"/>
+      <c r="K134" s="6"/>
+      <c r="L134" s="6"/>
+      <c r="M134" s="6"/>
+    </row>
+    <row r="135" spans="1:13">
+      <c r="A135" s="9">
+        <v>44032</v>
+      </c>
+      <c r="B135" s="6">
+        <v>54426</v>
+      </c>
+      <c r="C135" s="10">
+        <f>IFERROR(B135-B134,"")</f>
+        <v>958</v>
+      </c>
+      <c r="D135" s="6"/>
+      <c r="E135" s="10">
+        <f>C135-D135</f>
+        <v>958</v>
+      </c>
+      <c r="F135" s="6"/>
+      <c r="G135" s="6"/>
+      <c r="H135" s="6"/>
+      <c r="I135" s="6"/>
+      <c r="J135" s="6"/>
+      <c r="K135" s="6"/>
+      <c r="L135" s="6"/>
+      <c r="M135" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22025,249 +22172,249 @@
       </c>
     </row>
     <row r="133" spans="1:20">
-      <c r="A133" s="4" t="str">
+      <c r="A133" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B133" t="str">
+        <v>44030</v>
+      </c>
+      <c r="B133">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C133" t="str">
+        <v>52261</v>
+      </c>
+      <c r="C133">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>853</v>
       </c>
       <c r="D133">
         <f>+IFERROR('Fallecidos Diarios'!B132,"")</f>
-        <v>0</v>
+        <v>1071</v>
       </c>
       <c r="E133">
         <f>+IFERROR('Fallecidos Diarios'!C132,"")</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F133">
         <f>+IFERROR('Recuperados Diarios'!B132,"")</f>
-        <v>0</v>
+        <v>27494</v>
       </c>
       <c r="G133">
         <f>+IFERROR('Recuperados Diarios'!C132,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H133" t="str">
+        <v>974</v>
+      </c>
+      <c r="H133">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I133" t="str">
+        <v>23696</v>
+      </c>
+      <c r="I133">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J133" t="str">
+        <v>-154</v>
+      </c>
+      <c r="J133">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K133" t="str">
+        <v>2.0493293277970188E-2</v>
+      </c>
+      <c r="K133">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L133" t="str">
+        <v>0.52609020110598725</v>
+      </c>
+      <c r="L133">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M133" t="str">
+        <v>0.45341650561604258</v>
+      </c>
+      <c r="M133">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N133" t="str">
+        <v>1881.2724932478054</v>
+      </c>
+      <c r="N133">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O133" t="str">
+        <v>3.081232492997199E-2</v>
+      </c>
+      <c r="O133">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P133" t="str">
+        <v>3.5425911107878086E-2</v>
+      </c>
+      <c r="P133">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q133" t="str">
+        <v>-6.4989871708305202E-3</v>
+      </c>
+      <c r="Q133">
         <f t="shared" si="34"/>
-        <v/>
+        <v>12565.761000240444</v>
       </c>
       <c r="R133">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>257.51382543880743</v>
       </c>
       <c r="S133">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T133" t="str">
+        <v>6610.7237316662658</v>
+      </c>
+      <c r="T133">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5697.5234431353692</v>
       </c>
     </row>
     <row r="134" spans="1:20">
-      <c r="A134" s="4" t="str">
+      <c r="A134" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B134" t="str">
+        <v>44031</v>
+      </c>
+      <c r="B134">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C134" t="str">
+        <v>53468</v>
+      </c>
+      <c r="C134">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1207</v>
       </c>
       <c r="D134">
         <f>+IFERROR('Fallecidos Diarios'!B133,"")</f>
-        <v>0</v>
+        <v>1096</v>
       </c>
       <c r="E134">
         <f>+IFERROR('Fallecidos Diarios'!C133,"")</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F134">
         <f>+IFERROR('Recuperados Diarios'!B133,"")</f>
-        <v>0</v>
+        <v>28482</v>
       </c>
       <c r="G134">
         <f>+IFERROR('Recuperados Diarios'!C133,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H134" t="str">
+        <v>988</v>
+      </c>
+      <c r="H134">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I134" t="str">
+        <v>23890</v>
+      </c>
+      <c r="I134">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J134" t="str">
+        <v>194</v>
+      </c>
+      <c r="J134">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K134" t="str">
+        <v>2.0498241939103764E-2</v>
+      </c>
+      <c r="K134">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L134" t="str">
+        <v>0.53269245155981149</v>
+      </c>
+      <c r="L134">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M134" t="str">
+        <v>0.44680930650108475</v>
+      </c>
+      <c r="M134">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N134" t="str">
+        <v>2701.376140644621</v>
+      </c>
+      <c r="N134">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O134" t="str">
+        <v>2.281021897810219E-2</v>
+      </c>
+      <c r="O134">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P134" t="str">
+        <v>3.4688575240502777E-2</v>
+      </c>
+      <c r="P134">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q134" t="str">
+        <v>8.1205525324403519E-3</v>
+      </c>
+      <c r="Q134">
         <f t="shared" si="34"/>
-        <v/>
+        <v>12855.974993988941</v>
       </c>
       <c r="R134">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>263.52488578985333</v>
       </c>
       <c r="S134">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T134" t="str">
+        <v>6848.280836739601</v>
+      </c>
+      <c r="T134">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5744.1692714594856</v>
       </c>
     </row>
     <row r="135" spans="1:20">
-      <c r="A135" s="4" t="str">
+      <c r="A135" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B135" t="str">
+        <v>44032</v>
+      </c>
+      <c r="B135">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C135" t="str">
+        <v>54426</v>
+      </c>
+      <c r="C135">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>958</v>
       </c>
       <c r="D135">
         <f>+IFERROR('Fallecidos Diarios'!B134,"")</f>
-        <v>0</v>
+        <v>1127</v>
       </c>
       <c r="E135">
         <f>+IFERROR('Fallecidos Diarios'!C134,"")</f>
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F135">
         <f>+IFERROR('Recuperados Diarios'!B134,"")</f>
-        <v>0</v>
+        <v>29164</v>
       </c>
       <c r="G135">
         <f>+IFERROR('Recuperados Diarios'!C134,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H135" t="str">
+        <v>682</v>
+      </c>
+      <c r="H135">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I135" t="str">
+        <v>24135</v>
+      </c>
+      <c r="I135">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J135" t="str">
+        <v>245</v>
+      </c>
+      <c r="J135">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K135" t="str">
+        <v>2.0707015029581451E-2</v>
+      </c>
+      <c r="K135">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L135" t="str">
+        <v>0.53584683790835264</v>
+      </c>
+      <c r="L135">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M135" t="str">
+        <v>0.44344614706206592</v>
+      </c>
+      <c r="M135">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N135" t="str">
+        <v>2160.3525170913613</v>
+      </c>
+      <c r="N135">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O135" t="str">
+        <v>2.7506654835847383E-2</v>
+      </c>
+      <c r="O135">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P135" t="str">
+        <v>2.3384995199561102E-2</v>
+      </c>
+      <c r="P135">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q135" t="str">
+        <v>1.015123264967889E-2</v>
+      </c>
+      <c r="Q135">
         <f t="shared" si="34"/>
-        <v/>
+        <v>13086.31882664102</v>
       </c>
       <c r="R135">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>270.97860062515031</v>
       </c>
       <c r="S135">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T135" t="str">
+        <v>7012.2625631161336</v>
+      </c>
+      <c r="T135">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5803.0776628997355</v>
       </c>
     </row>
     <row r="136" spans="1:20">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-01-2020 16-53-22
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2103" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C3D51BFC-738D-455A-AF68-FD5D76A36FD5}"/>
+  <xr:revisionPtr revIDLastSave="2169" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E54D0D07-2D4A-4AF2-86FC-194854E45BD1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$145</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C134" totalsRowShown="0">
-  <autoFilter ref="A1:C134" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C145" totalsRowShown="0">
+  <autoFilter ref="A1:C145" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C134" totalsRowShown="0">
-  <autoFilter ref="A1:C134" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C145" totalsRowShown="0">
+  <autoFilter ref="A1:C145" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M135" totalsRowShown="0">
-  <autoFilter ref="A1:M135" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M146" totalsRowShown="0">
+  <autoFilter ref="A1:M146" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC134"/>
+  <dimension ref="A1:BC145"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4148,9 +4148,141 @@
         <v>682</v>
       </c>
     </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="4">
+        <v>44033</v>
+      </c>
+      <c r="B135">
+        <v>30075</v>
+      </c>
+      <c r="C135">
+        <f t="shared" ref="C135:C145" si="3">B135-B134</f>
+        <v>911</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="4">
+        <v>44034</v>
+      </c>
+      <c r="B136">
+        <v>31122</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="3"/>
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="4">
+        <v>44035</v>
+      </c>
+      <c r="B137">
+        <v>31828</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="3"/>
+        <v>706</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="4">
+        <v>44036</v>
+      </c>
+      <c r="B138">
+        <v>32704</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="3"/>
+        <v>876</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="4">
+        <v>44037</v>
+      </c>
+      <c r="B139">
+        <v>33428</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="3"/>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="4">
+        <v>44038</v>
+      </c>
+      <c r="B140">
+        <v>34131</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="3"/>
+        <v>703</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="4">
+        <v>44039</v>
+      </c>
+      <c r="B141">
+        <v>35086</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="3"/>
+        <v>955</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="4">
+        <v>44040</v>
+      </c>
+      <c r="B142">
+        <v>36181</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="3"/>
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="4">
+        <v>44041</v>
+      </c>
+      <c r="B143">
+        <v>37316</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="3"/>
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="4">
+        <v>44042</v>
+      </c>
+      <c r="B144">
+        <v>38218</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="3"/>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="4">
+        <v>44043</v>
+      </c>
+      <c r="B145">
+        <v>39166</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="3"/>
+        <v>948</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048573">
-    <sortCondition descending="1" ref="A72:A1048573"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048576">
+    <sortCondition descending="1" ref="A72:A1048576"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4161,10 +4293,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F152" sqref="F152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5343,7 +5475,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C134" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C145" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -5753,6 +5885,138 @@
       <c r="C134">
         <f t="shared" si="1"/>
         <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="4">
+        <v>44033</v>
+      </c>
+      <c r="B135">
+        <v>1159</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="4">
+        <v>44034</v>
+      </c>
+      <c r="B136">
+        <v>1180</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="4">
+        <v>44035</v>
+      </c>
+      <c r="B137">
+        <v>1209</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="4">
+        <v>44036</v>
+      </c>
+      <c r="B138">
+        <v>1250</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="4">
+        <v>44037</v>
+      </c>
+      <c r="B139">
+        <v>1275</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="4">
+        <v>44038</v>
+      </c>
+      <c r="B140">
+        <v>1294</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="4">
+        <v>44039</v>
+      </c>
+      <c r="B141">
+        <v>1322</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="4">
+        <v>44040</v>
+      </c>
+      <c r="B142">
+        <v>1349</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="4">
+        <v>44041</v>
+      </c>
+      <c r="B143">
+        <v>1374</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="4">
+        <v>44042</v>
+      </c>
+      <c r="B144">
+        <v>1397</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="4">
+        <v>44043</v>
+      </c>
+      <c r="B145">
+        <v>1421</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5765,11 +6029,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M135"/>
+  <dimension ref="A1:M146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
+      <pane ySplit="1" topLeftCell="C2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -10972,11 +11236,11 @@
         <v>1041</v>
       </c>
       <c r="D125" s="6">
-        <v>967</v>
+        <v>482</v>
       </c>
       <c r="E125" s="10">
         <f>C125-D125</f>
-        <v>74</v>
+        <v>559</v>
       </c>
       <c r="F125" s="6">
         <v>128</v>
@@ -11015,11 +11279,11 @@
         <v>1075</v>
       </c>
       <c r="D126" s="6">
-        <v>572</v>
+        <v>485</v>
       </c>
       <c r="E126" s="10">
         <f>C126-D126</f>
-        <v>503</v>
+        <v>590</v>
       </c>
       <c r="F126" s="6">
         <v>72</v>
@@ -11058,11 +11322,11 @@
         <v>1301</v>
       </c>
       <c r="D127" s="6">
-        <v>748</v>
+        <v>570</v>
       </c>
       <c r="E127" s="10">
         <f>C127-D127</f>
-        <v>553</v>
+        <v>731</v>
       </c>
       <c r="F127" s="6">
         <v>114</v>
@@ -11101,11 +11365,11 @@
         <v>1540</v>
       </c>
       <c r="D128" s="6">
-        <v>413</v>
+        <v>752</v>
       </c>
       <c r="E128" s="10">
         <f>C128-D128</f>
-        <v>1127</v>
+        <v>788</v>
       </c>
       <c r="F128" s="6">
         <v>69</v>
@@ -11144,11 +11408,11 @@
         <v>923</v>
       </c>
       <c r="D129" s="6">
-        <v>586</v>
+        <v>410</v>
       </c>
       <c r="E129" s="10">
         <f>C129-D129</f>
-        <v>337</v>
+        <v>513</v>
       </c>
       <c r="F129" s="6">
         <v>57</v>
@@ -11187,11 +11451,11 @@
         <v>1147</v>
       </c>
       <c r="D130" s="6">
-        <v>346</v>
+        <v>587</v>
       </c>
       <c r="E130" s="10">
         <f>C130-D130</f>
-        <v>801</v>
+        <v>560</v>
       </c>
       <c r="F130" s="6">
         <v>60</v>
@@ -11229,10 +11493,12 @@
         <f>IFERROR(B131-B130,"")</f>
         <v>1130</v>
       </c>
-      <c r="D131" s="6"/>
+      <c r="D131" s="6">
+        <v>518</v>
+      </c>
       <c r="E131" s="10">
         <f>C131-D131</f>
-        <v>1130</v>
+        <v>612</v>
       </c>
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
@@ -11254,10 +11520,12 @@
         <f>IFERROR(B132-B131,"")</f>
         <v>1035</v>
       </c>
-      <c r="D132" s="6"/>
+      <c r="D132" s="6">
+        <v>485</v>
+      </c>
       <c r="E132" s="10">
         <f>C132-D132</f>
-        <v>1035</v>
+        <v>550</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
@@ -11279,10 +11547,12 @@
         <f>IFERROR(B133-B132,"")</f>
         <v>853</v>
       </c>
-      <c r="D133" s="6"/>
+      <c r="D133" s="6">
+        <v>368</v>
+      </c>
       <c r="E133" s="10">
         <f>C133-D133</f>
-        <v>853</v>
+        <v>485</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
@@ -11304,10 +11574,12 @@
         <f>IFERROR(B134-B133,"")</f>
         <v>1207</v>
       </c>
-      <c r="D134" s="6"/>
+      <c r="D134" s="6">
+        <v>570</v>
+      </c>
       <c r="E134" s="10">
         <f>C134-D134</f>
-        <v>1207</v>
+        <v>637</v>
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="6"/>
@@ -11329,10 +11601,12 @@
         <f>IFERROR(B135-B134,"")</f>
         <v>958</v>
       </c>
-      <c r="D135" s="6"/>
+      <c r="D135" s="6">
+        <v>478</v>
+      </c>
       <c r="E135" s="10">
         <f>C135-D135</f>
-        <v>958</v>
+        <v>480</v>
       </c>
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
@@ -11342,6 +11616,215 @@
       <c r="K135" s="6"/>
       <c r="L135" s="6"/>
       <c r="M135" s="6"/>
+    </row>
+    <row r="136" spans="1:13">
+      <c r="A136" s="9">
+        <v>44033</v>
+      </c>
+      <c r="B136">
+        <v>55153</v>
+      </c>
+      <c r="C136" s="8">
+        <f t="shared" ref="C136:C140" si="7">IFERROR(B136-B135,"")</f>
+        <v>727</v>
+      </c>
+      <c r="D136">
+        <v>351</v>
+      </c>
+      <c r="E136" s="8">
+        <f t="shared" ref="E136:E140" si="8">C136-D136</f>
+        <v>376</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13">
+      <c r="A137" s="9">
+        <v>44034</v>
+      </c>
+      <c r="B137">
+        <v>55906</v>
+      </c>
+      <c r="C137" s="8">
+        <f t="shared" si="7"/>
+        <v>753</v>
+      </c>
+      <c r="D137">
+        <v>323</v>
+      </c>
+      <c r="E137" s="8">
+        <f t="shared" si="8"/>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13">
+      <c r="A138" s="9">
+        <v>44035</v>
+      </c>
+      <c r="B138">
+        <v>56817</v>
+      </c>
+      <c r="C138" s="8">
+        <f t="shared" si="7"/>
+        <v>911</v>
+      </c>
+      <c r="D138">
+        <v>458</v>
+      </c>
+      <c r="E138" s="8">
+        <f t="shared" si="8"/>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13">
+      <c r="A139" s="9">
+        <v>44036</v>
+      </c>
+      <c r="B139">
+        <v>57993</v>
+      </c>
+      <c r="C139" s="8">
+        <f t="shared" si="7"/>
+        <v>1176</v>
+      </c>
+      <c r="D139">
+        <v>548</v>
+      </c>
+      <c r="E139" s="8">
+        <f t="shared" si="8"/>
+        <v>628</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13">
+      <c r="A140" s="9">
+        <v>44037</v>
+      </c>
+      <c r="B140">
+        <v>58864</v>
+      </c>
+      <c r="C140" s="8">
+        <f t="shared" si="7"/>
+        <v>871</v>
+      </c>
+      <c r="D140">
+        <v>420</v>
+      </c>
+      <c r="E140" s="8">
+        <f t="shared" si="8"/>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13">
+      <c r="A141" s="9">
+        <v>44038</v>
+      </c>
+      <c r="B141">
+        <v>60296</v>
+      </c>
+      <c r="C141" s="8">
+        <f t="shared" ref="C141:C145" si="9">IFERROR(B141-B140,"")</f>
+        <v>1432</v>
+      </c>
+      <c r="D141">
+        <v>705</v>
+      </c>
+      <c r="E141" s="8">
+        <f t="shared" ref="E141:E145" si="10">C141-D141</f>
+        <v>727</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13">
+      <c r="A142" s="9">
+        <v>44039</v>
+      </c>
+      <c r="B142">
+        <v>61442</v>
+      </c>
+      <c r="C142" s="8">
+        <f t="shared" si="9"/>
+        <v>1146</v>
+      </c>
+      <c r="D142">
+        <v>564</v>
+      </c>
+      <c r="E142" s="8">
+        <f t="shared" si="10"/>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13">
+      <c r="A143" s="9">
+        <v>44040</v>
+      </c>
+      <c r="B143">
+        <v>62223</v>
+      </c>
+      <c r="C143" s="8">
+        <f t="shared" si="9"/>
+        <v>781</v>
+      </c>
+      <c r="D143">
+        <v>389</v>
+      </c>
+      <c r="E143" s="8">
+        <f t="shared" si="10"/>
+        <v>392</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13">
+      <c r="A144" s="9">
+        <v>44041</v>
+      </c>
+      <c r="B144">
+        <v>63269</v>
+      </c>
+      <c r="C144" s="8">
+        <f t="shared" si="9"/>
+        <v>1046</v>
+      </c>
+      <c r="D144">
+        <v>487</v>
+      </c>
+      <c r="E144" s="8">
+        <f t="shared" si="10"/>
+        <v>559</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="9">
+        <v>44042</v>
+      </c>
+      <c r="B145">
+        <v>64191</v>
+      </c>
+      <c r="C145" s="8">
+        <f t="shared" si="9"/>
+        <v>922</v>
+      </c>
+      <c r="D145">
+        <v>447</v>
+      </c>
+      <c r="E145" s="8">
+        <f t="shared" si="10"/>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="9">
+        <v>44043</v>
+      </c>
+      <c r="B146">
+        <v>65256</v>
+      </c>
+      <c r="C146" s="8">
+        <f>IFERROR(B146-B145,"")</f>
+        <v>1065</v>
+      </c>
+      <c r="D146">
+        <v>510</v>
+      </c>
+      <c r="E146" s="8">
+        <f>C146-D146</f>
+        <v>555</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11358,8 +11841,8 @@
   </sheetPr>
   <dimension ref="A1:T277"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -22418,905 +22901,905 @@
       </c>
     </row>
     <row r="136" spans="1:20">
-      <c r="A136" s="4" t="str">
+      <c r="A136" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B136" t="str">
+        <v>44033</v>
+      </c>
+      <c r="B136">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C136" t="str">
+        <v>55153</v>
+      </c>
+      <c r="C136">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>727</v>
       </c>
       <c r="D136">
         <f>+IFERROR('Fallecidos Diarios'!B135,"")</f>
-        <v>0</v>
+        <v>1159</v>
       </c>
       <c r="E136">
         <f>+IFERROR('Fallecidos Diarios'!C135,"")</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F136">
         <f>+IFERROR('Recuperados Diarios'!B135,"")</f>
-        <v>0</v>
+        <v>30075</v>
       </c>
       <c r="G136">
         <f>+IFERROR('Recuperados Diarios'!C135,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H136" t="str">
+        <v>911</v>
+      </c>
+      <c r="H136">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I136" t="str">
+        <v>23919</v>
+      </c>
+      <c r="I136">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J136" t="str">
+        <v>-216</v>
+      </c>
+      <c r="J136">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K136" t="str">
+        <v>2.1014269396043735E-2</v>
+      </c>
+      <c r="K136">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L136" t="str">
+        <v>0.54530125287835662</v>
+      </c>
+      <c r="L136">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M136" t="str">
+        <v>0.4336844777255997</v>
+      </c>
+      <c r="M136">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N136" t="str">
+        <v>1676.3339186420837</v>
+      </c>
+      <c r="N136">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O136" t="str">
+        <v>2.7610008628127698E-2</v>
+      </c>
+      <c r="O136">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P136" t="str">
+        <v>3.0290939318370739E-2</v>
+      </c>
+      <c r="P136">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q136" t="str">
+        <v>-9.0304778627869065E-3</v>
+      </c>
+      <c r="Q136">
         <f t="shared" si="34"/>
-        <v/>
+        <v>13261.120461649436</v>
       </c>
       <c r="R136">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>278.67275787448909</v>
       </c>
       <c r="S136">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T136" t="str">
+        <v>7231.3056023082472</v>
+      </c>
+      <c r="T136">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5751.1421014666994</v>
       </c>
     </row>
     <row r="137" spans="1:20">
-      <c r="A137" s="4" t="str">
+      <c r="A137" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B137" t="str">
+        <v>44034</v>
+      </c>
+      <c r="B137">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C137" t="str">
+        <v>55906</v>
+      </c>
+      <c r="C137">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>753</v>
       </c>
       <c r="D137">
         <f>+IFERROR('Fallecidos Diarios'!B136,"")</f>
-        <v>0</v>
+        <v>1180</v>
       </c>
       <c r="E137">
         <f>+IFERROR('Fallecidos Diarios'!C136,"")</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F137">
         <f>+IFERROR('Recuperados Diarios'!B136,"")</f>
-        <v>0</v>
+        <v>31122</v>
       </c>
       <c r="G137">
         <f>+IFERROR('Recuperados Diarios'!C136,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H137" t="str">
+        <v>1047</v>
+      </c>
+      <c r="H137">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I137" t="str">
+        <v>23604</v>
+      </c>
+      <c r="I137">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J137" t="str">
+        <v>-315</v>
+      </c>
+      <c r="J137">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K137" t="str">
+        <v>2.1106857940113761E-2</v>
+      </c>
+      <c r="K137">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L137" t="str">
+        <v>0.55668443458662753</v>
+      </c>
+      <c r="L137">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M137" t="str">
+        <v>0.42220870747325867</v>
+      </c>
+      <c r="M137">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N137" t="str">
+        <v>1783.4781392984241</v>
+      </c>
+      <c r="N137">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O137" t="str">
+        <v>1.7796610169491526E-2</v>
+      </c>
+      <c r="O137">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P137" t="str">
+        <v>3.3641796799691537E-2</v>
+      </c>
+      <c r="P137">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q137" t="str">
+        <v>-1.3345195729537367E-2</v>
+      </c>
+      <c r="Q137">
         <f t="shared" si="34"/>
-        <v/>
+        <v>13442.173599422938</v>
       </c>
       <c r="R137">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>283.72204856936764</v>
       </c>
       <c r="S137">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T137" t="str">
+        <v>7483.0488098100504</v>
+      </c>
+      <c r="T137">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5675.4027410435201</v>
       </c>
     </row>
     <row r="138" spans="1:20">
-      <c r="A138" s="4" t="str">
+      <c r="A138" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B138" t="str">
+        <v>44035</v>
+      </c>
+      <c r="B138">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C138" t="str">
+        <v>56817</v>
+      </c>
+      <c r="C138">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>911</v>
       </c>
       <c r="D138">
         <f>+IFERROR('Fallecidos Diarios'!B137,"")</f>
-        <v>0</v>
+        <v>1209</v>
       </c>
       <c r="E138">
         <f>+IFERROR('Fallecidos Diarios'!C137,"")</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="F138">
         <f>+IFERROR('Recuperados Diarios'!B137,"")</f>
-        <v>0</v>
+        <v>31828</v>
       </c>
       <c r="G138">
         <f>+IFERROR('Recuperados Diarios'!C137,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H138" t="str">
+        <v>706</v>
+      </c>
+      <c r="H138">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I138" t="str">
+        <v>23780</v>
+      </c>
+      <c r="I138">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J138" t="str">
+        <v>176</v>
+      </c>
+      <c r="J138">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K138" t="str">
+        <v>2.1278842599926077E-2</v>
+      </c>
+      <c r="K138">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L138" t="str">
+        <v>0.56018445183659815</v>
+      </c>
+      <c r="L138">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M138" t="str">
+        <v>0.41853670556347572</v>
+      </c>
+      <c r="M138">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N138" t="str">
+        <v>2176.6310765349031</v>
+      </c>
+      <c r="N138">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O138" t="str">
+        <v>2.3986765922249794E-2</v>
+      </c>
+      <c r="O138">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P138" t="str">
+        <v>2.2181726781450296E-2</v>
+      </c>
+      <c r="P138">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q138" t="str">
+        <v>7.4011774600504622E-3</v>
+      </c>
+      <c r="Q138">
         <f t="shared" si="34"/>
-        <v/>
+        <v>13661.216638615053</v>
       </c>
       <c r="R138">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>290.69487857658095</v>
       </c>
       <c r="S138">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T138" t="str">
+        <v>7652.8011541235874</v>
+      </c>
+      <c r="T138">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5717.7206059148839</v>
       </c>
     </row>
     <row r="139" spans="1:20">
-      <c r="A139" s="4" t="str">
+      <c r="A139" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B139" t="str">
+        <v>44036</v>
+      </c>
+      <c r="B139">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C139" t="str">
+        <v>57993</v>
+      </c>
+      <c r="C139">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1176</v>
       </c>
       <c r="D139">
         <f>+IFERROR('Fallecidos Diarios'!B138,"")</f>
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="E139">
         <f>+IFERROR('Fallecidos Diarios'!C138,"")</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="F139">
         <f>+IFERROR('Recuperados Diarios'!B138,"")</f>
-        <v>0</v>
+        <v>32704</v>
       </c>
       <c r="G139">
         <f>+IFERROR('Recuperados Diarios'!C138,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H139" t="str">
+        <v>876</v>
+      </c>
+      <c r="H139">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I139" t="str">
+        <v>24039</v>
+      </c>
+      <c r="I139">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J139" t="str">
+        <v>259</v>
+      </c>
+      <c r="J139">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K139" t="str">
+        <v>2.1554325522045763E-2</v>
+      </c>
+      <c r="K139">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L139" t="str">
+        <v>0.56393012949838772</v>
+      </c>
+      <c r="L139">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M139" t="str">
+        <v>0.4145155449795665</v>
+      </c>
+      <c r="M139">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N139" t="str">
+        <v>2837.0467989517033</v>
+      </c>
+      <c r="N139">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O139" t="str">
+        <v>3.2800000000000003E-2</v>
+      </c>
+      <c r="O139">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P139" t="str">
+        <v>2.6785714285714284E-2</v>
+      </c>
+      <c r="P139">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q139" t="str">
+        <v>1.0774158658846043E-2</v>
+      </c>
+      <c r="Q139">
         <f t="shared" si="34"/>
-        <v/>
+        <v>13943.976917528253</v>
       </c>
       <c r="R139">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>300.55301755229624</v>
       </c>
       <c r="S139">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T139" t="str">
+        <v>7863.4287088242372</v>
+      </c>
+      <c r="T139">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5779.9951911517192</v>
       </c>
     </row>
     <row r="140" spans="1:20">
-      <c r="A140" s="4" t="str">
+      <c r="A140" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B140" t="str">
+        <v>44037</v>
+      </c>
+      <c r="B140">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C140" t="str">
+        <v>58864</v>
+      </c>
+      <c r="C140">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>871</v>
       </c>
       <c r="D140">
         <f>+IFERROR('Fallecidos Diarios'!B139,"")</f>
-        <v>0</v>
+        <v>1275</v>
       </c>
       <c r="E140">
         <f>+IFERROR('Fallecidos Diarios'!C139,"")</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F140">
         <f>+IFERROR('Recuperados Diarios'!B139,"")</f>
-        <v>0</v>
+        <v>33428</v>
       </c>
       <c r="G140">
         <f>+IFERROR('Recuperados Diarios'!C139,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H140" t="str">
+        <v>724</v>
+      </c>
+      <c r="H140">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I140" t="str">
+        <v>24161</v>
+      </c>
+      <c r="I140">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J140" t="str">
+        <v>122</v>
+      </c>
+      <c r="J140">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K140" t="str">
+        <v>2.1660097852677359E-2</v>
+      </c>
+      <c r="K140">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L140" t="str">
+        <v>0.56788529491709705</v>
+      </c>
+      <c r="L140">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M140" t="str">
+        <v>0.41045460723022559</v>
+      </c>
+      <c r="M140">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N140" t="str">
+        <v>2122.0373328918504</v>
+      </c>
+      <c r="N140">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O140" t="str">
+        <v>1.9607843137254902E-2</v>
+      </c>
+      <c r="O140">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P140" t="str">
+        <v>2.1658489888716045E-2</v>
+      </c>
+      <c r="P140">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q140" t="str">
+        <v>5.0494598733496132E-3</v>
+      </c>
+      <c r="Q140">
         <f t="shared" si="34"/>
-        <v/>
+        <v>14153.402260158693</v>
       </c>
       <c r="R140">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>306.56407790334214</v>
       </c>
       <c r="S140">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T140" t="str">
+        <v>8037.5090165905267</v>
+      </c>
+      <c r="T140">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5809.3291656648234</v>
       </c>
     </row>
     <row r="141" spans="1:20">
-      <c r="A141" s="4" t="str">
+      <c r="A141" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B141" t="str">
+        <v>44038</v>
+      </c>
+      <c r="B141">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C141" t="str">
+        <v>60296</v>
+      </c>
+      <c r="C141">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1432</v>
       </c>
       <c r="D141">
         <f>+IFERROR('Fallecidos Diarios'!B140,"")</f>
-        <v>0</v>
+        <v>1294</v>
       </c>
       <c r="E141">
         <f>+IFERROR('Fallecidos Diarios'!C140,"")</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F141">
         <f>+IFERROR('Recuperados Diarios'!B140,"")</f>
-        <v>0</v>
+        <v>34131</v>
       </c>
       <c r="G141">
         <f>+IFERROR('Recuperados Diarios'!C140,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H141" t="str">
+        <v>703</v>
+      </c>
+      <c r="H141">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I141" t="str">
+        <v>24871</v>
+      </c>
+      <c r="I141">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J141" t="str">
+        <v>710</v>
+      </c>
+      <c r="J141">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K141" t="str">
+        <v>2.146079341913228E-2</v>
+      </c>
+      <c r="K141">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L141" t="str">
+        <v>0.56605744991375884</v>
+      </c>
+      <c r="L141">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M141" t="str">
+        <v>0.41248175666710896</v>
+      </c>
+      <c r="M141">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N141" t="str">
+        <v>3471.6686904426842</v>
+      </c>
+      <c r="N141">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O141" t="str">
+        <v>1.4683153013910355E-2</v>
+      </c>
+      <c r="O141">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P141" t="str">
+        <v>2.0597111130643695E-2</v>
+      </c>
+      <c r="P141">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q141" t="str">
+        <v>2.8547304089099754E-2</v>
+      </c>
+      <c r="Q141">
         <f t="shared" si="34"/>
-        <v/>
+        <v>14497.715797066603</v>
       </c>
       <c r="R141">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>311.13248377013707</v>
       </c>
       <c r="S141">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T141" t="str">
+        <v>8206.5400336619387</v>
+      </c>
+      <c r="T141">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5980.0432796345276</v>
       </c>
     </row>
     <row r="142" spans="1:20">
-      <c r="A142" s="4" t="str">
+      <c r="A142" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B142" t="str">
+        <v>44039</v>
+      </c>
+      <c r="B142">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C142" t="str">
+        <v>61442</v>
+      </c>
+      <c r="C142">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1146</v>
       </c>
       <c r="D142">
         <f>+IFERROR('Fallecidos Diarios'!B141,"")</f>
-        <v>0</v>
+        <v>1322</v>
       </c>
       <c r="E142">
         <f>+IFERROR('Fallecidos Diarios'!C141,"")</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F142">
         <f>+IFERROR('Recuperados Diarios'!B141,"")</f>
-        <v>0</v>
+        <v>35086</v>
       </c>
       <c r="G142">
         <f>+IFERROR('Recuperados Diarios'!C141,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H142" t="str">
+        <v>955</v>
+      </c>
+      <c r="H142">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I142" t="str">
+        <v>25034</v>
+      </c>
+      <c r="I142">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J142" t="str">
+        <v>163</v>
+      </c>
+      <c r="J142">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K142" t="str">
+        <v>2.1516226685329255E-2</v>
+      </c>
+      <c r="K142">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L142" t="str">
+        <v>0.57104260929006212</v>
+      </c>
+      <c r="L142">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M142" t="str">
+        <v>0.40744116402460856</v>
+      </c>
+      <c r="M142">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N142" t="str">
+        <v>2812.6760405848049</v>
+      </c>
+      <c r="N142">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O142" t="str">
+        <v>2.118003025718608E-2</v>
+      </c>
+      <c r="O142">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P142" t="str">
+        <v>2.7218833722852418E-2</v>
+      </c>
+      <c r="P142">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q142" t="str">
+        <v>6.5111448430135018E-3</v>
+      </c>
+      <c r="Q142">
         <f t="shared" si="34"/>
-        <v/>
+        <v>14773.262803558548</v>
       </c>
       <c r="R142">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>317.86487136330851</v>
       </c>
       <c r="S142">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T142" t="str">
+        <v>8436.1625390718928</v>
+      </c>
+      <c r="T142">
         <f t="shared" si="37"/>
-        <v/>
+        <v>6019.2353931233474</v>
       </c>
     </row>
     <row r="143" spans="1:20">
-      <c r="A143" s="4" t="str">
+      <c r="A143" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B143" t="str">
+        <v>44040</v>
+      </c>
+      <c r="B143">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C143" t="str">
+        <v>62223</v>
+      </c>
+      <c r="C143">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>781</v>
       </c>
       <c r="D143">
         <f>+IFERROR('Fallecidos Diarios'!B142,"")</f>
-        <v>0</v>
+        <v>1349</v>
       </c>
       <c r="E143">
         <f>+IFERROR('Fallecidos Diarios'!C142,"")</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F143">
         <f>+IFERROR('Recuperados Diarios'!B142,"")</f>
-        <v>0</v>
+        <v>36181</v>
       </c>
       <c r="G143">
         <f>+IFERROR('Recuperados Diarios'!C142,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H143" t="str">
+        <v>1095</v>
+      </c>
+      <c r="H143">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I143" t="str">
+        <v>24693</v>
+      </c>
+      <c r="I143">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J143" t="str">
+        <v>-341</v>
+      </c>
+      <c r="J143">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K143" t="str">
+        <v>2.168008614178037E-2</v>
+      </c>
+      <c r="K143">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L143" t="str">
+        <v>0.58147308872924808</v>
+      </c>
+      <c r="L143">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M143" t="str">
+        <v>0.39684682512897163</v>
+      </c>
+      <c r="M143">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N143" t="str">
+        <v>1968.0137285870489</v>
+      </c>
+      <c r="N143">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O143" t="str">
+        <v>2.0014825796886581E-2</v>
+      </c>
+      <c r="O143">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P143" t="str">
+        <v>3.0264503468671402E-2</v>
+      </c>
+      <c r="P143">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q143" t="str">
+        <v>-1.3809581662819422E-2</v>
+      </c>
+      <c r="Q143">
         <f t="shared" si="34"/>
-        <v/>
+        <v>14961.048328925222</v>
       </c>
       <c r="R143">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>324.35681654243808</v>
       </c>
       <c r="S143">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T143" t="str">
+        <v>8699.4469824477037</v>
+      </c>
+      <c r="T143">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5937.2445299350811</v>
       </c>
     </row>
     <row r="144" spans="1:20">
-      <c r="A144" s="4" t="str">
+      <c r="A144" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B144" t="str">
+        <v>44041</v>
+      </c>
+      <c r="B144">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C144" t="str">
+        <v>63269</v>
+      </c>
+      <c r="C144">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1046</v>
       </c>
       <c r="D144">
         <f>+IFERROR('Fallecidos Diarios'!B143,"")</f>
-        <v>0</v>
+        <v>1374</v>
       </c>
       <c r="E144">
         <f>+IFERROR('Fallecidos Diarios'!C143,"")</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="F144">
         <f>+IFERROR('Recuperados Diarios'!B143,"")</f>
-        <v>0</v>
+        <v>37316</v>
       </c>
       <c r="G144">
         <f>+IFERROR('Recuperados Diarios'!C143,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H144" t="str">
+        <v>1135</v>
+      </c>
+      <c r="H144">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I144" t="str">
+        <v>24579</v>
+      </c>
+      <c r="I144">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J144" t="str">
+        <v>-114</v>
+      </c>
+      <c r="J144">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K144" t="str">
+        <v>2.1716796535428094E-2</v>
+      </c>
+      <c r="K144">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L144" t="str">
+        <v>0.5897991117292829</v>
+      </c>
+      <c r="L144">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M144" t="str">
+        <v>0.38848409173528903</v>
+      </c>
+      <c r="M144">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N144" t="str">
+        <v>2692.5169453598601</v>
+      </c>
+      <c r="N144">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O144" t="str">
+        <v>1.8195050946142648E-2</v>
+      </c>
+      <c r="O144">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P144" t="str">
+        <v>3.0415907385571872E-2</v>
+      </c>
+      <c r="P144">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q144" t="str">
+        <v>-4.6381056999877943E-3</v>
+      </c>
+      <c r="Q144">
         <f t="shared" si="34"/>
-        <v/>
+        <v>15212.551094012984</v>
       </c>
       <c r="R144">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>330.36787689348404</v>
       </c>
       <c r="S144">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T144" t="str">
+        <v>8972.3491223851888</v>
+      </c>
+      <c r="T144">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5909.8340947343113</v>
       </c>
     </row>
     <row r="145" spans="1:20">
-      <c r="A145" s="4" t="str">
+      <c r="A145" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B145" t="str">
+        <v>44042</v>
+      </c>
+      <c r="B145">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C145" t="str">
+        <v>64191</v>
+      </c>
+      <c r="C145">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>922</v>
       </c>
       <c r="D145">
         <f>+IFERROR('Fallecidos Diarios'!B144,"")</f>
-        <v>0</v>
+        <v>1397</v>
       </c>
       <c r="E145">
         <f>+IFERROR('Fallecidos Diarios'!C144,"")</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F145">
         <f>+IFERROR('Recuperados Diarios'!B144,"")</f>
-        <v>0</v>
+        <v>38218</v>
       </c>
       <c r="G145">
         <f>+IFERROR('Recuperados Diarios'!C144,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H145" t="str">
+        <v>902</v>
+      </c>
+      <c r="H145">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I145" t="str">
+        <v>24576</v>
+      </c>
+      <c r="I145">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J145" t="str">
+        <v>-3</v>
+      </c>
+      <c r="J145">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K145" t="str">
+        <v>2.1763175523048402E-2</v>
+      </c>
+      <c r="K145">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L145" t="str">
+        <v>0.59537941455967347</v>
+      </c>
+      <c r="L145">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M145" t="str">
+        <v>0.38285740991727812</v>
+      </c>
+      <c r="M145">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N145" t="str">
+        <v>2408.207275390625</v>
+      </c>
+      <c r="N145">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O145" t="str">
+        <v>1.6463851109520401E-2</v>
+      </c>
+      <c r="O145">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P145" t="str">
+        <v>2.3601444345596315E-2</v>
+      </c>
+      <c r="P145">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q145" t="str">
+        <v>-1.220703125E-4</v>
+      </c>
+      <c r="Q145">
         <f t="shared" si="34"/>
-        <v/>
+        <v>15434.238999759558</v>
       </c>
       <c r="R145">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>335.89805241644626</v>
       </c>
       <c r="S145">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T145" t="str">
+        <v>9189.2281798509266</v>
+      </c>
+      <c r="T145">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5909.1127674921863</v>
       </c>
     </row>
     <row r="146" spans="1:20">
-      <c r="A146" s="4" t="str">
+      <c r="A146" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B146" t="str">
+        <v>44043</v>
+      </c>
+      <c r="B146">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C146" t="str">
+        <v>65256</v>
+      </c>
+      <c r="C146">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1065</v>
       </c>
       <c r="D146">
         <f>+IFERROR('Fallecidos Diarios'!B145,"")</f>
-        <v>0</v>
+        <v>1421</v>
       </c>
       <c r="E146">
         <f>+IFERROR('Fallecidos Diarios'!C145,"")</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F146">
         <f>+IFERROR('Recuperados Diarios'!B145,"")</f>
-        <v>0</v>
+        <v>39166</v>
       </c>
       <c r="G146">
         <f>+IFERROR('Recuperados Diarios'!C145,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H146" t="str">
+        <v>948</v>
+      </c>
+      <c r="H146">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I146" t="str">
+        <v>24669</v>
+      </c>
+      <c r="I146">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J146" t="str">
+        <v>93</v>
+      </c>
+      <c r="J146">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K146" t="str">
+        <v>2.1775775407625351E-2</v>
+      </c>
+      <c r="K146">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L146" t="str">
+        <v>0.60019002084099549</v>
+      </c>
+      <c r="L146">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M146" t="str">
+        <v>0.37803420375137919</v>
+      </c>
+      <c r="M146">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N146" t="str">
+        <v>2817.2053994892376</v>
+      </c>
+      <c r="N146">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O146" t="str">
+        <v>1.688951442646024E-2</v>
+      </c>
+      <c r="O146">
         <f t="shared" si="32"/>
-        <v/>
-      </c>
-      <c r="P146" t="str">
+        <v>2.4204667313486188E-2</v>
+      </c>
+      <c r="P146">
         <f t="shared" si="33"/>
-        <v/>
-      </c>
-      <c r="Q146" t="str">
+        <v>3.769913656816247E-3</v>
+      </c>
+      <c r="Q146">
         <f t="shared" si="34"/>
-        <v/>
+        <v>15690.310170714114</v>
       </c>
       <c r="R146">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>341.66867035345035</v>
       </c>
       <c r="S146">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T146" t="str">
+        <v>9417.1675883625885</v>
+      </c>
+      <c r="T146">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5931.4739119980768</v>
       </c>
     </row>
     <row r="147" spans="1:20">
@@ -23332,13 +23815,13 @@
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
         <v/>
       </c>
-      <c r="D147">
-        <f>+IFERROR('Fallecidos Diarios'!B146,"")</f>
-        <v>0</v>
-      </c>
-      <c r="E147">
-        <f>+IFERROR('Fallecidos Diarios'!C146,"")</f>
-        <v>0</v>
+      <c r="D147" t="str">
+        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
+        <v/>
+      </c>
+      <c r="E147" t="str">
+        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
+        <v/>
       </c>
       <c r="F147">
         <f>+IFERROR('Recuperados Diarios'!B146,"")</f>
@@ -23388,9 +23871,9 @@
         <f t="shared" si="34"/>
         <v/>
       </c>
-      <c r="R147">
+      <c r="R147" t="str">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="S147">
         <f t="shared" si="36"/>
@@ -23415,11 +23898,11 @@
         <v/>
       </c>
       <c r="D148">
-        <f>+IFERROR('Fallecidos Diarios'!B147,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B146,"")</f>
         <v>0</v>
       </c>
       <c r="E148">
-        <f>+IFERROR('Fallecidos Diarios'!C147,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C146,"")</f>
         <v>0</v>
       </c>
       <c r="F148">
@@ -23497,11 +23980,11 @@
         <v/>
       </c>
       <c r="D149">
-        <f>+IFERROR('Fallecidos Diarios'!B148,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B147,"")</f>
         <v>0</v>
       </c>
       <c r="E149">
-        <f>+IFERROR('Fallecidos Diarios'!C148,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C147,"")</f>
         <v>0</v>
       </c>
       <c r="F149">
@@ -23579,11 +24062,11 @@
         <v/>
       </c>
       <c r="D150">
-        <f>+IFERROR('Fallecidos Diarios'!B149,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B148,"")</f>
         <v>0</v>
       </c>
       <c r="E150">
-        <f>+IFERROR('Fallecidos Diarios'!C149,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C148,"")</f>
         <v>0</v>
       </c>
       <c r="F150">
@@ -23661,11 +24144,11 @@
         <v/>
       </c>
       <c r="D151">
-        <f>+IFERROR('Fallecidos Diarios'!B150,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B149,"")</f>
         <v>0</v>
       </c>
       <c r="E151">
-        <f>+IFERROR('Fallecidos Diarios'!C150,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C149,"")</f>
         <v>0</v>
       </c>
       <c r="F151">
@@ -23743,11 +24226,11 @@
         <v/>
       </c>
       <c r="D152">
-        <f>+IFERROR('Fallecidos Diarios'!B151,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B150,"")</f>
         <v>0</v>
       </c>
       <c r="E152">
-        <f>+IFERROR('Fallecidos Diarios'!C151,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C150,"")</f>
         <v>0</v>
       </c>
       <c r="F152">
@@ -23825,11 +24308,11 @@
         <v/>
       </c>
       <c r="D153">
-        <f>+IFERROR('Fallecidos Diarios'!B152,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B151,"")</f>
         <v>0</v>
       </c>
       <c r="E153">
-        <f>+IFERROR('Fallecidos Diarios'!C152,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C151,"")</f>
         <v>0</v>
       </c>
       <c r="F153">
@@ -23907,11 +24390,11 @@
         <v/>
       </c>
       <c r="D154">
-        <f>+IFERROR('Fallecidos Diarios'!B153,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B152,"")</f>
         <v>0</v>
       </c>
       <c r="E154">
-        <f>+IFERROR('Fallecidos Diarios'!C153,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C152,"")</f>
         <v>0</v>
       </c>
       <c r="F154">
@@ -23989,11 +24472,11 @@
         <v/>
       </c>
       <c r="D155">
-        <f>+IFERROR('Fallecidos Diarios'!B154,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B153,"")</f>
         <v>0</v>
       </c>
       <c r="E155">
-        <f>+IFERROR('Fallecidos Diarios'!C154,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C153,"")</f>
         <v>0</v>
       </c>
       <c r="F155">
@@ -24071,11 +24554,11 @@
         <v/>
       </c>
       <c r="D156">
-        <f>+IFERROR('Fallecidos Diarios'!B155,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B154,"")</f>
         <v>0</v>
       </c>
       <c r="E156">
-        <f>+IFERROR('Fallecidos Diarios'!C155,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C154,"")</f>
         <v>0</v>
       </c>
       <c r="F156">
@@ -24153,11 +24636,11 @@
         <v/>
       </c>
       <c r="D157">
-        <f>+IFERROR('Fallecidos Diarios'!B156,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B155,"")</f>
         <v>0</v>
       </c>
       <c r="E157">
-        <f>+IFERROR('Fallecidos Diarios'!C156,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C155,"")</f>
         <v>0</v>
       </c>
       <c r="F157">
@@ -24235,11 +24718,11 @@
         <v/>
       </c>
       <c r="D158">
-        <f>+IFERROR('Fallecidos Diarios'!B157,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B156,"")</f>
         <v>0</v>
       </c>
       <c r="E158">
-        <f>+IFERROR('Fallecidos Diarios'!C157,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C156,"")</f>
         <v>0</v>
       </c>
       <c r="F158">
@@ -24317,11 +24800,11 @@
         <v/>
       </c>
       <c r="D159">
-        <f>+IFERROR('Fallecidos Diarios'!B158,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B157,"")</f>
         <v>0</v>
       </c>
       <c r="E159">
-        <f>+IFERROR('Fallecidos Diarios'!C158,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C157,"")</f>
         <v>0</v>
       </c>
       <c r="F159">
@@ -24399,11 +24882,11 @@
         <v/>
       </c>
       <c r="D160">
-        <f>+IFERROR('Fallecidos Diarios'!B159,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B158,"")</f>
         <v>0</v>
       </c>
       <c r="E160">
-        <f>+IFERROR('Fallecidos Diarios'!C159,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C158,"")</f>
         <v>0</v>
       </c>
       <c r="F160">
@@ -24481,11 +24964,11 @@
         <v/>
       </c>
       <c r="D161">
-        <f>+IFERROR('Fallecidos Diarios'!B160,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B159,"")</f>
         <v>0</v>
       </c>
       <c r="E161">
-        <f>+IFERROR('Fallecidos Diarios'!C160,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C159,"")</f>
         <v>0</v>
       </c>
       <c r="F161">
@@ -24563,11 +25046,11 @@
         <v/>
       </c>
       <c r="D162">
-        <f>+IFERROR('Fallecidos Diarios'!B161,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B160,"")</f>
         <v>0</v>
       </c>
       <c r="E162">
-        <f>+IFERROR('Fallecidos Diarios'!C161,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C160,"")</f>
         <v>0</v>
       </c>
       <c r="F162">
@@ -24645,11 +25128,11 @@
         <v/>
       </c>
       <c r="D163">
-        <f>+IFERROR('Fallecidos Diarios'!B162,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B161,"")</f>
         <v>0</v>
       </c>
       <c r="E163">
-        <f>+IFERROR('Fallecidos Diarios'!C162,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C161,"")</f>
         <v>0</v>
       </c>
       <c r="F163">
@@ -24727,11 +25210,11 @@
         <v/>
       </c>
       <c r="D164">
-        <f>+IFERROR('Fallecidos Diarios'!B163,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B162,"")</f>
         <v>0</v>
       </c>
       <c r="E164">
-        <f>+IFERROR('Fallecidos Diarios'!C163,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C162,"")</f>
         <v>0</v>
       </c>
       <c r="F164">
@@ -24809,11 +25292,11 @@
         <v/>
       </c>
       <c r="D165">
-        <f>+IFERROR('Fallecidos Diarios'!B164,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B163,"")</f>
         <v>0</v>
       </c>
       <c r="E165">
-        <f>+IFERROR('Fallecidos Diarios'!C164,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C163,"")</f>
         <v>0</v>
       </c>
       <c r="F165">
@@ -24891,11 +25374,11 @@
         <v/>
       </c>
       <c r="D166">
-        <f>+IFERROR('Fallecidos Diarios'!B165,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B164,"")</f>
         <v>0</v>
       </c>
       <c r="E166">
-        <f>+IFERROR('Fallecidos Diarios'!C165,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C164,"")</f>
         <v>0</v>
       </c>
       <c r="F166">
@@ -24973,11 +25456,11 @@
         <v/>
       </c>
       <c r="D167">
-        <f>+IFERROR('Fallecidos Diarios'!B166,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B165,"")</f>
         <v>0</v>
       </c>
       <c r="E167">
-        <f>+IFERROR('Fallecidos Diarios'!C166,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C165,"")</f>
         <v>0</v>
       </c>
       <c r="F167">
@@ -25055,11 +25538,11 @@
         <v/>
       </c>
       <c r="D168">
-        <f>+IFERROR('Fallecidos Diarios'!B167,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B166,"")</f>
         <v>0</v>
       </c>
       <c r="E168">
-        <f>+IFERROR('Fallecidos Diarios'!C167,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C166,"")</f>
         <v>0</v>
       </c>
       <c r="F168">
@@ -25137,11 +25620,11 @@
         <v/>
       </c>
       <c r="D169">
-        <f>+IFERROR('Fallecidos Diarios'!B168,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B167,"")</f>
         <v>0</v>
       </c>
       <c r="E169">
-        <f>+IFERROR('Fallecidos Diarios'!C168,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C167,"")</f>
         <v>0</v>
       </c>
       <c r="F169">
@@ -25219,11 +25702,11 @@
         <v/>
       </c>
       <c r="D170">
-        <f>+IFERROR('Fallecidos Diarios'!B169,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B168,"")</f>
         <v>0</v>
       </c>
       <c r="E170">
-        <f>+IFERROR('Fallecidos Diarios'!C169,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C168,"")</f>
         <v>0</v>
       </c>
       <c r="F170">
@@ -25301,11 +25784,11 @@
         <v/>
       </c>
       <c r="D171">
-        <f>+IFERROR('Fallecidos Diarios'!B170,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B169,"")</f>
         <v>0</v>
       </c>
       <c r="E171">
-        <f>+IFERROR('Fallecidos Diarios'!C170,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C169,"")</f>
         <v>0</v>
       </c>
       <c r="F171">
@@ -25383,11 +25866,11 @@
         <v/>
       </c>
       <c r="D172">
-        <f>+IFERROR('Fallecidos Diarios'!B171,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B170,"")</f>
         <v>0</v>
       </c>
       <c r="E172">
-        <f>+IFERROR('Fallecidos Diarios'!C171,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C170,"")</f>
         <v>0</v>
       </c>
       <c r="F172">
@@ -25465,11 +25948,11 @@
         <v/>
       </c>
       <c r="D173">
-        <f>+IFERROR('Fallecidos Diarios'!B172,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B171,"")</f>
         <v>0</v>
       </c>
       <c r="E173">
-        <f>+IFERROR('Fallecidos Diarios'!C172,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C171,"")</f>
         <v>0</v>
       </c>
       <c r="F173">
@@ -25547,11 +26030,11 @@
         <v/>
       </c>
       <c r="D174">
-        <f>+IFERROR('Fallecidos Diarios'!B173,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B172,"")</f>
         <v>0</v>
       </c>
       <c r="E174">
-        <f>+IFERROR('Fallecidos Diarios'!C173,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C172,"")</f>
         <v>0</v>
       </c>
       <c r="F174">
@@ -25629,11 +26112,11 @@
         <v/>
       </c>
       <c r="D175">
-        <f>+IFERROR('Fallecidos Diarios'!B174,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B173,"")</f>
         <v>0</v>
       </c>
       <c r="E175">
-        <f>+IFERROR('Fallecidos Diarios'!C174,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C173,"")</f>
         <v>0</v>
       </c>
       <c r="F175">
@@ -25711,11 +26194,11 @@
         <v/>
       </c>
       <c r="D176">
-        <f>+IFERROR('Fallecidos Diarios'!B175,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B174,"")</f>
         <v>0</v>
       </c>
       <c r="E176">
-        <f>+IFERROR('Fallecidos Diarios'!C175,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C174,"")</f>
         <v>0</v>
       </c>
       <c r="F176">
@@ -25793,11 +26276,11 @@
         <v/>
       </c>
       <c r="D177">
-        <f>+IFERROR('Fallecidos Diarios'!B176,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B175,"")</f>
         <v>0</v>
       </c>
       <c r="E177">
-        <f>+IFERROR('Fallecidos Diarios'!C176,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C175,"")</f>
         <v>0</v>
       </c>
       <c r="F177">
@@ -25875,11 +26358,11 @@
         <v/>
       </c>
       <c r="D178">
-        <f>+IFERROR('Fallecidos Diarios'!B177,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B176,"")</f>
         <v>0</v>
       </c>
       <c r="E178">
-        <f>+IFERROR('Fallecidos Diarios'!C177,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C176,"")</f>
         <v>0</v>
       </c>
       <c r="F178">
@@ -25957,11 +26440,11 @@
         <v/>
       </c>
       <c r="D179">
-        <f>+IFERROR('Fallecidos Diarios'!B178,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B177,"")</f>
         <v>0</v>
       </c>
       <c r="E179">
-        <f>+IFERROR('Fallecidos Diarios'!C178,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C177,"")</f>
         <v>0</v>
       </c>
       <c r="F179">
@@ -26039,11 +26522,11 @@
         <v/>
       </c>
       <c r="D180">
-        <f>+IFERROR('Fallecidos Diarios'!B179,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B178,"")</f>
         <v>0</v>
       </c>
       <c r="E180">
-        <f>+IFERROR('Fallecidos Diarios'!C179,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C178,"")</f>
         <v>0</v>
       </c>
       <c r="F180">
@@ -26121,11 +26604,11 @@
         <v/>
       </c>
       <c r="D181">
-        <f>+IFERROR('Fallecidos Diarios'!B180,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B179,"")</f>
         <v>0</v>
       </c>
       <c r="E181">
-        <f>+IFERROR('Fallecidos Diarios'!C180,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C179,"")</f>
         <v>0</v>
       </c>
       <c r="F181">
@@ -26203,11 +26686,11 @@
         <v/>
       </c>
       <c r="D182">
-        <f>+IFERROR('Fallecidos Diarios'!B181,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B180,"")</f>
         <v>0</v>
       </c>
       <c r="E182">
-        <f>+IFERROR('Fallecidos Diarios'!C181,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C180,"")</f>
         <v>0</v>
       </c>
       <c r="F182">
@@ -26285,11 +26768,11 @@
         <v/>
       </c>
       <c r="D183">
-        <f>+IFERROR('Fallecidos Diarios'!B182,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B181,"")</f>
         <v>0</v>
       </c>
       <c r="E183">
-        <f>+IFERROR('Fallecidos Diarios'!C182,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C181,"")</f>
         <v>0</v>
       </c>
       <c r="F183">
@@ -26367,11 +26850,11 @@
         <v/>
       </c>
       <c r="D184">
-        <f>+IFERROR('Fallecidos Diarios'!B183,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B182,"")</f>
         <v>0</v>
       </c>
       <c r="E184">
-        <f>+IFERROR('Fallecidos Diarios'!C183,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C182,"")</f>
         <v>0</v>
       </c>
       <c r="F184">
@@ -26449,11 +26932,11 @@
         <v/>
       </c>
       <c r="D185">
-        <f>+IFERROR('Fallecidos Diarios'!B184,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B183,"")</f>
         <v>0</v>
       </c>
       <c r="E185">
-        <f>+IFERROR('Fallecidos Diarios'!C184,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C183,"")</f>
         <v>0</v>
       </c>
       <c r="F185">
@@ -26531,11 +27014,11 @@
         <v/>
       </c>
       <c r="D186">
-        <f>+IFERROR('Fallecidos Diarios'!B185,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B184,"")</f>
         <v>0</v>
       </c>
       <c r="E186">
-        <f>+IFERROR('Fallecidos Diarios'!C185,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C184,"")</f>
         <v>0</v>
       </c>
       <c r="F186">
@@ -26613,11 +27096,11 @@
         <v/>
       </c>
       <c r="D187">
-        <f>+IFERROR('Fallecidos Diarios'!B186,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B185,"")</f>
         <v>0</v>
       </c>
       <c r="E187">
-        <f>+IFERROR('Fallecidos Diarios'!C186,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C185,"")</f>
         <v>0</v>
       </c>
       <c r="F187">
@@ -26695,11 +27178,11 @@
         <v/>
       </c>
       <c r="D188">
-        <f>+IFERROR('Fallecidos Diarios'!B187,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B186,"")</f>
         <v>0</v>
       </c>
       <c r="E188">
-        <f>+IFERROR('Fallecidos Diarios'!C187,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C186,"")</f>
         <v>0</v>
       </c>
       <c r="F188">
@@ -26777,11 +27260,11 @@
         <v/>
       </c>
       <c r="D189">
-        <f>+IFERROR('Fallecidos Diarios'!B188,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B187,"")</f>
         <v>0</v>
       </c>
       <c r="E189">
-        <f>+IFERROR('Fallecidos Diarios'!C188,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C187,"")</f>
         <v>0</v>
       </c>
       <c r="F189">
@@ -26859,11 +27342,11 @@
         <v/>
       </c>
       <c r="D190">
-        <f>+IFERROR('Fallecidos Diarios'!B189,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B188,"")</f>
         <v>0</v>
       </c>
       <c r="E190">
-        <f>+IFERROR('Fallecidos Diarios'!C189,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C188,"")</f>
         <v>0</v>
       </c>
       <c r="F190">
@@ -26941,11 +27424,11 @@
         <v/>
       </c>
       <c r="D191">
-        <f>+IFERROR('Fallecidos Diarios'!B190,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B189,"")</f>
         <v>0</v>
       </c>
       <c r="E191">
-        <f>+IFERROR('Fallecidos Diarios'!C190,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C189,"")</f>
         <v>0</v>
       </c>
       <c r="F191">
@@ -27023,11 +27506,11 @@
         <v/>
       </c>
       <c r="D192">
-        <f>+IFERROR('Fallecidos Diarios'!B191,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B190,"")</f>
         <v>0</v>
       </c>
       <c r="E192">
-        <f>+IFERROR('Fallecidos Diarios'!C191,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C190,"")</f>
         <v>0</v>
       </c>
       <c r="F192">
@@ -27105,11 +27588,11 @@
         <v/>
       </c>
       <c r="D193">
-        <f>+IFERROR('Fallecidos Diarios'!B192,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B191,"")</f>
         <v>0</v>
       </c>
       <c r="E193">
-        <f>+IFERROR('Fallecidos Diarios'!C192,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C191,"")</f>
         <v>0</v>
       </c>
       <c r="F193">
@@ -27187,11 +27670,11 @@
         <v/>
       </c>
       <c r="D194">
-        <f>+IFERROR('Fallecidos Diarios'!B193,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B192,"")</f>
         <v>0</v>
       </c>
       <c r="E194">
-        <f>+IFERROR('Fallecidos Diarios'!C193,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C192,"")</f>
         <v>0</v>
       </c>
       <c r="F194">
@@ -27269,11 +27752,11 @@
         <v/>
       </c>
       <c r="D195">
-        <f>+IFERROR('Fallecidos Diarios'!B194,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B193,"")</f>
         <v>0</v>
       </c>
       <c r="E195">
-        <f>+IFERROR('Fallecidos Diarios'!C194,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C193,"")</f>
         <v>0</v>
       </c>
       <c r="F195">
@@ -27351,11 +27834,11 @@
         <v/>
       </c>
       <c r="D196">
-        <f>+IFERROR('Fallecidos Diarios'!B195,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B194,"")</f>
         <v>0</v>
       </c>
       <c r="E196">
-        <f>+IFERROR('Fallecidos Diarios'!C195,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C194,"")</f>
         <v>0</v>
       </c>
       <c r="F196">
@@ -27433,11 +27916,11 @@
         <v/>
       </c>
       <c r="D197">
-        <f>+IFERROR('Fallecidos Diarios'!B196,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B195,"")</f>
         <v>0</v>
       </c>
       <c r="E197">
-        <f>+IFERROR('Fallecidos Diarios'!C196,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C195,"")</f>
         <v>0</v>
       </c>
       <c r="F197">
@@ -27515,11 +27998,11 @@
         <v/>
       </c>
       <c r="D198">
-        <f>+IFERROR('Fallecidos Diarios'!B197,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B196,"")</f>
         <v>0</v>
       </c>
       <c r="E198">
-        <f>+IFERROR('Fallecidos Diarios'!C197,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C196,"")</f>
         <v>0</v>
       </c>
       <c r="F198">
@@ -27597,11 +28080,11 @@
         <v/>
       </c>
       <c r="D199">
-        <f>+IFERROR('Fallecidos Diarios'!B198,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B197,"")</f>
         <v>0</v>
       </c>
       <c r="E199">
-        <f>+IFERROR('Fallecidos Diarios'!C198,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C197,"")</f>
         <v>0</v>
       </c>
       <c r="F199">
@@ -27679,11 +28162,11 @@
         <v/>
       </c>
       <c r="D200">
-        <f>+IFERROR('Fallecidos Diarios'!B199,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B198,"")</f>
         <v>0</v>
       </c>
       <c r="E200">
-        <f>+IFERROR('Fallecidos Diarios'!C199,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C198,"")</f>
         <v>0</v>
       </c>
       <c r="F200">
@@ -27761,11 +28244,11 @@
         <v/>
       </c>
       <c r="D201">
-        <f>+IFERROR('Fallecidos Diarios'!B200,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B199,"")</f>
         <v>0</v>
       </c>
       <c r="E201">
-        <f>+IFERROR('Fallecidos Diarios'!C200,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C199,"")</f>
         <v>0</v>
       </c>
       <c r="F201">
@@ -27843,11 +28326,11 @@
         <v/>
       </c>
       <c r="D202">
-        <f>+IFERROR('Fallecidos Diarios'!B201,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B200,"")</f>
         <v>0</v>
       </c>
       <c r="E202">
-        <f>+IFERROR('Fallecidos Diarios'!C201,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C200,"")</f>
         <v>0</v>
       </c>
       <c r="F202">
@@ -27925,11 +28408,11 @@
         <v/>
       </c>
       <c r="D203">
-        <f>+IFERROR('Fallecidos Diarios'!B202,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B201,"")</f>
         <v>0</v>
       </c>
       <c r="E203">
-        <f>+IFERROR('Fallecidos Diarios'!C202,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C201,"")</f>
         <v>0</v>
       </c>
       <c r="F203">
@@ -28007,11 +28490,11 @@
         <v/>
       </c>
       <c r="D204">
-        <f>+IFERROR('Fallecidos Diarios'!B203,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B202,"")</f>
         <v>0</v>
       </c>
       <c r="E204">
-        <f>+IFERROR('Fallecidos Diarios'!C203,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C202,"")</f>
         <v>0</v>
       </c>
       <c r="F204">
@@ -28089,11 +28572,11 @@
         <v/>
       </c>
       <c r="D205">
-        <f>+IFERROR('Fallecidos Diarios'!B204,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B203,"")</f>
         <v>0</v>
       </c>
       <c r="E205">
-        <f>+IFERROR('Fallecidos Diarios'!C204,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C203,"")</f>
         <v>0</v>
       </c>
       <c r="F205">
@@ -28171,11 +28654,11 @@
         <v/>
       </c>
       <c r="D206">
-        <f>+IFERROR('Fallecidos Diarios'!B205,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B204,"")</f>
         <v>0</v>
       </c>
       <c r="E206">
-        <f>+IFERROR('Fallecidos Diarios'!C205,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C204,"")</f>
         <v>0</v>
       </c>
       <c r="F206">
@@ -28253,11 +28736,11 @@
         <v/>
       </c>
       <c r="D207">
-        <f>+IFERROR('Fallecidos Diarios'!B206,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B205,"")</f>
         <v>0</v>
       </c>
       <c r="E207">
-        <f>+IFERROR('Fallecidos Diarios'!C206,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C205,"")</f>
         <v>0</v>
       </c>
       <c r="F207">
@@ -28335,11 +28818,11 @@
         <v/>
       </c>
       <c r="D208">
-        <f>+IFERROR('Fallecidos Diarios'!B207,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B206,"")</f>
         <v>0</v>
       </c>
       <c r="E208">
-        <f>+IFERROR('Fallecidos Diarios'!C207,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C206,"")</f>
         <v>0</v>
       </c>
       <c r="F208">
@@ -28417,11 +28900,11 @@
         <v/>
       </c>
       <c r="D209">
-        <f>+IFERROR('Fallecidos Diarios'!B208,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B207,"")</f>
         <v>0</v>
       </c>
       <c r="E209">
-        <f>+IFERROR('Fallecidos Diarios'!C208,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C207,"")</f>
         <v>0</v>
       </c>
       <c r="F209">
@@ -28499,11 +28982,11 @@
         <v/>
       </c>
       <c r="D210">
-        <f>+IFERROR('Fallecidos Diarios'!B209,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B208,"")</f>
         <v>0</v>
       </c>
       <c r="E210">
-        <f>+IFERROR('Fallecidos Diarios'!C209,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C208,"")</f>
         <v>0</v>
       </c>
       <c r="F210">
@@ -28581,11 +29064,11 @@
         <v/>
       </c>
       <c r="D211">
-        <f>+IFERROR('Fallecidos Diarios'!B210,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B209,"")</f>
         <v>0</v>
       </c>
       <c r="E211">
-        <f>+IFERROR('Fallecidos Diarios'!C210,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C209,"")</f>
         <v>0</v>
       </c>
       <c r="F211">
@@ -28663,11 +29146,11 @@
         <v/>
       </c>
       <c r="D212">
-        <f>+IFERROR('Fallecidos Diarios'!B211,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B210,"")</f>
         <v>0</v>
       </c>
       <c r="E212">
-        <f>+IFERROR('Fallecidos Diarios'!C211,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C210,"")</f>
         <v>0</v>
       </c>
       <c r="F212">
@@ -28745,11 +29228,11 @@
         <v/>
       </c>
       <c r="D213">
-        <f>+IFERROR('Fallecidos Diarios'!B212,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B211,"")</f>
         <v>0</v>
       </c>
       <c r="E213">
-        <f>+IFERROR('Fallecidos Diarios'!C212,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C211,"")</f>
         <v>0</v>
       </c>
       <c r="F213">
@@ -28827,11 +29310,11 @@
         <v/>
       </c>
       <c r="D214">
-        <f>+IFERROR('Fallecidos Diarios'!B213,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B212,"")</f>
         <v>0</v>
       </c>
       <c r="E214">
-        <f>+IFERROR('Fallecidos Diarios'!C213,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C212,"")</f>
         <v>0</v>
       </c>
       <c r="F214">
@@ -28909,11 +29392,11 @@
         <v/>
       </c>
       <c r="D215">
-        <f>+IFERROR('Fallecidos Diarios'!B214,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B213,"")</f>
         <v>0</v>
       </c>
       <c r="E215">
-        <f>+IFERROR('Fallecidos Diarios'!C214,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C213,"")</f>
         <v>0</v>
       </c>
       <c r="F215">
@@ -28991,11 +29474,11 @@
         <v/>
       </c>
       <c r="D216">
-        <f>+IFERROR('Fallecidos Diarios'!B215,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B214,"")</f>
         <v>0</v>
       </c>
       <c r="E216">
-        <f>+IFERROR('Fallecidos Diarios'!C215,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C214,"")</f>
         <v>0</v>
       </c>
       <c r="F216">
@@ -29073,11 +29556,11 @@
         <v/>
       </c>
       <c r="D217">
-        <f>+IFERROR('Fallecidos Diarios'!B216,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B215,"")</f>
         <v>0</v>
       </c>
       <c r="E217">
-        <f>+IFERROR('Fallecidos Diarios'!C216,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C215,"")</f>
         <v>0</v>
       </c>
       <c r="F217">
@@ -29155,11 +29638,11 @@
         <v/>
       </c>
       <c r="D218">
-        <f>+IFERROR('Fallecidos Diarios'!B217,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B216,"")</f>
         <v>0</v>
       </c>
       <c r="E218">
-        <f>+IFERROR('Fallecidos Diarios'!C217,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C216,"")</f>
         <v>0</v>
       </c>
       <c r="F218">
@@ -29237,11 +29720,11 @@
         <v/>
       </c>
       <c r="D219">
-        <f>+IFERROR('Fallecidos Diarios'!B218,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B217,"")</f>
         <v>0</v>
       </c>
       <c r="E219">
-        <f>+IFERROR('Fallecidos Diarios'!C218,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C217,"")</f>
         <v>0</v>
       </c>
       <c r="F219">
@@ -29319,11 +29802,11 @@
         <v/>
       </c>
       <c r="D220">
-        <f>+IFERROR('Fallecidos Diarios'!B219,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B218,"")</f>
         <v>0</v>
       </c>
       <c r="E220">
-        <f>+IFERROR('Fallecidos Diarios'!C219,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C218,"")</f>
         <v>0</v>
       </c>
       <c r="F220">
@@ -29401,11 +29884,11 @@
         <v/>
       </c>
       <c r="D221">
-        <f>+IFERROR('Fallecidos Diarios'!B220,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B219,"")</f>
         <v>0</v>
       </c>
       <c r="E221">
-        <f>+IFERROR('Fallecidos Diarios'!C220,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C219,"")</f>
         <v>0</v>
       </c>
       <c r="F221">
@@ -29483,11 +29966,11 @@
         <v/>
       </c>
       <c r="D222">
-        <f>+IFERROR('Fallecidos Diarios'!B221,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B220,"")</f>
         <v>0</v>
       </c>
       <c r="E222">
-        <f>+IFERROR('Fallecidos Diarios'!C221,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C220,"")</f>
         <v>0</v>
       </c>
       <c r="F222">
@@ -29565,11 +30048,11 @@
         <v/>
       </c>
       <c r="D223">
-        <f>+IFERROR('Fallecidos Diarios'!B222,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B221,"")</f>
         <v>0</v>
       </c>
       <c r="E223">
-        <f>+IFERROR('Fallecidos Diarios'!C222,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C221,"")</f>
         <v>0</v>
       </c>
       <c r="F223">
@@ -29647,11 +30130,11 @@
         <v/>
       </c>
       <c r="D224">
-        <f>+IFERROR('Fallecidos Diarios'!B223,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B222,"")</f>
         <v>0</v>
       </c>
       <c r="E224">
-        <f>+IFERROR('Fallecidos Diarios'!C223,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C222,"")</f>
         <v>0</v>
       </c>
       <c r="F224">
@@ -29729,11 +30212,11 @@
         <v/>
       </c>
       <c r="D225">
-        <f>+IFERROR('Fallecidos Diarios'!B224,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B223,"")</f>
         <v>0</v>
       </c>
       <c r="E225">
-        <f>+IFERROR('Fallecidos Diarios'!C224,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C223,"")</f>
         <v>0</v>
       </c>
       <c r="F225">
@@ -29811,11 +30294,11 @@
         <v/>
       </c>
       <c r="D226">
-        <f>+IFERROR('Fallecidos Diarios'!B225,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B224,"")</f>
         <v>0</v>
       </c>
       <c r="E226">
-        <f>+IFERROR('Fallecidos Diarios'!C225,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C224,"")</f>
         <v>0</v>
       </c>
       <c r="F226">
@@ -29893,11 +30376,11 @@
         <v/>
       </c>
       <c r="D227">
-        <f>+IFERROR('Fallecidos Diarios'!B226,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B225,"")</f>
         <v>0</v>
       </c>
       <c r="E227">
-        <f>+IFERROR('Fallecidos Diarios'!C226,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C225,"")</f>
         <v>0</v>
       </c>
       <c r="F227">
@@ -29975,11 +30458,11 @@
         <v/>
       </c>
       <c r="D228">
-        <f>+IFERROR('Fallecidos Diarios'!B227,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B226,"")</f>
         <v>0</v>
       </c>
       <c r="E228">
-        <f>+IFERROR('Fallecidos Diarios'!C227,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C226,"")</f>
         <v>0</v>
       </c>
       <c r="F228">
@@ -30057,11 +30540,11 @@
         <v/>
       </c>
       <c r="D229">
-        <f>+IFERROR('Fallecidos Diarios'!B228,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B227,"")</f>
         <v>0</v>
       </c>
       <c r="E229">
-        <f>+IFERROR('Fallecidos Diarios'!C228,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C227,"")</f>
         <v>0</v>
       </c>
       <c r="F229">
@@ -30139,11 +30622,11 @@
         <v/>
       </c>
       <c r="D230">
-        <f>+IFERROR('Fallecidos Diarios'!B229,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B228,"")</f>
         <v>0</v>
       </c>
       <c r="E230">
-        <f>+IFERROR('Fallecidos Diarios'!C229,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C228,"")</f>
         <v>0</v>
       </c>
       <c r="F230">
@@ -30221,11 +30704,11 @@
         <v/>
       </c>
       <c r="D231">
-        <f>+IFERROR('Fallecidos Diarios'!B230,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B229,"")</f>
         <v>0</v>
       </c>
       <c r="E231">
-        <f>+IFERROR('Fallecidos Diarios'!C230,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C229,"")</f>
         <v>0</v>
       </c>
       <c r="F231">
@@ -30303,11 +30786,11 @@
         <v/>
       </c>
       <c r="D232">
-        <f>+IFERROR('Fallecidos Diarios'!B231,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B230,"")</f>
         <v>0</v>
       </c>
       <c r="E232">
-        <f>+IFERROR('Fallecidos Diarios'!C231,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C230,"")</f>
         <v>0</v>
       </c>
       <c r="F232">
@@ -30385,11 +30868,11 @@
         <v/>
       </c>
       <c r="D233">
-        <f>+IFERROR('Fallecidos Diarios'!B232,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B231,"")</f>
         <v>0</v>
       </c>
       <c r="E233">
-        <f>+IFERROR('Fallecidos Diarios'!C232,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C231,"")</f>
         <v>0</v>
       </c>
       <c r="F233">
@@ -30467,11 +30950,11 @@
         <v/>
       </c>
       <c r="D234">
-        <f>+IFERROR('Fallecidos Diarios'!B233,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B232,"")</f>
         <v>0</v>
       </c>
       <c r="E234">
-        <f>+IFERROR('Fallecidos Diarios'!C233,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C232,"")</f>
         <v>0</v>
       </c>
       <c r="F234">
@@ -30549,11 +31032,11 @@
         <v/>
       </c>
       <c r="D235">
-        <f>+IFERROR('Fallecidos Diarios'!B234,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B233,"")</f>
         <v>0</v>
       </c>
       <c r="E235">
-        <f>+IFERROR('Fallecidos Diarios'!C234,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C233,"")</f>
         <v>0</v>
       </c>
       <c r="F235">
@@ -30631,11 +31114,11 @@
         <v/>
       </c>
       <c r="D236">
-        <f>+IFERROR('Fallecidos Diarios'!B235,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B234,"")</f>
         <v>0</v>
       </c>
       <c r="E236">
-        <f>+IFERROR('Fallecidos Diarios'!C235,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C234,"")</f>
         <v>0</v>
       </c>
       <c r="F236">
@@ -30713,11 +31196,11 @@
         <v/>
       </c>
       <c r="D237">
-        <f>+IFERROR('Fallecidos Diarios'!B236,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B235,"")</f>
         <v>0</v>
       </c>
       <c r="E237">
-        <f>+IFERROR('Fallecidos Diarios'!C236,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C235,"")</f>
         <v>0</v>
       </c>
       <c r="F237">
@@ -30795,11 +31278,11 @@
         <v/>
       </c>
       <c r="D238">
-        <f>+IFERROR('Fallecidos Diarios'!B237,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B236,"")</f>
         <v>0</v>
       </c>
       <c r="E238">
-        <f>+IFERROR('Fallecidos Diarios'!C237,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C236,"")</f>
         <v>0</v>
       </c>
       <c r="F238">
@@ -30877,11 +31360,11 @@
         <v/>
       </c>
       <c r="D239">
-        <f>+IFERROR('Fallecidos Diarios'!B238,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B237,"")</f>
         <v>0</v>
       </c>
       <c r="E239">
-        <f>+IFERROR('Fallecidos Diarios'!C238,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C237,"")</f>
         <v>0</v>
       </c>
       <c r="F239">
@@ -30959,11 +31442,11 @@
         <v/>
       </c>
       <c r="D240">
-        <f>+IFERROR('Fallecidos Diarios'!B239,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B238,"")</f>
         <v>0</v>
       </c>
       <c r="E240">
-        <f>+IFERROR('Fallecidos Diarios'!C239,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C238,"")</f>
         <v>0</v>
       </c>
       <c r="F240">
@@ -31041,11 +31524,11 @@
         <v/>
       </c>
       <c r="D241">
-        <f>+IFERROR('Fallecidos Diarios'!B240,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B239,"")</f>
         <v>0</v>
       </c>
       <c r="E241">
-        <f>+IFERROR('Fallecidos Diarios'!C240,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C239,"")</f>
         <v>0</v>
       </c>
       <c r="F241">
@@ -31123,11 +31606,11 @@
         <v/>
       </c>
       <c r="D242">
-        <f>+IFERROR('Fallecidos Diarios'!B241,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B240,"")</f>
         <v>0</v>
       </c>
       <c r="E242">
-        <f>+IFERROR('Fallecidos Diarios'!C241,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C240,"")</f>
         <v>0</v>
       </c>
       <c r="F242">
@@ -31205,11 +31688,11 @@
         <v/>
       </c>
       <c r="D243">
-        <f>+IFERROR('Fallecidos Diarios'!B242,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B241,"")</f>
         <v>0</v>
       </c>
       <c r="E243">
-        <f>+IFERROR('Fallecidos Diarios'!C242,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C241,"")</f>
         <v>0</v>
       </c>
       <c r="F243">
@@ -31287,11 +31770,11 @@
         <v/>
       </c>
       <c r="D244">
-        <f>+IFERROR('Fallecidos Diarios'!B243,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B242,"")</f>
         <v>0</v>
       </c>
       <c r="E244">
-        <f>+IFERROR('Fallecidos Diarios'!C243,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C242,"")</f>
         <v>0</v>
       </c>
       <c r="F244">
@@ -31369,11 +31852,11 @@
         <v/>
       </c>
       <c r="D245">
-        <f>+IFERROR('Fallecidos Diarios'!B244,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B243,"")</f>
         <v>0</v>
       </c>
       <c r="E245">
-        <f>+IFERROR('Fallecidos Diarios'!C244,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C243,"")</f>
         <v>0</v>
       </c>
       <c r="F245">
@@ -31451,11 +31934,11 @@
         <v/>
       </c>
       <c r="D246">
-        <f>+IFERROR('Fallecidos Diarios'!B245,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B244,"")</f>
         <v>0</v>
       </c>
       <c r="E246">
-        <f>+IFERROR('Fallecidos Diarios'!C245,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C244,"")</f>
         <v>0</v>
       </c>
       <c r="F246">
@@ -31533,11 +32016,11 @@
         <v/>
       </c>
       <c r="D247">
-        <f>+IFERROR('Fallecidos Diarios'!B246,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B245,"")</f>
         <v>0</v>
       </c>
       <c r="E247">
-        <f>+IFERROR('Fallecidos Diarios'!C246,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C245,"")</f>
         <v>0</v>
       </c>
       <c r="F247">
@@ -31615,11 +32098,11 @@
         <v/>
       </c>
       <c r="D248">
-        <f>+IFERROR('Fallecidos Diarios'!B247,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B246,"")</f>
         <v>0</v>
       </c>
       <c r="E248">
-        <f>+IFERROR('Fallecidos Diarios'!C247,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C246,"")</f>
         <v>0</v>
       </c>
       <c r="F248">
@@ -31697,11 +32180,11 @@
         <v/>
       </c>
       <c r="D249">
-        <f>+IFERROR('Fallecidos Diarios'!B248,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B247,"")</f>
         <v>0</v>
       </c>
       <c r="E249">
-        <f>+IFERROR('Fallecidos Diarios'!C248,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C247,"")</f>
         <v>0</v>
       </c>
       <c r="F249">
@@ -31779,11 +32262,11 @@
         <v/>
       </c>
       <c r="D250">
-        <f>+IFERROR('Fallecidos Diarios'!B249,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B248,"")</f>
         <v>0</v>
       </c>
       <c r="E250">
-        <f>+IFERROR('Fallecidos Diarios'!C249,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C248,"")</f>
         <v>0</v>
       </c>
       <c r="F250">
@@ -31861,11 +32344,11 @@
         <v/>
       </c>
       <c r="D251">
-        <f>+IFERROR('Fallecidos Diarios'!B250,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B249,"")</f>
         <v>0</v>
       </c>
       <c r="E251">
-        <f>+IFERROR('Fallecidos Diarios'!C250,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C249,"")</f>
         <v>0</v>
       </c>
       <c r="F251">
@@ -31943,11 +32426,11 @@
         <v/>
       </c>
       <c r="D252">
-        <f>+IFERROR('Fallecidos Diarios'!B251,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B250,"")</f>
         <v>0</v>
       </c>
       <c r="E252">
-        <f>+IFERROR('Fallecidos Diarios'!C251,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C250,"")</f>
         <v>0</v>
       </c>
       <c r="F252">
@@ -32025,11 +32508,11 @@
         <v/>
       </c>
       <c r="D253">
-        <f>+IFERROR('Fallecidos Diarios'!B252,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B251,"")</f>
         <v>0</v>
       </c>
       <c r="E253">
-        <f>+IFERROR('Fallecidos Diarios'!C252,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C251,"")</f>
         <v>0</v>
       </c>
       <c r="F253">
@@ -32107,11 +32590,11 @@
         <v/>
       </c>
       <c r="D254">
-        <f>+IFERROR('Fallecidos Diarios'!B253,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B252,"")</f>
         <v>0</v>
       </c>
       <c r="E254">
-        <f>+IFERROR('Fallecidos Diarios'!C253,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C252,"")</f>
         <v>0</v>
       </c>
       <c r="F254">
@@ -32189,11 +32672,11 @@
         <v/>
       </c>
       <c r="D255">
-        <f>+IFERROR('Fallecidos Diarios'!B254,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B253,"")</f>
         <v>0</v>
       </c>
       <c r="E255">
-        <f>+IFERROR('Fallecidos Diarios'!C254,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C253,"")</f>
         <v>0</v>
       </c>
       <c r="F255">
@@ -32271,11 +32754,11 @@
         <v/>
       </c>
       <c r="D256">
-        <f>+IFERROR('Fallecidos Diarios'!B255,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B254,"")</f>
         <v>0</v>
       </c>
       <c r="E256">
-        <f>+IFERROR('Fallecidos Diarios'!C255,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C254,"")</f>
         <v>0</v>
       </c>
       <c r="F256">
@@ -32353,11 +32836,11 @@
         <v/>
       </c>
       <c r="D257">
-        <f>+IFERROR('Fallecidos Diarios'!B256,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B255,"")</f>
         <v>0</v>
       </c>
       <c r="E257">
-        <f>+IFERROR('Fallecidos Diarios'!C256,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C255,"")</f>
         <v>0</v>
       </c>
       <c r="F257">
@@ -32435,11 +32918,11 @@
         <v/>
       </c>
       <c r="D258">
-        <f>+IFERROR('Fallecidos Diarios'!B257,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B256,"")</f>
         <v>0</v>
       </c>
       <c r="E258">
-        <f>+IFERROR('Fallecidos Diarios'!C257,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C256,"")</f>
         <v>0</v>
       </c>
       <c r="F258">
@@ -32517,11 +33000,11 @@
         <v/>
       </c>
       <c r="D259">
-        <f>+IFERROR('Fallecidos Diarios'!B258,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B257,"")</f>
         <v>0</v>
       </c>
       <c r="E259">
-        <f>+IFERROR('Fallecidos Diarios'!C258,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C257,"")</f>
         <v>0</v>
       </c>
       <c r="F259">
@@ -32599,11 +33082,11 @@
         <v/>
       </c>
       <c r="D260">
-        <f>+IFERROR('Fallecidos Diarios'!B259,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B258,"")</f>
         <v>0</v>
       </c>
       <c r="E260">
-        <f>+IFERROR('Fallecidos Diarios'!C259,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C258,"")</f>
         <v>0</v>
       </c>
       <c r="F260">
@@ -32681,11 +33164,11 @@
         <v/>
       </c>
       <c r="D261">
-        <f>+IFERROR('Fallecidos Diarios'!B260,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B259,"")</f>
         <v>0</v>
       </c>
       <c r="E261">
-        <f>+IFERROR('Fallecidos Diarios'!C260,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C259,"")</f>
         <v>0</v>
       </c>
       <c r="F261">
@@ -32763,11 +33246,11 @@
         <v/>
       </c>
       <c r="D262">
-        <f>+IFERROR('Fallecidos Diarios'!B261,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B260,"")</f>
         <v>0</v>
       </c>
       <c r="E262">
-        <f>+IFERROR('Fallecidos Diarios'!C261,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C260,"")</f>
         <v>0</v>
       </c>
       <c r="F262">
@@ -32845,11 +33328,11 @@
         <v/>
       </c>
       <c r="D263">
-        <f>+IFERROR('Fallecidos Diarios'!B262,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B261,"")</f>
         <v>0</v>
       </c>
       <c r="E263">
-        <f>+IFERROR('Fallecidos Diarios'!C262,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C261,"")</f>
         <v>0</v>
       </c>
       <c r="F263">
@@ -32927,11 +33410,11 @@
         <v/>
       </c>
       <c r="D264">
-        <f>+IFERROR('Fallecidos Diarios'!B263,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B262,"")</f>
         <v>0</v>
       </c>
       <c r="E264">
-        <f>+IFERROR('Fallecidos Diarios'!C263,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C262,"")</f>
         <v>0</v>
       </c>
       <c r="F264">
@@ -33009,11 +33492,11 @@
         <v/>
       </c>
       <c r="D265">
-        <f>+IFERROR('Fallecidos Diarios'!B264,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B263,"")</f>
         <v>0</v>
       </c>
       <c r="E265">
-        <f>+IFERROR('Fallecidos Diarios'!C264,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C263,"")</f>
         <v>0</v>
       </c>
       <c r="F265">
@@ -33091,11 +33574,11 @@
         <v/>
       </c>
       <c r="D266">
-        <f>+IFERROR('Fallecidos Diarios'!B265,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B264,"")</f>
         <v>0</v>
       </c>
       <c r="E266">
-        <f>+IFERROR('Fallecidos Diarios'!C265,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C264,"")</f>
         <v>0</v>
       </c>
       <c r="F266">
@@ -33173,11 +33656,11 @@
         <v/>
       </c>
       <c r="D267">
-        <f>+IFERROR('Fallecidos Diarios'!B266,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B265,"")</f>
         <v>0</v>
       </c>
       <c r="E267">
-        <f>+IFERROR('Fallecidos Diarios'!C266,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C265,"")</f>
         <v>0</v>
       </c>
       <c r="F267">
@@ -33255,11 +33738,11 @@
         <v/>
       </c>
       <c r="D268">
-        <f>+IFERROR('Fallecidos Diarios'!B267,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B266,"")</f>
         <v>0</v>
       </c>
       <c r="E268">
-        <f>+IFERROR('Fallecidos Diarios'!C267,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C266,"")</f>
         <v>0</v>
       </c>
       <c r="F268">
@@ -33337,11 +33820,11 @@
         <v/>
       </c>
       <c r="D269">
-        <f>+IFERROR('Fallecidos Diarios'!B268,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B267,"")</f>
         <v>0</v>
       </c>
       <c r="E269">
-        <f>+IFERROR('Fallecidos Diarios'!C268,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C267,"")</f>
         <v>0</v>
       </c>
       <c r="F269">
@@ -33419,11 +33902,11 @@
         <v/>
       </c>
       <c r="D270">
-        <f>+IFERROR('Fallecidos Diarios'!B269,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B268,"")</f>
         <v>0</v>
       </c>
       <c r="E270">
-        <f>+IFERROR('Fallecidos Diarios'!C269,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C268,"")</f>
         <v>0</v>
       </c>
       <c r="F270">
@@ -33501,11 +33984,11 @@
         <v/>
       </c>
       <c r="D271">
-        <f>+IFERROR('Fallecidos Diarios'!B270,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B269,"")</f>
         <v>0</v>
       </c>
       <c r="E271">
-        <f>+IFERROR('Fallecidos Diarios'!C270,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C269,"")</f>
         <v>0</v>
       </c>
       <c r="F271">
@@ -33583,11 +34066,11 @@
         <v/>
       </c>
       <c r="D272">
-        <f>+IFERROR('Fallecidos Diarios'!B271,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B270,"")</f>
         <v>0</v>
       </c>
       <c r="E272">
-        <f>+IFERROR('Fallecidos Diarios'!C271,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C270,"")</f>
         <v>0</v>
       </c>
       <c r="F272">
@@ -33665,11 +34148,11 @@
         <v/>
       </c>
       <c r="D273">
-        <f>+IFERROR('Fallecidos Diarios'!B272,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B271,"")</f>
         <v>0</v>
       </c>
       <c r="E273">
-        <f>+IFERROR('Fallecidos Diarios'!C272,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C271,"")</f>
         <v>0</v>
       </c>
       <c r="F273">
@@ -33747,11 +34230,11 @@
         <v/>
       </c>
       <c r="D274">
-        <f>+IFERROR('Fallecidos Diarios'!B273,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B272,"")</f>
         <v>0</v>
       </c>
       <c r="E274">
-        <f>+IFERROR('Fallecidos Diarios'!C273,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C272,"")</f>
         <v>0</v>
       </c>
       <c r="F274">
@@ -33829,11 +34312,11 @@
         <v/>
       </c>
       <c r="D275">
-        <f>+IFERROR('Fallecidos Diarios'!B274,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B273,"")</f>
         <v>0</v>
       </c>
       <c r="E275">
-        <f>+IFERROR('Fallecidos Diarios'!C274,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C273,"")</f>
         <v>0</v>
       </c>
       <c r="F275">
@@ -33911,11 +34394,11 @@
         <v/>
       </c>
       <c r="D276">
-        <f>+IFERROR('Fallecidos Diarios'!B275,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B274,"")</f>
         <v>0</v>
       </c>
       <c r="E276">
-        <f>+IFERROR('Fallecidos Diarios'!C275,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C274,"")</f>
         <v>0</v>
       </c>
       <c r="F276">
@@ -33993,11 +34476,11 @@
         <v/>
       </c>
       <c r="D277">
-        <f>+IFERROR('Fallecidos Diarios'!B276,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B275,"")</f>
         <v>0</v>
       </c>
       <c r="E277">
-        <f>+IFERROR('Fallecidos Diarios'!C276,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C275,"")</f>
         <v>0</v>
       </c>
       <c r="F277">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-03-2020 21-08-32
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2169" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E54D0D07-2D4A-4AF2-86FC-194854E45BD1}"/>
+  <xr:revisionPtr revIDLastSave="2183" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DB681A54-03F9-4A39-A440-2B7EC1DE9DCB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Fallecidos Diarios'!$A$1:$C$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Recuperados Diarios'!$A$1:$C$147</definedName>
   </definedNames>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -335,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C145" totalsRowShown="0">
-  <autoFilter ref="A1:C145" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2A66899C-BBC2-4424-A1E7-B1948EF59DC9}" name="Tabla2" displayName="Tabla2" ref="A1:C147" totalsRowShown="0">
+  <autoFilter ref="A1:C147" xr:uid="{F728434E-A725-4812-B399-71BF4F83CC85}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{8EC2316A-7046-4097-90A4-64373053E002}" name="Fecha" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D201B563-B400-44EC-9308-0689C8B650F2}" name="Recuperados Acumulados"/>
@@ -349,8 +349,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C145" totalsRowShown="0">
-  <autoFilter ref="A1:C145" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52D6FB1D-35C8-4895-84FA-09D0EA9D4B35}" name="Tabla1" displayName="Tabla1" ref="A1:C147" totalsRowShown="0">
+  <autoFilter ref="A1:C147" xr:uid="{517D9367-0240-4C2D-ADFF-4AF09B613BBD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0885F415-77E4-4B4C-9B60-6BEC0001A890}" name="Fecha" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{EF6B2D91-8C0A-4DE9-801E-4F11E28B825F}" name="Fallecidos Acumulados"/>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M146" totalsRowShown="0">
-  <autoFilter ref="A1:M146" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D9BA8B8B-0F8F-4242-B2E7-7A363E740AE3}" name="Tabla3" displayName="Tabla3" ref="A1:M148" totalsRowShown="0">
+  <autoFilter ref="A1:M148" xr:uid="{4D9B2783-E960-4987-881E-175B768F31D3}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{0057B26E-FB62-446F-BDF0-7F3E0DE0835E}" name="Fecha" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{FD7DC77B-0B9F-46ED-A1AC-3680468FCD48}" name="Confirmados Acumulados"/>
@@ -752,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
-  <dimension ref="A1:BC145"/>
+  <dimension ref="A1:BC147"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4280,6 +4280,30 @@
         <v>948</v>
       </c>
     </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B146">
+        <v>40081</v>
+      </c>
+      <c r="C146">
+        <f>B146-B145</f>
+        <v>915</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="4">
+        <v>44045</v>
+      </c>
+      <c r="B147">
+        <v>41038</v>
+      </c>
+      <c r="C147">
+        <f>B147-B146</f>
+        <v>957</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A72:C1048576">
     <sortCondition descending="1" ref="A72:A1048576"/>
@@ -4293,10 +4317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
-  <dimension ref="A1:E145"/>
+  <dimension ref="A1:E147"/>
   <sheetViews>
     <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="F152" sqref="F152"/>
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -5475,7 +5499,7 @@
         <v>457</v>
       </c>
       <c r="C100">
-        <f t="shared" ref="C100:C145" si="1">B100-B99</f>
+        <f t="shared" ref="C100:C147" si="1">B100-B99</f>
         <v>9</v>
       </c>
     </row>
@@ -6017,6 +6041,30 @@
       <c r="C145">
         <f t="shared" si="1"/>
         <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="4">
+        <v>44044</v>
+      </c>
+      <c r="B146">
+        <v>1449</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="4">
+        <v>44045</v>
+      </c>
+      <c r="B147">
+        <v>1471</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -6029,11 +6077,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12899D86-5B86-49AD-AFB2-4561F885F47E}">
-  <dimension ref="A1:M146"/>
+  <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="C2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -11788,7 +11836,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:13">
       <c r="A145" s="9">
         <v>44042</v>
       </c>
@@ -11807,7 +11855,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:13">
       <c r="A146" s="9">
         <v>44043</v>
       </c>
@@ -11825,6 +11873,58 @@
         <f>C146-D146</f>
         <v>555</v>
       </c>
+    </row>
+    <row r="147" spans="1:13">
+      <c r="A147" s="9">
+        <v>44044</v>
+      </c>
+      <c r="B147" s="6">
+        <v>66383</v>
+      </c>
+      <c r="C147" s="10">
+        <f>IFERROR(B147-B146,"")</f>
+        <v>1127</v>
+      </c>
+      <c r="D147" s="6">
+        <v>537</v>
+      </c>
+      <c r="E147" s="10">
+        <f>C147-D147</f>
+        <v>590</v>
+      </c>
+      <c r="F147" s="6"/>
+      <c r="G147" s="6"/>
+      <c r="H147" s="6"/>
+      <c r="I147" s="6"/>
+      <c r="J147" s="6"/>
+      <c r="K147" s="6"/>
+      <c r="L147" s="6"/>
+      <c r="M147" s="6"/>
+    </row>
+    <row r="148" spans="1:13">
+      <c r="A148" s="9">
+        <v>44045</v>
+      </c>
+      <c r="B148" s="6">
+        <v>67453</v>
+      </c>
+      <c r="C148" s="10">
+        <f>IFERROR(B148-B147,"")</f>
+        <v>1070</v>
+      </c>
+      <c r="D148" s="6"/>
+      <c r="E148" s="10">
+        <f>C148-D148</f>
+        <v>1070</v>
+      </c>
+      <c r="F148" s="6"/>
+      <c r="G148" s="6"/>
+      <c r="H148" s="6"/>
+      <c r="I148" s="6"/>
+      <c r="J148" s="6"/>
+      <c r="K148" s="6"/>
+      <c r="L148" s="6"/>
+      <c r="M148" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11841,7 +11941,7 @@
   </sheetPr>
   <dimension ref="A1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A135" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -23803,17 +23903,17 @@
       </c>
     </row>
     <row r="147" spans="1:20">
-      <c r="A147" s="4" t="str">
+      <c r="A147" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B147" t="str">
+        <v>44044</v>
+      </c>
+      <c r="B147">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C147" t="str">
+        <v>66383</v>
+      </c>
+      <c r="C147">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1127</v>
       </c>
       <c r="D147" t="str">
         <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
@@ -23825,11 +23925,11 @@
       </c>
       <c r="F147">
         <f>+IFERROR('Recuperados Diarios'!B146,"")</f>
-        <v>0</v>
+        <v>40081</v>
       </c>
       <c r="G147">
         <f>+IFERROR('Recuperados Diarios'!C146,"")</f>
-        <v>0</v>
+        <v>915</v>
       </c>
       <c r="H147" t="str">
         <f t="shared" si="26"/>
@@ -23843,9 +23943,9 @@
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="K147" t="str">
+      <c r="K147">
         <f t="shared" si="28"/>
-        <v/>
+        <v>0.6037841013512496</v>
       </c>
       <c r="L147" t="str">
         <f t="shared" si="29"/>
@@ -23859,17 +23959,17 @@
         <f t="shared" si="31"/>
         <v/>
       </c>
-      <c r="O147" t="str">
+      <c r="O147">
         <f t="shared" si="32"/>
-        <v/>
+        <v>2.2828771737232106E-2</v>
       </c>
       <c r="P147" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="Q147" t="str">
+      <c r="Q147">
         <f t="shared" si="34"/>
-        <v/>
+        <v>15961.288771339265</v>
       </c>
       <c r="R147" t="str">
         <f t="shared" si="35"/>
@@ -23877,7 +23977,7 @@
       </c>
       <c r="S147">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>9637.1723972108684</v>
       </c>
       <c r="T147" t="str">
         <f t="shared" si="37"/>
@@ -23885,85 +23985,85 @@
       </c>
     </row>
     <row r="148" spans="1:20">
-      <c r="A148" s="4" t="str">
+      <c r="A148" s="4">
         <f>+IFERROR(Tabla3[[#This Row],[Fecha]],"")</f>
-        <v/>
-      </c>
-      <c r="B148" t="str">
+        <v>44045</v>
+      </c>
+      <c r="B148">
         <f>+IFERROR(Tabla3[[#This Row],[Confirmados Acumulados]],"")</f>
-        <v/>
-      </c>
-      <c r="C148" t="str">
+        <v>67453</v>
+      </c>
+      <c r="C148">
         <f>+IFERROR(Tabla3[[#This Row],[Nuevos Confirmados]],"")</f>
-        <v/>
+        <v>1070</v>
       </c>
       <c r="D148">
         <f>+IFERROR('Fallecidos Diarios'!B146,"")</f>
-        <v>0</v>
+        <v>1449</v>
       </c>
       <c r="E148">
         <f>+IFERROR('Fallecidos Diarios'!C146,"")</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F148">
         <f>+IFERROR('Recuperados Diarios'!B147,"")</f>
-        <v>0</v>
+        <v>41038</v>
       </c>
       <c r="G148">
         <f>+IFERROR('Recuperados Diarios'!C147,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H148" t="str">
+        <v>957</v>
+      </c>
+      <c r="H148">
         <f t="shared" si="26"/>
-        <v/>
+        <v>24966</v>
       </c>
       <c r="I148" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="J148" t="str">
+      <c r="J148">
         <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="K148" t="str">
+        <v>2.1481624242064845E-2</v>
+      </c>
+      <c r="K148">
         <f t="shared" si="28"/>
-        <v/>
-      </c>
-      <c r="L148" t="str">
+        <v>0.60839399285428375</v>
+      </c>
+      <c r="L148">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M148" t="str">
+        <v>0.37012438290365141</v>
+      </c>
+      <c r="M148">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N148" t="str">
+        <v>2890.9200512697271</v>
+      </c>
+      <c r="N148">
         <f t="shared" si="31"/>
-        <v/>
-      </c>
-      <c r="O148" t="str">
+        <v>1.932367149758454E-2</v>
+      </c>
+      <c r="O148">
         <f t="shared" si="32"/>
-        <v/>
+        <v>2.3319849895219066E-2</v>
       </c>
       <c r="P148" t="str">
         <f t="shared" si="33"/>
         <v/>
       </c>
-      <c r="Q148" t="str">
+      <c r="Q148">
         <f t="shared" si="34"/>
-        <v/>
+        <v>16218.56215436403</v>
       </c>
       <c r="R148">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>348.40105794662179</v>
       </c>
       <c r="S148">
         <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="T148" t="str">
+        <v>9867.2757874489071</v>
+      </c>
+      <c r="T148">
         <f t="shared" si="37"/>
-        <v/>
+        <v>6002.8853089685026</v>
       </c>
     </row>
     <row r="149" spans="1:20">
@@ -23981,11 +24081,11 @@
       </c>
       <c r="D149">
         <f>+IFERROR('Fallecidos Diarios'!B147,"")</f>
-        <v>0</v>
+        <v>1471</v>
       </c>
       <c r="E149">
         <f>+IFERROR('Fallecidos Diarios'!C147,"")</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F149">
         <f>+IFERROR('Recuperados Diarios'!B148,"")</f>
@@ -24019,9 +24119,9 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
-      <c r="N149" t="str">
+      <c r="N149">
         <f t="shared" si="31"/>
-        <v/>
+        <v>1.495581237253569E-2</v>
       </c>
       <c r="O149" t="str">
         <f t="shared" si="32"/>
@@ -24037,7 +24137,7 @@
       </c>
       <c r="R149">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>353.69079105554221</v>
       </c>
       <c r="S149">
         <f t="shared" si="36"/>

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2020 13-22-08
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2199" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BE1677C-2D06-444D-835E-95631A1E01EC}"/>
+  <xr:revisionPtr revIDLastSave="2202" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADBA0678-B85F-4483-8DF0-53CD4E7E3E50}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recuperados Diarios" sheetId="3" r:id="rId1"/>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4309,9 +4309,12 @@
       <c r="A148" s="4">
         <v>44046</v>
       </c>
+      <c r="B148">
+        <v>42093</v>
+      </c>
       <c r="C148">
         <f>B148-B147</f>
-        <v>-41038</v>
+        <v>1055</v>
       </c>
     </row>
   </sheetData>
@@ -4329,7 +4332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC392382-2E38-495D-A066-EE170A1325D6}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
@@ -6189,7 +6192,7 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12075,8 +12078,8 @@
   </sheetPr>
   <dimension ref="A1:T277"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -24049,13 +24052,13 @@
         <f>+IFERROR(Confirmados_diarios[[#This Row],[Nuevos Confirmados]],"")</f>
         <v>1127</v>
       </c>
-      <c r="D147" t="str">
-        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
-        <v/>
-      </c>
-      <c r="E147" t="str">
-        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
-        <v/>
+      <c r="D147">
+        <f>+IFERROR('Fallecidos Diarios'!B146,"")</f>
+        <v>1449</v>
+      </c>
+      <c r="E147">
+        <f>+IFERROR('Fallecidos Diarios'!C146,"")</f>
+        <v>28</v>
       </c>
       <c r="F147">
         <f>+IFERROR('Recuperados Diarios'!B146,"")</f>
@@ -24065,57 +24068,57 @@
         <f>+IFERROR('Recuperados Diarios'!C146,"")</f>
         <v>915</v>
       </c>
-      <c r="H147" t="str">
+      <c r="H147">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I147" t="str">
+        <v>24853</v>
+      </c>
+      <c r="I147">
         <f t="shared" si="38"/>
-        <v/>
-      </c>
-      <c r="J147" t="str">
+        <v>184</v>
+      </c>
+      <c r="J147">
         <f t="shared" si="27"/>
-        <v/>
+        <v>2.1827877619269995E-2</v>
       </c>
       <c r="K147">
         <f t="shared" si="28"/>
         <v>0.6037841013512496</v>
       </c>
-      <c r="L147" t="str">
+      <c r="L147">
         <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="M147" t="str">
+        <v>0.37438802102948043</v>
+      </c>
+      <c r="M147">
         <f t="shared" si="30"/>
-        <v/>
-      </c>
-      <c r="N147" t="str">
+        <v>3010.2458858085542</v>
+      </c>
+      <c r="N147">
         <f t="shared" si="31"/>
-        <v/>
+        <v>1.932367149758454E-2</v>
       </c>
       <c r="O147">
         <f t="shared" si="32"/>
         <v>2.2828771737232106E-2</v>
       </c>
-      <c r="P147" t="str">
+      <c r="P147">
         <f t="shared" si="33"/>
-        <v/>
+        <v>7.4035327727034967E-3</v>
       </c>
       <c r="Q147">
         <f t="shared" si="34"/>
         <v>15961.288771339265</v>
       </c>
-      <c r="R147" t="str">
+      <c r="R147">
         <f t="shared" si="35"/>
-        <v/>
+        <v>348.40105794662179</v>
       </c>
       <c r="S147">
         <f t="shared" si="36"/>
         <v>9637.1723972108684</v>
       </c>
-      <c r="T147" t="str">
+      <c r="T147">
         <f t="shared" si="37"/>
-        <v/>
+        <v>5975.7153161817751</v>
       </c>
     </row>
     <row r="148" spans="1:20">
@@ -24132,12 +24135,12 @@
         <v>1070</v>
       </c>
       <c r="D148">
-        <f>+IFERROR('Fallecidos Diarios'!B146,"")</f>
-        <v>1449</v>
+        <f>+IFERROR('Fallecidos Diarios'!B147,"")</f>
+        <v>1471</v>
       </c>
       <c r="E148">
-        <f>+IFERROR('Fallecidos Diarios'!C146,"")</f>
-        <v>28</v>
+        <f>+IFERROR('Fallecidos Diarios'!C147,"")</f>
+        <v>22</v>
       </c>
       <c r="F148">
         <f>+IFERROR('Recuperados Diarios'!B147,"")</f>
@@ -24149,15 +24152,15 @@
       </c>
       <c r="H148">
         <f t="shared" si="26"/>
-        <v>24966</v>
-      </c>
-      <c r="I148" t="str">
+        <v>24944</v>
+      </c>
+      <c r="I148">
         <f t="shared" si="38"/>
-        <v/>
+        <v>91</v>
       </c>
       <c r="J148">
         <f t="shared" si="27"/>
-        <v>2.1481624242064845E-2</v>
+        <v>2.1807777267134152E-2</v>
       </c>
       <c r="K148">
         <f t="shared" si="28"/>
@@ -24165,23 +24168,23 @@
       </c>
       <c r="L148">
         <f t="shared" si="29"/>
-        <v>0.37012438290365141</v>
+        <v>0.36979822987858213</v>
       </c>
       <c r="M148">
         <f t="shared" si="30"/>
-        <v>2890.9200512697271</v>
+        <v>2893.4697722899296</v>
       </c>
       <c r="N148">
         <f t="shared" si="31"/>
-        <v>1.932367149758454E-2</v>
+        <v>1.495581237253569E-2</v>
       </c>
       <c r="O148">
         <f t="shared" si="32"/>
         <v>2.3319849895219066E-2</v>
       </c>
-      <c r="P148" t="str">
+      <c r="P148">
         <f t="shared" si="33"/>
-        <v/>
+        <v>3.6481719050673509E-3</v>
       </c>
       <c r="Q148">
         <f t="shared" si="34"/>
@@ -24189,7 +24192,7 @@
       </c>
       <c r="R148">
         <f t="shared" si="35"/>
-        <v>348.40105794662179</v>
+        <v>353.69079105554221</v>
       </c>
       <c r="S148">
         <f t="shared" si="36"/>
@@ -24197,7 +24200,7 @@
       </c>
       <c r="T148">
         <f t="shared" si="37"/>
-        <v>6002.8853089685026</v>
+        <v>5997.5955758595819</v>
       </c>
     </row>
     <row r="149" spans="1:20">
@@ -24214,56 +24217,56 @@
         <v>1003</v>
       </c>
       <c r="D149">
-        <f>+IFERROR('Fallecidos Diarios'!B147,"")</f>
-        <v>1471</v>
+        <f>+IFERROR('Fallecidos Diarios'!B148,"")</f>
+        <v>1497</v>
       </c>
       <c r="E149">
-        <f>+IFERROR('Fallecidos Diarios'!C147,"")</f>
-        <v>22</v>
+        <f>+IFERROR('Fallecidos Diarios'!C148,"")</f>
+        <v>26</v>
       </c>
       <c r="F149">
         <f>+IFERROR('Recuperados Diarios'!B148,"")</f>
-        <v>0</v>
+        <v>42093</v>
       </c>
       <c r="G149">
         <f>+IFERROR('Recuperados Diarios'!C148,"")</f>
-        <v>-41038</v>
+        <v>1055</v>
       </c>
       <c r="H149">
         <f t="shared" si="26"/>
-        <v>66985</v>
+        <v>24866</v>
       </c>
       <c r="I149">
         <f t="shared" si="38"/>
-        <v>42019</v>
+        <v>-78</v>
       </c>
       <c r="J149">
         <f t="shared" si="27"/>
-        <v>2.1488255229636554E-2</v>
+        <v>2.1868061236414632E-2</v>
       </c>
       <c r="K149">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>0.61489131705036815</v>
       </c>
       <c r="L149">
         <f t="shared" si="29"/>
-        <v>0.9785117447703634</v>
+        <v>0.36324062171321725</v>
       </c>
       <c r="M149">
         <f t="shared" si="30"/>
-        <v>1025.0260207509145</v>
+        <v>2761.2550470521996</v>
       </c>
       <c r="N149">
         <f t="shared" si="31"/>
-        <v>1.495581237253569E-2</v>
-      </c>
-      <c r="O149" t="str">
+        <v>1.736806947227789E-2</v>
+      </c>
+      <c r="O149">
         <f t="shared" si="32"/>
-        <v/>
+        <v>2.5063549758867269E-2</v>
       </c>
       <c r="P149">
         <f t="shared" si="33"/>
-        <v>0.62728969172202731</v>
+        <v>-3.1368133193919409E-3</v>
       </c>
       <c r="Q149">
         <f t="shared" si="34"/>
@@ -24271,15 +24274,15 @@
       </c>
       <c r="R149">
         <f t="shared" si="35"/>
-        <v>353.69079105554221</v>
+        <v>359.94229382062997</v>
       </c>
       <c r="S149">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>10120.942534263044</v>
       </c>
       <c r="T149">
         <f t="shared" si="37"/>
-        <v>16106.035104592451</v>
+        <v>5978.841067564319</v>
       </c>
     </row>
     <row r="150" spans="1:20">
@@ -24295,13 +24298,13 @@
         <f>+IFERROR(Confirmados_diarios[[#This Row],[Nuevos Confirmados]],"")</f>
         <v/>
       </c>
-      <c r="D150" t="str">
-        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
-        <v/>
-      </c>
-      <c r="E150" t="str">
-        <f>+IFERROR('Fallecidos Diarios'!#REF!,"")</f>
-        <v/>
+      <c r="D150">
+        <f>+IFERROR('Fallecidos Diarios'!B149,"")</f>
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <f>+IFERROR('Fallecidos Diarios'!C149,"")</f>
+        <v>0</v>
       </c>
       <c r="F150">
         <f>+IFERROR('Recuperados Diarios'!B149,"")</f>
@@ -24351,9 +24354,9 @@
         <f t="shared" si="34"/>
         <v/>
       </c>
-      <c r="R150" t="str">
+      <c r="R150">
         <f t="shared" si="35"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S150">
         <f t="shared" si="36"/>
@@ -24378,12 +24381,12 @@
         <v/>
       </c>
       <c r="D151">
-        <f>+IFERROR('Fallecidos Diarios'!B148,"")</f>
-        <v>1497</v>
+        <f>+IFERROR('Fallecidos Diarios'!B150,"")</f>
+        <v>0</v>
       </c>
       <c r="E151">
-        <f>+IFERROR('Fallecidos Diarios'!C148,"")</f>
-        <v>26</v>
+        <f>+IFERROR('Fallecidos Diarios'!C150,"")</f>
+        <v>0</v>
       </c>
       <c r="F151">
         <f>+IFERROR('Recuperados Diarios'!B150,"")</f>
@@ -24417,9 +24420,9 @@
         <f t="shared" si="30"/>
         <v/>
       </c>
-      <c r="N151">
+      <c r="N151" t="str">
         <f t="shared" si="31"/>
-        <v>1.736806947227789E-2</v>
+        <v/>
       </c>
       <c r="O151" t="str">
         <f t="shared" si="32"/>
@@ -24435,7 +24438,7 @@
       </c>
       <c r="R151">
         <f t="shared" si="35"/>
-        <v>359.94229382062997</v>
+        <v>0</v>
       </c>
       <c r="S151">
         <f t="shared" si="36"/>
@@ -24460,11 +24463,11 @@
         <v/>
       </c>
       <c r="D152">
-        <f>+IFERROR('Fallecidos Diarios'!B149,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B151,"")</f>
         <v>0</v>
       </c>
       <c r="E152">
-        <f>+IFERROR('Fallecidos Diarios'!C149,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C151,"")</f>
         <v>0</v>
       </c>
       <c r="F152">
@@ -24542,11 +24545,11 @@
         <v/>
       </c>
       <c r="D153">
-        <f>+IFERROR('Fallecidos Diarios'!B150,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B152,"")</f>
         <v>0</v>
       </c>
       <c r="E153">
-        <f>+IFERROR('Fallecidos Diarios'!C150,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C152,"")</f>
         <v>0</v>
       </c>
       <c r="F153">
@@ -24624,11 +24627,11 @@
         <v/>
       </c>
       <c r="D154">
-        <f>+IFERROR('Fallecidos Diarios'!B151,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B153,"")</f>
         <v>0</v>
       </c>
       <c r="E154">
-        <f>+IFERROR('Fallecidos Diarios'!C151,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C153,"")</f>
         <v>0</v>
       </c>
       <c r="F154">
@@ -24706,11 +24709,11 @@
         <v/>
       </c>
       <c r="D155">
-        <f>+IFERROR('Fallecidos Diarios'!B152,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B154,"")</f>
         <v>0</v>
       </c>
       <c r="E155">
-        <f>+IFERROR('Fallecidos Diarios'!C152,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C154,"")</f>
         <v>0</v>
       </c>
       <c r="F155">
@@ -24788,11 +24791,11 @@
         <v/>
       </c>
       <c r="D156">
-        <f>+IFERROR('Fallecidos Diarios'!B153,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B155,"")</f>
         <v>0</v>
       </c>
       <c r="E156">
-        <f>+IFERROR('Fallecidos Diarios'!C153,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C155,"")</f>
         <v>0</v>
       </c>
       <c r="F156">
@@ -24870,11 +24873,11 @@
         <v/>
       </c>
       <c r="D157">
-        <f>+IFERROR('Fallecidos Diarios'!B154,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B156,"")</f>
         <v>0</v>
       </c>
       <c r="E157">
-        <f>+IFERROR('Fallecidos Diarios'!C154,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C156,"")</f>
         <v>0</v>
       </c>
       <c r="F157">
@@ -24952,11 +24955,11 @@
         <v/>
       </c>
       <c r="D158">
-        <f>+IFERROR('Fallecidos Diarios'!B155,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B157,"")</f>
         <v>0</v>
       </c>
       <c r="E158">
-        <f>+IFERROR('Fallecidos Diarios'!C155,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C157,"")</f>
         <v>0</v>
       </c>
       <c r="F158">
@@ -25034,11 +25037,11 @@
         <v/>
       </c>
       <c r="D159">
-        <f>+IFERROR('Fallecidos Diarios'!B156,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B158,"")</f>
         <v>0</v>
       </c>
       <c r="E159">
-        <f>+IFERROR('Fallecidos Diarios'!C156,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C158,"")</f>
         <v>0</v>
       </c>
       <c r="F159">
@@ -25116,11 +25119,11 @@
         <v/>
       </c>
       <c r="D160">
-        <f>+IFERROR('Fallecidos Diarios'!B157,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B159,"")</f>
         <v>0</v>
       </c>
       <c r="E160">
-        <f>+IFERROR('Fallecidos Diarios'!C157,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C159,"")</f>
         <v>0</v>
       </c>
       <c r="F160">
@@ -25198,11 +25201,11 @@
         <v/>
       </c>
       <c r="D161">
-        <f>+IFERROR('Fallecidos Diarios'!B158,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B160,"")</f>
         <v>0</v>
       </c>
       <c r="E161">
-        <f>+IFERROR('Fallecidos Diarios'!C158,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C160,"")</f>
         <v>0</v>
       </c>
       <c r="F161">
@@ -25280,11 +25283,11 @@
         <v/>
       </c>
       <c r="D162">
-        <f>+IFERROR('Fallecidos Diarios'!B159,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B161,"")</f>
         <v>0</v>
       </c>
       <c r="E162">
-        <f>+IFERROR('Fallecidos Diarios'!C159,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C161,"")</f>
         <v>0</v>
       </c>
       <c r="F162">
@@ -25362,11 +25365,11 @@
         <v/>
       </c>
       <c r="D163">
-        <f>+IFERROR('Fallecidos Diarios'!B160,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B162,"")</f>
         <v>0</v>
       </c>
       <c r="E163">
-        <f>+IFERROR('Fallecidos Diarios'!C160,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C162,"")</f>
         <v>0</v>
       </c>
       <c r="F163">
@@ -25444,11 +25447,11 @@
         <v/>
       </c>
       <c r="D164">
-        <f>+IFERROR('Fallecidos Diarios'!B161,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B163,"")</f>
         <v>0</v>
       </c>
       <c r="E164">
-        <f>+IFERROR('Fallecidos Diarios'!C161,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C163,"")</f>
         <v>0</v>
       </c>
       <c r="F164">
@@ -25526,11 +25529,11 @@
         <v/>
       </c>
       <c r="D165">
-        <f>+IFERROR('Fallecidos Diarios'!B162,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B164,"")</f>
         <v>0</v>
       </c>
       <c r="E165">
-        <f>+IFERROR('Fallecidos Diarios'!C162,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C164,"")</f>
         <v>0</v>
       </c>
       <c r="F165">
@@ -25608,11 +25611,11 @@
         <v/>
       </c>
       <c r="D166">
-        <f>+IFERROR('Fallecidos Diarios'!B163,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B165,"")</f>
         <v>0</v>
       </c>
       <c r="E166">
-        <f>+IFERROR('Fallecidos Diarios'!C163,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C165,"")</f>
         <v>0</v>
       </c>
       <c r="F166">
@@ -25690,11 +25693,11 @@
         <v/>
       </c>
       <c r="D167">
-        <f>+IFERROR('Fallecidos Diarios'!B164,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B166,"")</f>
         <v>0</v>
       </c>
       <c r="E167">
-        <f>+IFERROR('Fallecidos Diarios'!C164,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C166,"")</f>
         <v>0</v>
       </c>
       <c r="F167">
@@ -25772,11 +25775,11 @@
         <v/>
       </c>
       <c r="D168">
-        <f>+IFERROR('Fallecidos Diarios'!B165,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B167,"")</f>
         <v>0</v>
       </c>
       <c r="E168">
-        <f>+IFERROR('Fallecidos Diarios'!C165,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C167,"")</f>
         <v>0</v>
       </c>
       <c r="F168">
@@ -25854,11 +25857,11 @@
         <v/>
       </c>
       <c r="D169">
-        <f>+IFERROR('Fallecidos Diarios'!B166,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B168,"")</f>
         <v>0</v>
       </c>
       <c r="E169">
-        <f>+IFERROR('Fallecidos Diarios'!C166,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C168,"")</f>
         <v>0</v>
       </c>
       <c r="F169">
@@ -25936,11 +25939,11 @@
         <v/>
       </c>
       <c r="D170">
-        <f>+IFERROR('Fallecidos Diarios'!B167,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B169,"")</f>
         <v>0</v>
       </c>
       <c r="E170">
-        <f>+IFERROR('Fallecidos Diarios'!C167,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C169,"")</f>
         <v>0</v>
       </c>
       <c r="F170">
@@ -26018,11 +26021,11 @@
         <v/>
       </c>
       <c r="D171">
-        <f>+IFERROR('Fallecidos Diarios'!B168,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B170,"")</f>
         <v>0</v>
       </c>
       <c r="E171">
-        <f>+IFERROR('Fallecidos Diarios'!C168,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C170,"")</f>
         <v>0</v>
       </c>
       <c r="F171">
@@ -26100,11 +26103,11 @@
         <v/>
       </c>
       <c r="D172">
-        <f>+IFERROR('Fallecidos Diarios'!B169,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B171,"")</f>
         <v>0</v>
       </c>
       <c r="E172">
-        <f>+IFERROR('Fallecidos Diarios'!C169,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C171,"")</f>
         <v>0</v>
       </c>
       <c r="F172">
@@ -26182,11 +26185,11 @@
         <v/>
       </c>
       <c r="D173">
-        <f>+IFERROR('Fallecidos Diarios'!B170,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B172,"")</f>
         <v>0</v>
       </c>
       <c r="E173">
-        <f>+IFERROR('Fallecidos Diarios'!C170,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C172,"")</f>
         <v>0</v>
       </c>
       <c r="F173">
@@ -26264,11 +26267,11 @@
         <v/>
       </c>
       <c r="D174">
-        <f>+IFERROR('Fallecidos Diarios'!B171,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B173,"")</f>
         <v>0</v>
       </c>
       <c r="E174">
-        <f>+IFERROR('Fallecidos Diarios'!C171,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C173,"")</f>
         <v>0</v>
       </c>
       <c r="F174">
@@ -26346,11 +26349,11 @@
         <v/>
       </c>
       <c r="D175">
-        <f>+IFERROR('Fallecidos Diarios'!B172,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B174,"")</f>
         <v>0</v>
       </c>
       <c r="E175">
-        <f>+IFERROR('Fallecidos Diarios'!C172,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C174,"")</f>
         <v>0</v>
       </c>
       <c r="F175">
@@ -26428,11 +26431,11 @@
         <v/>
       </c>
       <c r="D176">
-        <f>+IFERROR('Fallecidos Diarios'!B173,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B175,"")</f>
         <v>0</v>
       </c>
       <c r="E176">
-        <f>+IFERROR('Fallecidos Diarios'!C173,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C175,"")</f>
         <v>0</v>
       </c>
       <c r="F176">
@@ -26510,11 +26513,11 @@
         <v/>
       </c>
       <c r="D177">
-        <f>+IFERROR('Fallecidos Diarios'!B174,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B176,"")</f>
         <v>0</v>
       </c>
       <c r="E177">
-        <f>+IFERROR('Fallecidos Diarios'!C174,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C176,"")</f>
         <v>0</v>
       </c>
       <c r="F177">
@@ -26592,11 +26595,11 @@
         <v/>
       </c>
       <c r="D178">
-        <f>+IFERROR('Fallecidos Diarios'!B175,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B177,"")</f>
         <v>0</v>
       </c>
       <c r="E178">
-        <f>+IFERROR('Fallecidos Diarios'!C175,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C177,"")</f>
         <v>0</v>
       </c>
       <c r="F178">
@@ -26674,11 +26677,11 @@
         <v/>
       </c>
       <c r="D179">
-        <f>+IFERROR('Fallecidos Diarios'!B176,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B178,"")</f>
         <v>0</v>
       </c>
       <c r="E179">
-        <f>+IFERROR('Fallecidos Diarios'!C176,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C178,"")</f>
         <v>0</v>
       </c>
       <c r="F179">
@@ -26756,11 +26759,11 @@
         <v/>
       </c>
       <c r="D180">
-        <f>+IFERROR('Fallecidos Diarios'!B177,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B179,"")</f>
         <v>0</v>
       </c>
       <c r="E180">
-        <f>+IFERROR('Fallecidos Diarios'!C177,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C179,"")</f>
         <v>0</v>
       </c>
       <c r="F180">
@@ -26838,11 +26841,11 @@
         <v/>
       </c>
       <c r="D181">
-        <f>+IFERROR('Fallecidos Diarios'!B178,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B180,"")</f>
         <v>0</v>
       </c>
       <c r="E181">
-        <f>+IFERROR('Fallecidos Diarios'!C178,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C180,"")</f>
         <v>0</v>
       </c>
       <c r="F181">
@@ -26920,11 +26923,11 @@
         <v/>
       </c>
       <c r="D182">
-        <f>+IFERROR('Fallecidos Diarios'!B179,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B181,"")</f>
         <v>0</v>
       </c>
       <c r="E182">
-        <f>+IFERROR('Fallecidos Diarios'!C179,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C181,"")</f>
         <v>0</v>
       </c>
       <c r="F182">
@@ -27002,11 +27005,11 @@
         <v/>
       </c>
       <c r="D183">
-        <f>+IFERROR('Fallecidos Diarios'!B180,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B182,"")</f>
         <v>0</v>
       </c>
       <c r="E183">
-        <f>+IFERROR('Fallecidos Diarios'!C180,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C182,"")</f>
         <v>0</v>
       </c>
       <c r="F183">
@@ -27084,11 +27087,11 @@
         <v/>
       </c>
       <c r="D184">
-        <f>+IFERROR('Fallecidos Diarios'!B181,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B183,"")</f>
         <v>0</v>
       </c>
       <c r="E184">
-        <f>+IFERROR('Fallecidos Diarios'!C181,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C183,"")</f>
         <v>0</v>
       </c>
       <c r="F184">
@@ -27166,11 +27169,11 @@
         <v/>
       </c>
       <c r="D185">
-        <f>+IFERROR('Fallecidos Diarios'!B182,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B184,"")</f>
         <v>0</v>
       </c>
       <c r="E185">
-        <f>+IFERROR('Fallecidos Diarios'!C182,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C184,"")</f>
         <v>0</v>
       </c>
       <c r="F185">
@@ -27248,11 +27251,11 @@
         <v/>
       </c>
       <c r="D186">
-        <f>+IFERROR('Fallecidos Diarios'!B183,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B185,"")</f>
         <v>0</v>
       </c>
       <c r="E186">
-        <f>+IFERROR('Fallecidos Diarios'!C183,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C185,"")</f>
         <v>0</v>
       </c>
       <c r="F186">
@@ -27330,11 +27333,11 @@
         <v/>
       </c>
       <c r="D187">
-        <f>+IFERROR('Fallecidos Diarios'!B184,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B186,"")</f>
         <v>0</v>
       </c>
       <c r="E187">
-        <f>+IFERROR('Fallecidos Diarios'!C184,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C186,"")</f>
         <v>0</v>
       </c>
       <c r="F187">
@@ -27412,11 +27415,11 @@
         <v/>
       </c>
       <c r="D188">
-        <f>+IFERROR('Fallecidos Diarios'!B185,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B187,"")</f>
         <v>0</v>
       </c>
       <c r="E188">
-        <f>+IFERROR('Fallecidos Diarios'!C185,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C187,"")</f>
         <v>0</v>
       </c>
       <c r="F188">
@@ -27494,11 +27497,11 @@
         <v/>
       </c>
       <c r="D189">
-        <f>+IFERROR('Fallecidos Diarios'!B186,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B188,"")</f>
         <v>0</v>
       </c>
       <c r="E189">
-        <f>+IFERROR('Fallecidos Diarios'!C186,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C188,"")</f>
         <v>0</v>
       </c>
       <c r="F189">
@@ -27576,11 +27579,11 @@
         <v/>
       </c>
       <c r="D190">
-        <f>+IFERROR('Fallecidos Diarios'!B187,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B189,"")</f>
         <v>0</v>
       </c>
       <c r="E190">
-        <f>+IFERROR('Fallecidos Diarios'!C187,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C189,"")</f>
         <v>0</v>
       </c>
       <c r="F190">
@@ -27658,11 +27661,11 @@
         <v/>
       </c>
       <c r="D191">
-        <f>+IFERROR('Fallecidos Diarios'!B188,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B190,"")</f>
         <v>0</v>
       </c>
       <c r="E191">
-        <f>+IFERROR('Fallecidos Diarios'!C188,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C190,"")</f>
         <v>0</v>
       </c>
       <c r="F191">
@@ -27740,11 +27743,11 @@
         <v/>
       </c>
       <c r="D192">
-        <f>+IFERROR('Fallecidos Diarios'!B189,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B191,"")</f>
         <v>0</v>
       </c>
       <c r="E192">
-        <f>+IFERROR('Fallecidos Diarios'!C189,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C191,"")</f>
         <v>0</v>
       </c>
       <c r="F192">
@@ -27822,11 +27825,11 @@
         <v/>
       </c>
       <c r="D193">
-        <f>+IFERROR('Fallecidos Diarios'!B190,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B192,"")</f>
         <v>0</v>
       </c>
       <c r="E193">
-        <f>+IFERROR('Fallecidos Diarios'!C190,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C192,"")</f>
         <v>0</v>
       </c>
       <c r="F193">
@@ -27904,11 +27907,11 @@
         <v/>
       </c>
       <c r="D194">
-        <f>+IFERROR('Fallecidos Diarios'!B191,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B193,"")</f>
         <v>0</v>
       </c>
       <c r="E194">
-        <f>+IFERROR('Fallecidos Diarios'!C191,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C193,"")</f>
         <v>0</v>
       </c>
       <c r="F194">
@@ -27986,11 +27989,11 @@
         <v/>
       </c>
       <c r="D195">
-        <f>+IFERROR('Fallecidos Diarios'!B192,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B194,"")</f>
         <v>0</v>
       </c>
       <c r="E195">
-        <f>+IFERROR('Fallecidos Diarios'!C192,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C194,"")</f>
         <v>0</v>
       </c>
       <c r="F195">
@@ -28068,11 +28071,11 @@
         <v/>
       </c>
       <c r="D196">
-        <f>+IFERROR('Fallecidos Diarios'!B193,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B195,"")</f>
         <v>0</v>
       </c>
       <c r="E196">
-        <f>+IFERROR('Fallecidos Diarios'!C193,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C195,"")</f>
         <v>0</v>
       </c>
       <c r="F196">
@@ -28150,11 +28153,11 @@
         <v/>
       </c>
       <c r="D197">
-        <f>+IFERROR('Fallecidos Diarios'!B194,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B196,"")</f>
         <v>0</v>
       </c>
       <c r="E197">
-        <f>+IFERROR('Fallecidos Diarios'!C194,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C196,"")</f>
         <v>0</v>
       </c>
       <c r="F197">
@@ -28232,11 +28235,11 @@
         <v/>
       </c>
       <c r="D198">
-        <f>+IFERROR('Fallecidos Diarios'!B195,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B197,"")</f>
         <v>0</v>
       </c>
       <c r="E198">
-        <f>+IFERROR('Fallecidos Diarios'!C195,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C197,"")</f>
         <v>0</v>
       </c>
       <c r="F198">
@@ -28314,11 +28317,11 @@
         <v/>
       </c>
       <c r="D199">
-        <f>+IFERROR('Fallecidos Diarios'!B196,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B198,"")</f>
         <v>0</v>
       </c>
       <c r="E199">
-        <f>+IFERROR('Fallecidos Diarios'!C196,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C198,"")</f>
         <v>0</v>
       </c>
       <c r="F199">
@@ -28396,11 +28399,11 @@
         <v/>
       </c>
       <c r="D200">
-        <f>+IFERROR('Fallecidos Diarios'!B197,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B199,"")</f>
         <v>0</v>
       </c>
       <c r="E200">
-        <f>+IFERROR('Fallecidos Diarios'!C197,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C199,"")</f>
         <v>0</v>
       </c>
       <c r="F200">
@@ -28478,11 +28481,11 @@
         <v/>
       </c>
       <c r="D201">
-        <f>+IFERROR('Fallecidos Diarios'!B198,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B200,"")</f>
         <v>0</v>
       </c>
       <c r="E201">
-        <f>+IFERROR('Fallecidos Diarios'!C198,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C200,"")</f>
         <v>0</v>
       </c>
       <c r="F201">
@@ -28560,11 +28563,11 @@
         <v/>
       </c>
       <c r="D202">
-        <f>+IFERROR('Fallecidos Diarios'!B199,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B201,"")</f>
         <v>0</v>
       </c>
       <c r="E202">
-        <f>+IFERROR('Fallecidos Diarios'!C199,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C201,"")</f>
         <v>0</v>
       </c>
       <c r="F202">
@@ -28642,11 +28645,11 @@
         <v/>
       </c>
       <c r="D203">
-        <f>+IFERROR('Fallecidos Diarios'!B200,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B202,"")</f>
         <v>0</v>
       </c>
       <c r="E203">
-        <f>+IFERROR('Fallecidos Diarios'!C200,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C202,"")</f>
         <v>0</v>
       </c>
       <c r="F203">
@@ -28724,11 +28727,11 @@
         <v/>
       </c>
       <c r="D204">
-        <f>+IFERROR('Fallecidos Diarios'!B201,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B203,"")</f>
         <v>0</v>
       </c>
       <c r="E204">
-        <f>+IFERROR('Fallecidos Diarios'!C201,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C203,"")</f>
         <v>0</v>
       </c>
       <c r="F204">
@@ -28806,11 +28809,11 @@
         <v/>
       </c>
       <c r="D205">
-        <f>+IFERROR('Fallecidos Diarios'!B202,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B204,"")</f>
         <v>0</v>
       </c>
       <c r="E205">
-        <f>+IFERROR('Fallecidos Diarios'!C202,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C204,"")</f>
         <v>0</v>
       </c>
       <c r="F205">
@@ -28888,11 +28891,11 @@
         <v/>
       </c>
       <c r="D206">
-        <f>+IFERROR('Fallecidos Diarios'!B203,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B205,"")</f>
         <v>0</v>
       </c>
       <c r="E206">
-        <f>+IFERROR('Fallecidos Diarios'!C203,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C205,"")</f>
         <v>0</v>
       </c>
       <c r="F206">
@@ -28970,11 +28973,11 @@
         <v/>
       </c>
       <c r="D207">
-        <f>+IFERROR('Fallecidos Diarios'!B204,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B206,"")</f>
         <v>0</v>
       </c>
       <c r="E207">
-        <f>+IFERROR('Fallecidos Diarios'!C204,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C206,"")</f>
         <v>0</v>
       </c>
       <c r="F207">
@@ -29052,11 +29055,11 @@
         <v/>
       </c>
       <c r="D208">
-        <f>+IFERROR('Fallecidos Diarios'!B205,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B207,"")</f>
         <v>0</v>
       </c>
       <c r="E208">
-        <f>+IFERROR('Fallecidos Diarios'!C205,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C207,"")</f>
         <v>0</v>
       </c>
       <c r="F208">
@@ -29134,11 +29137,11 @@
         <v/>
       </c>
       <c r="D209">
-        <f>+IFERROR('Fallecidos Diarios'!B206,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B208,"")</f>
         <v>0</v>
       </c>
       <c r="E209">
-        <f>+IFERROR('Fallecidos Diarios'!C206,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C208,"")</f>
         <v>0</v>
       </c>
       <c r="F209">
@@ -29216,11 +29219,11 @@
         <v/>
       </c>
       <c r="D210">
-        <f>+IFERROR('Fallecidos Diarios'!B207,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B209,"")</f>
         <v>0</v>
       </c>
       <c r="E210">
-        <f>+IFERROR('Fallecidos Diarios'!C207,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C209,"")</f>
         <v>0</v>
       </c>
       <c r="F210">
@@ -29298,11 +29301,11 @@
         <v/>
       </c>
       <c r="D211">
-        <f>+IFERROR('Fallecidos Diarios'!B208,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B210,"")</f>
         <v>0</v>
       </c>
       <c r="E211">
-        <f>+IFERROR('Fallecidos Diarios'!C208,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C210,"")</f>
         <v>0</v>
       </c>
       <c r="F211">
@@ -29380,11 +29383,11 @@
         <v/>
       </c>
       <c r="D212">
-        <f>+IFERROR('Fallecidos Diarios'!B209,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B211,"")</f>
         <v>0</v>
       </c>
       <c r="E212">
-        <f>+IFERROR('Fallecidos Diarios'!C209,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C211,"")</f>
         <v>0</v>
       </c>
       <c r="F212">
@@ -29462,11 +29465,11 @@
         <v/>
       </c>
       <c r="D213">
-        <f>+IFERROR('Fallecidos Diarios'!B210,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B212,"")</f>
         <v>0</v>
       </c>
       <c r="E213">
-        <f>+IFERROR('Fallecidos Diarios'!C210,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C212,"")</f>
         <v>0</v>
       </c>
       <c r="F213">
@@ -29544,11 +29547,11 @@
         <v/>
       </c>
       <c r="D214">
-        <f>+IFERROR('Fallecidos Diarios'!B211,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B213,"")</f>
         <v>0</v>
       </c>
       <c r="E214">
-        <f>+IFERROR('Fallecidos Diarios'!C211,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C213,"")</f>
         <v>0</v>
       </c>
       <c r="F214">
@@ -29626,11 +29629,11 @@
         <v/>
       </c>
       <c r="D215">
-        <f>+IFERROR('Fallecidos Diarios'!B212,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B214,"")</f>
         <v>0</v>
       </c>
       <c r="E215">
-        <f>+IFERROR('Fallecidos Diarios'!C212,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C214,"")</f>
         <v>0</v>
       </c>
       <c r="F215">
@@ -29708,11 +29711,11 @@
         <v/>
       </c>
       <c r="D216">
-        <f>+IFERROR('Fallecidos Diarios'!B213,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B215,"")</f>
         <v>0</v>
       </c>
       <c r="E216">
-        <f>+IFERROR('Fallecidos Diarios'!C213,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C215,"")</f>
         <v>0</v>
       </c>
       <c r="F216">
@@ -29790,11 +29793,11 @@
         <v/>
       </c>
       <c r="D217">
-        <f>+IFERROR('Fallecidos Diarios'!B214,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B216,"")</f>
         <v>0</v>
       </c>
       <c r="E217">
-        <f>+IFERROR('Fallecidos Diarios'!C214,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C216,"")</f>
         <v>0</v>
       </c>
       <c r="F217">
@@ -29872,11 +29875,11 @@
         <v/>
       </c>
       <c r="D218">
-        <f>+IFERROR('Fallecidos Diarios'!B215,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B217,"")</f>
         <v>0</v>
       </c>
       <c r="E218">
-        <f>+IFERROR('Fallecidos Diarios'!C215,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C217,"")</f>
         <v>0</v>
       </c>
       <c r="F218">
@@ -29954,11 +29957,11 @@
         <v/>
       </c>
       <c r="D219">
-        <f>+IFERROR('Fallecidos Diarios'!B216,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B218,"")</f>
         <v>0</v>
       </c>
       <c r="E219">
-        <f>+IFERROR('Fallecidos Diarios'!C216,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C218,"")</f>
         <v>0</v>
       </c>
       <c r="F219">
@@ -30036,11 +30039,11 @@
         <v/>
       </c>
       <c r="D220">
-        <f>+IFERROR('Fallecidos Diarios'!B217,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B219,"")</f>
         <v>0</v>
       </c>
       <c r="E220">
-        <f>+IFERROR('Fallecidos Diarios'!C217,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C219,"")</f>
         <v>0</v>
       </c>
       <c r="F220">
@@ -30118,11 +30121,11 @@
         <v/>
       </c>
       <c r="D221">
-        <f>+IFERROR('Fallecidos Diarios'!B218,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B220,"")</f>
         <v>0</v>
       </c>
       <c r="E221">
-        <f>+IFERROR('Fallecidos Diarios'!C218,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C220,"")</f>
         <v>0</v>
       </c>
       <c r="F221">
@@ -30200,11 +30203,11 @@
         <v/>
       </c>
       <c r="D222">
-        <f>+IFERROR('Fallecidos Diarios'!B219,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B221,"")</f>
         <v>0</v>
       </c>
       <c r="E222">
-        <f>+IFERROR('Fallecidos Diarios'!C219,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C221,"")</f>
         <v>0</v>
       </c>
       <c r="F222">
@@ -30282,11 +30285,11 @@
         <v/>
       </c>
       <c r="D223">
-        <f>+IFERROR('Fallecidos Diarios'!B220,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B222,"")</f>
         <v>0</v>
       </c>
       <c r="E223">
-        <f>+IFERROR('Fallecidos Diarios'!C220,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C222,"")</f>
         <v>0</v>
       </c>
       <c r="F223">
@@ -30364,11 +30367,11 @@
         <v/>
       </c>
       <c r="D224">
-        <f>+IFERROR('Fallecidos Diarios'!B221,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B223,"")</f>
         <v>0</v>
       </c>
       <c r="E224">
-        <f>+IFERROR('Fallecidos Diarios'!C221,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C223,"")</f>
         <v>0</v>
       </c>
       <c r="F224">
@@ -30446,11 +30449,11 @@
         <v/>
       </c>
       <c r="D225">
-        <f>+IFERROR('Fallecidos Diarios'!B222,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B224,"")</f>
         <v>0</v>
       </c>
       <c r="E225">
-        <f>+IFERROR('Fallecidos Diarios'!C222,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C224,"")</f>
         <v>0</v>
       </c>
       <c r="F225">
@@ -30528,11 +30531,11 @@
         <v/>
       </c>
       <c r="D226">
-        <f>+IFERROR('Fallecidos Diarios'!B223,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B225,"")</f>
         <v>0</v>
       </c>
       <c r="E226">
-        <f>+IFERROR('Fallecidos Diarios'!C223,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C225,"")</f>
         <v>0</v>
       </c>
       <c r="F226">
@@ -30610,11 +30613,11 @@
         <v/>
       </c>
       <c r="D227">
-        <f>+IFERROR('Fallecidos Diarios'!B224,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B226,"")</f>
         <v>0</v>
       </c>
       <c r="E227">
-        <f>+IFERROR('Fallecidos Diarios'!C224,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C226,"")</f>
         <v>0</v>
       </c>
       <c r="F227">
@@ -30692,11 +30695,11 @@
         <v/>
       </c>
       <c r="D228">
-        <f>+IFERROR('Fallecidos Diarios'!B225,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B227,"")</f>
         <v>0</v>
       </c>
       <c r="E228">
-        <f>+IFERROR('Fallecidos Diarios'!C225,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C227,"")</f>
         <v>0</v>
       </c>
       <c r="F228">
@@ -30774,11 +30777,11 @@
         <v/>
       </c>
       <c r="D229">
-        <f>+IFERROR('Fallecidos Diarios'!B226,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B228,"")</f>
         <v>0</v>
       </c>
       <c r="E229">
-        <f>+IFERROR('Fallecidos Diarios'!C226,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C228,"")</f>
         <v>0</v>
       </c>
       <c r="F229">
@@ -30856,11 +30859,11 @@
         <v/>
       </c>
       <c r="D230">
-        <f>+IFERROR('Fallecidos Diarios'!B227,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B229,"")</f>
         <v>0</v>
       </c>
       <c r="E230">
-        <f>+IFERROR('Fallecidos Diarios'!C227,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C229,"")</f>
         <v>0</v>
       </c>
       <c r="F230">
@@ -30938,11 +30941,11 @@
         <v/>
       </c>
       <c r="D231">
-        <f>+IFERROR('Fallecidos Diarios'!B228,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B230,"")</f>
         <v>0</v>
       </c>
       <c r="E231">
-        <f>+IFERROR('Fallecidos Diarios'!C228,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C230,"")</f>
         <v>0</v>
       </c>
       <c r="F231">
@@ -31020,11 +31023,11 @@
         <v/>
       </c>
       <c r="D232">
-        <f>+IFERROR('Fallecidos Diarios'!B229,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B231,"")</f>
         <v>0</v>
       </c>
       <c r="E232">
-        <f>+IFERROR('Fallecidos Diarios'!C229,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C231,"")</f>
         <v>0</v>
       </c>
       <c r="F232">
@@ -31102,11 +31105,11 @@
         <v/>
       </c>
       <c r="D233">
-        <f>+IFERROR('Fallecidos Diarios'!B230,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B232,"")</f>
         <v>0</v>
       </c>
       <c r="E233">
-        <f>+IFERROR('Fallecidos Diarios'!C230,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C232,"")</f>
         <v>0</v>
       </c>
       <c r="F233">
@@ -31184,11 +31187,11 @@
         <v/>
       </c>
       <c r="D234">
-        <f>+IFERROR('Fallecidos Diarios'!B231,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B233,"")</f>
         <v>0</v>
       </c>
       <c r="E234">
-        <f>+IFERROR('Fallecidos Diarios'!C231,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C233,"")</f>
         <v>0</v>
       </c>
       <c r="F234">
@@ -31266,11 +31269,11 @@
         <v/>
       </c>
       <c r="D235">
-        <f>+IFERROR('Fallecidos Diarios'!B232,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B234,"")</f>
         <v>0</v>
       </c>
       <c r="E235">
-        <f>+IFERROR('Fallecidos Diarios'!C232,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C234,"")</f>
         <v>0</v>
       </c>
       <c r="F235">
@@ -31348,11 +31351,11 @@
         <v/>
       </c>
       <c r="D236">
-        <f>+IFERROR('Fallecidos Diarios'!B233,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B235,"")</f>
         <v>0</v>
       </c>
       <c r="E236">
-        <f>+IFERROR('Fallecidos Diarios'!C233,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C235,"")</f>
         <v>0</v>
       </c>
       <c r="F236">
@@ -31430,11 +31433,11 @@
         <v/>
       </c>
       <c r="D237">
-        <f>+IFERROR('Fallecidos Diarios'!B234,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B236,"")</f>
         <v>0</v>
       </c>
       <c r="E237">
-        <f>+IFERROR('Fallecidos Diarios'!C234,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C236,"")</f>
         <v>0</v>
       </c>
       <c r="F237">
@@ -31512,11 +31515,11 @@
         <v/>
       </c>
       <c r="D238">
-        <f>+IFERROR('Fallecidos Diarios'!B235,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B237,"")</f>
         <v>0</v>
       </c>
       <c r="E238">
-        <f>+IFERROR('Fallecidos Diarios'!C235,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C237,"")</f>
         <v>0</v>
       </c>
       <c r="F238">
@@ -31594,11 +31597,11 @@
         <v/>
       </c>
       <c r="D239">
-        <f>+IFERROR('Fallecidos Diarios'!B236,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B238,"")</f>
         <v>0</v>
       </c>
       <c r="E239">
-        <f>+IFERROR('Fallecidos Diarios'!C236,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C238,"")</f>
         <v>0</v>
       </c>
       <c r="F239">
@@ -31676,11 +31679,11 @@
         <v/>
       </c>
       <c r="D240">
-        <f>+IFERROR('Fallecidos Diarios'!B237,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B239,"")</f>
         <v>0</v>
       </c>
       <c r="E240">
-        <f>+IFERROR('Fallecidos Diarios'!C237,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C239,"")</f>
         <v>0</v>
       </c>
       <c r="F240">
@@ -31758,11 +31761,11 @@
         <v/>
       </c>
       <c r="D241">
-        <f>+IFERROR('Fallecidos Diarios'!B238,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B240,"")</f>
         <v>0</v>
       </c>
       <c r="E241">
-        <f>+IFERROR('Fallecidos Diarios'!C238,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C240,"")</f>
         <v>0</v>
       </c>
       <c r="F241">
@@ -31840,11 +31843,11 @@
         <v/>
       </c>
       <c r="D242">
-        <f>+IFERROR('Fallecidos Diarios'!B239,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B241,"")</f>
         <v>0</v>
       </c>
       <c r="E242">
-        <f>+IFERROR('Fallecidos Diarios'!C239,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C241,"")</f>
         <v>0</v>
       </c>
       <c r="F242">
@@ -31922,11 +31925,11 @@
         <v/>
       </c>
       <c r="D243">
-        <f>+IFERROR('Fallecidos Diarios'!B240,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B242,"")</f>
         <v>0</v>
       </c>
       <c r="E243">
-        <f>+IFERROR('Fallecidos Diarios'!C240,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C242,"")</f>
         <v>0</v>
       </c>
       <c r="F243">
@@ -32004,11 +32007,11 @@
         <v/>
       </c>
       <c r="D244">
-        <f>+IFERROR('Fallecidos Diarios'!B241,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B243,"")</f>
         <v>0</v>
       </c>
       <c r="E244">
-        <f>+IFERROR('Fallecidos Diarios'!C241,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C243,"")</f>
         <v>0</v>
       </c>
       <c r="F244">
@@ -32086,11 +32089,11 @@
         <v/>
       </c>
       <c r="D245">
-        <f>+IFERROR('Fallecidos Diarios'!B242,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B244,"")</f>
         <v>0</v>
       </c>
       <c r="E245">
-        <f>+IFERROR('Fallecidos Diarios'!C242,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C244,"")</f>
         <v>0</v>
       </c>
       <c r="F245">
@@ -32168,11 +32171,11 @@
         <v/>
       </c>
       <c r="D246">
-        <f>+IFERROR('Fallecidos Diarios'!B243,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B245,"")</f>
         <v>0</v>
       </c>
       <c r="E246">
-        <f>+IFERROR('Fallecidos Diarios'!C243,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C245,"")</f>
         <v>0</v>
       </c>
       <c r="F246">
@@ -32250,11 +32253,11 @@
         <v/>
       </c>
       <c r="D247">
-        <f>+IFERROR('Fallecidos Diarios'!B244,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B246,"")</f>
         <v>0</v>
       </c>
       <c r="E247">
-        <f>+IFERROR('Fallecidos Diarios'!C244,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C246,"")</f>
         <v>0</v>
       </c>
       <c r="F247">
@@ -32332,11 +32335,11 @@
         <v/>
       </c>
       <c r="D248">
-        <f>+IFERROR('Fallecidos Diarios'!B245,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B247,"")</f>
         <v>0</v>
       </c>
       <c r="E248">
-        <f>+IFERROR('Fallecidos Diarios'!C245,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C247,"")</f>
         <v>0</v>
       </c>
       <c r="F248">
@@ -32414,11 +32417,11 @@
         <v/>
       </c>
       <c r="D249">
-        <f>+IFERROR('Fallecidos Diarios'!B246,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B248,"")</f>
         <v>0</v>
       </c>
       <c r="E249">
-        <f>+IFERROR('Fallecidos Diarios'!C246,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C248,"")</f>
         <v>0</v>
       </c>
       <c r="F249">
@@ -32496,11 +32499,11 @@
         <v/>
       </c>
       <c r="D250">
-        <f>+IFERROR('Fallecidos Diarios'!B247,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B249,"")</f>
         <v>0</v>
       </c>
       <c r="E250">
-        <f>+IFERROR('Fallecidos Diarios'!C247,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C249,"")</f>
         <v>0</v>
       </c>
       <c r="F250">
@@ -32578,11 +32581,11 @@
         <v/>
       </c>
       <c r="D251">
-        <f>+IFERROR('Fallecidos Diarios'!B248,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B250,"")</f>
         <v>0</v>
       </c>
       <c r="E251">
-        <f>+IFERROR('Fallecidos Diarios'!C248,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C250,"")</f>
         <v>0</v>
       </c>
       <c r="F251">
@@ -32660,11 +32663,11 @@
         <v/>
       </c>
       <c r="D252">
-        <f>+IFERROR('Fallecidos Diarios'!B249,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B251,"")</f>
         <v>0</v>
       </c>
       <c r="E252">
-        <f>+IFERROR('Fallecidos Diarios'!C249,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C251,"")</f>
         <v>0</v>
       </c>
       <c r="F252">
@@ -32742,11 +32745,11 @@
         <v/>
       </c>
       <c r="D253">
-        <f>+IFERROR('Fallecidos Diarios'!B250,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B252,"")</f>
         <v>0</v>
       </c>
       <c r="E253">
-        <f>+IFERROR('Fallecidos Diarios'!C250,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C252,"")</f>
         <v>0</v>
       </c>
       <c r="F253">
@@ -32824,11 +32827,11 @@
         <v/>
       </c>
       <c r="D254">
-        <f>+IFERROR('Fallecidos Diarios'!B251,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B253,"")</f>
         <v>0</v>
       </c>
       <c r="E254">
-        <f>+IFERROR('Fallecidos Diarios'!C251,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C253,"")</f>
         <v>0</v>
       </c>
       <c r="F254">
@@ -32906,11 +32909,11 @@
         <v/>
       </c>
       <c r="D255">
-        <f>+IFERROR('Fallecidos Diarios'!B252,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B254,"")</f>
         <v>0</v>
       </c>
       <c r="E255">
-        <f>+IFERROR('Fallecidos Diarios'!C252,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C254,"")</f>
         <v>0</v>
       </c>
       <c r="F255">
@@ -32988,11 +32991,11 @@
         <v/>
       </c>
       <c r="D256">
-        <f>+IFERROR('Fallecidos Diarios'!B253,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B255,"")</f>
         <v>0</v>
       </c>
       <c r="E256">
-        <f>+IFERROR('Fallecidos Diarios'!C253,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C255,"")</f>
         <v>0</v>
       </c>
       <c r="F256">
@@ -33070,11 +33073,11 @@
         <v/>
       </c>
       <c r="D257">
-        <f>+IFERROR('Fallecidos Diarios'!B254,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B256,"")</f>
         <v>0</v>
       </c>
       <c r="E257">
-        <f>+IFERROR('Fallecidos Diarios'!C254,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C256,"")</f>
         <v>0</v>
       </c>
       <c r="F257">
@@ -33152,11 +33155,11 @@
         <v/>
       </c>
       <c r="D258">
-        <f>+IFERROR('Fallecidos Diarios'!B255,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B257,"")</f>
         <v>0</v>
       </c>
       <c r="E258">
-        <f>+IFERROR('Fallecidos Diarios'!C255,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C257,"")</f>
         <v>0</v>
       </c>
       <c r="F258">
@@ -33234,11 +33237,11 @@
         <v/>
       </c>
       <c r="D259">
-        <f>+IFERROR('Fallecidos Diarios'!B256,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B258,"")</f>
         <v>0</v>
       </c>
       <c r="E259">
-        <f>+IFERROR('Fallecidos Diarios'!C256,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C258,"")</f>
         <v>0</v>
       </c>
       <c r="F259">
@@ -33316,11 +33319,11 @@
         <v/>
       </c>
       <c r="D260">
-        <f>+IFERROR('Fallecidos Diarios'!B257,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B259,"")</f>
         <v>0</v>
       </c>
       <c r="E260">
-        <f>+IFERROR('Fallecidos Diarios'!C257,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C259,"")</f>
         <v>0</v>
       </c>
       <c r="F260">
@@ -33398,11 +33401,11 @@
         <v/>
       </c>
       <c r="D261">
-        <f>+IFERROR('Fallecidos Diarios'!B258,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B260,"")</f>
         <v>0</v>
       </c>
       <c r="E261">
-        <f>+IFERROR('Fallecidos Diarios'!C258,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C260,"")</f>
         <v>0</v>
       </c>
       <c r="F261">
@@ -33480,11 +33483,11 @@
         <v/>
       </c>
       <c r="D262">
-        <f>+IFERROR('Fallecidos Diarios'!B259,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B261,"")</f>
         <v>0</v>
       </c>
       <c r="E262">
-        <f>+IFERROR('Fallecidos Diarios'!C259,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C261,"")</f>
         <v>0</v>
       </c>
       <c r="F262">
@@ -33562,11 +33565,11 @@
         <v/>
       </c>
       <c r="D263">
-        <f>+IFERROR('Fallecidos Diarios'!B260,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B262,"")</f>
         <v>0</v>
       </c>
       <c r="E263">
-        <f>+IFERROR('Fallecidos Diarios'!C260,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C262,"")</f>
         <v>0</v>
       </c>
       <c r="F263">
@@ -33644,11 +33647,11 @@
         <v/>
       </c>
       <c r="D264">
-        <f>+IFERROR('Fallecidos Diarios'!B261,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B263,"")</f>
         <v>0</v>
       </c>
       <c r="E264">
-        <f>+IFERROR('Fallecidos Diarios'!C261,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C263,"")</f>
         <v>0</v>
       </c>
       <c r="F264">
@@ -33726,11 +33729,11 @@
         <v/>
       </c>
       <c r="D265">
-        <f>+IFERROR('Fallecidos Diarios'!B262,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B264,"")</f>
         <v>0</v>
       </c>
       <c r="E265">
-        <f>+IFERROR('Fallecidos Diarios'!C262,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C264,"")</f>
         <v>0</v>
       </c>
       <c r="F265">
@@ -33808,11 +33811,11 @@
         <v/>
       </c>
       <c r="D266">
-        <f>+IFERROR('Fallecidos Diarios'!B263,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B265,"")</f>
         <v>0</v>
       </c>
       <c r="E266">
-        <f>+IFERROR('Fallecidos Diarios'!C263,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C265,"")</f>
         <v>0</v>
       </c>
       <c r="F266">
@@ -33890,11 +33893,11 @@
         <v/>
       </c>
       <c r="D267">
-        <f>+IFERROR('Fallecidos Diarios'!B264,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B266,"")</f>
         <v>0</v>
       </c>
       <c r="E267">
-        <f>+IFERROR('Fallecidos Diarios'!C264,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C266,"")</f>
         <v>0</v>
       </c>
       <c r="F267">
@@ -33972,11 +33975,11 @@
         <v/>
       </c>
       <c r="D268">
-        <f>+IFERROR('Fallecidos Diarios'!B265,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B267,"")</f>
         <v>0</v>
       </c>
       <c r="E268">
-        <f>+IFERROR('Fallecidos Diarios'!C265,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C267,"")</f>
         <v>0</v>
       </c>
       <c r="F268">
@@ -34054,11 +34057,11 @@
         <v/>
       </c>
       <c r="D269">
-        <f>+IFERROR('Fallecidos Diarios'!B266,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B268,"")</f>
         <v>0</v>
       </c>
       <c r="E269">
-        <f>+IFERROR('Fallecidos Diarios'!C266,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C268,"")</f>
         <v>0</v>
       </c>
       <c r="F269">
@@ -34136,11 +34139,11 @@
         <v/>
       </c>
       <c r="D270">
-        <f>+IFERROR('Fallecidos Diarios'!B267,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B269,"")</f>
         <v>0</v>
       </c>
       <c r="E270">
-        <f>+IFERROR('Fallecidos Diarios'!C267,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C269,"")</f>
         <v>0</v>
       </c>
       <c r="F270">
@@ -34218,11 +34221,11 @@
         <v/>
       </c>
       <c r="D271">
-        <f>+IFERROR('Fallecidos Diarios'!B268,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B270,"")</f>
         <v>0</v>
       </c>
       <c r="E271">
-        <f>+IFERROR('Fallecidos Diarios'!C268,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C270,"")</f>
         <v>0</v>
       </c>
       <c r="F271">
@@ -34300,11 +34303,11 @@
         <v/>
       </c>
       <c r="D272">
-        <f>+IFERROR('Fallecidos Diarios'!B269,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B271,"")</f>
         <v>0</v>
       </c>
       <c r="E272">
-        <f>+IFERROR('Fallecidos Diarios'!C269,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C271,"")</f>
         <v>0</v>
       </c>
       <c r="F272">
@@ -34382,11 +34385,11 @@
         <v/>
       </c>
       <c r="D273">
-        <f>+IFERROR('Fallecidos Diarios'!B270,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B272,"")</f>
         <v>0</v>
       </c>
       <c r="E273">
-        <f>+IFERROR('Fallecidos Diarios'!C270,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C272,"")</f>
         <v>0</v>
       </c>
       <c r="F273">
@@ -34464,11 +34467,11 @@
         <v/>
       </c>
       <c r="D274">
-        <f>+IFERROR('Fallecidos Diarios'!B271,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B273,"")</f>
         <v>0</v>
       </c>
       <c r="E274">
-        <f>+IFERROR('Fallecidos Diarios'!C271,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C273,"")</f>
         <v>0</v>
       </c>
       <c r="F274">
@@ -34546,11 +34549,11 @@
         <v/>
       </c>
       <c r="D275">
-        <f>+IFERROR('Fallecidos Diarios'!B272,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B274,"")</f>
         <v>0</v>
       </c>
       <c r="E275">
-        <f>+IFERROR('Fallecidos Diarios'!C272,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C274,"")</f>
         <v>0</v>
       </c>
       <c r="F275">
@@ -34628,11 +34631,11 @@
         <v/>
       </c>
       <c r="D276">
-        <f>+IFERROR('Fallecidos Diarios'!B273,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B275,"")</f>
         <v>0</v>
       </c>
       <c r="E276">
-        <f>+IFERROR('Fallecidos Diarios'!C273,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C275,"")</f>
         <v>0</v>
       </c>
       <c r="F276">
@@ -34710,11 +34713,11 @@
         <v/>
       </c>
       <c r="D277">
-        <f>+IFERROR('Fallecidos Diarios'!B274,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!B276,"")</f>
         <v>0</v>
       </c>
       <c r="E277">
-        <f>+IFERROR('Fallecidos Diarios'!C274,"")</f>
+        <f>+IFERROR('Fallecidos Diarios'!C276,"")</f>
         <v>0</v>
       </c>
       <c r="F277">

</xml_diff>

<commit_message>
Update automatico via Actualizar 08-04-2020 14-52-50
</commit_message>
<xml_diff>
--- a/datacovidpa/Casos PN Diarios.xlsx
+++ b/datacovidpa/Casos PN Diarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID PN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2202" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{ADBA0678-B85F-4483-8DF0-53CD4E7E3E50}"/>
+  <xr:revisionPtr revIDLastSave="2203" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F500BE8A-EB3C-4769-803F-1CCFF8C19C93}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4D4203-BE53-4B99-8CE3-A4DA4C5B1D6B}">
   <dimension ref="A1:BC148"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -4333,7 +4333,7 @@
   <dimension ref="A1:E148"/>
   <sheetViews>
     <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+      <selection activeCell="C1" sqref="C1:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -6192,8 +6192,8 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -12078,8 +12078,8 @@
   </sheetPr>
   <dimension ref="A1:T277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -13085,7 +13085,7 @@
         <v>198</v>
       </c>
       <c r="I13">
-        <f t="shared" si="12"/>
+        <f>+IFERROR(H13-H12,"")</f>
         <v>63</v>
       </c>
       <c r="J13">

</xml_diff>